<commit_message>
14sps for proto1 and averaged per 1sec (for my dad)
</commit_message>
<xml_diff>
--- a/BillOfMaterials/INVENTORY.xlsx
+++ b/BillOfMaterials/INVENTORY.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="INVENTORY" sheetId="1" r:id="rId1"/>
@@ -2328,11 +2328,20 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2340,9 +2349,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2357,12 +2363,6 @@
     </xf>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2884,9 +2884,9 @@
   </sheetPr>
   <dimension ref="A1:AB176"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G76" sqref="G76"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q48" sqref="Q48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2973,7 +2973,7 @@
       <c r="L3" s="35"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C4" s="203">
+      <c r="C4" s="204">
         <v>42882</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -2988,14 +2988,14 @@
       <c r="G4" s="27">
         <v>6.99</v>
       </c>
-      <c r="H4" s="204">
+      <c r="H4" s="207">
         <f>SUM(G4:G10)</f>
         <v>48.1</v>
       </c>
-      <c r="I4" s="202">
+      <c r="I4" s="205">
         <v>0</v>
       </c>
-      <c r="J4" s="204">
+      <c r="J4" s="207">
         <f>H4+I4</f>
         <v>48.1</v>
       </c>
@@ -3007,7 +3007,7 @@
       <c r="M4" s="206"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C5" s="203"/>
+      <c r="C5" s="204"/>
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
@@ -3020,9 +3020,9 @@
       <c r="G5" s="27">
         <v>6.99</v>
       </c>
-      <c r="H5" s="205"/>
-      <c r="I5" s="202"/>
-      <c r="J5" s="205"/>
+      <c r="H5" s="208"/>
+      <c r="I5" s="205"/>
+      <c r="J5" s="208"/>
       <c r="K5" s="206">
         <f t="shared" ref="K5:K10" si="0">G5/E5</f>
         <v>6.99</v>
@@ -3031,7 +3031,7 @@
       <c r="M5" s="206"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C6" s="203"/>
+      <c r="C6" s="204"/>
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
@@ -3044,9 +3044,9 @@
       <c r="G6" s="27">
         <v>4.97</v>
       </c>
-      <c r="H6" s="205"/>
-      <c r="I6" s="202"/>
-      <c r="J6" s="205"/>
+      <c r="H6" s="208"/>
+      <c r="I6" s="205"/>
+      <c r="J6" s="208"/>
       <c r="K6" s="206">
         <f t="shared" si="0"/>
         <v>0.2485</v>
@@ -3055,7 +3055,7 @@
       <c r="M6" s="206"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C7" s="203"/>
+      <c r="C7" s="204"/>
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
@@ -3068,9 +3068,9 @@
       <c r="G7" s="27">
         <v>5.99</v>
       </c>
-      <c r="H7" s="205"/>
-      <c r="I7" s="202"/>
-      <c r="J7" s="205"/>
+      <c r="H7" s="208"/>
+      <c r="I7" s="205"/>
+      <c r="J7" s="208"/>
       <c r="K7" s="206">
         <f t="shared" si="0"/>
         <v>0.29949999999999999</v>
@@ -3079,7 +3079,7 @@
       <c r="M7" s="206"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C8" s="203"/>
+      <c r="C8" s="204"/>
       <c r="D8" s="1" t="s">
         <v>155</v>
       </c>
@@ -3092,9 +3092,9 @@
       <c r="G8" s="27">
         <v>6.25</v>
       </c>
-      <c r="H8" s="205"/>
-      <c r="I8" s="202"/>
-      <c r="J8" s="205"/>
+      <c r="H8" s="208"/>
+      <c r="I8" s="205"/>
+      <c r="J8" s="208"/>
       <c r="K8" s="206">
         <f t="shared" si="0"/>
         <v>6.25</v>
@@ -3103,7 +3103,7 @@
       <c r="M8" s="206"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C9" s="203"/>
+      <c r="C9" s="204"/>
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3116,9 +3116,9 @@
       <c r="G9" s="27">
         <v>11.59</v>
       </c>
-      <c r="H9" s="205"/>
-      <c r="I9" s="202"/>
-      <c r="J9" s="205"/>
+      <c r="H9" s="208"/>
+      <c r="I9" s="205"/>
+      <c r="J9" s="208"/>
       <c r="K9" s="206">
         <f t="shared" si="0"/>
         <v>0.57950000000000002</v>
@@ -3127,7 +3127,7 @@
       <c r="M9" s="206"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C10" s="203"/>
+      <c r="C10" s="204"/>
       <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
@@ -3140,9 +3140,9 @@
       <c r="G10" s="27">
         <v>5.32</v>
       </c>
-      <c r="H10" s="205"/>
-      <c r="I10" s="202"/>
-      <c r="J10" s="205"/>
+      <c r="H10" s="208"/>
+      <c r="I10" s="205"/>
+      <c r="J10" s="208"/>
       <c r="K10" s="206">
         <f t="shared" si="0"/>
         <v>1.0640000000000001</v>
@@ -3255,14 +3255,14 @@
       <c r="G16" s="27">
         <v>6.56</v>
       </c>
-      <c r="H16" s="204">
+      <c r="H16" s="207">
         <f>SUM(G16:G17)</f>
         <v>7.55</v>
       </c>
-      <c r="I16" s="202">
+      <c r="I16" s="205">
         <v>0</v>
       </c>
-      <c r="J16" s="204">
+      <c r="J16" s="207">
         <f>H16+I16</f>
         <v>7.55</v>
       </c>
@@ -3283,9 +3283,9 @@
       <c r="G17" s="27">
         <v>0.99</v>
       </c>
-      <c r="H17" s="204"/>
-      <c r="I17" s="202"/>
-      <c r="J17" s="204"/>
+      <c r="H17" s="207"/>
+      <c r="I17" s="205"/>
+      <c r="J17" s="207"/>
     </row>
     <row r="18" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
@@ -3337,7 +3337,7 @@
       <c r="L20" s="35"/>
     </row>
     <row r="21" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C21" s="203">
+      <c r="C21" s="204">
         <v>42925</v>
       </c>
       <c r="D21" s="149" t="s">
@@ -3352,20 +3352,20 @@
       <c r="G21" s="27">
         <v>2.56</v>
       </c>
-      <c r="H21" s="204">
+      <c r="H21" s="207">
         <f>SUM(G21:G25)</f>
         <v>17.230000000000004</v>
       </c>
-      <c r="I21" s="202">
+      <c r="I21" s="205">
         <v>5.65</v>
       </c>
-      <c r="J21" s="204">
+      <c r="J21" s="207">
         <f>H21+I21</f>
         <v>22.880000000000003</v>
       </c>
     </row>
     <row r="22" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C22" s="203"/>
+      <c r="C22" s="204"/>
       <c r="D22" s="149" t="s">
         <v>21</v>
       </c>
@@ -3378,12 +3378,12 @@
       <c r="G22" s="27">
         <v>1.8</v>
       </c>
-      <c r="H22" s="205"/>
-      <c r="I22" s="202"/>
-      <c r="J22" s="205"/>
+      <c r="H22" s="208"/>
+      <c r="I22" s="205"/>
+      <c r="J22" s="208"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C23" s="203"/>
+      <c r="C23" s="204"/>
       <c r="D23" s="1" t="s">
         <v>20</v>
       </c>
@@ -3396,12 +3396,12 @@
       <c r="G23" s="27">
         <v>3.99</v>
       </c>
-      <c r="H23" s="205"/>
-      <c r="I23" s="202"/>
-      <c r="J23" s="205"/>
+      <c r="H23" s="208"/>
+      <c r="I23" s="205"/>
+      <c r="J23" s="208"/>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C24" s="203"/>
+      <c r="C24" s="204"/>
       <c r="D24" s="149" t="s">
         <v>13</v>
       </c>
@@ -3414,12 +3414,12 @@
       <c r="G24" s="27">
         <v>1.97</v>
       </c>
-      <c r="H24" s="205"/>
-      <c r="I24" s="202"/>
-      <c r="J24" s="205"/>
+      <c r="H24" s="208"/>
+      <c r="I24" s="205"/>
+      <c r="J24" s="208"/>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C25" s="203"/>
+      <c r="C25" s="204"/>
       <c r="D25" s="1" t="s">
         <v>2</v>
       </c>
@@ -3432,9 +3432,9 @@
       <c r="G25" s="27">
         <v>6.91</v>
       </c>
-      <c r="H25" s="205"/>
-      <c r="I25" s="202"/>
-      <c r="J25" s="205"/>
+      <c r="H25" s="208"/>
+      <c r="I25" s="205"/>
+      <c r="J25" s="208"/>
     </row>
     <row r="26" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
@@ -3448,7 +3448,7 @@
       <c r="L26" s="35"/>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C27" s="203">
+      <c r="C27" s="204">
         <v>42927</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -3463,20 +3463,20 @@
       <c r="G27" s="27">
         <v>0.75</v>
       </c>
-      <c r="H27" s="204">
+      <c r="H27" s="207">
         <f>SUM(G27:G29)</f>
         <v>3.44</v>
       </c>
-      <c r="I27" s="202">
+      <c r="I27" s="205">
         <v>4.99</v>
       </c>
-      <c r="J27" s="204">
+      <c r="J27" s="207">
         <f>H27+I27</f>
         <v>8.43</v>
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C28" s="203"/>
+      <c r="C28" s="204"/>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
@@ -3489,12 +3489,12 @@
       <c r="G28" s="27">
         <v>0.75</v>
       </c>
-      <c r="H28" s="205"/>
-      <c r="I28" s="202"/>
-      <c r="J28" s="205"/>
+      <c r="H28" s="208"/>
+      <c r="I28" s="205"/>
+      <c r="J28" s="208"/>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C29" s="203"/>
+      <c r="C29" s="204"/>
       <c r="D29" s="1" t="s">
         <v>154</v>
       </c>
@@ -3507,9 +3507,9 @@
       <c r="G29" s="27">
         <v>1.94</v>
       </c>
-      <c r="H29" s="205"/>
-      <c r="I29" s="202"/>
-      <c r="J29" s="205"/>
+      <c r="H29" s="208"/>
+      <c r="I29" s="205"/>
+      <c r="J29" s="208"/>
     </row>
     <row r="30" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="7"/>
@@ -3561,7 +3561,7 @@
       <c r="L32" s="35"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C33" s="203">
+      <c r="C33" s="204">
         <v>42929</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -3576,20 +3576,20 @@
       <c r="G33" s="27">
         <v>0.77</v>
       </c>
-      <c r="H33" s="204">
+      <c r="H33" s="207">
         <f>SUM(G33:G34)</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="I33" s="202">
+      <c r="I33" s="205">
         <v>3.39</v>
       </c>
-      <c r="J33" s="202">
+      <c r="J33" s="205">
         <f>SUM(H33:I34)</f>
         <v>5.6899999999999995</v>
       </c>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C34" s="203"/>
+      <c r="C34" s="204"/>
       <c r="D34" s="1" t="s">
         <v>76</v>
       </c>
@@ -3602,9 +3602,9 @@
       <c r="G34" s="27">
         <v>1.53</v>
       </c>
-      <c r="H34" s="205"/>
-      <c r="I34" s="202"/>
-      <c r="J34" s="202"/>
+      <c r="H34" s="208"/>
+      <c r="I34" s="205"/>
+      <c r="J34" s="205"/>
     </row>
     <row r="35" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="7"/>
@@ -3656,7 +3656,7 @@
       <c r="L37" s="35"/>
     </row>
     <row r="38" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C38" s="203">
+      <c r="C38" s="204">
         <v>42931</v>
       </c>
       <c r="D38" s="149" t="s">
@@ -3671,20 +3671,20 @@
       <c r="G38" s="27">
         <v>5.72</v>
       </c>
-      <c r="H38" s="202">
+      <c r="H38" s="205">
         <f>SUM(G38:G39)</f>
         <v>8.5500000000000007</v>
       </c>
-      <c r="I38" s="202">
+      <c r="I38" s="205">
         <v>4.99</v>
       </c>
-      <c r="J38" s="202">
+      <c r="J38" s="205">
         <f>SUM(H38:I39)</f>
         <v>13.540000000000001</v>
       </c>
     </row>
     <row r="39" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C39" s="203"/>
+      <c r="C39" s="204"/>
       <c r="D39" s="149" t="s">
         <v>122</v>
       </c>
@@ -3697,9 +3697,9 @@
       <c r="G39" s="27">
         <v>2.83</v>
       </c>
-      <c r="H39" s="202"/>
-      <c r="I39" s="202"/>
-      <c r="J39" s="202"/>
+      <c r="H39" s="205"/>
+      <c r="I39" s="205"/>
+      <c r="J39" s="205"/>
     </row>
     <row r="40" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="7"/>
@@ -3713,7 +3713,7 @@
       <c r="L40" s="35"/>
     </row>
     <row r="41" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C41" s="203">
+      <c r="C41" s="204">
         <v>42936</v>
       </c>
       <c r="D41" s="149" t="s">
@@ -3728,20 +3728,20 @@
       <c r="G41" s="27">
         <v>10.58</v>
       </c>
-      <c r="H41" s="202">
+      <c r="H41" s="205">
         <f>SUM(G41:G45)</f>
         <v>18.649999999999999</v>
       </c>
-      <c r="I41" s="202">
+      <c r="I41" s="205">
         <v>0.25</v>
       </c>
-      <c r="J41" s="202">
+      <c r="J41" s="205">
         <f>H41+I41</f>
         <v>18.899999999999999</v>
       </c>
     </row>
     <row r="42" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C42" s="203"/>
+      <c r="C42" s="204"/>
       <c r="D42" s="149" t="s">
         <v>150</v>
       </c>
@@ -3754,12 +3754,12 @@
       <c r="G42" s="27">
         <v>3.86</v>
       </c>
-      <c r="H42" s="202"/>
-      <c r="I42" s="202"/>
-      <c r="J42" s="202"/>
+      <c r="H42" s="205"/>
+      <c r="I42" s="205"/>
+      <c r="J42" s="205"/>
     </row>
     <row r="43" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C43" s="203"/>
+      <c r="C43" s="204"/>
       <c r="D43" s="149" t="s">
         <v>151</v>
       </c>
@@ -3773,12 +3773,12 @@
         <f>1.99-0.1</f>
         <v>1.89</v>
       </c>
-      <c r="H43" s="202"/>
-      <c r="I43" s="202"/>
-      <c r="J43" s="202"/>
+      <c r="H43" s="205"/>
+      <c r="I43" s="205"/>
+      <c r="J43" s="205"/>
     </row>
     <row r="44" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C44" s="203"/>
+      <c r="C44" s="204"/>
       <c r="D44" s="149" t="s">
         <v>152</v>
       </c>
@@ -3792,12 +3792,12 @@
         <f>0.99-0.05</f>
         <v>0.94</v>
       </c>
-      <c r="H44" s="202"/>
-      <c r="I44" s="202"/>
-      <c r="J44" s="202"/>
+      <c r="H44" s="205"/>
+      <c r="I44" s="205"/>
+      <c r="J44" s="205"/>
     </row>
     <row r="45" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C45" s="203"/>
+      <c r="C45" s="204"/>
       <c r="D45" s="149" t="s">
         <v>153</v>
       </c>
@@ -3811,9 +3811,9 @@
         <f>1.45-0.07</f>
         <v>1.38</v>
       </c>
-      <c r="H45" s="202"/>
-      <c r="I45" s="202"/>
-      <c r="J45" s="202"/>
+      <c r="H45" s="205"/>
+      <c r="I45" s="205"/>
+      <c r="J45" s="205"/>
     </row>
     <row r="46" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="51"/>
@@ -3830,7 +3830,7 @@
       <c r="C47" s="191">
         <v>42985</v>
       </c>
-      <c r="D47" s="212" t="s">
+      <c r="D47" s="202" t="s">
         <v>219</v>
       </c>
       <c r="E47" s="26">
@@ -3867,7 +3867,7 @@
       <c r="C49" s="200">
         <v>42986</v>
       </c>
-      <c r="D49" s="212" t="s">
+      <c r="D49" s="202" t="s">
         <v>220</v>
       </c>
       <c r="E49" s="26">
@@ -3902,10 +3902,10 @@
       <c r="L50" s="57"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C51" s="203">
+      <c r="C51" s="204">
         <v>42986</v>
       </c>
-      <c r="D51" s="212" t="s">
+      <c r="D51" s="202" t="s">
         <v>221</v>
       </c>
       <c r="E51" s="26">
@@ -3917,21 +3917,21 @@
       <c r="G51" s="27">
         <v>29.95</v>
       </c>
-      <c r="H51" s="202">
-        <f>G51+G52+G53</f>
-        <v>32.25</v>
-      </c>
-      <c r="I51" s="202">
-        <v>3.39</v>
-      </c>
-      <c r="J51" s="202">
+      <c r="H51" s="205">
+        <f>G51+G52+G53+2.13</f>
+        <v>34.380000000000003</v>
+      </c>
+      <c r="I51" s="205">
+        <v>3.03</v>
+      </c>
+      <c r="J51" s="205">
         <f>H51+I51</f>
-        <v>35.64</v>
+        <v>37.410000000000004</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C52" s="203"/>
-      <c r="D52" s="212" t="s">
+      <c r="C52" s="204"/>
+      <c r="D52" s="202" t="s">
         <v>222</v>
       </c>
       <c r="E52" s="26">
@@ -3943,13 +3943,13 @@
       <c r="G52" s="27">
         <v>0.77</v>
       </c>
-      <c r="H52" s="202"/>
-      <c r="I52" s="202"/>
-      <c r="J52" s="202"/>
+      <c r="H52" s="205"/>
+      <c r="I52" s="205"/>
+      <c r="J52" s="205"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C53" s="203"/>
-      <c r="D53" s="212" t="s">
+      <c r="C53" s="204"/>
+      <c r="D53" s="202" t="s">
         <v>223</v>
       </c>
       <c r="E53" s="26">
@@ -3961,9 +3961,9 @@
       <c r="G53" s="27">
         <v>1.53</v>
       </c>
-      <c r="H53" s="202"/>
-      <c r="I53" s="202"/>
-      <c r="J53" s="202"/>
+      <c r="H53" s="205"/>
+      <c r="I53" s="205"/>
+      <c r="J53" s="205"/>
     </row>
     <row r="54" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="7"/>
@@ -3982,7 +3982,7 @@
       </c>
       <c r="C55" s="41">
         <f ca="1">TODAY()</f>
-        <v>42986</v>
+        <v>42989</v>
       </c>
       <c r="E55" s="29"/>
       <c r="F55" s="29"/>
@@ -3993,14 +3993,14 @@
       </c>
       <c r="J55" s="30">
         <f>SUM(J4:J54)</f>
-        <v>246.49</v>
+        <v>248.26</v>
       </c>
       <c r="K55" s="24" t="s">
         <v>24</v>
       </c>
       <c r="L55" s="39">
         <f ca="1">(C55-C4)*0.0328767</f>
-        <v>3.4191768000000002</v>
+        <v>3.5178069000000001</v>
       </c>
       <c r="M55" s="24" t="s">
         <v>25</v>
@@ -4018,7 +4018,7 @@
       </c>
       <c r="J56" s="22">
         <f ca="1">J55/L55</f>
-        <v>72.090451713406566</v>
+        <v>70.572378489564045</v>
       </c>
       <c r="K56" s="32" t="s">
         <v>27</v>
@@ -4051,7 +4051,7 @@
       <c r="D58" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="E58" s="213" t="s">
+      <c r="E58" s="203" t="s">
         <v>227</v>
       </c>
       <c r="H58" s="10"/>
@@ -5451,6 +5451,28 @@
     <sortCondition ref="C4:C19"/>
   </sortState>
   <mergeCells count="38">
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="C4:C10"/>
+    <mergeCell ref="J4:J10"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="H4:H10"/>
+    <mergeCell ref="I4:I10"/>
+    <mergeCell ref="J21:J25"/>
+    <mergeCell ref="H21:H25"/>
+    <mergeCell ref="H27:H29"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="I21:I25"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="J27:J29"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="H33:H34"/>
     <mergeCell ref="C51:C53"/>
     <mergeCell ref="H51:H53"/>
     <mergeCell ref="I51:I53"/>
@@ -5467,28 +5489,6 @@
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="K10:M10"/>
     <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="J27:J29"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="C4:C10"/>
-    <mergeCell ref="J4:J10"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="H4:H10"/>
-    <mergeCell ref="I4:I10"/>
-    <mergeCell ref="J21:J25"/>
-    <mergeCell ref="H21:H25"/>
-    <mergeCell ref="H27:H29"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="I21:I25"/>
-    <mergeCell ref="H16:H17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6396,21 +6396,21 @@
       <c r="AB16" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="AN16" s="207" t="s">
+      <c r="AN16" s="209" t="s">
         <v>123</v>
       </c>
-      <c r="AO16" s="207"/>
-      <c r="AP16" s="207"/>
-      <c r="AQ16" s="207"/>
-      <c r="AT16" s="205" t="s">
+      <c r="AO16" s="209"/>
+      <c r="AP16" s="209"/>
+      <c r="AQ16" s="209"/>
+      <c r="AT16" s="208" t="s">
         <v>119</v>
       </c>
-      <c r="AU16" s="205"/>
-      <c r="AV16" s="205"/>
-      <c r="AW16" s="205"/>
-      <c r="AX16" s="205"/>
-      <c r="AY16" s="205"/>
-      <c r="AZ16" s="205"/>
+      <c r="AU16" s="208"/>
+      <c r="AV16" s="208"/>
+      <c r="AW16" s="208"/>
+      <c r="AX16" s="208"/>
+      <c r="AY16" s="208"/>
+      <c r="AZ16" s="208"/>
     </row>
     <row r="17" spans="25:59" x14ac:dyDescent="0.25">
       <c r="Y17" s="108" t="s">
@@ -6425,15 +6425,15 @@
       <c r="AB17" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="AJ17" s="205" t="s">
+      <c r="AJ17" s="208" t="s">
         <v>117</v>
       </c>
-      <c r="AK17" s="205"/>
-      <c r="AL17" s="205"/>
-      <c r="AN17" s="207"/>
-      <c r="AO17" s="207"/>
-      <c r="AP17" s="207"/>
-      <c r="AQ17" s="207"/>
+      <c r="AK17" s="208"/>
+      <c r="AL17" s="208"/>
+      <c r="AN17" s="209"/>
+      <c r="AO17" s="209"/>
+      <c r="AP17" s="209"/>
+      <c r="AQ17" s="209"/>
     </row>
     <row r="19" spans="25:59" x14ac:dyDescent="0.25">
       <c r="AP19" s="195" t="s">
@@ -6448,11 +6448,11 @@
       </c>
     </row>
     <row r="20" spans="25:59" x14ac:dyDescent="0.25">
-      <c r="AK20" s="208" t="s">
+      <c r="AK20" s="210" t="s">
         <v>120</v>
       </c>
-      <c r="AL20" s="208"/>
-      <c r="AM20" s="208"/>
+      <c r="AL20" s="210"/>
+      <c r="AM20" s="210"/>
       <c r="AP20" s="195" t="s">
         <v>217</v>
       </c>
@@ -6484,7 +6484,7 @@
   </sheetPr>
   <dimension ref="B1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -6747,7 +6747,7 @@
         <f t="shared" si="1"/>
         <v>6.6300000000000008</v>
       </c>
-      <c r="H11" s="209">
+      <c r="H11" s="211">
         <v>3.39</v>
       </c>
       <c r="I11" s="172" t="s">
@@ -6777,7 +6777,7 @@
         <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
-      <c r="H12" s="209"/>
+      <c r="H12" s="211"/>
       <c r="I12" s="172" t="s">
         <v>186</v>
       </c>
@@ -6833,7 +6833,7 @@
         <f t="shared" si="1"/>
         <v>57.199999999999996</v>
       </c>
-      <c r="H14" s="210">
+      <c r="H14" s="212">
         <v>4.99</v>
       </c>
       <c r="I14" s="172" t="s">
@@ -6862,7 +6862,7 @@
         <f t="shared" si="1"/>
         <v>28.3</v>
       </c>
-      <c r="H15" s="211"/>
+      <c r="H15" s="213"/>
       <c r="I15" s="182" t="s">
         <v>228</v>
       </c>

</xml_diff>

<commit_message>
Purchased flyskyhy on my wife's phone
</commit_message>
<xml_diff>
--- a/BillOfMaterials/INVENTORY.xlsx
+++ b/BillOfMaterials/INVENTORY.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="230">
   <si>
     <t>Arduino Nano</t>
   </si>
@@ -1315,6 +1315,9 @@
   </si>
   <si>
     <t>TODO -- FIND A CHEAPER ALTERNATIVE</t>
+  </si>
+  <si>
+    <t>FLYSKYHY IOS APP</t>
   </si>
 </sst>
 </file>
@@ -1879,7 +1882,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="214">
+  <cellXfs count="216">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2340,14 +2343,20 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2882,11 +2891,11 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:AB176"/>
+  <dimension ref="A1:AB178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q48" sqref="Q48"/>
+      <selection pane="bottomLeft" activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2973,7 +2982,7 @@
       <c r="L3" s="35"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C4" s="204">
+      <c r="C4" s="206">
         <v>42882</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -2988,26 +2997,26 @@
       <c r="G4" s="27">
         <v>6.99</v>
       </c>
-      <c r="H4" s="207">
+      <c r="H4" s="208">
         <f>SUM(G4:G10)</f>
         <v>48.1</v>
       </c>
-      <c r="I4" s="205">
+      <c r="I4" s="207">
         <v>0</v>
       </c>
-      <c r="J4" s="207">
+      <c r="J4" s="208">
         <f>H4+I4</f>
         <v>48.1</v>
       </c>
-      <c r="K4" s="206">
+      <c r="K4" s="210">
         <f>G4/E4</f>
         <v>6.99</v>
       </c>
-      <c r="L4" s="206"/>
-      <c r="M4" s="206"/>
+      <c r="L4" s="210"/>
+      <c r="M4" s="210"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C5" s="204"/>
+      <c r="C5" s="206"/>
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
@@ -3020,18 +3029,18 @@
       <c r="G5" s="27">
         <v>6.99</v>
       </c>
-      <c r="H5" s="208"/>
-      <c r="I5" s="205"/>
-      <c r="J5" s="208"/>
-      <c r="K5" s="206">
+      <c r="H5" s="209"/>
+      <c r="I5" s="207"/>
+      <c r="J5" s="209"/>
+      <c r="K5" s="210">
         <f t="shared" ref="K5:K10" si="0">G5/E5</f>
         <v>6.99</v>
       </c>
-      <c r="L5" s="206"/>
-      <c r="M5" s="206"/>
+      <c r="L5" s="210"/>
+      <c r="M5" s="210"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C6" s="204"/>
+      <c r="C6" s="206"/>
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
@@ -3044,18 +3053,18 @@
       <c r="G6" s="27">
         <v>4.97</v>
       </c>
-      <c r="H6" s="208"/>
-      <c r="I6" s="205"/>
-      <c r="J6" s="208"/>
-      <c r="K6" s="206">
+      <c r="H6" s="209"/>
+      <c r="I6" s="207"/>
+      <c r="J6" s="209"/>
+      <c r="K6" s="210">
         <f t="shared" si="0"/>
         <v>0.2485</v>
       </c>
-      <c r="L6" s="206"/>
-      <c r="M6" s="206"/>
+      <c r="L6" s="210"/>
+      <c r="M6" s="210"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C7" s="204"/>
+      <c r="C7" s="206"/>
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
@@ -3068,18 +3077,18 @@
       <c r="G7" s="27">
         <v>5.99</v>
       </c>
-      <c r="H7" s="208"/>
-      <c r="I7" s="205"/>
-      <c r="J7" s="208"/>
-      <c r="K7" s="206">
+      <c r="H7" s="209"/>
+      <c r="I7" s="207"/>
+      <c r="J7" s="209"/>
+      <c r="K7" s="210">
         <f t="shared" si="0"/>
         <v>0.29949999999999999</v>
       </c>
-      <c r="L7" s="206"/>
-      <c r="M7" s="206"/>
+      <c r="L7" s="210"/>
+      <c r="M7" s="210"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C8" s="204"/>
+      <c r="C8" s="206"/>
       <c r="D8" s="1" t="s">
         <v>155</v>
       </c>
@@ -3092,18 +3101,18 @@
       <c r="G8" s="27">
         <v>6.25</v>
       </c>
-      <c r="H8" s="208"/>
-      <c r="I8" s="205"/>
-      <c r="J8" s="208"/>
-      <c r="K8" s="206">
+      <c r="H8" s="209"/>
+      <c r="I8" s="207"/>
+      <c r="J8" s="209"/>
+      <c r="K8" s="210">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
-      <c r="L8" s="206"/>
-      <c r="M8" s="206"/>
+      <c r="L8" s="210"/>
+      <c r="M8" s="210"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C9" s="204"/>
+      <c r="C9" s="206"/>
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3116,18 +3125,18 @@
       <c r="G9" s="27">
         <v>11.59</v>
       </c>
-      <c r="H9" s="208"/>
-      <c r="I9" s="205"/>
-      <c r="J9" s="208"/>
-      <c r="K9" s="206">
+      <c r="H9" s="209"/>
+      <c r="I9" s="207"/>
+      <c r="J9" s="209"/>
+      <c r="K9" s="210">
         <f t="shared" si="0"/>
         <v>0.57950000000000002</v>
       </c>
-      <c r="L9" s="206"/>
-      <c r="M9" s="206"/>
+      <c r="L9" s="210"/>
+      <c r="M9" s="210"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C10" s="204"/>
+      <c r="C10" s="206"/>
       <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
@@ -3140,15 +3149,15 @@
       <c r="G10" s="27">
         <v>5.32</v>
       </c>
-      <c r="H10" s="208"/>
-      <c r="I10" s="205"/>
-      <c r="J10" s="208"/>
-      <c r="K10" s="206">
+      <c r="H10" s="209"/>
+      <c r="I10" s="207"/>
+      <c r="J10" s="209"/>
+      <c r="K10" s="210">
         <f t="shared" si="0"/>
         <v>1.0640000000000001</v>
       </c>
-      <c r="L10" s="206"/>
-      <c r="M10" s="206"/>
+      <c r="L10" s="210"/>
+      <c r="M10" s="210"/>
     </row>
     <row r="11" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C11" s="7"/>
@@ -3255,14 +3264,14 @@
       <c r="G16" s="27">
         <v>6.56</v>
       </c>
-      <c r="H16" s="207">
+      <c r="H16" s="208">
         <f>SUM(G16:G17)</f>
         <v>7.55</v>
       </c>
-      <c r="I16" s="205">
+      <c r="I16" s="207">
         <v>0</v>
       </c>
-      <c r="J16" s="207">
+      <c r="J16" s="208">
         <f>H16+I16</f>
         <v>7.55</v>
       </c>
@@ -3283,9 +3292,9 @@
       <c r="G17" s="27">
         <v>0.99</v>
       </c>
-      <c r="H17" s="207"/>
-      <c r="I17" s="205"/>
-      <c r="J17" s="207"/>
+      <c r="H17" s="208"/>
+      <c r="I17" s="207"/>
+      <c r="J17" s="208"/>
     </row>
     <row r="18" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
@@ -3337,7 +3346,7 @@
       <c r="L20" s="35"/>
     </row>
     <row r="21" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C21" s="204">
+      <c r="C21" s="206">
         <v>42925</v>
       </c>
       <c r="D21" s="149" t="s">
@@ -3352,20 +3361,20 @@
       <c r="G21" s="27">
         <v>2.56</v>
       </c>
-      <c r="H21" s="207">
+      <c r="H21" s="208">
         <f>SUM(G21:G25)</f>
         <v>17.230000000000004</v>
       </c>
-      <c r="I21" s="205">
+      <c r="I21" s="207">
         <v>5.65</v>
       </c>
-      <c r="J21" s="207">
+      <c r="J21" s="208">
         <f>H21+I21</f>
         <v>22.880000000000003</v>
       </c>
     </row>
     <row r="22" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C22" s="204"/>
+      <c r="C22" s="206"/>
       <c r="D22" s="149" t="s">
         <v>21</v>
       </c>
@@ -3378,12 +3387,12 @@
       <c r="G22" s="27">
         <v>1.8</v>
       </c>
-      <c r="H22" s="208"/>
-      <c r="I22" s="205"/>
-      <c r="J22" s="208"/>
+      <c r="H22" s="209"/>
+      <c r="I22" s="207"/>
+      <c r="J22" s="209"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C23" s="204"/>
+      <c r="C23" s="206"/>
       <c r="D23" s="1" t="s">
         <v>20</v>
       </c>
@@ -3396,12 +3405,12 @@
       <c r="G23" s="27">
         <v>3.99</v>
       </c>
-      <c r="H23" s="208"/>
-      <c r="I23" s="205"/>
-      <c r="J23" s="208"/>
+      <c r="H23" s="209"/>
+      <c r="I23" s="207"/>
+      <c r="J23" s="209"/>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C24" s="204"/>
+      <c r="C24" s="206"/>
       <c r="D24" s="149" t="s">
         <v>13</v>
       </c>
@@ -3414,12 +3423,12 @@
       <c r="G24" s="27">
         <v>1.97</v>
       </c>
-      <c r="H24" s="208"/>
-      <c r="I24" s="205"/>
-      <c r="J24" s="208"/>
+      <c r="H24" s="209"/>
+      <c r="I24" s="207"/>
+      <c r="J24" s="209"/>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C25" s="204"/>
+      <c r="C25" s="206"/>
       <c r="D25" s="1" t="s">
         <v>2</v>
       </c>
@@ -3432,9 +3441,9 @@
       <c r="G25" s="27">
         <v>6.91</v>
       </c>
-      <c r="H25" s="208"/>
-      <c r="I25" s="205"/>
-      <c r="J25" s="208"/>
+      <c r="H25" s="209"/>
+      <c r="I25" s="207"/>
+      <c r="J25" s="209"/>
     </row>
     <row r="26" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
@@ -3448,7 +3457,7 @@
       <c r="L26" s="35"/>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C27" s="204">
+      <c r="C27" s="206">
         <v>42927</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -3463,20 +3472,20 @@
       <c r="G27" s="27">
         <v>0.75</v>
       </c>
-      <c r="H27" s="207">
+      <c r="H27" s="208">
         <f>SUM(G27:G29)</f>
         <v>3.44</v>
       </c>
-      <c r="I27" s="205">
+      <c r="I27" s="207">
         <v>4.99</v>
       </c>
-      <c r="J27" s="207">
+      <c r="J27" s="208">
         <f>H27+I27</f>
         <v>8.43</v>
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C28" s="204"/>
+      <c r="C28" s="206"/>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
@@ -3489,12 +3498,12 @@
       <c r="G28" s="27">
         <v>0.75</v>
       </c>
-      <c r="H28" s="208"/>
-      <c r="I28" s="205"/>
-      <c r="J28" s="208"/>
+      <c r="H28" s="209"/>
+      <c r="I28" s="207"/>
+      <c r="J28" s="209"/>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C29" s="204"/>
+      <c r="C29" s="206"/>
       <c r="D29" s="1" t="s">
         <v>154</v>
       </c>
@@ -3507,9 +3516,9 @@
       <c r="G29" s="27">
         <v>1.94</v>
       </c>
-      <c r="H29" s="208"/>
-      <c r="I29" s="205"/>
-      <c r="J29" s="208"/>
+      <c r="H29" s="209"/>
+      <c r="I29" s="207"/>
+      <c r="J29" s="209"/>
     </row>
     <row r="30" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="7"/>
@@ -3561,7 +3570,7 @@
       <c r="L32" s="35"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C33" s="204">
+      <c r="C33" s="206">
         <v>42929</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -3576,20 +3585,20 @@
       <c r="G33" s="27">
         <v>0.77</v>
       </c>
-      <c r="H33" s="207">
+      <c r="H33" s="208">
         <f>SUM(G33:G34)</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="I33" s="205">
+      <c r="I33" s="207">
         <v>3.39</v>
       </c>
-      <c r="J33" s="205">
+      <c r="J33" s="207">
         <f>SUM(H33:I34)</f>
         <v>5.6899999999999995</v>
       </c>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C34" s="204"/>
+      <c r="C34" s="206"/>
       <c r="D34" s="1" t="s">
         <v>76</v>
       </c>
@@ -3602,9 +3611,9 @@
       <c r="G34" s="27">
         <v>1.53</v>
       </c>
-      <c r="H34" s="208"/>
-      <c r="I34" s="205"/>
-      <c r="J34" s="205"/>
+      <c r="H34" s="209"/>
+      <c r="I34" s="207"/>
+      <c r="J34" s="207"/>
     </row>
     <row r="35" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="7"/>
@@ -3656,7 +3665,7 @@
       <c r="L37" s="35"/>
     </row>
     <row r="38" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C38" s="204">
+      <c r="C38" s="206">
         <v>42931</v>
       </c>
       <c r="D38" s="149" t="s">
@@ -3671,20 +3680,20 @@
       <c r="G38" s="27">
         <v>5.72</v>
       </c>
-      <c r="H38" s="205">
+      <c r="H38" s="207">
         <f>SUM(G38:G39)</f>
         <v>8.5500000000000007</v>
       </c>
-      <c r="I38" s="205">
+      <c r="I38" s="207">
         <v>4.99</v>
       </c>
-      <c r="J38" s="205">
+      <c r="J38" s="207">
         <f>SUM(H38:I39)</f>
         <v>13.540000000000001</v>
       </c>
     </row>
     <row r="39" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C39" s="204"/>
+      <c r="C39" s="206"/>
       <c r="D39" s="149" t="s">
         <v>122</v>
       </c>
@@ -3697,9 +3706,9 @@
       <c r="G39" s="27">
         <v>2.83</v>
       </c>
-      <c r="H39" s="205"/>
-      <c r="I39" s="205"/>
-      <c r="J39" s="205"/>
+      <c r="H39" s="207"/>
+      <c r="I39" s="207"/>
+      <c r="J39" s="207"/>
     </row>
     <row r="40" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="7"/>
@@ -3713,7 +3722,7 @@
       <c r="L40" s="35"/>
     </row>
     <row r="41" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C41" s="204">
+      <c r="C41" s="206">
         <v>42936</v>
       </c>
       <c r="D41" s="149" t="s">
@@ -3728,20 +3737,20 @@
       <c r="G41" s="27">
         <v>10.58</v>
       </c>
-      <c r="H41" s="205">
+      <c r="H41" s="207">
         <f>SUM(G41:G45)</f>
         <v>18.649999999999999</v>
       </c>
-      <c r="I41" s="205">
+      <c r="I41" s="207">
         <v>0.25</v>
       </c>
-      <c r="J41" s="205">
+      <c r="J41" s="207">
         <f>H41+I41</f>
         <v>18.899999999999999</v>
       </c>
     </row>
     <row r="42" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C42" s="204"/>
+      <c r="C42" s="206"/>
       <c r="D42" s="149" t="s">
         <v>150</v>
       </c>
@@ -3754,12 +3763,12 @@
       <c r="G42" s="27">
         <v>3.86</v>
       </c>
-      <c r="H42" s="205"/>
-      <c r="I42" s="205"/>
-      <c r="J42" s="205"/>
+      <c r="H42" s="207"/>
+      <c r="I42" s="207"/>
+      <c r="J42" s="207"/>
     </row>
     <row r="43" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C43" s="204"/>
+      <c r="C43" s="206"/>
       <c r="D43" s="149" t="s">
         <v>151</v>
       </c>
@@ -3773,12 +3782,12 @@
         <f>1.99-0.1</f>
         <v>1.89</v>
       </c>
-      <c r="H43" s="205"/>
-      <c r="I43" s="205"/>
-      <c r="J43" s="205"/>
+      <c r="H43" s="207"/>
+      <c r="I43" s="207"/>
+      <c r="J43" s="207"/>
     </row>
     <row r="44" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C44" s="204"/>
+      <c r="C44" s="206"/>
       <c r="D44" s="149" t="s">
         <v>152</v>
       </c>
@@ -3792,12 +3801,12 @@
         <f>0.99-0.05</f>
         <v>0.94</v>
       </c>
-      <c r="H44" s="205"/>
-      <c r="I44" s="205"/>
-      <c r="J44" s="205"/>
+      <c r="H44" s="207"/>
+      <c r="I44" s="207"/>
+      <c r="J44" s="207"/>
     </row>
     <row r="45" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C45" s="204"/>
+      <c r="C45" s="206"/>
       <c r="D45" s="149" t="s">
         <v>153</v>
       </c>
@@ -3811,9 +3820,9 @@
         <f>1.45-0.07</f>
         <v>1.38</v>
       </c>
-      <c r="H45" s="205"/>
-      <c r="I45" s="205"/>
-      <c r="J45" s="205"/>
+      <c r="H45" s="207"/>
+      <c r="I45" s="207"/>
+      <c r="J45" s="207"/>
     </row>
     <row r="46" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="51"/>
@@ -3902,7 +3911,7 @@
       <c r="L50" s="57"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C51" s="204">
+      <c r="C51" s="206">
         <v>42986</v>
       </c>
       <c r="D51" s="202" t="s">
@@ -3917,20 +3926,20 @@
       <c r="G51" s="27">
         <v>29.95</v>
       </c>
-      <c r="H51" s="205">
+      <c r="H51" s="207">
         <f>G51+G52+G53+2.13</f>
         <v>34.380000000000003</v>
       </c>
-      <c r="I51" s="205">
+      <c r="I51" s="207">
         <v>3.03</v>
       </c>
-      <c r="J51" s="205">
+      <c r="J51" s="207">
         <f>H51+I51</f>
         <v>37.410000000000004</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C52" s="204"/>
+      <c r="C52" s="206"/>
       <c r="D52" s="202" t="s">
         <v>222</v>
       </c>
@@ -3943,12 +3952,12 @@
       <c r="G52" s="27">
         <v>0.77</v>
       </c>
-      <c r="H52" s="205"/>
-      <c r="I52" s="205"/>
-      <c r="J52" s="205"/>
+      <c r="H52" s="207"/>
+      <c r="I52" s="207"/>
+      <c r="J52" s="207"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C53" s="204"/>
+      <c r="C53" s="206"/>
       <c r="D53" s="202" t="s">
         <v>223</v>
       </c>
@@ -3961,49 +3970,45 @@
       <c r="G53" s="27">
         <v>1.53</v>
       </c>
-      <c r="H53" s="205"/>
-      <c r="I53" s="205"/>
-      <c r="J53" s="205"/>
-    </row>
-    <row r="54" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C54" s="7"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24"/>
-      <c r="G54" s="25"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="13"/>
-      <c r="J54" s="9"/>
-      <c r="L54" s="35"/>
-    </row>
-    <row r="55" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="C55" s="41">
-        <f ca="1">TODAY()</f>
-        <v>42989</v>
-      </c>
-      <c r="E55" s="29"/>
-      <c r="F55" s="29"/>
-      <c r="G55" s="29"/>
-      <c r="H55" s="29"/>
-      <c r="I55" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="J55" s="30">
-        <f>SUM(J4:J54)</f>
-        <v>248.26</v>
-      </c>
-      <c r="K55" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="L55" s="39">
-        <f ca="1">(C55-C4)*0.0328767</f>
-        <v>3.5178069000000001</v>
-      </c>
-      <c r="M55" s="24" t="s">
-        <v>25</v>
+      <c r="H53" s="207"/>
+      <c r="I53" s="207"/>
+      <c r="J53" s="207"/>
+    </row>
+    <row r="54" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C54" s="51"/>
+      <c r="D54" s="52"/>
+      <c r="E54" s="53"/>
+      <c r="F54" s="53"/>
+      <c r="G54" s="54"/>
+      <c r="H54" s="158"/>
+      <c r="I54" s="158"/>
+      <c r="J54" s="158"/>
+      <c r="L54" s="57"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C55" s="204">
+        <v>42991</v>
+      </c>
+      <c r="D55" s="149" t="s">
+        <v>229</v>
+      </c>
+      <c r="E55" s="26">
+        <v>1</v>
+      </c>
+      <c r="F55" s="26">
+        <v>1</v>
+      </c>
+      <c r="G55" s="27">
+        <v>8.99</v>
+      </c>
+      <c r="H55" s="205">
+        <v>8.99</v>
+      </c>
+      <c r="I55" s="205">
+        <v>0</v>
+      </c>
+      <c r="J55" s="205">
+        <v>8.99</v>
       </c>
     </row>
     <row r="56" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4012,80 +4017,97 @@
       <c r="E56" s="24"/>
       <c r="F56" s="24"/>
       <c r="G56" s="25"/>
-      <c r="H56" s="31"/>
-      <c r="I56" s="34" t="s">
+      <c r="H56" s="9"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="9"/>
+      <c r="L56" s="35"/>
+    </row>
+    <row r="57" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C57" s="41">
+        <f ca="1">TODAY()</f>
+        <v>42991</v>
+      </c>
+      <c r="E57" s="29"/>
+      <c r="F57" s="29"/>
+      <c r="G57" s="29"/>
+      <c r="H57" s="29"/>
+      <c r="I57" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="J57" s="30">
+        <f>SUM(J4:J56)</f>
+        <v>257.25</v>
+      </c>
+      <c r="K57" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="L57" s="39">
+        <f ca="1">(C57-C4)*0.0328767</f>
+        <v>3.5835603000000003</v>
+      </c>
+      <c r="M57" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="7"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="25"/>
+      <c r="H58" s="31"/>
+      <c r="I58" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="J56" s="22">
-        <f ca="1">J55/L55</f>
-        <v>70.572378489564045</v>
-      </c>
-      <c r="K56" s="32" t="s">
+      <c r="J58" s="22">
+        <f ca="1">J57/L57</f>
+        <v>71.786150773017539</v>
+      </c>
+      <c r="K58" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="L56" s="36"/>
-      <c r="M56" s="32" t="s">
+      <c r="L58" s="36"/>
+      <c r="M58" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="N56" s="33"/>
-    </row>
-    <row r="57" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="58"/>
-      <c r="B57" s="58"/>
-      <c r="C57" s="44"/>
-      <c r="D57" s="45"/>
-      <c r="E57" s="46"/>
-      <c r="F57" s="46"/>
-      <c r="G57" s="47"/>
-      <c r="H57" s="48"/>
-      <c r="I57" s="59"/>
-      <c r="J57" s="48"/>
-      <c r="K57" s="58"/>
-      <c r="L57" s="60"/>
-      <c r="M57" s="58"/>
-      <c r="N57" s="58"/>
-      <c r="O57" s="58"/>
-    </row>
-    <row r="58" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C58" s="7"/>
-      <c r="D58" s="63" t="s">
-        <v>75</v>
-      </c>
-      <c r="E58" s="203" t="s">
-        <v>227</v>
-      </c>
-      <c r="H58" s="10"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="10"/>
-      <c r="L58" s="35"/>
+      <c r="N58" s="33"/>
     </row>
     <row r="59" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C59" s="7"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="24"/>
-      <c r="F59" s="24"/>
-      <c r="G59" s="25"/>
-      <c r="H59" s="10"/>
-      <c r="I59" s="11"/>
-      <c r="J59" s="10"/>
-      <c r="L59" s="35"/>
+      <c r="A59" s="58"/>
+      <c r="B59" s="58"/>
+      <c r="C59" s="44"/>
+      <c r="D59" s="45"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="46"/>
+      <c r="G59" s="47"/>
+      <c r="H59" s="48"/>
+      <c r="I59" s="59"/>
+      <c r="J59" s="48"/>
+      <c r="K59" s="58"/>
+      <c r="L59" s="60"/>
+      <c r="M59" s="58"/>
+      <c r="N59" s="58"/>
+      <c r="O59" s="58"/>
     </row>
     <row r="60" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C60" s="7"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24"/>
-      <c r="G60" s="25"/>
+      <c r="D60" s="63" t="s">
+        <v>75</v>
+      </c>
+      <c r="E60" s="203" t="s">
+        <v>227</v>
+      </c>
       <c r="H60" s="10"/>
       <c r="I60" s="11"/>
       <c r="J60" s="10"/>
       <c r="L60" s="35"/>
     </row>
     <row r="61" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C61" s="147" t="s">
-        <v>164</v>
-      </c>
-      <c r="D61" s="148"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="8"/>
       <c r="E61" s="24"/>
       <c r="F61" s="24"/>
       <c r="G61" s="25"/>
@@ -4095,50 +4117,40 @@
       <c r="L61" s="35"/>
     </row>
     <row r="62" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C62" s="49"/>
-      <c r="D62" s="95" t="s">
-        <v>0</v>
-      </c>
-      <c r="E62" s="98"/>
-      <c r="F62" s="98" t="s">
-        <v>160</v>
-      </c>
-      <c r="G62" s="99">
-        <v>3.39</v>
-      </c>
+      <c r="C62" s="7"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="25"/>
       <c r="H62" s="10"/>
       <c r="I62" s="11"/>
       <c r="J62" s="10"/>
       <c r="L62" s="35"/>
     </row>
     <row r="63" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C63" s="7"/>
-      <c r="D63" s="95" t="s">
-        <v>1</v>
-      </c>
-      <c r="E63" s="98"/>
-      <c r="F63" s="98" t="s">
-        <v>160</v>
-      </c>
-      <c r="G63" s="99">
-        <v>1.39</v>
-      </c>
+      <c r="C63" s="147" t="s">
+        <v>164</v>
+      </c>
+      <c r="D63" s="148"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="25"/>
       <c r="H63" s="10"/>
       <c r="I63" s="11"/>
       <c r="J63" s="10"/>
       <c r="L63" s="35"/>
     </row>
     <row r="64" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C64" s="7"/>
-      <c r="D64" s="95" t="str">
-        <f>D24</f>
-        <v>NOKIA 5110 LCD</v>
+      <c r="C64" s="49"/>
+      <c r="D64" s="95" t="s">
+        <v>0</v>
       </c>
       <c r="E64" s="98"/>
-      <c r="F64" s="98"/>
+      <c r="F64" s="98" t="s">
+        <v>160</v>
+      </c>
       <c r="G64" s="99">
-        <f>G24</f>
-        <v>1.97</v>
+        <v>3.39</v>
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="11"/>
@@ -4148,12 +4160,14 @@
     <row r="65" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C65" s="7"/>
       <c r="D65" s="95" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E65" s="98"/>
-      <c r="F65" s="98"/>
+      <c r="F65" s="98" t="s">
+        <v>160</v>
+      </c>
       <c r="G65" s="99">
-        <v>0.2485</v>
+        <v>1.39</v>
       </c>
       <c r="H65" s="10"/>
       <c r="I65" s="11"/>
@@ -4162,13 +4176,15 @@
     </row>
     <row r="66" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C66" s="7"/>
-      <c r="D66" s="95" t="s">
-        <v>156</v>
+      <c r="D66" s="95" t="str">
+        <f>D24</f>
+        <v>NOKIA 5110 LCD</v>
       </c>
       <c r="E66" s="98"/>
       <c r="F66" s="98"/>
       <c r="G66" s="99">
-        <v>0.29949999999999999</v>
+        <f>G24</f>
+        <v>1.97</v>
       </c>
       <c r="H66" s="10"/>
       <c r="I66" s="11"/>
@@ -4178,12 +4194,12 @@
     <row r="67" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C67" s="7"/>
       <c r="D67" s="95" t="s">
-        <v>158</v>
+        <v>5</v>
       </c>
       <c r="E67" s="98"/>
       <c r="F67" s="98"/>
       <c r="G67" s="99">
-        <v>1</v>
+        <v>0.2485</v>
       </c>
       <c r="H67" s="10"/>
       <c r="I67" s="11"/>
@@ -4193,12 +4209,12 @@
     <row r="68" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C68" s="7"/>
       <c r="D68" s="95" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E68" s="98"/>
       <c r="F68" s="98"/>
       <c r="G68" s="99">
-        <v>6.25</v>
+        <v>0.29949999999999999</v>
       </c>
       <c r="H68" s="10"/>
       <c r="I68" s="11"/>
@@ -4208,12 +4224,12 @@
     <row r="69" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C69" s="7"/>
       <c r="D69" s="95" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E69" s="98"/>
       <c r="F69" s="98"/>
       <c r="G69" s="99">
-        <v>0.57950000000000002</v>
+        <v>1</v>
       </c>
       <c r="H69" s="10"/>
       <c r="I69" s="11"/>
@@ -4223,12 +4239,12 @@
     <row r="70" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C70" s="7"/>
       <c r="D70" s="95" t="s">
-        <v>17</v>
+        <v>155</v>
       </c>
       <c r="E70" s="98"/>
       <c r="F70" s="98"/>
       <c r="G70" s="99">
-        <v>1.0640000000000001</v>
+        <v>6.25</v>
       </c>
       <c r="H70" s="10"/>
       <c r="I70" s="11"/>
@@ -4238,12 +4254,12 @@
     <row r="71" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C71" s="7"/>
       <c r="D71" s="95" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E71" s="98"/>
       <c r="F71" s="98"/>
       <c r="G71" s="99">
-        <v>0.5</v>
+        <v>0.57950000000000002</v>
       </c>
       <c r="H71" s="10"/>
       <c r="I71" s="11"/>
@@ -4251,61 +4267,69 @@
       <c r="L71" s="35"/>
     </row>
     <row r="72" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C72" s="44"/>
-      <c r="D72" s="96" t="s">
-        <v>159</v>
-      </c>
-      <c r="E72" s="100"/>
-      <c r="F72" s="100"/>
-      <c r="G72" s="101">
-        <v>2</v>
-      </c>
-      <c r="H72" s="48"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="E72" s="98"/>
+      <c r="F72" s="98"/>
+      <c r="G72" s="99">
+        <v>1.0640000000000001</v>
+      </c>
+      <c r="H72" s="10"/>
       <c r="I72" s="11"/>
       <c r="J72" s="10"/>
       <c r="L72" s="35"/>
     </row>
     <row r="73" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="58"/>
-      <c r="B73" s="58"/>
-      <c r="C73" s="44"/>
-      <c r="D73" s="45"/>
-      <c r="E73" s="46"/>
-      <c r="F73" s="46"/>
-      <c r="G73" s="97">
-        <f>SUM(G62:G72)</f>
-        <v>18.691499999999998</v>
-      </c>
-      <c r="H73" s="48"/>
-      <c r="I73" s="59"/>
-      <c r="J73" s="48"/>
-      <c r="K73" s="58"/>
-      <c r="L73" s="60"/>
-      <c r="M73" s="58"/>
-      <c r="N73" s="58"/>
-      <c r="O73" s="58"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="95" t="s">
+        <v>161</v>
+      </c>
+      <c r="E73" s="98"/>
+      <c r="F73" s="98"/>
+      <c r="G73" s="99">
+        <v>0.5</v>
+      </c>
+      <c r="H73" s="10"/>
+      <c r="I73" s="11"/>
+      <c r="J73" s="10"/>
+      <c r="L73" s="35"/>
     </row>
     <row r="74" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C74" s="7"/>
-      <c r="D74" s="8"/>
-      <c r="E74" s="24"/>
-      <c r="F74" s="24"/>
-      <c r="G74" s="25"/>
-      <c r="H74" s="10"/>
+      <c r="C74" s="44"/>
+      <c r="D74" s="96" t="s">
+        <v>159</v>
+      </c>
+      <c r="E74" s="100"/>
+      <c r="F74" s="100"/>
+      <c r="G74" s="101">
+        <v>2</v>
+      </c>
+      <c r="H74" s="48"/>
       <c r="I74" s="11"/>
       <c r="J74" s="10"/>
       <c r="L74" s="35"/>
     </row>
     <row r="75" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C75" s="7"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="24"/>
-      <c r="F75" s="24"/>
-      <c r="G75" s="25"/>
-      <c r="H75" s="10"/>
-      <c r="I75" s="11"/>
-      <c r="J75" s="10"/>
-      <c r="L75" s="35"/>
+      <c r="A75" s="58"/>
+      <c r="B75" s="58"/>
+      <c r="C75" s="44"/>
+      <c r="D75" s="45"/>
+      <c r="E75" s="46"/>
+      <c r="F75" s="46"/>
+      <c r="G75" s="97">
+        <f>SUM(G64:G74)</f>
+        <v>18.691499999999998</v>
+      </c>
+      <c r="H75" s="48"/>
+      <c r="I75" s="59"/>
+      <c r="J75" s="48"/>
+      <c r="K75" s="58"/>
+      <c r="L75" s="60"/>
+      <c r="M75" s="58"/>
+      <c r="N75" s="58"/>
+      <c r="O75" s="58"/>
     </row>
     <row r="76" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C76" s="7"/>
@@ -4329,59 +4353,49 @@
       <c r="J77" s="10"/>
       <c r="L77" s="35"/>
     </row>
-    <row r="78" spans="1:15" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C78" s="93" t="s">
+    <row r="78" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C78" s="7"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="24"/>
+      <c r="G78" s="25"/>
+      <c r="H78" s="10"/>
+      <c r="I78" s="11"/>
+      <c r="J78" s="10"/>
+      <c r="L78" s="35"/>
+    </row>
+    <row r="79" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C79" s="7"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="24"/>
+      <c r="G79" s="25"/>
+      <c r="H79" s="10"/>
+      <c r="I79" s="11"/>
+      <c r="J79" s="10"/>
+      <c r="L79" s="35"/>
+    </row>
+    <row r="80" spans="1:15" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C80" s="93" t="s">
         <v>163</v>
       </c>
-      <c r="D78" s="94"/>
-      <c r="E78" s="18"/>
-      <c r="H78" s="14"/>
-      <c r="I78" s="17"/>
-      <c r="J78" s="14"/>
-      <c r="K78" s="14"/>
-      <c r="L78" s="14"/>
-    </row>
-    <row r="79" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C79" s="144"/>
-      <c r="D79" s="151" t="s">
-        <v>226</v>
-      </c>
-      <c r="E79" s="98"/>
-      <c r="F79" s="98"/>
-      <c r="G79" s="99">
-        <v>1.53</v>
-      </c>
-      <c r="H79" s="157"/>
-      <c r="I79" s="158"/>
-      <c r="J79" s="157"/>
-      <c r="K79" s="157"/>
-      <c r="L79" s="159"/>
-    </row>
-    <row r="80" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C80" s="144"/>
-      <c r="D80" s="151" t="s">
-        <v>30</v>
-      </c>
-      <c r="E80" s="98"/>
-      <c r="F80" s="98"/>
-      <c r="G80" s="99">
-        <v>33.57</v>
-      </c>
-      <c r="H80" s="157"/>
-      <c r="I80" s="158"/>
-      <c r="J80" s="157"/>
-      <c r="K80" s="157"/>
-      <c r="L80" s="159"/>
+      <c r="D80" s="94"/>
+      <c r="E80" s="18"/>
+      <c r="H80" s="14"/>
+      <c r="I80" s="17"/>
+      <c r="J80" s="14"/>
+      <c r="K80" s="14"/>
+      <c r="L80" s="14"/>
     </row>
     <row r="81" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C81" s="144"/>
       <c r="D81" s="151" t="s">
-        <v>2</v>
+        <v>226</v>
       </c>
       <c r="E81" s="98"/>
       <c r="F81" s="98"/>
       <c r="G81" s="99">
-        <v>6.56</v>
+        <v>1.53</v>
       </c>
       <c r="H81" s="157"/>
       <c r="I81" s="158"/>
@@ -4392,12 +4406,12 @@
     <row r="82" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C82" s="144"/>
       <c r="D82" s="151" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="E82" s="98"/>
       <c r="F82" s="98"/>
       <c r="G82" s="99">
-        <v>2.57</v>
+        <v>33.57</v>
       </c>
       <c r="H82" s="157"/>
       <c r="I82" s="158"/>
@@ -4408,12 +4422,12 @@
     <row r="83" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C83" s="144"/>
       <c r="D83" s="151" t="s">
-        <v>61</v>
+        <v>2</v>
       </c>
       <c r="E83" s="98"/>
       <c r="F83" s="98"/>
       <c r="G83" s="99">
-        <v>5.22</v>
+        <v>6.56</v>
       </c>
       <c r="H83" s="157"/>
       <c r="I83" s="158"/>
@@ -4424,12 +4438,12 @@
     <row r="84" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C84" s="144"/>
       <c r="D84" s="151" t="s">
-        <v>162</v>
+        <v>11</v>
       </c>
       <c r="E84" s="98"/>
       <c r="F84" s="98"/>
       <c r="G84" s="99">
-        <v>0.39900000000000002</v>
+        <v>2.57</v>
       </c>
       <c r="H84" s="157"/>
       <c r="I84" s="158"/>
@@ -4437,48 +4451,47 @@
       <c r="K84" s="157"/>
       <c r="L84" s="159"/>
     </row>
-    <row r="85" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C85" s="145"/>
+    <row r="85" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C85" s="144"/>
       <c r="D85" s="151" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="E85" s="98"/>
       <c r="F85" s="98"/>
       <c r="G85" s="99">
-        <v>0.77</v>
-      </c>
-      <c r="H85" s="9"/>
-      <c r="I85" s="13"/>
-      <c r="J85" s="9"/>
-      <c r="K85" s="9"/>
-      <c r="L85" s="38"/>
-    </row>
-    <row r="86" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C86" s="145"/>
+        <v>5.22</v>
+      </c>
+      <c r="H85" s="157"/>
+      <c r="I85" s="158"/>
+      <c r="J85" s="157"/>
+      <c r="K85" s="157"/>
+      <c r="L85" s="159"/>
+    </row>
+    <row r="86" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C86" s="144"/>
       <c r="D86" s="151" t="s">
-        <v>6</v>
+        <v>162</v>
       </c>
       <c r="E86" s="98"/>
       <c r="F86" s="98"/>
       <c r="G86" s="99">
-        <v>0.02</v>
-      </c>
-      <c r="H86" s="9"/>
-      <c r="I86" s="13"/>
-      <c r="J86" s="9"/>
-      <c r="K86" s="9"/>
-      <c r="L86" s="38"/>
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="H86" s="157"/>
+      <c r="I86" s="158"/>
+      <c r="J86" s="157"/>
+      <c r="K86" s="157"/>
+      <c r="L86" s="159"/>
     </row>
     <row r="87" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C87" s="145"/>
-      <c r="D87" s="153" t="s">
-        <v>168</v>
+      <c r="D87" s="151" t="s">
+        <v>73</v>
       </c>
       <c r="E87" s="98"/>
       <c r="F87" s="98"/>
       <c r="G87" s="99">
-        <f>5.72+(0.5*4.99)</f>
-        <v>8.2149999999999999</v>
+        <v>0.77</v>
       </c>
       <c r="H87" s="9"/>
       <c r="I87" s="13"/>
@@ -4489,13 +4502,12 @@
     <row r="88" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C88" s="145"/>
       <c r="D88" s="151" t="s">
-        <v>169</v>
+        <v>6</v>
       </c>
       <c r="E88" s="98"/>
       <c r="F88" s="98"/>
       <c r="G88" s="99">
-        <f>2.83+(0.5*4.99)</f>
-        <v>5.3250000000000002</v>
+        <v>0.02</v>
       </c>
       <c r="H88" s="9"/>
       <c r="I88" s="13"/>
@@ -4504,130 +4516,134 @@
       <c r="L88" s="38"/>
     </row>
     <row r="89" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C89" s="146"/>
-      <c r="D89" s="152" t="s">
-        <v>74</v>
-      </c>
-      <c r="E89" s="100"/>
-      <c r="F89" s="100"/>
-      <c r="G89" s="101">
-        <v>1.53</v>
-      </c>
-      <c r="H89" s="160"/>
+      <c r="C89" s="145"/>
+      <c r="D89" s="153" t="s">
+        <v>168</v>
+      </c>
+      <c r="E89" s="98"/>
+      <c r="F89" s="98"/>
+      <c r="G89" s="99">
+        <f>5.72+(0.5*4.99)</f>
+        <v>8.2149999999999999</v>
+      </c>
+      <c r="H89" s="9"/>
       <c r="I89" s="13"/>
       <c r="J89" s="9"/>
       <c r="K89" s="9"/>
       <c r="L89" s="38"/>
     </row>
-    <row r="90" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="67"/>
-      <c r="B90" s="67"/>
-      <c r="C90" s="68"/>
-      <c r="D90" s="69"/>
-      <c r="E90" s="70"/>
-      <c r="F90" s="70"/>
-      <c r="G90" s="97">
-        <f>SUM(G79:G89)</f>
+    <row r="90" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C90" s="145"/>
+      <c r="D90" s="151" t="s">
+        <v>169</v>
+      </c>
+      <c r="E90" s="98"/>
+      <c r="F90" s="98"/>
+      <c r="G90" s="99">
+        <f>2.83+(0.5*4.99)</f>
+        <v>5.3250000000000002</v>
+      </c>
+      <c r="H90" s="9"/>
+      <c r="I90" s="13"/>
+      <c r="J90" s="9"/>
+      <c r="K90" s="9"/>
+      <c r="L90" s="38"/>
+    </row>
+    <row r="91" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C91" s="146"/>
+      <c r="D91" s="152" t="s">
+        <v>74</v>
+      </c>
+      <c r="E91" s="100"/>
+      <c r="F91" s="100"/>
+      <c r="G91" s="101">
+        <v>1.53</v>
+      </c>
+      <c r="H91" s="160"/>
+      <c r="I91" s="13"/>
+      <c r="J91" s="9"/>
+      <c r="K91" s="9"/>
+      <c r="L91" s="38"/>
+    </row>
+    <row r="92" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="67"/>
+      <c r="B92" s="67"/>
+      <c r="C92" s="68"/>
+      <c r="D92" s="69"/>
+      <c r="E92" s="70"/>
+      <c r="F92" s="70"/>
+      <c r="G92" s="97">
+        <f>SUM(G81:G91)</f>
         <v>65.709000000000017</v>
       </c>
-      <c r="H90" s="71"/>
-      <c r="I90" s="72"/>
-      <c r="J90" s="71"/>
-      <c r="K90" s="67"/>
-      <c r="L90" s="67"/>
-      <c r="M90" s="67"/>
-      <c r="N90" s="67"/>
-      <c r="O90" s="67"/>
-    </row>
-    <row r="91" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C91" s="51"/>
-      <c r="D91" s="73"/>
-      <c r="E91" s="74"/>
-      <c r="F91" s="74"/>
-      <c r="G91" s="75"/>
-      <c r="H91" s="55"/>
-      <c r="I91" s="56"/>
-      <c r="J91" s="55"/>
-      <c r="L91" s="57"/>
-    </row>
-    <row r="92" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="79"/>
-      <c r="B93" s="79"/>
-      <c r="C93" s="80"/>
-      <c r="D93" s="81"/>
-      <c r="E93" s="82"/>
-      <c r="F93" s="82"/>
-      <c r="G93" s="83"/>
-      <c r="H93" s="84"/>
-      <c r="I93" s="85"/>
-      <c r="J93" s="84"/>
-      <c r="K93" s="79"/>
-      <c r="L93" s="79"/>
-      <c r="M93" s="79"/>
-      <c r="N93" s="79"/>
-      <c r="O93" s="79"/>
-    </row>
-    <row r="94" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C94" s="87"/>
-      <c r="D94" s="88"/>
-      <c r="E94" s="61"/>
-      <c r="F94" s="61"/>
-      <c r="G94" s="89"/>
-      <c r="H94" s="90"/>
-      <c r="I94" s="91"/>
-      <c r="J94" s="90"/>
-      <c r="L94" s="92"/>
-    </row>
-    <row r="95" spans="1:15" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C95" s="93" t="s">
+      <c r="H92" s="71"/>
+      <c r="I92" s="72"/>
+      <c r="J92" s="71"/>
+      <c r="K92" s="67"/>
+      <c r="L92" s="67"/>
+      <c r="M92" s="67"/>
+      <c r="N92" s="67"/>
+      <c r="O92" s="67"/>
+    </row>
+    <row r="93" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C93" s="51"/>
+      <c r="D93" s="73"/>
+      <c r="E93" s="74"/>
+      <c r="F93" s="74"/>
+      <c r="G93" s="75"/>
+      <c r="H93" s="55"/>
+      <c r="I93" s="56"/>
+      <c r="J93" s="55"/>
+      <c r="L93" s="57"/>
+    </row>
+    <row r="94" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="79"/>
+      <c r="B95" s="79"/>
+      <c r="C95" s="80"/>
+      <c r="D95" s="81"/>
+      <c r="E95" s="82"/>
+      <c r="F95" s="82"/>
+      <c r="G95" s="83"/>
+      <c r="H95" s="84"/>
+      <c r="I95" s="85"/>
+      <c r="J95" s="84"/>
+      <c r="K95" s="79"/>
+      <c r="L95" s="79"/>
+      <c r="M95" s="79"/>
+      <c r="N95" s="79"/>
+      <c r="O95" s="79"/>
+    </row>
+    <row r="96" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C96" s="87"/>
+      <c r="D96" s="88"/>
+      <c r="E96" s="61"/>
+      <c r="F96" s="61"/>
+      <c r="G96" s="89"/>
+      <c r="H96" s="90"/>
+      <c r="I96" s="91"/>
+      <c r="J96" s="90"/>
+      <c r="L96" s="92"/>
+    </row>
+    <row r="97" spans="1:15" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C97" s="93" t="s">
         <v>165</v>
       </c>
-      <c r="D95" s="94"/>
-      <c r="E95" s="18"/>
-      <c r="H95" s="64"/>
-      <c r="I95" s="65"/>
-      <c r="J95" s="64"/>
-    </row>
-    <row r="96" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C96" s="144"/>
-      <c r="D96" s="151" t="s">
-        <v>225</v>
-      </c>
-      <c r="E96" s="98"/>
-      <c r="F96" s="98"/>
-      <c r="G96" s="99">
-        <v>1.53</v>
-      </c>
-      <c r="H96" s="55"/>
-      <c r="I96" s="56"/>
-      <c r="J96" s="55"/>
-      <c r="L96" s="57"/>
-    </row>
-    <row r="97" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C97" s="144"/>
-      <c r="D97" s="151" t="s">
-        <v>166</v>
-      </c>
-      <c r="E97" s="98"/>
-      <c r="F97" s="98"/>
-      <c r="G97" s="99">
-        <v>33.57</v>
-      </c>
-      <c r="H97" s="55"/>
-      <c r="I97" s="56"/>
-      <c r="J97" s="55"/>
-      <c r="L97" s="57"/>
+      <c r="D97" s="94"/>
+      <c r="E97" s="18"/>
+      <c r="H97" s="64"/>
+      <c r="I97" s="65"/>
+      <c r="J97" s="64"/>
     </row>
     <row r="98" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C98" s="144"/>
       <c r="D98" s="151" t="s">
-        <v>2</v>
+        <v>225</v>
       </c>
       <c r="E98" s="98"/>
       <c r="F98" s="98"/>
       <c r="G98" s="99">
-        <v>6.56</v>
+        <v>1.53</v>
       </c>
       <c r="H98" s="55"/>
       <c r="I98" s="56"/>
@@ -4637,57 +4653,57 @@
     <row r="99" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C99" s="144"/>
       <c r="D99" s="151" t="s">
-        <v>61</v>
+        <v>166</v>
       </c>
       <c r="E99" s="98"/>
       <c r="F99" s="98"/>
       <c r="G99" s="99">
-        <v>6.91</v>
+        <v>33.57</v>
       </c>
       <c r="H99" s="55"/>
       <c r="I99" s="56"/>
       <c r="J99" s="55"/>
       <c r="L99" s="57"/>
     </row>
-    <row r="100" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C100" s="145"/>
+    <row r="100" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C100" s="144"/>
       <c r="D100" s="151" t="s">
-        <v>162</v>
+        <v>2</v>
       </c>
       <c r="E100" s="98"/>
       <c r="F100" s="98"/>
       <c r="G100" s="99">
-        <v>0.39900000000000002</v>
-      </c>
-      <c r="H100" s="10"/>
-      <c r="I100" s="11"/>
-      <c r="J100" s="10"/>
-      <c r="L100" s="35"/>
-    </row>
-    <row r="101" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C101" s="145"/>
+        <v>6.56</v>
+      </c>
+      <c r="H100" s="55"/>
+      <c r="I100" s="56"/>
+      <c r="J100" s="55"/>
+      <c r="L100" s="57"/>
+    </row>
+    <row r="101" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C101" s="144"/>
       <c r="D101" s="151" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="E101" s="98"/>
       <c r="F101" s="98"/>
       <c r="G101" s="99">
-        <v>2.57</v>
-      </c>
-      <c r="H101" s="10"/>
-      <c r="I101" s="11"/>
-      <c r="J101" s="10"/>
-      <c r="L101" s="35"/>
+        <v>6.91</v>
+      </c>
+      <c r="H101" s="55"/>
+      <c r="I101" s="56"/>
+      <c r="J101" s="55"/>
+      <c r="L101" s="57"/>
     </row>
     <row r="102" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C102" s="145"/>
       <c r="D102" s="151" t="s">
-        <v>6</v>
+        <v>162</v>
       </c>
       <c r="E102" s="98"/>
       <c r="F102" s="98"/>
       <c r="G102" s="99">
-        <v>0.02</v>
+        <v>0.39900000000000002</v>
       </c>
       <c r="H102" s="10"/>
       <c r="I102" s="11"/>
@@ -4695,86 +4711,95 @@
       <c r="L102" s="35"/>
     </row>
     <row r="103" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C103" s="145"/>
       <c r="D103" s="151" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="E103" s="98"/>
       <c r="F103" s="98"/>
       <c r="G103" s="99">
+        <v>2.57</v>
+      </c>
+      <c r="H103" s="10"/>
+      <c r="I103" s="11"/>
+      <c r="J103" s="10"/>
+      <c r="L103" s="35"/>
+    </row>
+    <row r="104" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C104" s="145"/>
+      <c r="D104" s="151" t="s">
+        <v>6</v>
+      </c>
+      <c r="E104" s="98"/>
+      <c r="F104" s="98"/>
+      <c r="G104" s="99">
+        <v>0.02</v>
+      </c>
+      <c r="H104" s="10"/>
+      <c r="I104" s="11"/>
+      <c r="J104" s="10"/>
+      <c r="L104" s="35"/>
+    </row>
+    <row r="105" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D105" s="151" t="s">
+        <v>73</v>
+      </c>
+      <c r="E105" s="98"/>
+      <c r="F105" s="98"/>
+      <c r="G105" s="99">
         <v>0.77</v>
       </c>
     </row>
-    <row r="104" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D104" s="154" t="s">
+    <row r="106" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D106" s="154" t="s">
         <v>74</v>
       </c>
-      <c r="E104" s="155"/>
-      <c r="F104" s="155"/>
-      <c r="G104" s="156">
+      <c r="E106" s="155"/>
+      <c r="F106" s="155"/>
+      <c r="G106" s="156">
         <v>1.53</v>
       </c>
     </row>
-    <row r="105" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C105" s="146"/>
-      <c r="D105" s="152" t="s">
+    <row r="107" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C107" s="146"/>
+      <c r="D107" s="152" t="s">
         <v>224</v>
       </c>
-      <c r="E105" s="100"/>
-      <c r="F105" s="100"/>
-      <c r="G105" s="101">
+      <c r="E107" s="100"/>
+      <c r="F107" s="100"/>
+      <c r="G107" s="101">
         <v>3.78</v>
       </c>
-      <c r="H105" s="48"/>
-      <c r="I105" s="11"/>
-      <c r="J105" s="10"/>
-      <c r="K105" s="12"/>
-      <c r="L105" s="35"/>
-      <c r="M105" s="12"/>
-      <c r="N105" s="12"/>
-      <c r="O105" s="12"/>
-    </row>
-    <row r="106" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="67"/>
-      <c r="B106" s="67"/>
-      <c r="C106" s="68"/>
-      <c r="D106" s="69"/>
-      <c r="E106" s="70"/>
-      <c r="F106" s="70"/>
-      <c r="G106" s="97">
-        <f>SUM(G96:G105)</f>
+      <c r="H107" s="48"/>
+      <c r="I107" s="11"/>
+      <c r="J107" s="10"/>
+      <c r="K107" s="12"/>
+      <c r="L107" s="35"/>
+      <c r="M107" s="12"/>
+      <c r="N107" s="12"/>
+      <c r="O107" s="12"/>
+    </row>
+    <row r="108" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="67"/>
+      <c r="B108" s="67"/>
+      <c r="C108" s="68"/>
+      <c r="D108" s="69"/>
+      <c r="E108" s="70"/>
+      <c r="F108" s="70"/>
+      <c r="G108" s="97">
+        <f>SUM(G98:G107)</f>
         <v>57.639000000000017</v>
       </c>
-      <c r="H106" s="71"/>
-      <c r="I106" s="72"/>
-      <c r="J106" s="71"/>
-      <c r="K106" s="67"/>
-      <c r="L106" s="67"/>
-      <c r="M106" s="67"/>
-      <c r="N106" s="67"/>
-      <c r="O106" s="67"/>
-    </row>
-    <row r="107" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C107" s="51"/>
-      <c r="D107" s="52"/>
-      <c r="E107" s="53"/>
-      <c r="F107" s="53"/>
-      <c r="G107" s="54"/>
-      <c r="H107" s="55"/>
-      <c r="I107" s="56"/>
-      <c r="J107" s="55"/>
-      <c r="L107" s="57"/>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C108" s="51"/>
-      <c r="D108" s="52"/>
-      <c r="E108" s="53"/>
-      <c r="F108" s="53"/>
-      <c r="G108" s="54"/>
-      <c r="H108" s="55"/>
-      <c r="I108" s="56"/>
-      <c r="J108" s="55"/>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H108" s="71"/>
+      <c r="I108" s="72"/>
+      <c r="J108" s="71"/>
+      <c r="K108" s="67"/>
+      <c r="L108" s="67"/>
+      <c r="M108" s="67"/>
+      <c r="N108" s="67"/>
+      <c r="O108" s="67"/>
+    </row>
+    <row r="109" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C109" s="51"/>
       <c r="D109" s="52"/>
       <c r="E109" s="53"/>
@@ -4783,6 +4808,7 @@
       <c r="H109" s="55"/>
       <c r="I109" s="56"/>
       <c r="J109" s="55"/>
+      <c r="L109" s="57"/>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C110" s="51"/>
@@ -5435,22 +5461,64 @@
       <c r="J174" s="55"/>
     </row>
     <row r="175" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C175" s="51"/>
       <c r="D175" s="52"/>
       <c r="E175" s="53"/>
       <c r="F175" s="53"/>
       <c r="G175" s="54"/>
+      <c r="H175" s="55"/>
+      <c r="I175" s="56"/>
+      <c r="J175" s="55"/>
     </row>
     <row r="176" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C176" s="51"/>
       <c r="D176" s="52"/>
       <c r="E176" s="53"/>
       <c r="F176" s="53"/>
       <c r="G176" s="54"/>
+      <c r="H176" s="55"/>
+      <c r="I176" s="56"/>
+      <c r="J176" s="55"/>
+    </row>
+    <row r="177" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D177" s="52"/>
+      <c r="E177" s="53"/>
+      <c r="F177" s="53"/>
+      <c r="G177" s="54"/>
+    </row>
+    <row r="178" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D178" s="52"/>
+      <c r="E178" s="53"/>
+      <c r="F178" s="53"/>
+      <c r="G178" s="54"/>
     </row>
   </sheetData>
   <sortState ref="C4:H19">
     <sortCondition ref="C4:C19"/>
   </sortState>
   <mergeCells count="38">
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="H51:H53"/>
+    <mergeCell ref="I51:I53"/>
+    <mergeCell ref="J51:J53"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="C41:C45"/>
+    <mergeCell ref="H41:H45"/>
+    <mergeCell ref="I41:I45"/>
+    <mergeCell ref="J41:J45"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="J27:J29"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="H33:H34"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="H38:H39"/>
     <mergeCell ref="I38:I39"/>
@@ -5467,28 +5535,6 @@
     <mergeCell ref="I27:I29"/>
     <mergeCell ref="I21:I25"/>
     <mergeCell ref="H16:H17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="J27:J29"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="H51:H53"/>
-    <mergeCell ref="I51:I53"/>
-    <mergeCell ref="J51:J53"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="C41:C45"/>
-    <mergeCell ref="H41:H45"/>
-    <mergeCell ref="I41:I45"/>
-    <mergeCell ref="J41:J45"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="I16:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6396,21 +6442,21 @@
       <c r="AB16" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="AN16" s="209" t="s">
+      <c r="AN16" s="211" t="s">
         <v>123</v>
       </c>
-      <c r="AO16" s="209"/>
-      <c r="AP16" s="209"/>
-      <c r="AQ16" s="209"/>
-      <c r="AT16" s="208" t="s">
+      <c r="AO16" s="211"/>
+      <c r="AP16" s="211"/>
+      <c r="AQ16" s="211"/>
+      <c r="AT16" s="209" t="s">
         <v>119</v>
       </c>
-      <c r="AU16" s="208"/>
-      <c r="AV16" s="208"/>
-      <c r="AW16" s="208"/>
-      <c r="AX16" s="208"/>
-      <c r="AY16" s="208"/>
-      <c r="AZ16" s="208"/>
+      <c r="AU16" s="209"/>
+      <c r="AV16" s="209"/>
+      <c r="AW16" s="209"/>
+      <c r="AX16" s="209"/>
+      <c r="AY16" s="209"/>
+      <c r="AZ16" s="209"/>
     </row>
     <row r="17" spans="25:59" x14ac:dyDescent="0.25">
       <c r="Y17" s="108" t="s">
@@ -6425,22 +6471,22 @@
       <c r="AB17" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="AJ17" s="208" t="s">
+      <c r="AJ17" s="209" t="s">
         <v>117</v>
       </c>
-      <c r="AK17" s="208"/>
-      <c r="AL17" s="208"/>
-      <c r="AN17" s="209"/>
-      <c r="AO17" s="209"/>
-      <c r="AP17" s="209"/>
-      <c r="AQ17" s="209"/>
+      <c r="AK17" s="209"/>
+      <c r="AL17" s="209"/>
+      <c r="AN17" s="211"/>
+      <c r="AO17" s="211"/>
+      <c r="AP17" s="211"/>
+      <c r="AQ17" s="211"/>
     </row>
     <row r="19" spans="25:59" x14ac:dyDescent="0.25">
       <c r="AP19" s="195" t="s">
         <v>216</v>
       </c>
       <c r="AQ19" s="117">
-        <f>INVENTORY!G90</f>
+        <f>INVENTORY!G92</f>
         <v>65.709000000000017</v>
       </c>
       <c r="AS19" s="196" t="s">
@@ -6448,11 +6494,11 @@
       </c>
     </row>
     <row r="20" spans="25:59" x14ac:dyDescent="0.25">
-      <c r="AK20" s="210" t="s">
+      <c r="AK20" s="212" t="s">
         <v>120</v>
       </c>
-      <c r="AL20" s="210"/>
-      <c r="AM20" s="210"/>
+      <c r="AL20" s="212"/>
+      <c r="AM20" s="212"/>
       <c r="AP20" s="195" t="s">
         <v>217</v>
       </c>
@@ -6747,7 +6793,7 @@
         <f t="shared" si="1"/>
         <v>6.6300000000000008</v>
       </c>
-      <c r="H11" s="211">
+      <c r="H11" s="213">
         <v>3.39</v>
       </c>
       <c r="I11" s="172" t="s">
@@ -6777,7 +6823,7 @@
         <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
-      <c r="H12" s="211"/>
+      <c r="H12" s="213"/>
       <c r="I12" s="172" t="s">
         <v>186</v>
       </c>
@@ -6833,7 +6879,7 @@
         <f t="shared" si="1"/>
         <v>57.199999999999996</v>
       </c>
-      <c r="H14" s="212">
+      <c r="H14" s="214">
         <v>4.99</v>
       </c>
       <c r="I14" s="172" t="s">
@@ -6862,7 +6908,7 @@
         <f t="shared" si="1"/>
         <v>28.3</v>
       </c>
-      <c r="H15" s="213"/>
+      <c r="H15" s="215"/>
       <c r="I15" s="182" t="s">
         <v>228</v>
       </c>

</xml_diff>

<commit_message>
Trying to make PROTOTYPE3 code work.
TODO -- FIGURE OUT WHY THE M0 GLITCHES AND LAGS... POSSIBLY HARDWARE BUGS? SOLDER JOINTS?
</commit_message>
<xml_diff>
--- a/BillOfMaterials/INVENTORY.xlsx
+++ b/BillOfMaterials/INVENTORY.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INVENTORY" sheetId="1" r:id="rId1"/>
@@ -2349,14 +2349,14 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2893,9 +2893,9 @@
   </sheetPr>
   <dimension ref="A1:AB178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E56" sqref="E56"/>
+      <selection pane="bottomLeft" activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2997,23 +2997,23 @@
       <c r="G4" s="27">
         <v>6.99</v>
       </c>
-      <c r="H4" s="208">
+      <c r="H4" s="209">
         <f>SUM(G4:G10)</f>
         <v>48.1</v>
       </c>
       <c r="I4" s="207">
         <v>0</v>
       </c>
-      <c r="J4" s="208">
+      <c r="J4" s="209">
         <f>H4+I4</f>
         <v>48.1</v>
       </c>
-      <c r="K4" s="210">
+      <c r="K4" s="208">
         <f>G4/E4</f>
         <v>6.99</v>
       </c>
-      <c r="L4" s="210"/>
-      <c r="M4" s="210"/>
+      <c r="L4" s="208"/>
+      <c r="M4" s="208"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C5" s="206"/>
@@ -3029,15 +3029,15 @@
       <c r="G5" s="27">
         <v>6.99</v>
       </c>
-      <c r="H5" s="209"/>
+      <c r="H5" s="210"/>
       <c r="I5" s="207"/>
-      <c r="J5" s="209"/>
-      <c r="K5" s="210">
+      <c r="J5" s="210"/>
+      <c r="K5" s="208">
         <f t="shared" ref="K5:K10" si="0">G5/E5</f>
         <v>6.99</v>
       </c>
-      <c r="L5" s="210"/>
-      <c r="M5" s="210"/>
+      <c r="L5" s="208"/>
+      <c r="M5" s="208"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C6" s="206"/>
@@ -3053,15 +3053,15 @@
       <c r="G6" s="27">
         <v>4.97</v>
       </c>
-      <c r="H6" s="209"/>
+      <c r="H6" s="210"/>
       <c r="I6" s="207"/>
-      <c r="J6" s="209"/>
-      <c r="K6" s="210">
+      <c r="J6" s="210"/>
+      <c r="K6" s="208">
         <f t="shared" si="0"/>
         <v>0.2485</v>
       </c>
-      <c r="L6" s="210"/>
-      <c r="M6" s="210"/>
+      <c r="L6" s="208"/>
+      <c r="M6" s="208"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C7" s="206"/>
@@ -3077,15 +3077,15 @@
       <c r="G7" s="27">
         <v>5.99</v>
       </c>
-      <c r="H7" s="209"/>
+      <c r="H7" s="210"/>
       <c r="I7" s="207"/>
-      <c r="J7" s="209"/>
-      <c r="K7" s="210">
+      <c r="J7" s="210"/>
+      <c r="K7" s="208">
         <f t="shared" si="0"/>
         <v>0.29949999999999999</v>
       </c>
-      <c r="L7" s="210"/>
-      <c r="M7" s="210"/>
+      <c r="L7" s="208"/>
+      <c r="M7" s="208"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C8" s="206"/>
@@ -3101,15 +3101,15 @@
       <c r="G8" s="27">
         <v>6.25</v>
       </c>
-      <c r="H8" s="209"/>
+      <c r="H8" s="210"/>
       <c r="I8" s="207"/>
-      <c r="J8" s="209"/>
-      <c r="K8" s="210">
+      <c r="J8" s="210"/>
+      <c r="K8" s="208">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
-      <c r="L8" s="210"/>
-      <c r="M8" s="210"/>
+      <c r="L8" s="208"/>
+      <c r="M8" s="208"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C9" s="206"/>
@@ -3125,15 +3125,15 @@
       <c r="G9" s="27">
         <v>11.59</v>
       </c>
-      <c r="H9" s="209"/>
+      <c r="H9" s="210"/>
       <c r="I9" s="207"/>
-      <c r="J9" s="209"/>
-      <c r="K9" s="210">
+      <c r="J9" s="210"/>
+      <c r="K9" s="208">
         <f t="shared" si="0"/>
         <v>0.57950000000000002</v>
       </c>
-      <c r="L9" s="210"/>
-      <c r="M9" s="210"/>
+      <c r="L9" s="208"/>
+      <c r="M9" s="208"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C10" s="206"/>
@@ -3149,15 +3149,15 @@
       <c r="G10" s="27">
         <v>5.32</v>
       </c>
-      <c r="H10" s="209"/>
+      <c r="H10" s="210"/>
       <c r="I10" s="207"/>
-      <c r="J10" s="209"/>
-      <c r="K10" s="210">
+      <c r="J10" s="210"/>
+      <c r="K10" s="208">
         <f t="shared" si="0"/>
         <v>1.0640000000000001</v>
       </c>
-      <c r="L10" s="210"/>
-      <c r="M10" s="210"/>
+      <c r="L10" s="208"/>
+      <c r="M10" s="208"/>
     </row>
     <row r="11" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C11" s="7"/>
@@ -3264,14 +3264,14 @@
       <c r="G16" s="27">
         <v>6.56</v>
       </c>
-      <c r="H16" s="208">
+      <c r="H16" s="209">
         <f>SUM(G16:G17)</f>
         <v>7.55</v>
       </c>
       <c r="I16" s="207">
         <v>0</v>
       </c>
-      <c r="J16" s="208">
+      <c r="J16" s="209">
         <f>H16+I16</f>
         <v>7.55</v>
       </c>
@@ -3292,9 +3292,9 @@
       <c r="G17" s="27">
         <v>0.99</v>
       </c>
-      <c r="H17" s="208"/>
+      <c r="H17" s="209"/>
       <c r="I17" s="207"/>
-      <c r="J17" s="208"/>
+      <c r="J17" s="209"/>
     </row>
     <row r="18" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
@@ -3361,14 +3361,14 @@
       <c r="G21" s="27">
         <v>2.56</v>
       </c>
-      <c r="H21" s="208">
+      <c r="H21" s="209">
         <f>SUM(G21:G25)</f>
         <v>17.230000000000004</v>
       </c>
       <c r="I21" s="207">
         <v>5.65</v>
       </c>
-      <c r="J21" s="208">
+      <c r="J21" s="209">
         <f>H21+I21</f>
         <v>22.880000000000003</v>
       </c>
@@ -3387,9 +3387,9 @@
       <c r="G22" s="27">
         <v>1.8</v>
       </c>
-      <c r="H22" s="209"/>
+      <c r="H22" s="210"/>
       <c r="I22" s="207"/>
-      <c r="J22" s="209"/>
+      <c r="J22" s="210"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C23" s="206"/>
@@ -3405,9 +3405,9 @@
       <c r="G23" s="27">
         <v>3.99</v>
       </c>
-      <c r="H23" s="209"/>
+      <c r="H23" s="210"/>
       <c r="I23" s="207"/>
-      <c r="J23" s="209"/>
+      <c r="J23" s="210"/>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C24" s="206"/>
@@ -3423,9 +3423,9 @@
       <c r="G24" s="27">
         <v>1.97</v>
       </c>
-      <c r="H24" s="209"/>
+      <c r="H24" s="210"/>
       <c r="I24" s="207"/>
-      <c r="J24" s="209"/>
+      <c r="J24" s="210"/>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C25" s="206"/>
@@ -3441,9 +3441,9 @@
       <c r="G25" s="27">
         <v>6.91</v>
       </c>
-      <c r="H25" s="209"/>
+      <c r="H25" s="210"/>
       <c r="I25" s="207"/>
-      <c r="J25" s="209"/>
+      <c r="J25" s="210"/>
     </row>
     <row r="26" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
@@ -3472,14 +3472,14 @@
       <c r="G27" s="27">
         <v>0.75</v>
       </c>
-      <c r="H27" s="208">
+      <c r="H27" s="209">
         <f>SUM(G27:G29)</f>
         <v>3.44</v>
       </c>
       <c r="I27" s="207">
         <v>4.99</v>
       </c>
-      <c r="J27" s="208">
+      <c r="J27" s="209">
         <f>H27+I27</f>
         <v>8.43</v>
       </c>
@@ -3498,9 +3498,9 @@
       <c r="G28" s="27">
         <v>0.75</v>
       </c>
-      <c r="H28" s="209"/>
+      <c r="H28" s="210"/>
       <c r="I28" s="207"/>
-      <c r="J28" s="209"/>
+      <c r="J28" s="210"/>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C29" s="206"/>
@@ -3516,9 +3516,9 @@
       <c r="G29" s="27">
         <v>1.94</v>
       </c>
-      <c r="H29" s="209"/>
+      <c r="H29" s="210"/>
       <c r="I29" s="207"/>
-      <c r="J29" s="209"/>
+      <c r="J29" s="210"/>
     </row>
     <row r="30" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="7"/>
@@ -3585,7 +3585,7 @@
       <c r="G33" s="27">
         <v>0.77</v>
       </c>
-      <c r="H33" s="208">
+      <c r="H33" s="209">
         <f>SUM(G33:G34)</f>
         <v>2.2999999999999998</v>
       </c>
@@ -3611,7 +3611,7 @@
       <c r="G34" s="27">
         <v>1.53</v>
       </c>
-      <c r="H34" s="209"/>
+      <c r="H34" s="210"/>
       <c r="I34" s="207"/>
       <c r="J34" s="207"/>
     </row>
@@ -3839,7 +3839,7 @@
       <c r="C47" s="191">
         <v>42985</v>
       </c>
-      <c r="D47" s="202" t="s">
+      <c r="D47" s="149" t="s">
         <v>219</v>
       </c>
       <c r="E47" s="26">
@@ -3914,7 +3914,7 @@
       <c r="C51" s="206">
         <v>42986</v>
       </c>
-      <c r="D51" s="202" t="s">
+      <c r="D51" s="149" t="s">
         <v>221</v>
       </c>
       <c r="E51" s="26">
@@ -3940,7 +3940,7 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C52" s="206"/>
-      <c r="D52" s="202" t="s">
+      <c r="D52" s="149" t="s">
         <v>222</v>
       </c>
       <c r="E52" s="26">
@@ -3958,7 +3958,7 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C53" s="206"/>
-      <c r="D53" s="202" t="s">
+      <c r="D53" s="149" t="s">
         <v>223</v>
       </c>
       <c r="E53" s="26">
@@ -4028,7 +4028,7 @@
       </c>
       <c r="C57" s="41">
         <f ca="1">TODAY()</f>
-        <v>42991</v>
+        <v>42992</v>
       </c>
       <c r="E57" s="29"/>
       <c r="F57" s="29"/>
@@ -4046,7 +4046,7 @@
       </c>
       <c r="L57" s="39">
         <f ca="1">(C57-C4)*0.0328767</f>
-        <v>3.5835603000000003</v>
+        <v>3.6164370000000003</v>
       </c>
       <c r="M57" s="24" t="s">
         <v>25</v>
@@ -4064,7 +4064,7 @@
       </c>
       <c r="J58" s="22">
         <f ca="1">J57/L57</f>
-        <v>71.786150773017539</v>
+        <v>71.133549402353751</v>
       </c>
       <c r="K58" s="32" t="s">
         <v>27</v>
@@ -5497,6 +5497,28 @@
     <sortCondition ref="C4:C19"/>
   </sortState>
   <mergeCells count="38">
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="C4:C10"/>
+    <mergeCell ref="J4:J10"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="H4:H10"/>
+    <mergeCell ref="I4:I10"/>
+    <mergeCell ref="J21:J25"/>
+    <mergeCell ref="H21:H25"/>
+    <mergeCell ref="H27:H29"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="I21:I25"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="J27:J29"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="H33:H34"/>
     <mergeCell ref="C51:C53"/>
     <mergeCell ref="H51:H53"/>
     <mergeCell ref="I51:I53"/>
@@ -5513,28 +5535,6 @@
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="K10:M10"/>
     <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="J27:J29"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="C4:C10"/>
-    <mergeCell ref="J4:J10"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="H4:H10"/>
-    <mergeCell ref="I4:I10"/>
-    <mergeCell ref="J21:J25"/>
-    <mergeCell ref="H21:H25"/>
-    <mergeCell ref="H27:H29"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="I21:I25"/>
-    <mergeCell ref="H16:H17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5551,8 +5551,8 @@
   </sheetPr>
   <dimension ref="B3:BG20"/>
   <sheetViews>
-    <sheetView topLeftCell="AI1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AY19" sqref="AY19"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6448,15 +6448,15 @@
       <c r="AO16" s="211"/>
       <c r="AP16" s="211"/>
       <c r="AQ16" s="211"/>
-      <c r="AT16" s="209" t="s">
+      <c r="AT16" s="210" t="s">
         <v>119</v>
       </c>
-      <c r="AU16" s="209"/>
-      <c r="AV16" s="209"/>
-      <c r="AW16" s="209"/>
-      <c r="AX16" s="209"/>
-      <c r="AY16" s="209"/>
-      <c r="AZ16" s="209"/>
+      <c r="AU16" s="210"/>
+      <c r="AV16" s="210"/>
+      <c r="AW16" s="210"/>
+      <c r="AX16" s="210"/>
+      <c r="AY16" s="210"/>
+      <c r="AZ16" s="210"/>
     </row>
     <row r="17" spans="25:59" x14ac:dyDescent="0.25">
       <c r="Y17" s="108" t="s">
@@ -6471,11 +6471,11 @@
       <c r="AB17" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="AJ17" s="209" t="s">
+      <c r="AJ17" s="210" t="s">
         <v>117</v>
       </c>
-      <c r="AK17" s="209"/>
-      <c r="AL17" s="209"/>
+      <c r="AK17" s="210"/>
+      <c r="AL17" s="210"/>
       <c r="AN17" s="211"/>
       <c r="AO17" s="211"/>
       <c r="AP17" s="211"/>

</xml_diff>

<commit_message>
BOUGHT A NEW PRESSURE SENSOR FOR PROTOTYPE2. CURRENT ONE MALFUNCTIONED. MAYBE DEBRIS GOT INTO THE SENSOR?
</commit_message>
<xml_diff>
--- a/BillOfMaterials/INVENTORY.xlsx
+++ b/BillOfMaterials/INVENTORY.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="232">
   <si>
     <t>Arduino Nano</t>
   </si>
@@ -1318,6 +1318,12 @@
   </si>
   <si>
     <t>FLYSKYHY IOS APP</t>
+  </si>
+  <si>
+    <t>MS5611 (EBAY)</t>
+  </si>
+  <si>
+    <t>BREAK AWAY 40 PIN FEMAL HEADER (EBAY)</t>
   </si>
 </sst>
 </file>
@@ -1882,7 +1888,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="216">
+  <cellXfs count="220">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2336,6 +2342,18 @@
     </xf>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2891,11 +2909,11 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:AB178"/>
+  <dimension ref="A1:AB182"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R60" sqref="R60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2982,7 +3000,7 @@
       <c r="L3" s="35"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C4" s="206">
+      <c r="C4" s="210">
         <v>42882</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -2997,26 +3015,26 @@
       <c r="G4" s="27">
         <v>6.99</v>
       </c>
-      <c r="H4" s="209">
+      <c r="H4" s="213">
         <f>SUM(G4:G10)</f>
         <v>48.1</v>
       </c>
-      <c r="I4" s="207">
+      <c r="I4" s="211">
         <v>0</v>
       </c>
-      <c r="J4" s="209">
+      <c r="J4" s="213">
         <f>H4+I4</f>
         <v>48.1</v>
       </c>
-      <c r="K4" s="208">
+      <c r="K4" s="212">
         <f>G4/E4</f>
         <v>6.99</v>
       </c>
-      <c r="L4" s="208"/>
-      <c r="M4" s="208"/>
+      <c r="L4" s="212"/>
+      <c r="M4" s="212"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C5" s="206"/>
+      <c r="C5" s="210"/>
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
@@ -3029,18 +3047,18 @@
       <c r="G5" s="27">
         <v>6.99</v>
       </c>
-      <c r="H5" s="210"/>
-      <c r="I5" s="207"/>
-      <c r="J5" s="210"/>
-      <c r="K5" s="208">
+      <c r="H5" s="214"/>
+      <c r="I5" s="211"/>
+      <c r="J5" s="214"/>
+      <c r="K5" s="212">
         <f t="shared" ref="K5:K10" si="0">G5/E5</f>
         <v>6.99</v>
       </c>
-      <c r="L5" s="208"/>
-      <c r="M5" s="208"/>
+      <c r="L5" s="212"/>
+      <c r="M5" s="212"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C6" s="206"/>
+      <c r="C6" s="210"/>
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
@@ -3053,18 +3071,18 @@
       <c r="G6" s="27">
         <v>4.97</v>
       </c>
-      <c r="H6" s="210"/>
-      <c r="I6" s="207"/>
-      <c r="J6" s="210"/>
-      <c r="K6" s="208">
+      <c r="H6" s="214"/>
+      <c r="I6" s="211"/>
+      <c r="J6" s="214"/>
+      <c r="K6" s="212">
         <f t="shared" si="0"/>
         <v>0.2485</v>
       </c>
-      <c r="L6" s="208"/>
-      <c r="M6" s="208"/>
+      <c r="L6" s="212"/>
+      <c r="M6" s="212"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C7" s="206"/>
+      <c r="C7" s="210"/>
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
@@ -3077,18 +3095,18 @@
       <c r="G7" s="27">
         <v>5.99</v>
       </c>
-      <c r="H7" s="210"/>
-      <c r="I7" s="207"/>
-      <c r="J7" s="210"/>
-      <c r="K7" s="208">
+      <c r="H7" s="214"/>
+      <c r="I7" s="211"/>
+      <c r="J7" s="214"/>
+      <c r="K7" s="212">
         <f t="shared" si="0"/>
         <v>0.29949999999999999</v>
       </c>
-      <c r="L7" s="208"/>
-      <c r="M7" s="208"/>
+      <c r="L7" s="212"/>
+      <c r="M7" s="212"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C8" s="206"/>
+      <c r="C8" s="210"/>
       <c r="D8" s="1" t="s">
         <v>155</v>
       </c>
@@ -3101,18 +3119,18 @@
       <c r="G8" s="27">
         <v>6.25</v>
       </c>
-      <c r="H8" s="210"/>
-      <c r="I8" s="207"/>
-      <c r="J8" s="210"/>
-      <c r="K8" s="208">
+      <c r="H8" s="214"/>
+      <c r="I8" s="211"/>
+      <c r="J8" s="214"/>
+      <c r="K8" s="212">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
-      <c r="L8" s="208"/>
-      <c r="M8" s="208"/>
+      <c r="L8" s="212"/>
+      <c r="M8" s="212"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C9" s="206"/>
+      <c r="C9" s="210"/>
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3125,18 +3143,18 @@
       <c r="G9" s="27">
         <v>11.59</v>
       </c>
-      <c r="H9" s="210"/>
-      <c r="I9" s="207"/>
-      <c r="J9" s="210"/>
-      <c r="K9" s="208">
+      <c r="H9" s="214"/>
+      <c r="I9" s="211"/>
+      <c r="J9" s="214"/>
+      <c r="K9" s="212">
         <f t="shared" si="0"/>
         <v>0.57950000000000002</v>
       </c>
-      <c r="L9" s="208"/>
-      <c r="M9" s="208"/>
+      <c r="L9" s="212"/>
+      <c r="M9" s="212"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C10" s="206"/>
+      <c r="C10" s="210"/>
       <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
@@ -3149,15 +3167,15 @@
       <c r="G10" s="27">
         <v>5.32</v>
       </c>
-      <c r="H10" s="210"/>
-      <c r="I10" s="207"/>
-      <c r="J10" s="210"/>
-      <c r="K10" s="208">
+      <c r="H10" s="214"/>
+      <c r="I10" s="211"/>
+      <c r="J10" s="214"/>
+      <c r="K10" s="212">
         <f t="shared" si="0"/>
         <v>1.0640000000000001</v>
       </c>
-      <c r="L10" s="208"/>
-      <c r="M10" s="208"/>
+      <c r="L10" s="212"/>
+      <c r="M10" s="212"/>
     </row>
     <row r="11" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C11" s="7"/>
@@ -3264,14 +3282,14 @@
       <c r="G16" s="27">
         <v>6.56</v>
       </c>
-      <c r="H16" s="209">
+      <c r="H16" s="213">
         <f>SUM(G16:G17)</f>
         <v>7.55</v>
       </c>
-      <c r="I16" s="207">
+      <c r="I16" s="211">
         <v>0</v>
       </c>
-      <c r="J16" s="209">
+      <c r="J16" s="213">
         <f>H16+I16</f>
         <v>7.55</v>
       </c>
@@ -3292,9 +3310,9 @@
       <c r="G17" s="27">
         <v>0.99</v>
       </c>
-      <c r="H17" s="209"/>
-      <c r="I17" s="207"/>
-      <c r="J17" s="209"/>
+      <c r="H17" s="213"/>
+      <c r="I17" s="211"/>
+      <c r="J17" s="213"/>
     </row>
     <row r="18" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
@@ -3346,7 +3364,7 @@
       <c r="L20" s="35"/>
     </row>
     <row r="21" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C21" s="206">
+      <c r="C21" s="210">
         <v>42925</v>
       </c>
       <c r="D21" s="149" t="s">
@@ -3361,20 +3379,20 @@
       <c r="G21" s="27">
         <v>2.56</v>
       </c>
-      <c r="H21" s="209">
+      <c r="H21" s="213">
         <f>SUM(G21:G25)</f>
         <v>17.230000000000004</v>
       </c>
-      <c r="I21" s="207">
+      <c r="I21" s="211">
         <v>5.65</v>
       </c>
-      <c r="J21" s="209">
+      <c r="J21" s="213">
         <f>H21+I21</f>
         <v>22.880000000000003</v>
       </c>
     </row>
     <row r="22" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C22" s="206"/>
+      <c r="C22" s="210"/>
       <c r="D22" s="149" t="s">
         <v>21</v>
       </c>
@@ -3387,12 +3405,12 @@
       <c r="G22" s="27">
         <v>1.8</v>
       </c>
-      <c r="H22" s="210"/>
-      <c r="I22" s="207"/>
-      <c r="J22" s="210"/>
+      <c r="H22" s="214"/>
+      <c r="I22" s="211"/>
+      <c r="J22" s="214"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C23" s="206"/>
+      <c r="C23" s="210"/>
       <c r="D23" s="1" t="s">
         <v>20</v>
       </c>
@@ -3405,12 +3423,12 @@
       <c r="G23" s="27">
         <v>3.99</v>
       </c>
-      <c r="H23" s="210"/>
-      <c r="I23" s="207"/>
-      <c r="J23" s="210"/>
+      <c r="H23" s="214"/>
+      <c r="I23" s="211"/>
+      <c r="J23" s="214"/>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C24" s="206"/>
+      <c r="C24" s="210"/>
       <c r="D24" s="149" t="s">
         <v>13</v>
       </c>
@@ -3423,12 +3441,12 @@
       <c r="G24" s="27">
         <v>1.97</v>
       </c>
-      <c r="H24" s="210"/>
-      <c r="I24" s="207"/>
-      <c r="J24" s="210"/>
+      <c r="H24" s="214"/>
+      <c r="I24" s="211"/>
+      <c r="J24" s="214"/>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C25" s="206"/>
+      <c r="C25" s="210"/>
       <c r="D25" s="1" t="s">
         <v>2</v>
       </c>
@@ -3441,9 +3459,9 @@
       <c r="G25" s="27">
         <v>6.91</v>
       </c>
-      <c r="H25" s="210"/>
-      <c r="I25" s="207"/>
-      <c r="J25" s="210"/>
+      <c r="H25" s="214"/>
+      <c r="I25" s="211"/>
+      <c r="J25" s="214"/>
     </row>
     <row r="26" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
@@ -3457,7 +3475,7 @@
       <c r="L26" s="35"/>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C27" s="206">
+      <c r="C27" s="210">
         <v>42927</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -3472,20 +3490,20 @@
       <c r="G27" s="27">
         <v>0.75</v>
       </c>
-      <c r="H27" s="209">
+      <c r="H27" s="213">
         <f>SUM(G27:G29)</f>
         <v>3.44</v>
       </c>
-      <c r="I27" s="207">
+      <c r="I27" s="211">
         <v>4.99</v>
       </c>
-      <c r="J27" s="209">
+      <c r="J27" s="213">
         <f>H27+I27</f>
         <v>8.43</v>
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C28" s="206"/>
+      <c r="C28" s="210"/>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
@@ -3498,12 +3516,12 @@
       <c r="G28" s="27">
         <v>0.75</v>
       </c>
-      <c r="H28" s="210"/>
-      <c r="I28" s="207"/>
-      <c r="J28" s="210"/>
+      <c r="H28" s="214"/>
+      <c r="I28" s="211"/>
+      <c r="J28" s="214"/>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C29" s="206"/>
+      <c r="C29" s="210"/>
       <c r="D29" s="1" t="s">
         <v>154</v>
       </c>
@@ -3516,9 +3534,9 @@
       <c r="G29" s="27">
         <v>1.94</v>
       </c>
-      <c r="H29" s="210"/>
-      <c r="I29" s="207"/>
-      <c r="J29" s="210"/>
+      <c r="H29" s="214"/>
+      <c r="I29" s="211"/>
+      <c r="J29" s="214"/>
     </row>
     <row r="30" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="7"/>
@@ -3570,7 +3588,7 @@
       <c r="L32" s="35"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C33" s="206">
+      <c r="C33" s="210">
         <v>42929</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -3585,20 +3603,20 @@
       <c r="G33" s="27">
         <v>0.77</v>
       </c>
-      <c r="H33" s="209">
+      <c r="H33" s="213">
         <f>SUM(G33:G34)</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="I33" s="207">
+      <c r="I33" s="211">
         <v>3.39</v>
       </c>
-      <c r="J33" s="207">
+      <c r="J33" s="211">
         <f>SUM(H33:I34)</f>
         <v>5.6899999999999995</v>
       </c>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C34" s="206"/>
+      <c r="C34" s="210"/>
       <c r="D34" s="1" t="s">
         <v>76</v>
       </c>
@@ -3611,9 +3629,9 @@
       <c r="G34" s="27">
         <v>1.53</v>
       </c>
-      <c r="H34" s="210"/>
-      <c r="I34" s="207"/>
-      <c r="J34" s="207"/>
+      <c r="H34" s="214"/>
+      <c r="I34" s="211"/>
+      <c r="J34" s="211"/>
     </row>
     <row r="35" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="7"/>
@@ -3665,7 +3683,7 @@
       <c r="L37" s="35"/>
     </row>
     <row r="38" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C38" s="206">
+      <c r="C38" s="210">
         <v>42931</v>
       </c>
       <c r="D38" s="149" t="s">
@@ -3680,20 +3698,20 @@
       <c r="G38" s="27">
         <v>5.72</v>
       </c>
-      <c r="H38" s="207">
+      <c r="H38" s="211">
         <f>SUM(G38:G39)</f>
         <v>8.5500000000000007</v>
       </c>
-      <c r="I38" s="207">
+      <c r="I38" s="211">
         <v>4.99</v>
       </c>
-      <c r="J38" s="207">
+      <c r="J38" s="211">
         <f>SUM(H38:I39)</f>
         <v>13.540000000000001</v>
       </c>
     </row>
     <row r="39" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C39" s="206"/>
+      <c r="C39" s="210"/>
       <c r="D39" s="149" t="s">
         <v>122</v>
       </c>
@@ -3706,9 +3724,9 @@
       <c r="G39" s="27">
         <v>2.83</v>
       </c>
-      <c r="H39" s="207"/>
-      <c r="I39" s="207"/>
-      <c r="J39" s="207"/>
+      <c r="H39" s="211"/>
+      <c r="I39" s="211"/>
+      <c r="J39" s="211"/>
     </row>
     <row r="40" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="7"/>
@@ -3722,7 +3740,7 @@
       <c r="L40" s="35"/>
     </row>
     <row r="41" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C41" s="206">
+      <c r="C41" s="210">
         <v>42936</v>
       </c>
       <c r="D41" s="149" t="s">
@@ -3737,20 +3755,20 @@
       <c r="G41" s="27">
         <v>10.58</v>
       </c>
-      <c r="H41" s="207">
+      <c r="H41" s="211">
         <f>SUM(G41:G45)</f>
         <v>18.649999999999999</v>
       </c>
-      <c r="I41" s="207">
+      <c r="I41" s="211">
         <v>0.25</v>
       </c>
-      <c r="J41" s="207">
+      <c r="J41" s="211">
         <f>H41+I41</f>
         <v>18.899999999999999</v>
       </c>
     </row>
     <row r="42" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C42" s="206"/>
+      <c r="C42" s="210"/>
       <c r="D42" s="149" t="s">
         <v>150</v>
       </c>
@@ -3763,12 +3781,12 @@
       <c r="G42" s="27">
         <v>3.86</v>
       </c>
-      <c r="H42" s="207"/>
-      <c r="I42" s="207"/>
-      <c r="J42" s="207"/>
+      <c r="H42" s="211"/>
+      <c r="I42" s="211"/>
+      <c r="J42" s="211"/>
     </row>
     <row r="43" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C43" s="206"/>
+      <c r="C43" s="210"/>
       <c r="D43" s="149" t="s">
         <v>151</v>
       </c>
@@ -3782,12 +3800,12 @@
         <f>1.99-0.1</f>
         <v>1.89</v>
       </c>
-      <c r="H43" s="207"/>
-      <c r="I43" s="207"/>
-      <c r="J43" s="207"/>
+      <c r="H43" s="211"/>
+      <c r="I43" s="211"/>
+      <c r="J43" s="211"/>
     </row>
     <row r="44" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C44" s="206"/>
+      <c r="C44" s="210"/>
       <c r="D44" s="149" t="s">
         <v>152</v>
       </c>
@@ -3801,12 +3819,12 @@
         <f>0.99-0.05</f>
         <v>0.94</v>
       </c>
-      <c r="H44" s="207"/>
-      <c r="I44" s="207"/>
-      <c r="J44" s="207"/>
+      <c r="H44" s="211"/>
+      <c r="I44" s="211"/>
+      <c r="J44" s="211"/>
     </row>
     <row r="45" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C45" s="206"/>
+      <c r="C45" s="210"/>
       <c r="D45" s="149" t="s">
         <v>153</v>
       </c>
@@ -3820,9 +3838,9 @@
         <f>1.45-0.07</f>
         <v>1.38</v>
       </c>
-      <c r="H45" s="207"/>
-      <c r="I45" s="207"/>
-      <c r="J45" s="207"/>
+      <c r="H45" s="211"/>
+      <c r="I45" s="211"/>
+      <c r="J45" s="211"/>
     </row>
     <row r="46" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="51"/>
@@ -3911,7 +3929,7 @@
       <c r="L50" s="57"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C51" s="206">
+      <c r="C51" s="210">
         <v>42986</v>
       </c>
       <c r="D51" s="149" t="s">
@@ -3926,20 +3944,20 @@
       <c r="G51" s="27">
         <v>29.95</v>
       </c>
-      <c r="H51" s="207">
+      <c r="H51" s="211">
         <f>G51+G52+G53+2.13</f>
         <v>34.380000000000003</v>
       </c>
-      <c r="I51" s="207">
+      <c r="I51" s="211">
         <v>3.03</v>
       </c>
-      <c r="J51" s="207">
+      <c r="J51" s="211">
         <f>H51+I51</f>
         <v>37.410000000000004</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C52" s="206"/>
+      <c r="C52" s="210"/>
       <c r="D52" s="149" t="s">
         <v>222</v>
       </c>
@@ -3952,12 +3970,12 @@
       <c r="G52" s="27">
         <v>0.77</v>
       </c>
-      <c r="H52" s="207"/>
-      <c r="I52" s="207"/>
-      <c r="J52" s="207"/>
+      <c r="H52" s="211"/>
+      <c r="I52" s="211"/>
+      <c r="J52" s="211"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C53" s="206"/>
+      <c r="C53" s="210"/>
       <c r="D53" s="149" t="s">
         <v>223</v>
       </c>
@@ -3970,9 +3988,9 @@
       <c r="G53" s="27">
         <v>1.53</v>
       </c>
-      <c r="H53" s="207"/>
-      <c r="I53" s="207"/>
-      <c r="J53" s="207"/>
+      <c r="H53" s="211"/>
+      <c r="I53" s="211"/>
+      <c r="J53" s="211"/>
     </row>
     <row r="54" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="51"/>
@@ -4011,146 +4029,169 @@
         <v>8.99</v>
       </c>
     </row>
-    <row r="56" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="7"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="24"/>
-      <c r="F56" s="24"/>
-      <c r="G56" s="25"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="9"/>
-      <c r="L56" s="35"/>
-    </row>
-    <row r="57" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="40" t="s">
+    <row r="56" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C56" s="51"/>
+      <c r="D56" s="52"/>
+      <c r="E56" s="53"/>
+      <c r="F56" s="53"/>
+      <c r="G56" s="54"/>
+      <c r="H56" s="158"/>
+      <c r="I56" s="158"/>
+      <c r="J56" s="158"/>
+      <c r="L56" s="57"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C57" s="206">
+        <v>43017</v>
+      </c>
+      <c r="D57" s="202" t="s">
+        <v>230</v>
+      </c>
+      <c r="E57" s="26">
+        <v>1</v>
+      </c>
+      <c r="F57" s="26">
+        <v>1</v>
+      </c>
+      <c r="G57" s="27">
+        <v>4.99</v>
+      </c>
+      <c r="H57" s="207">
+        <v>4.99</v>
+      </c>
+      <c r="I57" s="207">
+        <v>1.39</v>
+      </c>
+      <c r="J57" s="207">
+        <f>H57+I57</f>
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C58" s="51"/>
+      <c r="D58" s="52"/>
+      <c r="E58" s="53"/>
+      <c r="F58" s="53"/>
+      <c r="G58" s="54"/>
+      <c r="H58" s="158"/>
+      <c r="I58" s="158"/>
+      <c r="J58" s="158"/>
+      <c r="L58" s="57"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C59" s="208">
+        <v>43017</v>
+      </c>
+      <c r="D59" s="202" t="s">
+        <v>231</v>
+      </c>
+      <c r="E59" s="26">
+        <v>10</v>
+      </c>
+      <c r="F59" s="26">
+        <v>1</v>
+      </c>
+      <c r="G59" s="27">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="H59" s="209">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="I59" s="209">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="J59" s="209">
+        <v>9.0500000000000007</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="7"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="25"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="9"/>
+      <c r="L60" s="35"/>
+    </row>
+    <row r="61" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C57" s="41">
+      <c r="C61" s="41">
         <f ca="1">TODAY()</f>
         <v>43016</v>
       </c>
-      <c r="E57" s="29"/>
-      <c r="F57" s="29"/>
-      <c r="G57" s="29"/>
-      <c r="H57" s="29"/>
-      <c r="I57" s="28" t="s">
+      <c r="E61" s="29"/>
+      <c r="F61" s="29"/>
+      <c r="G61" s="29"/>
+      <c r="H61" s="29"/>
+      <c r="I61" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="J57" s="30">
-        <f>SUM(J4:J56)</f>
-        <v>257.25</v>
-      </c>
-      <c r="K57" s="24" t="s">
+      <c r="J61" s="30">
+        <f>SUM(J4:J60)</f>
+        <v>272.68</v>
+      </c>
+      <c r="K61" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="L57" s="39">
-        <f ca="1">(C57-C4)*0.0328767</f>
+      <c r="L61" s="39">
+        <f ca="1">(C61-C4)*0.0328767</f>
         <v>4.4054777999999999</v>
       </c>
-      <c r="M57" s="24" t="s">
+      <c r="M61" s="24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C58" s="7"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="25"/>
-      <c r="H58" s="31"/>
-      <c r="I58" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="J58" s="22">
-        <f ca="1">J57/L57</f>
-        <v>58.393212195962036</v>
-      </c>
-      <c r="K58" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="L58" s="36"/>
-      <c r="M58" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="N58" s="33"/>
-    </row>
-    <row r="59" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="58"/>
-      <c r="B59" s="58"/>
-      <c r="C59" s="44"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="46"/>
-      <c r="F59" s="46"/>
-      <c r="G59" s="47"/>
-      <c r="H59" s="48"/>
-      <c r="I59" s="59"/>
-      <c r="J59" s="48"/>
-      <c r="K59" s="58"/>
-      <c r="L59" s="60"/>
-      <c r="M59" s="58"/>
-      <c r="N59" s="58"/>
-      <c r="O59" s="58"/>
-    </row>
-    <row r="60" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C60" s="7"/>
-      <c r="D60" s="63" t="s">
-        <v>75</v>
-      </c>
-      <c r="E60" s="203" t="s">
-        <v>227</v>
-      </c>
-      <c r="H60" s="10"/>
-      <c r="I60" s="11"/>
-      <c r="J60" s="10"/>
-      <c r="L60" s="35"/>
-    </row>
-    <row r="61" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C61" s="7"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="24"/>
-      <c r="F61" s="24"/>
-      <c r="G61" s="25"/>
-      <c r="H61" s="10"/>
-      <c r="I61" s="11"/>
-      <c r="J61" s="10"/>
-      <c r="L61" s="35"/>
-    </row>
-    <row r="62" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C62" s="7"/>
       <c r="D62" s="8"/>
       <c r="E62" s="24"/>
       <c r="F62" s="24"/>
       <c r="G62" s="25"/>
-      <c r="H62" s="10"/>
-      <c r="I62" s="11"/>
-      <c r="J62" s="10"/>
-      <c r="L62" s="35"/>
+      <c r="H62" s="31"/>
+      <c r="I62" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="J62" s="22">
+        <f ca="1">J61/L61</f>
+        <v>61.895669977045401</v>
+      </c>
+      <c r="K62" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="L62" s="36"/>
+      <c r="M62" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="N62" s="33"/>
     </row>
     <row r="63" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C63" s="147" t="s">
-        <v>164</v>
-      </c>
-      <c r="D63" s="148"/>
-      <c r="E63" s="24"/>
-      <c r="F63" s="24"/>
-      <c r="G63" s="25"/>
-      <c r="H63" s="10"/>
-      <c r="I63" s="11"/>
-      <c r="J63" s="10"/>
-      <c r="L63" s="35"/>
+      <c r="A63" s="58"/>
+      <c r="B63" s="58"/>
+      <c r="C63" s="44"/>
+      <c r="D63" s="45"/>
+      <c r="E63" s="46"/>
+      <c r="F63" s="46"/>
+      <c r="G63" s="47"/>
+      <c r="H63" s="48"/>
+      <c r="I63" s="59"/>
+      <c r="J63" s="48"/>
+      <c r="K63" s="58"/>
+      <c r="L63" s="60"/>
+      <c r="M63" s="58"/>
+      <c r="N63" s="58"/>
+      <c r="O63" s="58"/>
     </row>
     <row r="64" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C64" s="49"/>
-      <c r="D64" s="95" t="s">
-        <v>0</v>
-      </c>
-      <c r="E64" s="98"/>
-      <c r="F64" s="98" t="s">
-        <v>160</v>
-      </c>
-      <c r="G64" s="99">
-        <v>3.39</v>
+      <c r="C64" s="7"/>
+      <c r="D64" s="63" t="s">
+        <v>75</v>
+      </c>
+      <c r="E64" s="203" t="s">
+        <v>227</v>
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="11"/>
@@ -4159,16 +4200,10 @@
     </row>
     <row r="65" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C65" s="7"/>
-      <c r="D65" s="95" t="s">
-        <v>1</v>
-      </c>
-      <c r="E65" s="98"/>
-      <c r="F65" s="98" t="s">
-        <v>160</v>
-      </c>
-      <c r="G65" s="99">
-        <v>1.39</v>
-      </c>
+      <c r="D65" s="8"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="24"/>
+      <c r="G65" s="25"/>
       <c r="H65" s="10"/>
       <c r="I65" s="11"/>
       <c r="J65" s="10"/>
@@ -4176,45 +4211,39 @@
     </row>
     <row r="66" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C66" s="7"/>
-      <c r="D66" s="95" t="str">
-        <f>D24</f>
-        <v>NOKIA 5110 LCD</v>
-      </c>
-      <c r="E66" s="98"/>
-      <c r="F66" s="98"/>
-      <c r="G66" s="99">
-        <f>G24</f>
-        <v>1.97</v>
-      </c>
+      <c r="D66" s="8"/>
+      <c r="E66" s="24"/>
+      <c r="F66" s="24"/>
+      <c r="G66" s="25"/>
       <c r="H66" s="10"/>
       <c r="I66" s="11"/>
       <c r="J66" s="10"/>
       <c r="L66" s="35"/>
     </row>
     <row r="67" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C67" s="7"/>
-      <c r="D67" s="95" t="s">
-        <v>5</v>
-      </c>
-      <c r="E67" s="98"/>
-      <c r="F67" s="98"/>
-      <c r="G67" s="99">
-        <v>0.2485</v>
-      </c>
+      <c r="C67" s="147" t="s">
+        <v>164</v>
+      </c>
+      <c r="D67" s="148"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="25"/>
       <c r="H67" s="10"/>
       <c r="I67" s="11"/>
       <c r="J67" s="10"/>
       <c r="L67" s="35"/>
     </row>
     <row r="68" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C68" s="7"/>
+      <c r="C68" s="49"/>
       <c r="D68" s="95" t="s">
-        <v>156</v>
+        <v>0</v>
       </c>
       <c r="E68" s="98"/>
-      <c r="F68" s="98"/>
+      <c r="F68" s="98" t="s">
+        <v>160</v>
+      </c>
       <c r="G68" s="99">
-        <v>0.29949999999999999</v>
+        <v>3.39</v>
       </c>
       <c r="H68" s="10"/>
       <c r="I68" s="11"/>
@@ -4224,12 +4253,14 @@
     <row r="69" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C69" s="7"/>
       <c r="D69" s="95" t="s">
-        <v>158</v>
+        <v>1</v>
       </c>
       <c r="E69" s="98"/>
-      <c r="F69" s="98"/>
+      <c r="F69" s="98" t="s">
+        <v>160</v>
+      </c>
       <c r="G69" s="99">
-        <v>1</v>
+        <v>1.39</v>
       </c>
       <c r="H69" s="10"/>
       <c r="I69" s="11"/>
@@ -4238,13 +4269,15 @@
     </row>
     <row r="70" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C70" s="7"/>
-      <c r="D70" s="95" t="s">
-        <v>155</v>
+      <c r="D70" s="95" t="str">
+        <f>D24</f>
+        <v>NOKIA 5110 LCD</v>
       </c>
       <c r="E70" s="98"/>
       <c r="F70" s="98"/>
       <c r="G70" s="99">
-        <v>6.25</v>
+        <f>G24</f>
+        <v>1.97</v>
       </c>
       <c r="H70" s="10"/>
       <c r="I70" s="11"/>
@@ -4254,12 +4287,12 @@
     <row r="71" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C71" s="7"/>
       <c r="D71" s="95" t="s">
-        <v>157</v>
+        <v>5</v>
       </c>
       <c r="E71" s="98"/>
       <c r="F71" s="98"/>
       <c r="G71" s="99">
-        <v>0.57950000000000002</v>
+        <v>0.2485</v>
       </c>
       <c r="H71" s="10"/>
       <c r="I71" s="11"/>
@@ -4269,12 +4302,12 @@
     <row r="72" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C72" s="7"/>
       <c r="D72" s="95" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="E72" s="98"/>
       <c r="F72" s="98"/>
       <c r="G72" s="99">
-        <v>1.0640000000000001</v>
+        <v>0.29949999999999999</v>
       </c>
       <c r="H72" s="10"/>
       <c r="I72" s="11"/>
@@ -4284,12 +4317,12 @@
     <row r="73" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C73" s="7"/>
       <c r="D73" s="95" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E73" s="98"/>
       <c r="F73" s="98"/>
       <c r="G73" s="99">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H73" s="10"/>
       <c r="I73" s="11"/>
@@ -4297,46 +4330,45 @@
       <c r="L73" s="35"/>
     </row>
     <row r="74" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C74" s="44"/>
-      <c r="D74" s="96" t="s">
-        <v>159</v>
-      </c>
-      <c r="E74" s="100"/>
-      <c r="F74" s="100"/>
-      <c r="G74" s="101">
-        <v>2</v>
-      </c>
-      <c r="H74" s="48"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="95" t="s">
+        <v>155</v>
+      </c>
+      <c r="E74" s="98"/>
+      <c r="F74" s="98"/>
+      <c r="G74" s="99">
+        <v>6.25</v>
+      </c>
+      <c r="H74" s="10"/>
       <c r="I74" s="11"/>
       <c r="J74" s="10"/>
       <c r="L74" s="35"/>
     </row>
     <row r="75" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="58"/>
-      <c r="B75" s="58"/>
-      <c r="C75" s="44"/>
-      <c r="D75" s="45"/>
-      <c r="E75" s="46"/>
-      <c r="F75" s="46"/>
-      <c r="G75" s="97">
-        <f>SUM(G64:G74)</f>
-        <v>18.691499999999998</v>
-      </c>
-      <c r="H75" s="48"/>
-      <c r="I75" s="59"/>
-      <c r="J75" s="48"/>
-      <c r="K75" s="58"/>
-      <c r="L75" s="60"/>
-      <c r="M75" s="58"/>
-      <c r="N75" s="58"/>
-      <c r="O75" s="58"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="95" t="s">
+        <v>157</v>
+      </c>
+      <c r="E75" s="98"/>
+      <c r="F75" s="98"/>
+      <c r="G75" s="99">
+        <v>0.57950000000000002</v>
+      </c>
+      <c r="H75" s="10"/>
+      <c r="I75" s="11"/>
+      <c r="J75" s="10"/>
+      <c r="L75" s="35"/>
     </row>
     <row r="76" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C76" s="7"/>
-      <c r="D76" s="8"/>
-      <c r="E76" s="24"/>
-      <c r="F76" s="24"/>
-      <c r="G76" s="25"/>
+      <c r="D76" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="E76" s="98"/>
+      <c r="F76" s="98"/>
+      <c r="G76" s="99">
+        <v>1.0640000000000001</v>
+      </c>
       <c r="H76" s="10"/>
       <c r="I76" s="11"/>
       <c r="J76" s="10"/>
@@ -4344,122 +4376,119 @@
     </row>
     <row r="77" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C77" s="7"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="24"/>
-      <c r="F77" s="24"/>
-      <c r="G77" s="25"/>
+      <c r="D77" s="95" t="s">
+        <v>161</v>
+      </c>
+      <c r="E77" s="98"/>
+      <c r="F77" s="98"/>
+      <c r="G77" s="99">
+        <v>0.5</v>
+      </c>
       <c r="H77" s="10"/>
       <c r="I77" s="11"/>
       <c r="J77" s="10"/>
       <c r="L77" s="35"/>
     </row>
     <row r="78" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C78" s="7"/>
-      <c r="D78" s="8"/>
-      <c r="E78" s="24"/>
-      <c r="F78" s="24"/>
-      <c r="G78" s="25"/>
-      <c r="H78" s="10"/>
+      <c r="C78" s="44"/>
+      <c r="D78" s="96" t="s">
+        <v>159</v>
+      </c>
+      <c r="E78" s="100"/>
+      <c r="F78" s="100"/>
+      <c r="G78" s="101">
+        <v>2</v>
+      </c>
+      <c r="H78" s="48"/>
       <c r="I78" s="11"/>
       <c r="J78" s="10"/>
       <c r="L78" s="35"/>
     </row>
     <row r="79" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C79" s="7"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="24"/>
-      <c r="F79" s="24"/>
-      <c r="G79" s="25"/>
-      <c r="H79" s="10"/>
-      <c r="I79" s="11"/>
-      <c r="J79" s="10"/>
-      <c r="L79" s="35"/>
-    </row>
-    <row r="80" spans="1:15" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C80" s="93" t="s">
+      <c r="A79" s="58"/>
+      <c r="B79" s="58"/>
+      <c r="C79" s="44"/>
+      <c r="D79" s="45"/>
+      <c r="E79" s="46"/>
+      <c r="F79" s="46"/>
+      <c r="G79" s="97">
+        <f>SUM(G68:G78)</f>
+        <v>18.691499999999998</v>
+      </c>
+      <c r="H79" s="48"/>
+      <c r="I79" s="59"/>
+      <c r="J79" s="48"/>
+      <c r="K79" s="58"/>
+      <c r="L79" s="60"/>
+      <c r="M79" s="58"/>
+      <c r="N79" s="58"/>
+      <c r="O79" s="58"/>
+    </row>
+    <row r="80" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C80" s="7"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="24"/>
+      <c r="F80" s="24"/>
+      <c r="G80" s="25"/>
+      <c r="H80" s="10"/>
+      <c r="I80" s="11"/>
+      <c r="J80" s="10"/>
+      <c r="L80" s="35"/>
+    </row>
+    <row r="81" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C81" s="7"/>
+      <c r="D81" s="8"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="25"/>
+      <c r="H81" s="10"/>
+      <c r="I81" s="11"/>
+      <c r="J81" s="10"/>
+      <c r="L81" s="35"/>
+    </row>
+    <row r="82" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C82" s="7"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="24"/>
+      <c r="F82" s="24"/>
+      <c r="G82" s="25"/>
+      <c r="H82" s="10"/>
+      <c r="I82" s="11"/>
+      <c r="J82" s="10"/>
+      <c r="L82" s="35"/>
+    </row>
+    <row r="83" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C83" s="7"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="24"/>
+      <c r="F83" s="24"/>
+      <c r="G83" s="25"/>
+      <c r="H83" s="10"/>
+      <c r="I83" s="11"/>
+      <c r="J83" s="10"/>
+      <c r="L83" s="35"/>
+    </row>
+    <row r="84" spans="1:15" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C84" s="93" t="s">
         <v>163</v>
       </c>
-      <c r="D80" s="94"/>
-      <c r="E80" s="18"/>
-      <c r="H80" s="14"/>
-      <c r="I80" s="17"/>
-      <c r="J80" s="14"/>
-      <c r="K80" s="14"/>
-      <c r="L80" s="14"/>
-    </row>
-    <row r="81" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C81" s="144"/>
-      <c r="D81" s="151" t="s">
-        <v>226</v>
-      </c>
-      <c r="E81" s="98"/>
-      <c r="F81" s="98"/>
-      <c r="G81" s="99">
-        <v>1.53</v>
-      </c>
-      <c r="H81" s="157"/>
-      <c r="I81" s="158"/>
-      <c r="J81" s="157"/>
-      <c r="K81" s="157"/>
-      <c r="L81" s="159"/>
-    </row>
-    <row r="82" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C82" s="144"/>
-      <c r="D82" s="151" t="s">
-        <v>30</v>
-      </c>
-      <c r="E82" s="98"/>
-      <c r="F82" s="98"/>
-      <c r="G82" s="99">
-        <v>33.57</v>
-      </c>
-      <c r="H82" s="157"/>
-      <c r="I82" s="158"/>
-      <c r="J82" s="157"/>
-      <c r="K82" s="157"/>
-      <c r="L82" s="159"/>
-    </row>
-    <row r="83" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C83" s="144"/>
-      <c r="D83" s="151" t="s">
-        <v>2</v>
-      </c>
-      <c r="E83" s="98"/>
-      <c r="F83" s="98"/>
-      <c r="G83" s="99">
-        <v>6.56</v>
-      </c>
-      <c r="H83" s="157"/>
-      <c r="I83" s="158"/>
-      <c r="J83" s="157"/>
-      <c r="K83" s="157"/>
-      <c r="L83" s="159"/>
-    </row>
-    <row r="84" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C84" s="144"/>
-      <c r="D84" s="151" t="s">
-        <v>11</v>
-      </c>
-      <c r="E84" s="98"/>
-      <c r="F84" s="98"/>
-      <c r="G84" s="99">
-        <v>2.57</v>
-      </c>
-      <c r="H84" s="157"/>
-      <c r="I84" s="158"/>
-      <c r="J84" s="157"/>
-      <c r="K84" s="157"/>
-      <c r="L84" s="159"/>
+      <c r="D84" s="94"/>
+      <c r="E84" s="18"/>
+      <c r="H84" s="14"/>
+      <c r="I84" s="17"/>
+      <c r="J84" s="14"/>
+      <c r="K84" s="14"/>
+      <c r="L84" s="14"/>
     </row>
     <row r="85" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C85" s="144"/>
       <c r="D85" s="151" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="E85" s="98"/>
       <c r="F85" s="98"/>
       <c r="G85" s="99">
-        <v>5.22</v>
+        <v>1.53</v>
       </c>
       <c r="H85" s="157"/>
       <c r="I85" s="158"/>
@@ -4470,12 +4499,12 @@
     <row r="86" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C86" s="144"/>
       <c r="D86" s="151" t="s">
-        <v>162</v>
+        <v>30</v>
       </c>
       <c r="E86" s="98"/>
       <c r="F86" s="98"/>
       <c r="G86" s="99">
-        <v>0.39900000000000002</v>
+        <v>33.57</v>
       </c>
       <c r="H86" s="157"/>
       <c r="I86" s="158"/>
@@ -4483,364 +4512,387 @@
       <c r="K86" s="157"/>
       <c r="L86" s="159"/>
     </row>
-    <row r="87" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C87" s="145"/>
+    <row r="87" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C87" s="144"/>
       <c r="D87" s="151" t="s">
-        <v>73</v>
+        <v>2</v>
       </c>
       <c r="E87" s="98"/>
       <c r="F87" s="98"/>
       <c r="G87" s="99">
-        <v>0.77</v>
-      </c>
-      <c r="H87" s="9"/>
-      <c r="I87" s="13"/>
-      <c r="J87" s="9"/>
-      <c r="K87" s="9"/>
-      <c r="L87" s="38"/>
-    </row>
-    <row r="88" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C88" s="145"/>
+        <v>6.56</v>
+      </c>
+      <c r="H87" s="157"/>
+      <c r="I87" s="158"/>
+      <c r="J87" s="157"/>
+      <c r="K87" s="157"/>
+      <c r="L87" s="159"/>
+    </row>
+    <row r="88" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C88" s="144"/>
       <c r="D88" s="151" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E88" s="98"/>
       <c r="F88" s="98"/>
       <c r="G88" s="99">
-        <v>0.02</v>
-      </c>
-      <c r="H88" s="9"/>
-      <c r="I88" s="13"/>
-      <c r="J88" s="9"/>
-      <c r="K88" s="9"/>
-      <c r="L88" s="38"/>
-    </row>
-    <row r="89" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C89" s="145"/>
-      <c r="D89" s="153" t="s">
-        <v>168</v>
+        <v>2.57</v>
+      </c>
+      <c r="H88" s="157"/>
+      <c r="I88" s="158"/>
+      <c r="J88" s="157"/>
+      <c r="K88" s="157"/>
+      <c r="L88" s="159"/>
+    </row>
+    <row r="89" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C89" s="144"/>
+      <c r="D89" s="151" t="s">
+        <v>61</v>
       </c>
       <c r="E89" s="98"/>
       <c r="F89" s="98"/>
       <c r="G89" s="99">
-        <f>5.72+(0.5*4.99)</f>
-        <v>8.2149999999999999</v>
-      </c>
-      <c r="H89" s="9"/>
-      <c r="I89" s="13"/>
-      <c r="J89" s="9"/>
-      <c r="K89" s="9"/>
-      <c r="L89" s="38"/>
-    </row>
-    <row r="90" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C90" s="145"/>
+        <v>5.22</v>
+      </c>
+      <c r="H89" s="157"/>
+      <c r="I89" s="158"/>
+      <c r="J89" s="157"/>
+      <c r="K89" s="157"/>
+      <c r="L89" s="159"/>
+    </row>
+    <row r="90" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C90" s="144"/>
       <c r="D90" s="151" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E90" s="98"/>
       <c r="F90" s="98"/>
       <c r="G90" s="99">
-        <f>2.83+(0.5*4.99)</f>
-        <v>5.3250000000000002</v>
-      </c>
-      <c r="H90" s="9"/>
-      <c r="I90" s="13"/>
-      <c r="J90" s="9"/>
-      <c r="K90" s="9"/>
-      <c r="L90" s="38"/>
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="H90" s="157"/>
+      <c r="I90" s="158"/>
+      <c r="J90" s="157"/>
+      <c r="K90" s="157"/>
+      <c r="L90" s="159"/>
     </row>
     <row r="91" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C91" s="146"/>
-      <c r="D91" s="152" t="s">
-        <v>74</v>
-      </c>
-      <c r="E91" s="100"/>
-      <c r="F91" s="100"/>
-      <c r="G91" s="101">
-        <v>1.53</v>
-      </c>
-      <c r="H91" s="160"/>
+      <c r="C91" s="145"/>
+      <c r="D91" s="151" t="s">
+        <v>73</v>
+      </c>
+      <c r="E91" s="98"/>
+      <c r="F91" s="98"/>
+      <c r="G91" s="99">
+        <v>0.77</v>
+      </c>
+      <c r="H91" s="9"/>
       <c r="I91" s="13"/>
       <c r="J91" s="9"/>
       <c r="K91" s="9"/>
       <c r="L91" s="38"/>
     </row>
-    <row r="92" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="67"/>
-      <c r="B92" s="67"/>
-      <c r="C92" s="68"/>
-      <c r="D92" s="69"/>
-      <c r="E92" s="70"/>
-      <c r="F92" s="70"/>
-      <c r="G92" s="97">
-        <f>SUM(G81:G91)</f>
+    <row r="92" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C92" s="145"/>
+      <c r="D92" s="151" t="s">
+        <v>6</v>
+      </c>
+      <c r="E92" s="98"/>
+      <c r="F92" s="98"/>
+      <c r="G92" s="99">
+        <v>0.02</v>
+      </c>
+      <c r="H92" s="9"/>
+      <c r="I92" s="13"/>
+      <c r="J92" s="9"/>
+      <c r="K92" s="9"/>
+      <c r="L92" s="38"/>
+    </row>
+    <row r="93" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C93" s="145"/>
+      <c r="D93" s="153" t="s">
+        <v>168</v>
+      </c>
+      <c r="E93" s="98"/>
+      <c r="F93" s="98"/>
+      <c r="G93" s="99">
+        <f>5.72+(0.5*4.99)</f>
+        <v>8.2149999999999999</v>
+      </c>
+      <c r="H93" s="9"/>
+      <c r="I93" s="13"/>
+      <c r="J93" s="9"/>
+      <c r="K93" s="9"/>
+      <c r="L93" s="38"/>
+    </row>
+    <row r="94" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C94" s="145"/>
+      <c r="D94" s="151" t="s">
+        <v>169</v>
+      </c>
+      <c r="E94" s="98"/>
+      <c r="F94" s="98"/>
+      <c r="G94" s="99">
+        <f>2.83+(0.5*4.99)</f>
+        <v>5.3250000000000002</v>
+      </c>
+      <c r="H94" s="9"/>
+      <c r="I94" s="13"/>
+      <c r="J94" s="9"/>
+      <c r="K94" s="9"/>
+      <c r="L94" s="38"/>
+    </row>
+    <row r="95" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C95" s="146"/>
+      <c r="D95" s="152" t="s">
+        <v>74</v>
+      </c>
+      <c r="E95" s="100"/>
+      <c r="F95" s="100"/>
+      <c r="G95" s="101">
+        <v>1.53</v>
+      </c>
+      <c r="H95" s="160"/>
+      <c r="I95" s="13"/>
+      <c r="J95" s="9"/>
+      <c r="K95" s="9"/>
+      <c r="L95" s="38"/>
+    </row>
+    <row r="96" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="67"/>
+      <c r="B96" s="67"/>
+      <c r="C96" s="68"/>
+      <c r="D96" s="69"/>
+      <c r="E96" s="70"/>
+      <c r="F96" s="70"/>
+      <c r="G96" s="97">
+        <f>SUM(G85:G95)</f>
         <v>65.709000000000017</v>
       </c>
-      <c r="H92" s="71"/>
-      <c r="I92" s="72"/>
-      <c r="J92" s="71"/>
-      <c r="K92" s="67"/>
-      <c r="L92" s="67"/>
-      <c r="M92" s="67"/>
-      <c r="N92" s="67"/>
-      <c r="O92" s="67"/>
-    </row>
-    <row r="93" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C93" s="51"/>
-      <c r="D93" s="73"/>
-      <c r="E93" s="74"/>
-      <c r="F93" s="74"/>
-      <c r="G93" s="75"/>
-      <c r="H93" s="55"/>
-      <c r="I93" s="56"/>
-      <c r="J93" s="55"/>
-      <c r="L93" s="57"/>
-    </row>
-    <row r="94" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="79"/>
-      <c r="B95" s="79"/>
-      <c r="C95" s="80"/>
-      <c r="D95" s="81"/>
-      <c r="E95" s="82"/>
-      <c r="F95" s="82"/>
-      <c r="G95" s="83"/>
-      <c r="H95" s="84"/>
-      <c r="I95" s="85"/>
-      <c r="J95" s="84"/>
-      <c r="K95" s="79"/>
-      <c r="L95" s="79"/>
-      <c r="M95" s="79"/>
-      <c r="N95" s="79"/>
-      <c r="O95" s="79"/>
-    </row>
-    <row r="96" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C96" s="87"/>
-      <c r="D96" s="88"/>
-      <c r="E96" s="61"/>
-      <c r="F96" s="61"/>
-      <c r="G96" s="89"/>
-      <c r="H96" s="90"/>
-      <c r="I96" s="91"/>
-      <c r="J96" s="90"/>
-      <c r="L96" s="92"/>
-    </row>
-    <row r="97" spans="1:15" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C97" s="93" t="s">
+      <c r="H96" s="71"/>
+      <c r="I96" s="72"/>
+      <c r="J96" s="71"/>
+      <c r="K96" s="67"/>
+      <c r="L96" s="67"/>
+      <c r="M96" s="67"/>
+      <c r="N96" s="67"/>
+      <c r="O96" s="67"/>
+    </row>
+    <row r="97" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C97" s="51"/>
+      <c r="D97" s="73"/>
+      <c r="E97" s="74"/>
+      <c r="F97" s="74"/>
+      <c r="G97" s="75"/>
+      <c r="H97" s="55"/>
+      <c r="I97" s="56"/>
+      <c r="J97" s="55"/>
+      <c r="L97" s="57"/>
+    </row>
+    <row r="98" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="79"/>
+      <c r="B99" s="79"/>
+      <c r="C99" s="80"/>
+      <c r="D99" s="81"/>
+      <c r="E99" s="82"/>
+      <c r="F99" s="82"/>
+      <c r="G99" s="83"/>
+      <c r="H99" s="84"/>
+      <c r="I99" s="85"/>
+      <c r="J99" s="84"/>
+      <c r="K99" s="79"/>
+      <c r="L99" s="79"/>
+      <c r="M99" s="79"/>
+      <c r="N99" s="79"/>
+      <c r="O99" s="79"/>
+    </row>
+    <row r="100" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C100" s="87"/>
+      <c r="D100" s="88"/>
+      <c r="E100" s="61"/>
+      <c r="F100" s="61"/>
+      <c r="G100" s="89"/>
+      <c r="H100" s="90"/>
+      <c r="I100" s="91"/>
+      <c r="J100" s="90"/>
+      <c r="L100" s="92"/>
+    </row>
+    <row r="101" spans="1:15" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C101" s="93" t="s">
         <v>165</v>
       </c>
-      <c r="D97" s="94"/>
-      <c r="E97" s="18"/>
-      <c r="H97" s="64"/>
-      <c r="I97" s="65"/>
-      <c r="J97" s="64"/>
-    </row>
-    <row r="98" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C98" s="144"/>
-      <c r="D98" s="151" t="s">
+      <c r="D101" s="94"/>
+      <c r="E101" s="18"/>
+      <c r="H101" s="64"/>
+      <c r="I101" s="65"/>
+      <c r="J101" s="64"/>
+    </row>
+    <row r="102" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C102" s="144"/>
+      <c r="D102" s="151" t="s">
         <v>225</v>
-      </c>
-      <c r="E98" s="98"/>
-      <c r="F98" s="98"/>
-      <c r="G98" s="99">
-        <v>1.53</v>
-      </c>
-      <c r="H98" s="55"/>
-      <c r="I98" s="56"/>
-      <c r="J98" s="55"/>
-      <c r="L98" s="57"/>
-    </row>
-    <row r="99" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C99" s="144"/>
-      <c r="D99" s="151" t="s">
-        <v>166</v>
-      </c>
-      <c r="E99" s="98"/>
-      <c r="F99" s="98"/>
-      <c r="G99" s="99">
-        <v>33.57</v>
-      </c>
-      <c r="H99" s="55"/>
-      <c r="I99" s="56"/>
-      <c r="J99" s="55"/>
-      <c r="L99" s="57"/>
-    </row>
-    <row r="100" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C100" s="144"/>
-      <c r="D100" s="151" t="s">
-        <v>2</v>
-      </c>
-      <c r="E100" s="98"/>
-      <c r="F100" s="98"/>
-      <c r="G100" s="99">
-        <v>6.56</v>
-      </c>
-      <c r="H100" s="55"/>
-      <c r="I100" s="56"/>
-      <c r="J100" s="55"/>
-      <c r="L100" s="57"/>
-    </row>
-    <row r="101" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C101" s="144"/>
-      <c r="D101" s="151" t="s">
-        <v>61</v>
-      </c>
-      <c r="E101" s="98"/>
-      <c r="F101" s="98"/>
-      <c r="G101" s="99">
-        <v>6.91</v>
-      </c>
-      <c r="H101" s="55"/>
-      <c r="I101" s="56"/>
-      <c r="J101" s="55"/>
-      <c r="L101" s="57"/>
-    </row>
-    <row r="102" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C102" s="145"/>
-      <c r="D102" s="151" t="s">
-        <v>162</v>
       </c>
       <c r="E102" s="98"/>
       <c r="F102" s="98"/>
       <c r="G102" s="99">
-        <v>0.39900000000000002</v>
-      </c>
-      <c r="H102" s="10"/>
-      <c r="I102" s="11"/>
-      <c r="J102" s="10"/>
-      <c r="L102" s="35"/>
-    </row>
-    <row r="103" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C103" s="145"/>
+        <v>1.53</v>
+      </c>
+      <c r="H102" s="55"/>
+      <c r="I102" s="56"/>
+      <c r="J102" s="55"/>
+      <c r="L102" s="57"/>
+    </row>
+    <row r="103" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C103" s="144"/>
       <c r="D103" s="151" t="s">
-        <v>11</v>
+        <v>166</v>
       </c>
       <c r="E103" s="98"/>
       <c r="F103" s="98"/>
       <c r="G103" s="99">
-        <v>2.57</v>
-      </c>
-      <c r="H103" s="10"/>
-      <c r="I103" s="11"/>
-      <c r="J103" s="10"/>
-      <c r="L103" s="35"/>
-    </row>
-    <row r="104" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C104" s="145"/>
+        <v>33.57</v>
+      </c>
+      <c r="H103" s="55"/>
+      <c r="I103" s="56"/>
+      <c r="J103" s="55"/>
+      <c r="L103" s="57"/>
+    </row>
+    <row r="104" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C104" s="144"/>
       <c r="D104" s="151" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E104" s="98"/>
       <c r="F104" s="98"/>
       <c r="G104" s="99">
-        <v>0.02</v>
-      </c>
-      <c r="H104" s="10"/>
-      <c r="I104" s="11"/>
-      <c r="J104" s="10"/>
-      <c r="L104" s="35"/>
-    </row>
-    <row r="105" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>6.56</v>
+      </c>
+      <c r="H104" s="55"/>
+      <c r="I104" s="56"/>
+      <c r="J104" s="55"/>
+      <c r="L104" s="57"/>
+    </row>
+    <row r="105" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C105" s="144"/>
       <c r="D105" s="151" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="E105" s="98"/>
       <c r="F105" s="98"/>
       <c r="G105" s="99">
-        <v>0.77</v>
-      </c>
-    </row>
-    <row r="106" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D106" s="154" t="s">
-        <v>74</v>
-      </c>
-      <c r="E106" s="155"/>
-      <c r="F106" s="155"/>
-      <c r="G106" s="156">
-        <v>1.53</v>
-      </c>
-    </row>
-    <row r="107" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C107" s="146"/>
-      <c r="D107" s="152" t="s">
-        <v>224</v>
-      </c>
-      <c r="E107" s="100"/>
-      <c r="F107" s="100"/>
-      <c r="G107" s="101">
-        <v>3.78</v>
-      </c>
-      <c r="H107" s="48"/>
+        <v>6.91</v>
+      </c>
+      <c r="H105" s="55"/>
+      <c r="I105" s="56"/>
+      <c r="J105" s="55"/>
+      <c r="L105" s="57"/>
+    </row>
+    <row r="106" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C106" s="145"/>
+      <c r="D106" s="151" t="s">
+        <v>162</v>
+      </c>
+      <c r="E106" s="98"/>
+      <c r="F106" s="98"/>
+      <c r="G106" s="99">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="H106" s="10"/>
+      <c r="I106" s="11"/>
+      <c r="J106" s="10"/>
+      <c r="L106" s="35"/>
+    </row>
+    <row r="107" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C107" s="145"/>
+      <c r="D107" s="151" t="s">
+        <v>11</v>
+      </c>
+      <c r="E107" s="98"/>
+      <c r="F107" s="98"/>
+      <c r="G107" s="99">
+        <v>2.57</v>
+      </c>
+      <c r="H107" s="10"/>
       <c r="I107" s="11"/>
       <c r="J107" s="10"/>
-      <c r="K107" s="12"/>
       <c r="L107" s="35"/>
-      <c r="M107" s="12"/>
-      <c r="N107" s="12"/>
-      <c r="O107" s="12"/>
-    </row>
-    <row r="108" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="67"/>
-      <c r="B108" s="67"/>
-      <c r="C108" s="68"/>
-      <c r="D108" s="69"/>
-      <c r="E108" s="70"/>
-      <c r="F108" s="70"/>
-      <c r="G108" s="97">
-        <f>SUM(G98:G107)</f>
+    </row>
+    <row r="108" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C108" s="145"/>
+      <c r="D108" s="151" t="s">
+        <v>6</v>
+      </c>
+      <c r="E108" s="98"/>
+      <c r="F108" s="98"/>
+      <c r="G108" s="99">
+        <v>0.02</v>
+      </c>
+      <c r="H108" s="10"/>
+      <c r="I108" s="11"/>
+      <c r="J108" s="10"/>
+      <c r="L108" s="35"/>
+    </row>
+    <row r="109" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D109" s="151" t="s">
+        <v>73</v>
+      </c>
+      <c r="E109" s="98"/>
+      <c r="F109" s="98"/>
+      <c r="G109" s="99">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D110" s="154" t="s">
+        <v>74</v>
+      </c>
+      <c r="E110" s="155"/>
+      <c r="F110" s="155"/>
+      <c r="G110" s="156">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C111" s="146"/>
+      <c r="D111" s="152" t="s">
+        <v>224</v>
+      </c>
+      <c r="E111" s="100"/>
+      <c r="F111" s="100"/>
+      <c r="G111" s="101">
+        <v>3.78</v>
+      </c>
+      <c r="H111" s="48"/>
+      <c r="I111" s="11"/>
+      <c r="J111" s="10"/>
+      <c r="K111" s="12"/>
+      <c r="L111" s="35"/>
+      <c r="M111" s="12"/>
+      <c r="N111" s="12"/>
+      <c r="O111" s="12"/>
+    </row>
+    <row r="112" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="67"/>
+      <c r="B112" s="67"/>
+      <c r="C112" s="68"/>
+      <c r="D112" s="69"/>
+      <c r="E112" s="70"/>
+      <c r="F112" s="70"/>
+      <c r="G112" s="97">
+        <f>SUM(G102:G111)</f>
         <v>57.639000000000017</v>
       </c>
-      <c r="H108" s="71"/>
-      <c r="I108" s="72"/>
-      <c r="J108" s="71"/>
-      <c r="K108" s="67"/>
-      <c r="L108" s="67"/>
-      <c r="M108" s="67"/>
-      <c r="N108" s="67"/>
-      <c r="O108" s="67"/>
-    </row>
-    <row r="109" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C109" s="51"/>
-      <c r="D109" s="52"/>
-      <c r="E109" s="53"/>
-      <c r="F109" s="53"/>
-      <c r="G109" s="54"/>
-      <c r="H109" s="55"/>
-      <c r="I109" s="56"/>
-      <c r="J109" s="55"/>
-      <c r="L109" s="57"/>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C110" s="51"/>
-      <c r="D110" s="52"/>
-      <c r="E110" s="53"/>
-      <c r="F110" s="53"/>
-      <c r="G110" s="54"/>
-      <c r="H110" s="55"/>
-      <c r="I110" s="56"/>
-      <c r="J110" s="55"/>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C111" s="51"/>
-      <c r="D111" s="52"/>
-      <c r="E111" s="53"/>
-      <c r="F111" s="53"/>
-      <c r="G111" s="54"/>
-      <c r="H111" s="55"/>
-      <c r="I111" s="56"/>
-      <c r="J111" s="55"/>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C112" s="51"/>
-      <c r="D112" s="52"/>
-      <c r="E112" s="53"/>
-      <c r="F112" s="53"/>
-      <c r="G112" s="54"/>
-      <c r="H112" s="55"/>
-      <c r="I112" s="56"/>
-      <c r="J112" s="55"/>
-    </row>
-    <row r="113" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H112" s="71"/>
+      <c r="I112" s="72"/>
+      <c r="J112" s="71"/>
+      <c r="K112" s="67"/>
+      <c r="L112" s="67"/>
+      <c r="M112" s="67"/>
+      <c r="N112" s="67"/>
+      <c r="O112" s="67"/>
+    </row>
+    <row r="113" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C113" s="51"/>
       <c r="D113" s="52"/>
       <c r="E113" s="53"/>
@@ -4849,8 +4901,9 @@
       <c r="H113" s="55"/>
       <c r="I113" s="56"/>
       <c r="J113" s="55"/>
-    </row>
-    <row r="114" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="L113" s="57"/>
+    </row>
+    <row r="114" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C114" s="51"/>
       <c r="D114" s="52"/>
       <c r="E114" s="53"/>
@@ -4860,7 +4913,7 @@
       <c r="I114" s="56"/>
       <c r="J114" s="55"/>
     </row>
-    <row r="115" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C115" s="51"/>
       <c r="D115" s="52"/>
       <c r="E115" s="53"/>
@@ -4870,7 +4923,7 @@
       <c r="I115" s="56"/>
       <c r="J115" s="55"/>
     </row>
-    <row r="116" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C116" s="51"/>
       <c r="D116" s="52"/>
       <c r="E116" s="53"/>
@@ -4880,7 +4933,7 @@
       <c r="I116" s="56"/>
       <c r="J116" s="55"/>
     </row>
-    <row r="117" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C117" s="51"/>
       <c r="D117" s="52"/>
       <c r="E117" s="53"/>
@@ -4890,7 +4943,7 @@
       <c r="I117" s="56"/>
       <c r="J117" s="55"/>
     </row>
-    <row r="118" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C118" s="51"/>
       <c r="D118" s="52"/>
       <c r="E118" s="53"/>
@@ -4900,7 +4953,7 @@
       <c r="I118" s="56"/>
       <c r="J118" s="55"/>
     </row>
-    <row r="119" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C119" s="51"/>
       <c r="D119" s="52"/>
       <c r="E119" s="53"/>
@@ -4910,7 +4963,7 @@
       <c r="I119" s="56"/>
       <c r="J119" s="55"/>
     </row>
-    <row r="120" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C120" s="51"/>
       <c r="D120" s="52"/>
       <c r="E120" s="53"/>
@@ -4920,7 +4973,7 @@
       <c r="I120" s="56"/>
       <c r="J120" s="55"/>
     </row>
-    <row r="121" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C121" s="51"/>
       <c r="D121" s="52"/>
       <c r="E121" s="53"/>
@@ -4930,7 +4983,7 @@
       <c r="I121" s="56"/>
       <c r="J121" s="55"/>
     </row>
-    <row r="122" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C122" s="51"/>
       <c r="D122" s="52"/>
       <c r="E122" s="53"/>
@@ -4940,7 +4993,7 @@
       <c r="I122" s="56"/>
       <c r="J122" s="55"/>
     </row>
-    <row r="123" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C123" s="51"/>
       <c r="D123" s="52"/>
       <c r="E123" s="53"/>
@@ -4950,7 +5003,7 @@
       <c r="I123" s="56"/>
       <c r="J123" s="55"/>
     </row>
-    <row r="124" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C124" s="51"/>
       <c r="D124" s="52"/>
       <c r="E124" s="53"/>
@@ -4960,7 +5013,7 @@
       <c r="I124" s="56"/>
       <c r="J124" s="55"/>
     </row>
-    <row r="125" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C125" s="51"/>
       <c r="D125" s="52"/>
       <c r="E125" s="53"/>
@@ -4970,7 +5023,7 @@
       <c r="I125" s="56"/>
       <c r="J125" s="55"/>
     </row>
-    <row r="126" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C126" s="51"/>
       <c r="D126" s="52"/>
       <c r="E126" s="53"/>
@@ -4980,7 +5033,7 @@
       <c r="I126" s="56"/>
       <c r="J126" s="55"/>
     </row>
-    <row r="127" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C127" s="51"/>
       <c r="D127" s="52"/>
       <c r="E127" s="53"/>
@@ -4990,7 +5043,7 @@
       <c r="I127" s="56"/>
       <c r="J127" s="55"/>
     </row>
-    <row r="128" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C128" s="51"/>
       <c r="D128" s="52"/>
       <c r="E128" s="53"/>
@@ -5480,17 +5533,57 @@
       <c r="I176" s="56"/>
       <c r="J176" s="55"/>
     </row>
-    <row r="177" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C177" s="51"/>
       <c r="D177" s="52"/>
       <c r="E177" s="53"/>
       <c r="F177" s="53"/>
       <c r="G177" s="54"/>
-    </row>
-    <row r="178" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="H177" s="55"/>
+      <c r="I177" s="56"/>
+      <c r="J177" s="55"/>
+    </row>
+    <row r="178" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C178" s="51"/>
       <c r="D178" s="52"/>
       <c r="E178" s="53"/>
       <c r="F178" s="53"/>
       <c r="G178" s="54"/>
+      <c r="H178" s="55"/>
+      <c r="I178" s="56"/>
+      <c r="J178" s="55"/>
+    </row>
+    <row r="179" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C179" s="51"/>
+      <c r="D179" s="52"/>
+      <c r="E179" s="53"/>
+      <c r="F179" s="53"/>
+      <c r="G179" s="54"/>
+      <c r="H179" s="55"/>
+      <c r="I179" s="56"/>
+      <c r="J179" s="55"/>
+    </row>
+    <row r="180" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C180" s="51"/>
+      <c r="D180" s="52"/>
+      <c r="E180" s="53"/>
+      <c r="F180" s="53"/>
+      <c r="G180" s="54"/>
+      <c r="H180" s="55"/>
+      <c r="I180" s="56"/>
+      <c r="J180" s="55"/>
+    </row>
+    <row r="181" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D181" s="52"/>
+      <c r="E181" s="53"/>
+      <c r="F181" s="53"/>
+      <c r="G181" s="54"/>
+    </row>
+    <row r="182" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D182" s="52"/>
+      <c r="E182" s="53"/>
+      <c r="F182" s="53"/>
+      <c r="G182" s="54"/>
     </row>
   </sheetData>
   <sortState ref="C4:H19">
@@ -6442,21 +6535,21 @@
       <c r="AB16" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="AN16" s="211" t="s">
+      <c r="AN16" s="215" t="s">
         <v>123</v>
       </c>
-      <c r="AO16" s="211"/>
-      <c r="AP16" s="211"/>
-      <c r="AQ16" s="211"/>
-      <c r="AT16" s="210" t="s">
+      <c r="AO16" s="215"/>
+      <c r="AP16" s="215"/>
+      <c r="AQ16" s="215"/>
+      <c r="AT16" s="214" t="s">
         <v>119</v>
       </c>
-      <c r="AU16" s="210"/>
-      <c r="AV16" s="210"/>
-      <c r="AW16" s="210"/>
-      <c r="AX16" s="210"/>
-      <c r="AY16" s="210"/>
-      <c r="AZ16" s="210"/>
+      <c r="AU16" s="214"/>
+      <c r="AV16" s="214"/>
+      <c r="AW16" s="214"/>
+      <c r="AX16" s="214"/>
+      <c r="AY16" s="214"/>
+      <c r="AZ16" s="214"/>
     </row>
     <row r="17" spans="25:59" x14ac:dyDescent="0.25">
       <c r="Y17" s="108" t="s">
@@ -6471,22 +6564,22 @@
       <c r="AB17" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="AJ17" s="210" t="s">
+      <c r="AJ17" s="214" t="s">
         <v>117</v>
       </c>
-      <c r="AK17" s="210"/>
-      <c r="AL17" s="210"/>
-      <c r="AN17" s="211"/>
-      <c r="AO17" s="211"/>
-      <c r="AP17" s="211"/>
-      <c r="AQ17" s="211"/>
+      <c r="AK17" s="214"/>
+      <c r="AL17" s="214"/>
+      <c r="AN17" s="215"/>
+      <c r="AO17" s="215"/>
+      <c r="AP17" s="215"/>
+      <c r="AQ17" s="215"/>
     </row>
     <row r="19" spans="25:59" x14ac:dyDescent="0.25">
       <c r="AP19" s="195" t="s">
         <v>216</v>
       </c>
       <c r="AQ19" s="117">
-        <f>INVENTORY!G92</f>
+        <f>INVENTORY!G96</f>
         <v>65.709000000000017</v>
       </c>
       <c r="AS19" s="196" t="s">
@@ -6494,11 +6587,11 @@
       </c>
     </row>
     <row r="20" spans="25:59" x14ac:dyDescent="0.25">
-      <c r="AK20" s="212" t="s">
+      <c r="AK20" s="216" t="s">
         <v>120</v>
       </c>
-      <c r="AL20" s="212"/>
-      <c r="AM20" s="212"/>
+      <c r="AL20" s="216"/>
+      <c r="AM20" s="216"/>
       <c r="AP20" s="195" t="s">
         <v>217</v>
       </c>
@@ -6793,7 +6886,7 @@
         <f t="shared" si="1"/>
         <v>6.6300000000000008</v>
       </c>
-      <c r="H11" s="213">
+      <c r="H11" s="217">
         <v>3.39</v>
       </c>
       <c r="I11" s="172" t="s">
@@ -6823,7 +6916,7 @@
         <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
-      <c r="H12" s="213"/>
+      <c r="H12" s="217"/>
       <c r="I12" s="172" t="s">
         <v>186</v>
       </c>
@@ -6879,7 +6972,7 @@
         <f t="shared" si="1"/>
         <v>57.199999999999996</v>
       </c>
-      <c r="H14" s="214">
+      <c r="H14" s="218">
         <v>4.99</v>
       </c>
       <c r="I14" s="172" t="s">
@@ -6908,7 +7001,7 @@
         <f t="shared" si="1"/>
         <v>28.3</v>
       </c>
-      <c r="H15" s="215"/>
+      <c r="H15" s="219"/>
       <c r="I15" s="182" t="s">
         <v>228</v>
       </c>

</xml_diff>

<commit_message>
bought a digital potentiometer
</commit_message>
<xml_diff>
--- a/BillOfMaterials/INVENTORY.xlsx
+++ b/BillOfMaterials/INVENTORY.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="236">
   <si>
     <t>Arduino Nano</t>
   </si>
@@ -1324,6 +1324,18 @@
   </si>
   <si>
     <t>BREAK AWAY 40 PIN FEMAL HEADER (EBAY)</t>
+  </si>
+  <si>
+    <t>5PCS 40PIN SHORT FEMALE HEADER (EBAY)</t>
+  </si>
+  <si>
+    <t>668  SMT 0931 MAGNETIC BUZZER (DIGIKEY)</t>
+  </si>
+  <si>
+    <t>POT 1K THUMBWHEEL VERTICAL (DIGIKEY)</t>
+  </si>
+  <si>
+    <t>X9C102 DIP DIGITAL POT</t>
   </si>
 </sst>
 </file>
@@ -1888,7 +1900,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="220">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2342,6 +2354,12 @@
     </xf>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2909,11 +2927,11 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:AB182"/>
+  <dimension ref="A1:AB189"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R60" sqref="R60"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3000,7 +3018,7 @@
       <c r="L3" s="35"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C4" s="210">
+      <c r="C4" s="212">
         <v>42882</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -3015,26 +3033,26 @@
       <c r="G4" s="27">
         <v>6.99</v>
       </c>
-      <c r="H4" s="213">
+      <c r="H4" s="215">
         <f>SUM(G4:G10)</f>
         <v>48.1</v>
       </c>
-      <c r="I4" s="211">
+      <c r="I4" s="213">
         <v>0</v>
       </c>
-      <c r="J4" s="213">
+      <c r="J4" s="215">
         <f>H4+I4</f>
         <v>48.1</v>
       </c>
-      <c r="K4" s="212">
+      <c r="K4" s="214">
         <f>G4/E4</f>
         <v>6.99</v>
       </c>
-      <c r="L4" s="212"/>
-      <c r="M4" s="212"/>
+      <c r="L4" s="214"/>
+      <c r="M4" s="214"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C5" s="210"/>
+      <c r="C5" s="212"/>
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
@@ -3047,18 +3065,18 @@
       <c r="G5" s="27">
         <v>6.99</v>
       </c>
-      <c r="H5" s="214"/>
-      <c r="I5" s="211"/>
-      <c r="J5" s="214"/>
-      <c r="K5" s="212">
+      <c r="H5" s="216"/>
+      <c r="I5" s="213"/>
+      <c r="J5" s="216"/>
+      <c r="K5" s="214">
         <f t="shared" ref="K5:K10" si="0">G5/E5</f>
         <v>6.99</v>
       </c>
-      <c r="L5" s="212"/>
-      <c r="M5" s="212"/>
+      <c r="L5" s="214"/>
+      <c r="M5" s="214"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C6" s="210"/>
+      <c r="C6" s="212"/>
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
@@ -3071,18 +3089,18 @@
       <c r="G6" s="27">
         <v>4.97</v>
       </c>
-      <c r="H6" s="214"/>
-      <c r="I6" s="211"/>
-      <c r="J6" s="214"/>
-      <c r="K6" s="212">
+      <c r="H6" s="216"/>
+      <c r="I6" s="213"/>
+      <c r="J6" s="216"/>
+      <c r="K6" s="214">
         <f t="shared" si="0"/>
         <v>0.2485</v>
       </c>
-      <c r="L6" s="212"/>
-      <c r="M6" s="212"/>
+      <c r="L6" s="214"/>
+      <c r="M6" s="214"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C7" s="210"/>
+      <c r="C7" s="212"/>
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
@@ -3095,18 +3113,18 @@
       <c r="G7" s="27">
         <v>5.99</v>
       </c>
-      <c r="H7" s="214"/>
-      <c r="I7" s="211"/>
-      <c r="J7" s="214"/>
-      <c r="K7" s="212">
+      <c r="H7" s="216"/>
+      <c r="I7" s="213"/>
+      <c r="J7" s="216"/>
+      <c r="K7" s="214">
         <f t="shared" si="0"/>
         <v>0.29949999999999999</v>
       </c>
-      <c r="L7" s="212"/>
-      <c r="M7" s="212"/>
+      <c r="L7" s="214"/>
+      <c r="M7" s="214"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C8" s="210"/>
+      <c r="C8" s="212"/>
       <c r="D8" s="1" t="s">
         <v>155</v>
       </c>
@@ -3119,18 +3137,18 @@
       <c r="G8" s="27">
         <v>6.25</v>
       </c>
-      <c r="H8" s="214"/>
-      <c r="I8" s="211"/>
-      <c r="J8" s="214"/>
-      <c r="K8" s="212">
+      <c r="H8" s="216"/>
+      <c r="I8" s="213"/>
+      <c r="J8" s="216"/>
+      <c r="K8" s="214">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
-      <c r="L8" s="212"/>
-      <c r="M8" s="212"/>
+      <c r="L8" s="214"/>
+      <c r="M8" s="214"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C9" s="210"/>
+      <c r="C9" s="212"/>
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3143,18 +3161,18 @@
       <c r="G9" s="27">
         <v>11.59</v>
       </c>
-      <c r="H9" s="214"/>
-      <c r="I9" s="211"/>
-      <c r="J9" s="214"/>
-      <c r="K9" s="212">
+      <c r="H9" s="216"/>
+      <c r="I9" s="213"/>
+      <c r="J9" s="216"/>
+      <c r="K9" s="214">
         <f t="shared" si="0"/>
         <v>0.57950000000000002</v>
       </c>
-      <c r="L9" s="212"/>
-      <c r="M9" s="212"/>
+      <c r="L9" s="214"/>
+      <c r="M9" s="214"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C10" s="210"/>
+      <c r="C10" s="212"/>
       <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
@@ -3167,15 +3185,15 @@
       <c r="G10" s="27">
         <v>5.32</v>
       </c>
-      <c r="H10" s="214"/>
-      <c r="I10" s="211"/>
-      <c r="J10" s="214"/>
-      <c r="K10" s="212">
+      <c r="H10" s="216"/>
+      <c r="I10" s="213"/>
+      <c r="J10" s="216"/>
+      <c r="K10" s="214">
         <f t="shared" si="0"/>
         <v>1.0640000000000001</v>
       </c>
-      <c r="L10" s="212"/>
-      <c r="M10" s="212"/>
+      <c r="L10" s="214"/>
+      <c r="M10" s="214"/>
     </row>
     <row r="11" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C11" s="7"/>
@@ -3282,14 +3300,14 @@
       <c r="G16" s="27">
         <v>6.56</v>
       </c>
-      <c r="H16" s="213">
+      <c r="H16" s="215">
         <f>SUM(G16:G17)</f>
         <v>7.55</v>
       </c>
-      <c r="I16" s="211">
+      <c r="I16" s="213">
         <v>0</v>
       </c>
-      <c r="J16" s="213">
+      <c r="J16" s="215">
         <f>H16+I16</f>
         <v>7.55</v>
       </c>
@@ -3310,9 +3328,9 @@
       <c r="G17" s="27">
         <v>0.99</v>
       </c>
-      <c r="H17" s="213"/>
-      <c r="I17" s="211"/>
-      <c r="J17" s="213"/>
+      <c r="H17" s="215"/>
+      <c r="I17" s="213"/>
+      <c r="J17" s="215"/>
     </row>
     <row r="18" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
@@ -3364,7 +3382,7 @@
       <c r="L20" s="35"/>
     </row>
     <row r="21" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C21" s="210">
+      <c r="C21" s="212">
         <v>42925</v>
       </c>
       <c r="D21" s="149" t="s">
@@ -3379,20 +3397,20 @@
       <c r="G21" s="27">
         <v>2.56</v>
       </c>
-      <c r="H21" s="213">
+      <c r="H21" s="215">
         <f>SUM(G21:G25)</f>
         <v>17.230000000000004</v>
       </c>
-      <c r="I21" s="211">
+      <c r="I21" s="213">
         <v>5.65</v>
       </c>
-      <c r="J21" s="213">
+      <c r="J21" s="215">
         <f>H21+I21</f>
         <v>22.880000000000003</v>
       </c>
     </row>
     <row r="22" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C22" s="210"/>
+      <c r="C22" s="212"/>
       <c r="D22" s="149" t="s">
         <v>21</v>
       </c>
@@ -3405,12 +3423,12 @@
       <c r="G22" s="27">
         <v>1.8</v>
       </c>
-      <c r="H22" s="214"/>
-      <c r="I22" s="211"/>
-      <c r="J22" s="214"/>
+      <c r="H22" s="216"/>
+      <c r="I22" s="213"/>
+      <c r="J22" s="216"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C23" s="210"/>
+      <c r="C23" s="212"/>
       <c r="D23" s="1" t="s">
         <v>20</v>
       </c>
@@ -3423,12 +3441,12 @@
       <c r="G23" s="27">
         <v>3.99</v>
       </c>
-      <c r="H23" s="214"/>
-      <c r="I23" s="211"/>
-      <c r="J23" s="214"/>
+      <c r="H23" s="216"/>
+      <c r="I23" s="213"/>
+      <c r="J23" s="216"/>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C24" s="210"/>
+      <c r="C24" s="212"/>
       <c r="D24" s="149" t="s">
         <v>13</v>
       </c>
@@ -3441,12 +3459,12 @@
       <c r="G24" s="27">
         <v>1.97</v>
       </c>
-      <c r="H24" s="214"/>
-      <c r="I24" s="211"/>
-      <c r="J24" s="214"/>
+      <c r="H24" s="216"/>
+      <c r="I24" s="213"/>
+      <c r="J24" s="216"/>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C25" s="210"/>
+      <c r="C25" s="212"/>
       <c r="D25" s="1" t="s">
         <v>2</v>
       </c>
@@ -3459,9 +3477,9 @@
       <c r="G25" s="27">
         <v>6.91</v>
       </c>
-      <c r="H25" s="214"/>
-      <c r="I25" s="211"/>
-      <c r="J25" s="214"/>
+      <c r="H25" s="216"/>
+      <c r="I25" s="213"/>
+      <c r="J25" s="216"/>
     </row>
     <row r="26" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
@@ -3475,7 +3493,7 @@
       <c r="L26" s="35"/>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C27" s="210">
+      <c r="C27" s="212">
         <v>42927</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -3490,20 +3508,20 @@
       <c r="G27" s="27">
         <v>0.75</v>
       </c>
-      <c r="H27" s="213">
+      <c r="H27" s="215">
         <f>SUM(G27:G29)</f>
         <v>3.44</v>
       </c>
-      <c r="I27" s="211">
+      <c r="I27" s="213">
         <v>4.99</v>
       </c>
-      <c r="J27" s="213">
+      <c r="J27" s="215">
         <f>H27+I27</f>
         <v>8.43</v>
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C28" s="210"/>
+      <c r="C28" s="212"/>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
@@ -3516,12 +3534,12 @@
       <c r="G28" s="27">
         <v>0.75</v>
       </c>
-      <c r="H28" s="214"/>
-      <c r="I28" s="211"/>
-      <c r="J28" s="214"/>
+      <c r="H28" s="216"/>
+      <c r="I28" s="213"/>
+      <c r="J28" s="216"/>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C29" s="210"/>
+      <c r="C29" s="212"/>
       <c r="D29" s="1" t="s">
         <v>154</v>
       </c>
@@ -3534,9 +3552,9 @@
       <c r="G29" s="27">
         <v>1.94</v>
       </c>
-      <c r="H29" s="214"/>
-      <c r="I29" s="211"/>
-      <c r="J29" s="214"/>
+      <c r="H29" s="216"/>
+      <c r="I29" s="213"/>
+      <c r="J29" s="216"/>
     </row>
     <row r="30" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="7"/>
@@ -3588,7 +3606,7 @@
       <c r="L32" s="35"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C33" s="210">
+      <c r="C33" s="212">
         <v>42929</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -3603,20 +3621,20 @@
       <c r="G33" s="27">
         <v>0.77</v>
       </c>
-      <c r="H33" s="213">
+      <c r="H33" s="215">
         <f>SUM(G33:G34)</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="I33" s="211">
+      <c r="I33" s="213">
         <v>3.39</v>
       </c>
-      <c r="J33" s="211">
+      <c r="J33" s="213">
         <f>SUM(H33:I34)</f>
         <v>5.6899999999999995</v>
       </c>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C34" s="210"/>
+      <c r="C34" s="212"/>
       <c r="D34" s="1" t="s">
         <v>76</v>
       </c>
@@ -3629,9 +3647,9 @@
       <c r="G34" s="27">
         <v>1.53</v>
       </c>
-      <c r="H34" s="214"/>
-      <c r="I34" s="211"/>
-      <c r="J34" s="211"/>
+      <c r="H34" s="216"/>
+      <c r="I34" s="213"/>
+      <c r="J34" s="213"/>
     </row>
     <row r="35" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="7"/>
@@ -3683,7 +3701,7 @@
       <c r="L37" s="35"/>
     </row>
     <row r="38" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C38" s="210">
+      <c r="C38" s="212">
         <v>42931</v>
       </c>
       <c r="D38" s="149" t="s">
@@ -3698,20 +3716,20 @@
       <c r="G38" s="27">
         <v>5.72</v>
       </c>
-      <c r="H38" s="211">
+      <c r="H38" s="213">
         <f>SUM(G38:G39)</f>
         <v>8.5500000000000007</v>
       </c>
-      <c r="I38" s="211">
+      <c r="I38" s="213">
         <v>4.99</v>
       </c>
-      <c r="J38" s="211">
+      <c r="J38" s="213">
         <f>SUM(H38:I39)</f>
         <v>13.540000000000001</v>
       </c>
     </row>
     <row r="39" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C39" s="210"/>
+      <c r="C39" s="212"/>
       <c r="D39" s="149" t="s">
         <v>122</v>
       </c>
@@ -3724,9 +3742,9 @@
       <c r="G39" s="27">
         <v>2.83</v>
       </c>
-      <c r="H39" s="211"/>
-      <c r="I39" s="211"/>
-      <c r="J39" s="211"/>
+      <c r="H39" s="213"/>
+      <c r="I39" s="213"/>
+      <c r="J39" s="213"/>
     </row>
     <row r="40" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="7"/>
@@ -3740,7 +3758,7 @@
       <c r="L40" s="35"/>
     </row>
     <row r="41" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C41" s="210">
+      <c r="C41" s="212">
         <v>42936</v>
       </c>
       <c r="D41" s="149" t="s">
@@ -3755,20 +3773,20 @@
       <c r="G41" s="27">
         <v>10.58</v>
       </c>
-      <c r="H41" s="211">
+      <c r="H41" s="213">
         <f>SUM(G41:G45)</f>
         <v>18.649999999999999</v>
       </c>
-      <c r="I41" s="211">
+      <c r="I41" s="213">
         <v>0.25</v>
       </c>
-      <c r="J41" s="211">
+      <c r="J41" s="213">
         <f>H41+I41</f>
         <v>18.899999999999999</v>
       </c>
     </row>
     <row r="42" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C42" s="210"/>
+      <c r="C42" s="212"/>
       <c r="D42" s="149" t="s">
         <v>150</v>
       </c>
@@ -3781,12 +3799,12 @@
       <c r="G42" s="27">
         <v>3.86</v>
       </c>
-      <c r="H42" s="211"/>
-      <c r="I42" s="211"/>
-      <c r="J42" s="211"/>
+      <c r="H42" s="213"/>
+      <c r="I42" s="213"/>
+      <c r="J42" s="213"/>
     </row>
     <row r="43" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C43" s="210"/>
+      <c r="C43" s="212"/>
       <c r="D43" s="149" t="s">
         <v>151</v>
       </c>
@@ -3800,12 +3818,12 @@
         <f>1.99-0.1</f>
         <v>1.89</v>
       </c>
-      <c r="H43" s="211"/>
-      <c r="I43" s="211"/>
-      <c r="J43" s="211"/>
+      <c r="H43" s="213"/>
+      <c r="I43" s="213"/>
+      <c r="J43" s="213"/>
     </row>
     <row r="44" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C44" s="210"/>
+      <c r="C44" s="212"/>
       <c r="D44" s="149" t="s">
         <v>152</v>
       </c>
@@ -3819,12 +3837,12 @@
         <f>0.99-0.05</f>
         <v>0.94</v>
       </c>
-      <c r="H44" s="211"/>
-      <c r="I44" s="211"/>
-      <c r="J44" s="211"/>
+      <c r="H44" s="213"/>
+      <c r="I44" s="213"/>
+      <c r="J44" s="213"/>
     </row>
     <row r="45" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C45" s="210"/>
+      <c r="C45" s="212"/>
       <c r="D45" s="149" t="s">
         <v>153</v>
       </c>
@@ -3838,9 +3856,9 @@
         <f>1.45-0.07</f>
         <v>1.38</v>
       </c>
-      <c r="H45" s="211"/>
-      <c r="I45" s="211"/>
-      <c r="J45" s="211"/>
+      <c r="H45" s="213"/>
+      <c r="I45" s="213"/>
+      <c r="J45" s="213"/>
     </row>
     <row r="46" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="51"/>
@@ -3890,7 +3908,7 @@
       <c r="J48" s="158"/>
       <c r="L48" s="57"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C49" s="200">
         <v>42986</v>
       </c>
@@ -3917,7 +3935,7 @@
         <v>6.91</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C50" s="51"/>
       <c r="D50" s="52"/>
       <c r="E50" s="53"/>
@@ -3928,8 +3946,8 @@
       <c r="J50" s="158"/>
       <c r="L50" s="57"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C51" s="210">
+    <row r="51" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C51" s="212">
         <v>42986</v>
       </c>
       <c r="D51" s="149" t="s">
@@ -3944,20 +3962,20 @@
       <c r="G51" s="27">
         <v>29.95</v>
       </c>
-      <c r="H51" s="211">
+      <c r="H51" s="213">
         <f>G51+G52+G53+2.13</f>
         <v>34.380000000000003</v>
       </c>
-      <c r="I51" s="211">
+      <c r="I51" s="213">
         <v>3.03</v>
       </c>
-      <c r="J51" s="211">
+      <c r="J51" s="213">
         <f>H51+I51</f>
         <v>37.410000000000004</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C52" s="210"/>
+    <row r="52" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C52" s="212"/>
       <c r="D52" s="149" t="s">
         <v>222</v>
       </c>
@@ -3970,12 +3988,12 @@
       <c r="G52" s="27">
         <v>0.77</v>
       </c>
-      <c r="H52" s="211"/>
-      <c r="I52" s="211"/>
-      <c r="J52" s="211"/>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C53" s="210"/>
+      <c r="H52" s="213"/>
+      <c r="I52" s="213"/>
+      <c r="J52" s="213"/>
+    </row>
+    <row r="53" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C53" s="212"/>
       <c r="D53" s="149" t="s">
         <v>223</v>
       </c>
@@ -3988,11 +4006,11 @@
       <c r="G53" s="27">
         <v>1.53</v>
       </c>
-      <c r="H53" s="211"/>
-      <c r="I53" s="211"/>
-      <c r="J53" s="211"/>
-    </row>
-    <row r="54" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H53" s="213"/>
+      <c r="I53" s="213"/>
+      <c r="J53" s="213"/>
+    </row>
+    <row r="54" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="51"/>
       <c r="D54" s="52"/>
       <c r="E54" s="53"/>
@@ -4003,7 +4021,7 @@
       <c r="J54" s="158"/>
       <c r="L54" s="57"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C55" s="204">
         <v>42991</v>
       </c>
@@ -4029,7 +4047,7 @@
         <v>8.99</v>
       </c>
     </row>
-    <row r="56" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C56" s="51"/>
       <c r="D56" s="52"/>
       <c r="E56" s="53"/>
@@ -4040,7 +4058,7 @@
       <c r="J56" s="158"/>
       <c r="L56" s="57"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C57" s="206">
         <v>43017</v>
       </c>
@@ -4067,7 +4085,7 @@
         <v>6.38</v>
       </c>
     </row>
-    <row r="58" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C58" s="51"/>
       <c r="D58" s="52"/>
       <c r="E58" s="53"/>
@@ -4078,11 +4096,11 @@
       <c r="J58" s="158"/>
       <c r="L58" s="57"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C59" s="208">
         <v>43017</v>
       </c>
-      <c r="D59" s="202" t="s">
+      <c r="D59" s="149" t="s">
         <v>231</v>
       </c>
       <c r="E59" s="26">
@@ -4104,195 +4122,224 @@
         <v>9.0500000000000007</v>
       </c>
     </row>
-    <row r="60" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C60" s="7"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24"/>
-      <c r="G60" s="25"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="13"/>
-      <c r="J60" s="9"/>
-      <c r="L60" s="35"/>
-    </row>
-    <row r="61" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="C61" s="41">
-        <f ca="1">TODAY()</f>
-        <v>43016</v>
-      </c>
-      <c r="E61" s="29"/>
-      <c r="F61" s="29"/>
-      <c r="G61" s="29"/>
-      <c r="H61" s="29"/>
-      <c r="I61" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="J61" s="30">
-        <f>SUM(J4:J60)</f>
-        <v>272.68</v>
-      </c>
-      <c r="K61" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="L61" s="39">
-        <f ca="1">(C61-C4)*0.0328767</f>
-        <v>4.4054777999999999</v>
-      </c>
-      <c r="M61" s="24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C62" s="7"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="24"/>
-      <c r="F62" s="24"/>
-      <c r="G62" s="25"/>
-      <c r="H62" s="31"/>
-      <c r="I62" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="J62" s="22">
-        <f ca="1">J61/L61</f>
-        <v>61.895669977045401</v>
-      </c>
-      <c r="K62" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="L62" s="36"/>
-      <c r="M62" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="N62" s="33"/>
-    </row>
-    <row r="63" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="58"/>
-      <c r="B63" s="58"/>
-      <c r="C63" s="44"/>
-      <c r="D63" s="45"/>
-      <c r="E63" s="46"/>
-      <c r="F63" s="46"/>
-      <c r="G63" s="47"/>
-      <c r="H63" s="48"/>
-      <c r="I63" s="59"/>
-      <c r="J63" s="48"/>
-      <c r="K63" s="58"/>
-      <c r="L63" s="60"/>
-      <c r="M63" s="58"/>
-      <c r="N63" s="58"/>
-      <c r="O63" s="58"/>
-    </row>
-    <row r="64" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C64" s="7"/>
-      <c r="D64" s="63" t="s">
-        <v>75</v>
-      </c>
-      <c r="E64" s="203" t="s">
-        <v>227</v>
-      </c>
-      <c r="H64" s="10"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="10"/>
-      <c r="L64" s="35"/>
-    </row>
-    <row r="65" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C65" s="7"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="24"/>
-      <c r="F65" s="24"/>
-      <c r="G65" s="25"/>
-      <c r="H65" s="10"/>
-      <c r="I65" s="11"/>
-      <c r="J65" s="10"/>
-      <c r="L65" s="35"/>
-    </row>
-    <row r="66" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C66" s="7"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="24"/>
-      <c r="F66" s="24"/>
-      <c r="G66" s="25"/>
-      <c r="H66" s="10"/>
-      <c r="I66" s="11"/>
-      <c r="J66" s="10"/>
-      <c r="L66" s="35"/>
-    </row>
-    <row r="67" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C67" s="147" t="s">
-        <v>164</v>
-      </c>
-      <c r="D67" s="148"/>
+    <row r="60" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C60" s="51"/>
+      <c r="D60" s="52"/>
+      <c r="E60" s="53"/>
+      <c r="F60" s="53"/>
+      <c r="G60" s="54"/>
+      <c r="H60" s="158"/>
+      <c r="I60" s="158"/>
+      <c r="J60" s="158"/>
+      <c r="L60" s="57"/>
+    </row>
+    <row r="61" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C61" s="210">
+        <v>1019</v>
+      </c>
+      <c r="D61" s="202" t="s">
+        <v>232</v>
+      </c>
+      <c r="E61" s="26">
+        <v>5</v>
+      </c>
+      <c r="F61" s="26">
+        <v>1</v>
+      </c>
+      <c r="G61" s="27">
+        <v>4.99</v>
+      </c>
+      <c r="H61" s="211">
+        <v>4.99</v>
+      </c>
+      <c r="I61" s="211">
+        <v>0</v>
+      </c>
+      <c r="J61" s="211">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="62" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="51"/>
+      <c r="D62" s="52"/>
+      <c r="E62" s="53"/>
+      <c r="F62" s="53"/>
+      <c r="G62" s="54"/>
+      <c r="H62" s="158"/>
+      <c r="I62" s="158"/>
+      <c r="J62" s="158"/>
+      <c r="L62" s="57"/>
+    </row>
+    <row r="63" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C63" s="212">
+        <v>43027</v>
+      </c>
+      <c r="D63" s="202" t="s">
+        <v>233</v>
+      </c>
+      <c r="E63" s="26">
+        <v>1</v>
+      </c>
+      <c r="F63" s="26">
+        <v>1</v>
+      </c>
+      <c r="G63" s="27">
+        <v>2.66</v>
+      </c>
+      <c r="H63" s="213">
+        <f>SUM(G63:G66)</f>
+        <v>10.18</v>
+      </c>
+      <c r="I63" s="213">
+        <v>3.75</v>
+      </c>
+      <c r="J63" s="213">
+        <f>H63+I63</f>
+        <v>13.93</v>
+      </c>
+    </row>
+    <row r="64" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C64" s="212"/>
+      <c r="D64" s="202" t="s">
+        <v>234</v>
+      </c>
+      <c r="E64" s="26">
+        <v>1</v>
+      </c>
+      <c r="F64" s="26">
+        <v>1</v>
+      </c>
+      <c r="G64" s="27">
+        <v>1.53</v>
+      </c>
+      <c r="H64" s="213"/>
+      <c r="I64" s="213"/>
+      <c r="J64" s="213"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C65" s="212"/>
+      <c r="D65" s="202" t="s">
+        <v>73</v>
+      </c>
+      <c r="E65" s="26">
+        <v>1</v>
+      </c>
+      <c r="F65" s="26">
+        <v>1</v>
+      </c>
+      <c r="G65" s="27">
+        <v>0.77</v>
+      </c>
+      <c r="H65" s="213"/>
+      <c r="I65" s="213"/>
+      <c r="J65" s="213"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C66" s="212"/>
+      <c r="D66" s="202" t="s">
+        <v>235</v>
+      </c>
+      <c r="E66" s="26">
+        <v>1</v>
+      </c>
+      <c r="F66" s="26">
+        <v>1</v>
+      </c>
+      <c r="G66" s="27">
+        <v>5.22</v>
+      </c>
+      <c r="H66" s="213"/>
+      <c r="I66" s="213"/>
+      <c r="J66" s="213"/>
+    </row>
+    <row r="67" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C67" s="7"/>
+      <c r="D67" s="8"/>
       <c r="E67" s="24"/>
       <c r="F67" s="24"/>
       <c r="G67" s="25"/>
-      <c r="H67" s="10"/>
-      <c r="I67" s="11"/>
-      <c r="J67" s="10"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="9"/>
       <c r="L67" s="35"/>
     </row>
-    <row r="68" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C68" s="49"/>
-      <c r="D68" s="95" t="s">
-        <v>0</v>
-      </c>
-      <c r="E68" s="98"/>
-      <c r="F68" s="98" t="s">
-        <v>160</v>
-      </c>
-      <c r="G68" s="99">
-        <v>3.39</v>
-      </c>
-      <c r="H68" s="10"/>
-      <c r="I68" s="11"/>
-      <c r="J68" s="10"/>
-      <c r="L68" s="35"/>
-    </row>
-    <row r="69" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C68" s="41">
+        <f ca="1">TODAY()</f>
+        <v>43028</v>
+      </c>
+      <c r="E68" s="29"/>
+      <c r="F68" s="29"/>
+      <c r="G68" s="29"/>
+      <c r="H68" s="29"/>
+      <c r="I68" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="J68" s="30">
+        <f>SUM(J4:J67)</f>
+        <v>291.60000000000002</v>
+      </c>
+      <c r="K68" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="L68" s="39">
+        <f ca="1">(C68-C4)*0.0328767</f>
+        <v>4.7999982000000001</v>
+      </c>
+      <c r="M68" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C69" s="7"/>
-      <c r="D69" s="95" t="s">
-        <v>1</v>
-      </c>
-      <c r="E69" s="98"/>
-      <c r="F69" s="98" t="s">
-        <v>160</v>
-      </c>
-      <c r="G69" s="99">
-        <v>1.39</v>
-      </c>
-      <c r="H69" s="10"/>
-      <c r="I69" s="11"/>
-      <c r="J69" s="10"/>
-      <c r="L69" s="35"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="24"/>
+      <c r="G69" s="25"/>
+      <c r="H69" s="31"/>
+      <c r="I69" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="J69" s="22">
+        <f ca="1">J68/L68</f>
+        <v>60.750022781258544</v>
+      </c>
+      <c r="K69" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="L69" s="36"/>
+      <c r="M69" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="N69" s="33"/>
     </row>
     <row r="70" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="7"/>
-      <c r="D70" s="95" t="str">
-        <f>D24</f>
-        <v>NOKIA 5110 LCD</v>
-      </c>
-      <c r="E70" s="98"/>
-      <c r="F70" s="98"/>
-      <c r="G70" s="99">
-        <f>G24</f>
-        <v>1.97</v>
-      </c>
-      <c r="H70" s="10"/>
-      <c r="I70" s="11"/>
-      <c r="J70" s="10"/>
-      <c r="L70" s="35"/>
+      <c r="A70" s="58"/>
+      <c r="B70" s="58"/>
+      <c r="C70" s="44"/>
+      <c r="D70" s="45"/>
+      <c r="E70" s="46"/>
+      <c r="F70" s="46"/>
+      <c r="G70" s="47"/>
+      <c r="H70" s="48"/>
+      <c r="I70" s="59"/>
+      <c r="J70" s="48"/>
+      <c r="K70" s="58"/>
+      <c r="L70" s="60"/>
+      <c r="M70" s="58"/>
+      <c r="N70" s="58"/>
+      <c r="O70" s="58"/>
     </row>
     <row r="71" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C71" s="7"/>
-      <c r="D71" s="95" t="s">
-        <v>5</v>
-      </c>
-      <c r="E71" s="98"/>
-      <c r="F71" s="98"/>
-      <c r="G71" s="99">
-        <v>0.2485</v>
+      <c r="D71" s="63" t="s">
+        <v>75</v>
+      </c>
+      <c r="E71" s="203" t="s">
+        <v>227</v>
       </c>
       <c r="H71" s="10"/>
       <c r="I71" s="11"/>
@@ -4301,14 +4348,10 @@
     </row>
     <row r="72" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C72" s="7"/>
-      <c r="D72" s="95" t="s">
-        <v>156</v>
-      </c>
-      <c r="E72" s="98"/>
-      <c r="F72" s="98"/>
-      <c r="G72" s="99">
-        <v>0.29949999999999999</v>
-      </c>
+      <c r="D72" s="8"/>
+      <c r="E72" s="24"/>
+      <c r="F72" s="24"/>
+      <c r="G72" s="25"/>
       <c r="H72" s="10"/>
       <c r="I72" s="11"/>
       <c r="J72" s="10"/>
@@ -4316,43 +4359,39 @@
     </row>
     <row r="73" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C73" s="7"/>
-      <c r="D73" s="95" t="s">
-        <v>158</v>
-      </c>
-      <c r="E73" s="98"/>
-      <c r="F73" s="98"/>
-      <c r="G73" s="99">
-        <v>1</v>
-      </c>
+      <c r="D73" s="8"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="24"/>
+      <c r="G73" s="25"/>
       <c r="H73" s="10"/>
       <c r="I73" s="11"/>
       <c r="J73" s="10"/>
       <c r="L73" s="35"/>
     </row>
     <row r="74" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C74" s="7"/>
-      <c r="D74" s="95" t="s">
-        <v>155</v>
-      </c>
-      <c r="E74" s="98"/>
-      <c r="F74" s="98"/>
-      <c r="G74" s="99">
-        <v>6.25</v>
-      </c>
+      <c r="C74" s="147" t="s">
+        <v>164</v>
+      </c>
+      <c r="D74" s="148"/>
+      <c r="E74" s="24"/>
+      <c r="F74" s="24"/>
+      <c r="G74" s="25"/>
       <c r="H74" s="10"/>
       <c r="I74" s="11"/>
       <c r="J74" s="10"/>
       <c r="L74" s="35"/>
     </row>
     <row r="75" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C75" s="7"/>
+      <c r="C75" s="49"/>
       <c r="D75" s="95" t="s">
-        <v>157</v>
+        <v>0</v>
       </c>
       <c r="E75" s="98"/>
-      <c r="F75" s="98"/>
+      <c r="F75" s="98" t="s">
+        <v>160</v>
+      </c>
       <c r="G75" s="99">
-        <v>0.57950000000000002</v>
+        <v>2.19</v>
       </c>
       <c r="H75" s="10"/>
       <c r="I75" s="11"/>
@@ -4362,12 +4401,14 @@
     <row r="76" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C76" s="7"/>
       <c r="D76" s="95" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E76" s="98"/>
-      <c r="F76" s="98"/>
+      <c r="F76" s="98" t="s">
+        <v>160</v>
+      </c>
       <c r="G76" s="99">
-        <v>1.0640000000000001</v>
+        <v>1.06</v>
       </c>
       <c r="H76" s="10"/>
       <c r="I76" s="11"/>
@@ -4376,13 +4417,15 @@
     </row>
     <row r="77" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C77" s="7"/>
-      <c r="D77" s="95" t="s">
-        <v>161</v>
+      <c r="D77" s="95" t="str">
+        <f>D24</f>
+        <v>NOKIA 5110 LCD</v>
       </c>
       <c r="E77" s="98"/>
       <c r="F77" s="98"/>
       <c r="G77" s="99">
-        <v>0.5</v>
+        <f>G24</f>
+        <v>1.97</v>
       </c>
       <c r="H77" s="10"/>
       <c r="I77" s="11"/>
@@ -4390,46 +4433,45 @@
       <c r="L77" s="35"/>
     </row>
     <row r="78" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C78" s="44"/>
-      <c r="D78" s="96" t="s">
-        <v>159</v>
-      </c>
-      <c r="E78" s="100"/>
-      <c r="F78" s="100"/>
-      <c r="G78" s="101">
-        <v>2</v>
-      </c>
-      <c r="H78" s="48"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="95" t="s">
+        <v>5</v>
+      </c>
+      <c r="E78" s="98"/>
+      <c r="F78" s="98"/>
+      <c r="G78" s="99">
+        <v>0.2485</v>
+      </c>
+      <c r="H78" s="10"/>
       <c r="I78" s="11"/>
       <c r="J78" s="10"/>
       <c r="L78" s="35"/>
     </row>
     <row r="79" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="58"/>
-      <c r="B79" s="58"/>
-      <c r="C79" s="44"/>
-      <c r="D79" s="45"/>
-      <c r="E79" s="46"/>
-      <c r="F79" s="46"/>
-      <c r="G79" s="97">
-        <f>SUM(G68:G78)</f>
-        <v>18.691499999999998</v>
-      </c>
-      <c r="H79" s="48"/>
-      <c r="I79" s="59"/>
-      <c r="J79" s="48"/>
-      <c r="K79" s="58"/>
-      <c r="L79" s="60"/>
-      <c r="M79" s="58"/>
-      <c r="N79" s="58"/>
-      <c r="O79" s="58"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="95" t="s">
+        <v>156</v>
+      </c>
+      <c r="E79" s="98"/>
+      <c r="F79" s="98"/>
+      <c r="G79" s="99">
+        <v>0.29949999999999999</v>
+      </c>
+      <c r="H79" s="10"/>
+      <c r="I79" s="11"/>
+      <c r="J79" s="10"/>
+      <c r="L79" s="35"/>
     </row>
     <row r="80" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C80" s="7"/>
-      <c r="D80" s="8"/>
-      <c r="E80" s="24"/>
-      <c r="F80" s="24"/>
-      <c r="G80" s="25"/>
+      <c r="D80" s="95" t="s">
+        <v>158</v>
+      </c>
+      <c r="E80" s="98"/>
+      <c r="F80" s="98"/>
+      <c r="G80" s="99">
+        <v>1</v>
+      </c>
       <c r="H80" s="10"/>
       <c r="I80" s="11"/>
       <c r="J80" s="10"/>
@@ -4437,10 +4479,14 @@
     </row>
     <row r="81" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C81" s="7"/>
-      <c r="D81" s="8"/>
-      <c r="E81" s="24"/>
-      <c r="F81" s="24"/>
-      <c r="G81" s="25"/>
+      <c r="D81" s="95" t="s">
+        <v>155</v>
+      </c>
+      <c r="E81" s="98"/>
+      <c r="F81" s="98"/>
+      <c r="G81" s="99">
+        <v>6.25</v>
+      </c>
       <c r="H81" s="10"/>
       <c r="I81" s="11"/>
       <c r="J81" s="10"/>
@@ -4448,10 +4494,14 @@
     </row>
     <row r="82" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C82" s="7"/>
-      <c r="D82" s="8"/>
-      <c r="E82" s="24"/>
-      <c r="F82" s="24"/>
-      <c r="G82" s="25"/>
+      <c r="D82" s="95" t="s">
+        <v>157</v>
+      </c>
+      <c r="E82" s="98"/>
+      <c r="F82" s="98"/>
+      <c r="G82" s="99">
+        <v>0.57950000000000002</v>
+      </c>
       <c r="H82" s="10"/>
       <c r="I82" s="11"/>
       <c r="J82" s="10"/>
@@ -4459,511 +4509,538 @@
     </row>
     <row r="83" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C83" s="7"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="24"/>
-      <c r="F83" s="24"/>
-      <c r="G83" s="25"/>
+      <c r="D83" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="E83" s="98"/>
+      <c r="F83" s="98"/>
+      <c r="G83" s="99">
+        <v>1.0640000000000001</v>
+      </c>
       <c r="H83" s="10"/>
       <c r="I83" s="11"/>
       <c r="J83" s="10"/>
       <c r="L83" s="35"/>
     </row>
-    <row r="84" spans="1:15" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C84" s="93" t="s">
+    <row r="84" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C84" s="7"/>
+      <c r="D84" s="95" t="s">
+        <v>161</v>
+      </c>
+      <c r="E84" s="98"/>
+      <c r="F84" s="98"/>
+      <c r="G84" s="99">
+        <v>0.5</v>
+      </c>
+      <c r="H84" s="10"/>
+      <c r="I84" s="11"/>
+      <c r="J84" s="10"/>
+      <c r="L84" s="35"/>
+    </row>
+    <row r="85" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C85" s="44"/>
+      <c r="D85" s="96" t="s">
+        <v>159</v>
+      </c>
+      <c r="E85" s="100"/>
+      <c r="F85" s="100"/>
+      <c r="G85" s="101">
+        <v>2</v>
+      </c>
+      <c r="H85" s="48"/>
+      <c r="I85" s="11"/>
+      <c r="J85" s="10"/>
+      <c r="L85" s="35"/>
+    </row>
+    <row r="86" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="58"/>
+      <c r="B86" s="58"/>
+      <c r="C86" s="44"/>
+      <c r="D86" s="45"/>
+      <c r="E86" s="46"/>
+      <c r="F86" s="46"/>
+      <c r="G86" s="97">
+        <f>SUM(G75:G85)</f>
+        <v>17.1615</v>
+      </c>
+      <c r="H86" s="48"/>
+      <c r="I86" s="59"/>
+      <c r="J86" s="48"/>
+      <c r="K86" s="58"/>
+      <c r="L86" s="60"/>
+      <c r="M86" s="58"/>
+      <c r="N86" s="58"/>
+      <c r="O86" s="58"/>
+    </row>
+    <row r="87" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C87" s="7"/>
+      <c r="D87" s="8"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="25"/>
+      <c r="H87" s="10"/>
+      <c r="I87" s="11"/>
+      <c r="J87" s="10"/>
+      <c r="L87" s="35"/>
+    </row>
+    <row r="88" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C88" s="7"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="24"/>
+      <c r="F88" s="24"/>
+      <c r="G88" s="25"/>
+      <c r="H88" s="10"/>
+      <c r="I88" s="11"/>
+      <c r="J88" s="10"/>
+      <c r="L88" s="35"/>
+    </row>
+    <row r="89" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C89" s="7"/>
+      <c r="D89" s="8"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="24"/>
+      <c r="G89" s="25"/>
+      <c r="H89" s="10"/>
+      <c r="I89" s="11"/>
+      <c r="J89" s="10"/>
+      <c r="L89" s="35"/>
+    </row>
+    <row r="90" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C90" s="7"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="24"/>
+      <c r="F90" s="24"/>
+      <c r="G90" s="25"/>
+      <c r="H90" s="10"/>
+      <c r="I90" s="11"/>
+      <c r="J90" s="10"/>
+      <c r="L90" s="35"/>
+    </row>
+    <row r="91" spans="1:15" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C91" s="93" t="s">
         <v>163</v>
       </c>
-      <c r="D84" s="94"/>
-      <c r="E84" s="18"/>
-      <c r="H84" s="14"/>
-      <c r="I84" s="17"/>
-      <c r="J84" s="14"/>
-      <c r="K84" s="14"/>
-      <c r="L84" s="14"/>
-    </row>
-    <row r="85" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C85" s="144"/>
-      <c r="D85" s="151" t="s">
+      <c r="D91" s="94"/>
+      <c r="E91" s="18"/>
+      <c r="H91" s="14"/>
+      <c r="I91" s="17"/>
+      <c r="J91" s="14"/>
+      <c r="K91" s="14"/>
+      <c r="L91" s="14"/>
+    </row>
+    <row r="92" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C92" s="144"/>
+      <c r="D92" s="151" t="s">
         <v>226</v>
-      </c>
-      <c r="E85" s="98"/>
-      <c r="F85" s="98"/>
-      <c r="G85" s="99">
-        <v>1.53</v>
-      </c>
-      <c r="H85" s="157"/>
-      <c r="I85" s="158"/>
-      <c r="J85" s="157"/>
-      <c r="K85" s="157"/>
-      <c r="L85" s="159"/>
-    </row>
-    <row r="86" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C86" s="144"/>
-      <c r="D86" s="151" t="s">
-        <v>30</v>
-      </c>
-      <c r="E86" s="98"/>
-      <c r="F86" s="98"/>
-      <c r="G86" s="99">
-        <v>33.57</v>
-      </c>
-      <c r="H86" s="157"/>
-      <c r="I86" s="158"/>
-      <c r="J86" s="157"/>
-      <c r="K86" s="157"/>
-      <c r="L86" s="159"/>
-    </row>
-    <row r="87" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C87" s="144"/>
-      <c r="D87" s="151" t="s">
-        <v>2</v>
-      </c>
-      <c r="E87" s="98"/>
-      <c r="F87" s="98"/>
-      <c r="G87" s="99">
-        <v>6.56</v>
-      </c>
-      <c r="H87" s="157"/>
-      <c r="I87" s="158"/>
-      <c r="J87" s="157"/>
-      <c r="K87" s="157"/>
-      <c r="L87" s="159"/>
-    </row>
-    <row r="88" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C88" s="144"/>
-      <c r="D88" s="151" t="s">
-        <v>11</v>
-      </c>
-      <c r="E88" s="98"/>
-      <c r="F88" s="98"/>
-      <c r="G88" s="99">
-        <v>2.57</v>
-      </c>
-      <c r="H88" s="157"/>
-      <c r="I88" s="158"/>
-      <c r="J88" s="157"/>
-      <c r="K88" s="157"/>
-      <c r="L88" s="159"/>
-    </row>
-    <row r="89" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C89" s="144"/>
-      <c r="D89" s="151" t="s">
-        <v>61</v>
-      </c>
-      <c r="E89" s="98"/>
-      <c r="F89" s="98"/>
-      <c r="G89" s="99">
-        <v>5.22</v>
-      </c>
-      <c r="H89" s="157"/>
-      <c r="I89" s="158"/>
-      <c r="J89" s="157"/>
-      <c r="K89" s="157"/>
-      <c r="L89" s="159"/>
-    </row>
-    <row r="90" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C90" s="144"/>
-      <c r="D90" s="151" t="s">
-        <v>162</v>
-      </c>
-      <c r="E90" s="98"/>
-      <c r="F90" s="98"/>
-      <c r="G90" s="99">
-        <v>0.39900000000000002</v>
-      </c>
-      <c r="H90" s="157"/>
-      <c r="I90" s="158"/>
-      <c r="J90" s="157"/>
-      <c r="K90" s="157"/>
-      <c r="L90" s="159"/>
-    </row>
-    <row r="91" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C91" s="145"/>
-      <c r="D91" s="151" t="s">
-        <v>73</v>
-      </c>
-      <c r="E91" s="98"/>
-      <c r="F91" s="98"/>
-      <c r="G91" s="99">
-        <v>0.77</v>
-      </c>
-      <c r="H91" s="9"/>
-      <c r="I91" s="13"/>
-      <c r="J91" s="9"/>
-      <c r="K91" s="9"/>
-      <c r="L91" s="38"/>
-    </row>
-    <row r="92" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C92" s="145"/>
-      <c r="D92" s="151" t="s">
-        <v>6</v>
       </c>
       <c r="E92" s="98"/>
       <c r="F92" s="98"/>
       <c r="G92" s="99">
-        <v>0.02</v>
-      </c>
-      <c r="H92" s="9"/>
-      <c r="I92" s="13"/>
-      <c r="J92" s="9"/>
-      <c r="K92" s="9"/>
-      <c r="L92" s="38"/>
-    </row>
-    <row r="93" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C93" s="145"/>
-      <c r="D93" s="153" t="s">
-        <v>168</v>
+        <v>1.53</v>
+      </c>
+      <c r="H92" s="157"/>
+      <c r="I92" s="158"/>
+      <c r="J92" s="157"/>
+      <c r="K92" s="157"/>
+      <c r="L92" s="159"/>
+    </row>
+    <row r="93" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C93" s="144"/>
+      <c r="D93" s="151" t="s">
+        <v>30</v>
       </c>
       <c r="E93" s="98"/>
       <c r="F93" s="98"/>
       <c r="G93" s="99">
-        <f>5.72+(0.5*4.99)</f>
-        <v>8.2149999999999999</v>
-      </c>
-      <c r="H93" s="9"/>
-      <c r="I93" s="13"/>
-      <c r="J93" s="9"/>
-      <c r="K93" s="9"/>
-      <c r="L93" s="38"/>
-    </row>
-    <row r="94" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C94" s="145"/>
+        <v>33.57</v>
+      </c>
+      <c r="H93" s="157"/>
+      <c r="I93" s="158"/>
+      <c r="J93" s="157"/>
+      <c r="K93" s="157"/>
+      <c r="L93" s="159"/>
+    </row>
+    <row r="94" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C94" s="144"/>
       <c r="D94" s="151" t="s">
-        <v>169</v>
+        <v>2</v>
       </c>
       <c r="E94" s="98"/>
       <c r="F94" s="98"/>
       <c r="G94" s="99">
+        <v>6.56</v>
+      </c>
+      <c r="H94" s="157"/>
+      <c r="I94" s="158"/>
+      <c r="J94" s="157"/>
+      <c r="K94" s="157"/>
+      <c r="L94" s="159"/>
+    </row>
+    <row r="95" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C95" s="144"/>
+      <c r="D95" s="151" t="s">
+        <v>11</v>
+      </c>
+      <c r="E95" s="98"/>
+      <c r="F95" s="98"/>
+      <c r="G95" s="99">
+        <v>2.57</v>
+      </c>
+      <c r="H95" s="157"/>
+      <c r="I95" s="158"/>
+      <c r="J95" s="157"/>
+      <c r="K95" s="157"/>
+      <c r="L95" s="159"/>
+    </row>
+    <row r="96" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C96" s="144"/>
+      <c r="D96" s="151" t="s">
+        <v>61</v>
+      </c>
+      <c r="E96" s="98"/>
+      <c r="F96" s="98"/>
+      <c r="G96" s="99">
+        <v>5.22</v>
+      </c>
+      <c r="H96" s="157"/>
+      <c r="I96" s="158"/>
+      <c r="J96" s="157"/>
+      <c r="K96" s="157"/>
+      <c r="L96" s="159"/>
+    </row>
+    <row r="97" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C97" s="144"/>
+      <c r="D97" s="151" t="s">
+        <v>162</v>
+      </c>
+      <c r="E97" s="98"/>
+      <c r="F97" s="98"/>
+      <c r="G97" s="99">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="H97" s="157"/>
+      <c r="I97" s="158"/>
+      <c r="J97" s="157"/>
+      <c r="K97" s="157"/>
+      <c r="L97" s="159"/>
+    </row>
+    <row r="98" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C98" s="145"/>
+      <c r="D98" s="151" t="s">
+        <v>73</v>
+      </c>
+      <c r="E98" s="98"/>
+      <c r="F98" s="98"/>
+      <c r="G98" s="99">
+        <v>0.77</v>
+      </c>
+      <c r="H98" s="9"/>
+      <c r="I98" s="13"/>
+      <c r="J98" s="9"/>
+      <c r="K98" s="9"/>
+      <c r="L98" s="38"/>
+    </row>
+    <row r="99" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C99" s="145"/>
+      <c r="D99" s="151" t="s">
+        <v>6</v>
+      </c>
+      <c r="E99" s="98"/>
+      <c r="F99" s="98"/>
+      <c r="G99" s="99">
+        <v>0.02</v>
+      </c>
+      <c r="H99" s="9"/>
+      <c r="I99" s="13"/>
+      <c r="J99" s="9"/>
+      <c r="K99" s="9"/>
+      <c r="L99" s="38"/>
+    </row>
+    <row r="100" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C100" s="145"/>
+      <c r="D100" s="153" t="s">
+        <v>168</v>
+      </c>
+      <c r="E100" s="98"/>
+      <c r="F100" s="98"/>
+      <c r="G100" s="99">
+        <f>5.72+(0.5*4.99)</f>
+        <v>8.2149999999999999</v>
+      </c>
+      <c r="H100" s="9"/>
+      <c r="I100" s="13"/>
+      <c r="J100" s="9"/>
+      <c r="K100" s="9"/>
+      <c r="L100" s="38"/>
+    </row>
+    <row r="101" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C101" s="145"/>
+      <c r="D101" s="151" t="s">
+        <v>169</v>
+      </c>
+      <c r="E101" s="98"/>
+      <c r="F101" s="98"/>
+      <c r="G101" s="99">
         <f>2.83+(0.5*4.99)</f>
         <v>5.3250000000000002</v>
       </c>
-      <c r="H94" s="9"/>
-      <c r="I94" s="13"/>
-      <c r="J94" s="9"/>
-      <c r="K94" s="9"/>
-      <c r="L94" s="38"/>
-    </row>
-    <row r="95" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C95" s="146"/>
-      <c r="D95" s="152" t="s">
+      <c r="H101" s="9"/>
+      <c r="I101" s="13"/>
+      <c r="J101" s="9"/>
+      <c r="K101" s="9"/>
+      <c r="L101" s="38"/>
+    </row>
+    <row r="102" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C102" s="146"/>
+      <c r="D102" s="152" t="s">
         <v>74</v>
       </c>
-      <c r="E95" s="100"/>
-      <c r="F95" s="100"/>
-      <c r="G95" s="101">
+      <c r="E102" s="100"/>
+      <c r="F102" s="100"/>
+      <c r="G102" s="101">
         <v>1.53</v>
       </c>
-      <c r="H95" s="160"/>
-      <c r="I95" s="13"/>
-      <c r="J95" s="9"/>
-      <c r="K95" s="9"/>
-      <c r="L95" s="38"/>
-    </row>
-    <row r="96" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="67"/>
-      <c r="B96" s="67"/>
-      <c r="C96" s="68"/>
-      <c r="D96" s="69"/>
-      <c r="E96" s="70"/>
-      <c r="F96" s="70"/>
-      <c r="G96" s="97">
-        <f>SUM(G85:G95)</f>
+      <c r="H102" s="160"/>
+      <c r="I102" s="13"/>
+      <c r="J102" s="9"/>
+      <c r="K102" s="9"/>
+      <c r="L102" s="38"/>
+    </row>
+    <row r="103" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="67"/>
+      <c r="B103" s="67"/>
+      <c r="C103" s="68"/>
+      <c r="D103" s="69"/>
+      <c r="E103" s="70"/>
+      <c r="F103" s="70"/>
+      <c r="G103" s="97">
+        <f>SUM(G92:G102)</f>
         <v>65.709000000000017</v>
       </c>
-      <c r="H96" s="71"/>
-      <c r="I96" s="72"/>
-      <c r="J96" s="71"/>
-      <c r="K96" s="67"/>
-      <c r="L96" s="67"/>
-      <c r="M96" s="67"/>
-      <c r="N96" s="67"/>
-      <c r="O96" s="67"/>
-    </row>
-    <row r="97" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C97" s="51"/>
-      <c r="D97" s="73"/>
-      <c r="E97" s="74"/>
-      <c r="F97" s="74"/>
-      <c r="G97" s="75"/>
-      <c r="H97" s="55"/>
-      <c r="I97" s="56"/>
-      <c r="J97" s="55"/>
-      <c r="L97" s="57"/>
-    </row>
-    <row r="98" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="79"/>
-      <c r="B99" s="79"/>
-      <c r="C99" s="80"/>
-      <c r="D99" s="81"/>
-      <c r="E99" s="82"/>
-      <c r="F99" s="82"/>
-      <c r="G99" s="83"/>
-      <c r="H99" s="84"/>
-      <c r="I99" s="85"/>
-      <c r="J99" s="84"/>
-      <c r="K99" s="79"/>
-      <c r="L99" s="79"/>
-      <c r="M99" s="79"/>
-      <c r="N99" s="79"/>
-      <c r="O99" s="79"/>
-    </row>
-    <row r="100" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C100" s="87"/>
-      <c r="D100" s="88"/>
-      <c r="E100" s="61"/>
-      <c r="F100" s="61"/>
-      <c r="G100" s="89"/>
-      <c r="H100" s="90"/>
-      <c r="I100" s="91"/>
-      <c r="J100" s="90"/>
-      <c r="L100" s="92"/>
-    </row>
-    <row r="101" spans="1:15" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C101" s="93" t="s">
-        <v>165</v>
-      </c>
-      <c r="D101" s="94"/>
-      <c r="E101" s="18"/>
-      <c r="H101" s="64"/>
-      <c r="I101" s="65"/>
-      <c r="J101" s="64"/>
-    </row>
-    <row r="102" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C102" s="144"/>
-      <c r="D102" s="151" t="s">
-        <v>225</v>
-      </c>
-      <c r="E102" s="98"/>
-      <c r="F102" s="98"/>
-      <c r="G102" s="99">
-        <v>1.53</v>
-      </c>
-      <c r="H102" s="55"/>
-      <c r="I102" s="56"/>
-      <c r="J102" s="55"/>
-      <c r="L102" s="57"/>
-    </row>
-    <row r="103" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C103" s="144"/>
-      <c r="D103" s="151" t="s">
-        <v>166</v>
-      </c>
-      <c r="E103" s="98"/>
-      <c r="F103" s="98"/>
-      <c r="G103" s="99">
-        <v>33.57</v>
-      </c>
-      <c r="H103" s="55"/>
-      <c r="I103" s="56"/>
-      <c r="J103" s="55"/>
-      <c r="L103" s="57"/>
-    </row>
-    <row r="104" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C104" s="144"/>
-      <c r="D104" s="151" t="s">
-        <v>2</v>
-      </c>
-      <c r="E104" s="98"/>
-      <c r="F104" s="98"/>
-      <c r="G104" s="99">
-        <v>6.56</v>
-      </c>
+      <c r="H103" s="71"/>
+      <c r="I103" s="72"/>
+      <c r="J103" s="71"/>
+      <c r="K103" s="67"/>
+      <c r="L103" s="67"/>
+      <c r="M103" s="67"/>
+      <c r="N103" s="67"/>
+      <c r="O103" s="67"/>
+    </row>
+    <row r="104" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C104" s="51"/>
+      <c r="D104" s="73"/>
+      <c r="E104" s="74"/>
+      <c r="F104" s="74"/>
+      <c r="G104" s="75"/>
       <c r="H104" s="55"/>
       <c r="I104" s="56"/>
       <c r="J104" s="55"/>
       <c r="L104" s="57"/>
     </row>
-    <row r="105" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C105" s="144"/>
-      <c r="D105" s="151" t="s">
-        <v>61</v>
-      </c>
-      <c r="E105" s="98"/>
-      <c r="F105" s="98"/>
-      <c r="G105" s="99">
-        <v>6.91</v>
-      </c>
-      <c r="H105" s="55"/>
-      <c r="I105" s="56"/>
-      <c r="J105" s="55"/>
-      <c r="L105" s="57"/>
-    </row>
-    <row r="106" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C106" s="145"/>
-      <c r="D106" s="151" t="s">
-        <v>162</v>
-      </c>
-      <c r="E106" s="98"/>
-      <c r="F106" s="98"/>
-      <c r="G106" s="99">
-        <v>0.39900000000000002</v>
-      </c>
-      <c r="H106" s="10"/>
-      <c r="I106" s="11"/>
-      <c r="J106" s="10"/>
-      <c r="L106" s="35"/>
-    </row>
-    <row r="107" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C107" s="145"/>
-      <c r="D107" s="151" t="s">
-        <v>11</v>
-      </c>
-      <c r="E107" s="98"/>
-      <c r="F107" s="98"/>
-      <c r="G107" s="99">
-        <v>2.57</v>
-      </c>
-      <c r="H107" s="10"/>
-      <c r="I107" s="11"/>
-      <c r="J107" s="10"/>
-      <c r="L107" s="35"/>
-    </row>
-    <row r="108" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C108" s="145"/>
-      <c r="D108" s="151" t="s">
-        <v>6</v>
-      </c>
-      <c r="E108" s="98"/>
-      <c r="F108" s="98"/>
-      <c r="G108" s="99">
-        <v>0.02</v>
-      </c>
-      <c r="H108" s="10"/>
-      <c r="I108" s="11"/>
-      <c r="J108" s="10"/>
-      <c r="L108" s="35"/>
-    </row>
-    <row r="109" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="79"/>
+      <c r="B106" s="79"/>
+      <c r="C106" s="80"/>
+      <c r="D106" s="81"/>
+      <c r="E106" s="82"/>
+      <c r="F106" s="82"/>
+      <c r="G106" s="83"/>
+      <c r="H106" s="84"/>
+      <c r="I106" s="85"/>
+      <c r="J106" s="84"/>
+      <c r="K106" s="79"/>
+      <c r="L106" s="79"/>
+      <c r="M106" s="79"/>
+      <c r="N106" s="79"/>
+      <c r="O106" s="79"/>
+    </row>
+    <row r="107" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C107" s="87"/>
+      <c r="D107" s="88"/>
+      <c r="E107" s="61"/>
+      <c r="F107" s="61"/>
+      <c r="G107" s="89"/>
+      <c r="H107" s="90"/>
+      <c r="I107" s="91"/>
+      <c r="J107" s="90"/>
+      <c r="L107" s="92"/>
+    </row>
+    <row r="108" spans="1:15" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C108" s="93" t="s">
+        <v>165</v>
+      </c>
+      <c r="D108" s="94"/>
+      <c r="E108" s="18"/>
+      <c r="H108" s="64"/>
+      <c r="I108" s="65"/>
+      <c r="J108" s="64"/>
+    </row>
+    <row r="109" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C109" s="144"/>
       <c r="D109" s="151" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
       <c r="E109" s="98"/>
       <c r="F109" s="98"/>
       <c r="G109" s="99">
+        <v>1.53</v>
+      </c>
+      <c r="H109" s="55"/>
+      <c r="I109" s="56"/>
+      <c r="J109" s="55"/>
+      <c r="L109" s="57"/>
+    </row>
+    <row r="110" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C110" s="144"/>
+      <c r="D110" s="151" t="s">
+        <v>166</v>
+      </c>
+      <c r="E110" s="98"/>
+      <c r="F110" s="98"/>
+      <c r="G110" s="99">
+        <v>33.57</v>
+      </c>
+      <c r="H110" s="55"/>
+      <c r="I110" s="56"/>
+      <c r="J110" s="55"/>
+      <c r="L110" s="57"/>
+    </row>
+    <row r="111" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C111" s="144"/>
+      <c r="D111" s="151" t="s">
+        <v>2</v>
+      </c>
+      <c r="E111" s="98"/>
+      <c r="F111" s="98"/>
+      <c r="G111" s="99">
+        <v>6.56</v>
+      </c>
+      <c r="H111" s="55"/>
+      <c r="I111" s="56"/>
+      <c r="J111" s="55"/>
+      <c r="L111" s="57"/>
+    </row>
+    <row r="112" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C112" s="144"/>
+      <c r="D112" s="151" t="s">
+        <v>61</v>
+      </c>
+      <c r="E112" s="98"/>
+      <c r="F112" s="98"/>
+      <c r="G112" s="99">
+        <v>6.91</v>
+      </c>
+      <c r="H112" s="55"/>
+      <c r="I112" s="56"/>
+      <c r="J112" s="55"/>
+      <c r="L112" s="57"/>
+    </row>
+    <row r="113" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C113" s="145"/>
+      <c r="D113" s="151" t="s">
+        <v>162</v>
+      </c>
+      <c r="E113" s="98"/>
+      <c r="F113" s="98"/>
+      <c r="G113" s="99">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="H113" s="10"/>
+      <c r="I113" s="11"/>
+      <c r="J113" s="10"/>
+      <c r="L113" s="35"/>
+    </row>
+    <row r="114" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C114" s="145"/>
+      <c r="D114" s="151" t="s">
+        <v>11</v>
+      </c>
+      <c r="E114" s="98"/>
+      <c r="F114" s="98"/>
+      <c r="G114" s="99">
+        <v>2.57</v>
+      </c>
+      <c r="H114" s="10"/>
+      <c r="I114" s="11"/>
+      <c r="J114" s="10"/>
+      <c r="L114" s="35"/>
+    </row>
+    <row r="115" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C115" s="145"/>
+      <c r="D115" s="151" t="s">
+        <v>6</v>
+      </c>
+      <c r="E115" s="98"/>
+      <c r="F115" s="98"/>
+      <c r="G115" s="99">
+        <v>0.02</v>
+      </c>
+      <c r="H115" s="10"/>
+      <c r="I115" s="11"/>
+      <c r="J115" s="10"/>
+      <c r="L115" s="35"/>
+    </row>
+    <row r="116" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D116" s="151" t="s">
+        <v>73</v>
+      </c>
+      <c r="E116" s="98"/>
+      <c r="F116" s="98"/>
+      <c r="G116" s="99">
         <v>0.77</v>
       </c>
     </row>
-    <row r="110" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D110" s="154" t="s">
+    <row r="117" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D117" s="154" t="s">
         <v>74</v>
       </c>
-      <c r="E110" s="155"/>
-      <c r="F110" s="155"/>
-      <c r="G110" s="156">
+      <c r="E117" s="155"/>
+      <c r="F117" s="155"/>
+      <c r="G117" s="156">
         <v>1.53</v>
       </c>
     </row>
-    <row r="111" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C111" s="146"/>
-      <c r="D111" s="152" t="s">
+    <row r="118" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C118" s="146"/>
+      <c r="D118" s="152" t="s">
         <v>224</v>
       </c>
-      <c r="E111" s="100"/>
-      <c r="F111" s="100"/>
-      <c r="G111" s="101">
+      <c r="E118" s="100"/>
+      <c r="F118" s="100"/>
+      <c r="G118" s="101">
         <v>3.78</v>
       </c>
-      <c r="H111" s="48"/>
-      <c r="I111" s="11"/>
-      <c r="J111" s="10"/>
-      <c r="K111" s="12"/>
-      <c r="L111" s="35"/>
-      <c r="M111" s="12"/>
-      <c r="N111" s="12"/>
-      <c r="O111" s="12"/>
-    </row>
-    <row r="112" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="67"/>
-      <c r="B112" s="67"/>
-      <c r="C112" s="68"/>
-      <c r="D112" s="69"/>
-      <c r="E112" s="70"/>
-      <c r="F112" s="70"/>
-      <c r="G112" s="97">
-        <f>SUM(G102:G111)</f>
+      <c r="H118" s="48"/>
+      <c r="I118" s="11"/>
+      <c r="J118" s="10"/>
+      <c r="K118" s="12"/>
+      <c r="L118" s="35"/>
+      <c r="M118" s="12"/>
+      <c r="N118" s="12"/>
+      <c r="O118" s="12"/>
+    </row>
+    <row r="119" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="67"/>
+      <c r="B119" s="67"/>
+      <c r="C119" s="68"/>
+      <c r="D119" s="69"/>
+      <c r="E119" s="70"/>
+      <c r="F119" s="70"/>
+      <c r="G119" s="97">
+        <f>SUM(G109:G118)</f>
         <v>57.639000000000017</v>
       </c>
-      <c r="H112" s="71"/>
-      <c r="I112" s="72"/>
-      <c r="J112" s="71"/>
-      <c r="K112" s="67"/>
-      <c r="L112" s="67"/>
-      <c r="M112" s="67"/>
-      <c r="N112" s="67"/>
-      <c r="O112" s="67"/>
-    </row>
-    <row r="113" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C113" s="51"/>
-      <c r="D113" s="52"/>
-      <c r="E113" s="53"/>
-      <c r="F113" s="53"/>
-      <c r="G113" s="54"/>
-      <c r="H113" s="55"/>
-      <c r="I113" s="56"/>
-      <c r="J113" s="55"/>
-      <c r="L113" s="57"/>
-    </row>
-    <row r="114" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C114" s="51"/>
-      <c r="D114" s="52"/>
-      <c r="E114" s="53"/>
-      <c r="F114" s="53"/>
-      <c r="G114" s="54"/>
-      <c r="H114" s="55"/>
-      <c r="I114" s="56"/>
-      <c r="J114" s="55"/>
-    </row>
-    <row r="115" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C115" s="51"/>
-      <c r="D115" s="52"/>
-      <c r="E115" s="53"/>
-      <c r="F115" s="53"/>
-      <c r="G115" s="54"/>
-      <c r="H115" s="55"/>
-      <c r="I115" s="56"/>
-      <c r="J115" s="55"/>
-    </row>
-    <row r="116" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C116" s="51"/>
-      <c r="D116" s="52"/>
-      <c r="E116" s="53"/>
-      <c r="F116" s="53"/>
-      <c r="G116" s="54"/>
-      <c r="H116" s="55"/>
-      <c r="I116" s="56"/>
-      <c r="J116" s="55"/>
-    </row>
-    <row r="117" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C117" s="51"/>
-      <c r="D117" s="52"/>
-      <c r="E117" s="53"/>
-      <c r="F117" s="53"/>
-      <c r="G117" s="54"/>
-      <c r="H117" s="55"/>
-      <c r="I117" s="56"/>
-      <c r="J117" s="55"/>
-    </row>
-    <row r="118" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C118" s="51"/>
-      <c r="D118" s="52"/>
-      <c r="E118" s="53"/>
-      <c r="F118" s="53"/>
-      <c r="G118" s="54"/>
-      <c r="H118" s="55"/>
-      <c r="I118" s="56"/>
-      <c r="J118" s="55"/>
-    </row>
-    <row r="119" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C119" s="51"/>
-      <c r="D119" s="52"/>
-      <c r="E119" s="53"/>
-      <c r="F119" s="53"/>
-      <c r="G119" s="54"/>
-      <c r="H119" s="55"/>
-      <c r="I119" s="56"/>
-      <c r="J119" s="55"/>
-    </row>
-    <row r="120" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="H119" s="71"/>
+      <c r="I119" s="72"/>
+      <c r="J119" s="71"/>
+      <c r="K119" s="67"/>
+      <c r="L119" s="67"/>
+      <c r="M119" s="67"/>
+      <c r="N119" s="67"/>
+      <c r="O119" s="67"/>
+    </row>
+    <row r="120" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C120" s="51"/>
       <c r="D120" s="52"/>
       <c r="E120" s="53"/>
@@ -4972,8 +5049,9 @@
       <c r="H120" s="55"/>
       <c r="I120" s="56"/>
       <c r="J120" s="55"/>
-    </row>
-    <row r="121" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="L120" s="57"/>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C121" s="51"/>
       <c r="D121" s="52"/>
       <c r="E121" s="53"/>
@@ -4983,7 +5061,7 @@
       <c r="I121" s="56"/>
       <c r="J121" s="55"/>
     </row>
-    <row r="122" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C122" s="51"/>
       <c r="D122" s="52"/>
       <c r="E122" s="53"/>
@@ -4993,7 +5071,7 @@
       <c r="I122" s="56"/>
       <c r="J122" s="55"/>
     </row>
-    <row r="123" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C123" s="51"/>
       <c r="D123" s="52"/>
       <c r="E123" s="53"/>
@@ -5003,7 +5081,7 @@
       <c r="I123" s="56"/>
       <c r="J123" s="55"/>
     </row>
-    <row r="124" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C124" s="51"/>
       <c r="D124" s="52"/>
       <c r="E124" s="53"/>
@@ -5013,7 +5091,7 @@
       <c r="I124" s="56"/>
       <c r="J124" s="55"/>
     </row>
-    <row r="125" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C125" s="51"/>
       <c r="D125" s="52"/>
       <c r="E125" s="53"/>
@@ -5023,7 +5101,7 @@
       <c r="I125" s="56"/>
       <c r="J125" s="55"/>
     </row>
-    <row r="126" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C126" s="51"/>
       <c r="D126" s="52"/>
       <c r="E126" s="53"/>
@@ -5033,7 +5111,7 @@
       <c r="I126" s="56"/>
       <c r="J126" s="55"/>
     </row>
-    <row r="127" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C127" s="51"/>
       <c r="D127" s="52"/>
       <c r="E127" s="53"/>
@@ -5043,7 +5121,7 @@
       <c r="I127" s="56"/>
       <c r="J127" s="55"/>
     </row>
-    <row r="128" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C128" s="51"/>
       <c r="D128" s="52"/>
       <c r="E128" s="53"/>
@@ -5574,25 +5652,92 @@
       <c r="J180" s="55"/>
     </row>
     <row r="181" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C181" s="51"/>
       <c r="D181" s="52"/>
       <c r="E181" s="53"/>
       <c r="F181" s="53"/>
       <c r="G181" s="54"/>
+      <c r="H181" s="55"/>
+      <c r="I181" s="56"/>
+      <c r="J181" s="55"/>
     </row>
     <row r="182" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C182" s="51"/>
       <c r="D182" s="52"/>
       <c r="E182" s="53"/>
       <c r="F182" s="53"/>
       <c r="G182" s="54"/>
+      <c r="H182" s="55"/>
+      <c r="I182" s="56"/>
+      <c r="J182" s="55"/>
+    </row>
+    <row r="183" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C183" s="51"/>
+      <c r="D183" s="52"/>
+      <c r="E183" s="53"/>
+      <c r="F183" s="53"/>
+      <c r="G183" s="54"/>
+      <c r="H183" s="55"/>
+      <c r="I183" s="56"/>
+      <c r="J183" s="55"/>
+    </row>
+    <row r="184" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C184" s="51"/>
+      <c r="D184" s="52"/>
+      <c r="E184" s="53"/>
+      <c r="F184" s="53"/>
+      <c r="G184" s="54"/>
+      <c r="H184" s="55"/>
+      <c r="I184" s="56"/>
+      <c r="J184" s="55"/>
+    </row>
+    <row r="185" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C185" s="51"/>
+      <c r="D185" s="52"/>
+      <c r="E185" s="53"/>
+      <c r="F185" s="53"/>
+      <c r="G185" s="54"/>
+      <c r="H185" s="55"/>
+      <c r="I185" s="56"/>
+      <c r="J185" s="55"/>
+    </row>
+    <row r="186" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C186" s="51"/>
+      <c r="D186" s="52"/>
+      <c r="E186" s="53"/>
+      <c r="F186" s="53"/>
+      <c r="G186" s="54"/>
+      <c r="H186" s="55"/>
+      <c r="I186" s="56"/>
+      <c r="J186" s="55"/>
+    </row>
+    <row r="187" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C187" s="51"/>
+      <c r="D187" s="52"/>
+      <c r="E187" s="53"/>
+      <c r="F187" s="53"/>
+      <c r="G187" s="54"/>
+      <c r="H187" s="55"/>
+      <c r="I187" s="56"/>
+      <c r="J187" s="55"/>
+    </row>
+    <row r="188" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D188" s="52"/>
+      <c r="E188" s="53"/>
+      <c r="F188" s="53"/>
+      <c r="G188" s="54"/>
+    </row>
+    <row r="189" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D189" s="52"/>
+      <c r="E189" s="53"/>
+      <c r="F189" s="53"/>
+      <c r="G189" s="54"/>
     </row>
   </sheetData>
   <sortState ref="C4:H19">
     <sortCondition ref="C4:C19"/>
   </sortState>
-  <mergeCells count="38">
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="I38:I39"/>
+  <mergeCells count="42">
     <mergeCell ref="J38:J39"/>
     <mergeCell ref="C4:C10"/>
     <mergeCell ref="J4:J10"/>
@@ -5606,21 +5751,6 @@
     <mergeCell ref="I27:I29"/>
     <mergeCell ref="I21:I25"/>
     <mergeCell ref="H16:H17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="J27:J29"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="H51:H53"/>
-    <mergeCell ref="I51:I53"/>
-    <mergeCell ref="J51:J53"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="K9:M9"/>
     <mergeCell ref="C41:C45"/>
     <mergeCell ref="H41:H45"/>
     <mergeCell ref="I41:I45"/>
@@ -5628,6 +5758,28 @@
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="K10:M10"/>
     <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="J27:J29"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="H63:H66"/>
+    <mergeCell ref="I63:I66"/>
+    <mergeCell ref="J63:J66"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="H51:H53"/>
+    <mergeCell ref="I51:I53"/>
+    <mergeCell ref="J51:J53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6535,21 +6687,21 @@
       <c r="AB16" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="AN16" s="215" t="s">
+      <c r="AN16" s="217" t="s">
         <v>123</v>
       </c>
-      <c r="AO16" s="215"/>
-      <c r="AP16" s="215"/>
-      <c r="AQ16" s="215"/>
-      <c r="AT16" s="214" t="s">
+      <c r="AO16" s="217"/>
+      <c r="AP16" s="217"/>
+      <c r="AQ16" s="217"/>
+      <c r="AT16" s="216" t="s">
         <v>119</v>
       </c>
-      <c r="AU16" s="214"/>
-      <c r="AV16" s="214"/>
-      <c r="AW16" s="214"/>
-      <c r="AX16" s="214"/>
-      <c r="AY16" s="214"/>
-      <c r="AZ16" s="214"/>
+      <c r="AU16" s="216"/>
+      <c r="AV16" s="216"/>
+      <c r="AW16" s="216"/>
+      <c r="AX16" s="216"/>
+      <c r="AY16" s="216"/>
+      <c r="AZ16" s="216"/>
     </row>
     <row r="17" spans="25:59" x14ac:dyDescent="0.25">
       <c r="Y17" s="108" t="s">
@@ -6564,22 +6716,22 @@
       <c r="AB17" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="AJ17" s="214" t="s">
+      <c r="AJ17" s="216" t="s">
         <v>117</v>
       </c>
-      <c r="AK17" s="214"/>
-      <c r="AL17" s="214"/>
-      <c r="AN17" s="215"/>
-      <c r="AO17" s="215"/>
-      <c r="AP17" s="215"/>
-      <c r="AQ17" s="215"/>
+      <c r="AK17" s="216"/>
+      <c r="AL17" s="216"/>
+      <c r="AN17" s="217"/>
+      <c r="AO17" s="217"/>
+      <c r="AP17" s="217"/>
+      <c r="AQ17" s="217"/>
     </row>
     <row r="19" spans="25:59" x14ac:dyDescent="0.25">
       <c r="AP19" s="195" t="s">
         <v>216</v>
       </c>
       <c r="AQ19" s="117">
-        <f>INVENTORY!G96</f>
+        <f>INVENTORY!G103</f>
         <v>65.709000000000017</v>
       </c>
       <c r="AS19" s="196" t="s">
@@ -6587,11 +6739,11 @@
       </c>
     </row>
     <row r="20" spans="25:59" x14ac:dyDescent="0.25">
-      <c r="AK20" s="216" t="s">
+      <c r="AK20" s="218" t="s">
         <v>120</v>
       </c>
-      <c r="AL20" s="216"/>
-      <c r="AM20" s="216"/>
+      <c r="AL20" s="218"/>
+      <c r="AM20" s="218"/>
       <c r="AP20" s="195" t="s">
         <v>217</v>
       </c>
@@ -6886,7 +7038,7 @@
         <f t="shared" si="1"/>
         <v>6.6300000000000008</v>
       </c>
-      <c r="H11" s="217">
+      <c r="H11" s="219">
         <v>3.39</v>
       </c>
       <c r="I11" s="172" t="s">
@@ -6916,7 +7068,7 @@
         <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
-      <c r="H12" s="217"/>
+      <c r="H12" s="219"/>
       <c r="I12" s="172" t="s">
         <v>186</v>
       </c>
@@ -6972,7 +7124,7 @@
         <f t="shared" si="1"/>
         <v>57.199999999999996</v>
       </c>
-      <c r="H14" s="218">
+      <c r="H14" s="220">
         <v>4.99</v>
       </c>
       <c r="I14" s="172" t="s">
@@ -7001,7 +7153,7 @@
         <f t="shared" si="1"/>
         <v>28.3</v>
       </c>
-      <c r="H15" s="219"/>
+      <c r="H15" s="221"/>
       <c r="I15" s="182" t="s">
         <v>228</v>
       </c>

</xml_diff>

<commit_message>
TAKING A HUGE LEAP IN THE DARK TO ADD A MENU DRIVEN PROGRAM, AND HAVING SETTINGS SAVED TO A MICRO SD
</commit_message>
<xml_diff>
--- a/BillOfMaterials/INVENTORY.xlsx
+++ b/BillOfMaterials/INVENTORY.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="245">
   <si>
     <t>Arduino Nano</t>
   </si>
@@ -1339,6 +1339,30 @@
   </si>
   <si>
     <t>10PCS DIAL TOGGLE SWITCH (ALIEXPRESS)</t>
+  </si>
+  <si>
+    <t>RES 5.00M OHM 1/2W 1% AXIAL</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 50V X5R RADIAL</t>
+  </si>
+  <si>
+    <t>RES 30K OHM 1/4W 5% AXIAL</t>
+  </si>
+  <si>
+    <t>MJTP1236G SWITCH TACTILE</t>
+  </si>
+  <si>
+    <t>SN74HC00N IC GATE NAND 4CH 2-INP 14-DIP</t>
+  </si>
+  <si>
+    <t>SN74HC08N IC GATE AND 4CH 2-INP 14-DIP</t>
+  </si>
+  <si>
+    <t>RES 100K OHM 1/4W 5% AXIAL (DIGIKEY)</t>
+  </si>
+  <si>
+    <t>TAX</t>
   </si>
 </sst>
 </file>
@@ -1903,7 +1927,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="224">
+  <cellXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2417,6 +2441,13 @@
     </xf>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2936,11 +2967,11 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:AB191"/>
+  <dimension ref="A1:AB199"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q54" sqref="Q54"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L68" sqref="L68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2954,8 +2985,8 @@
     <col min="8" max="8" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.140625" style="12" customWidth="1"/>
-    <col min="12" max="12" width="5" style="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="35" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.140625" style="12" bestFit="1" customWidth="1"/>
     <col min="14" max="28" width="9.140625" style="12"/>
   </cols>
@@ -4299,210 +4330,249 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="69" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C69" s="7"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="24"/>
-      <c r="F69" s="24"/>
-      <c r="G69" s="25"/>
-      <c r="H69" s="9"/>
-      <c r="I69" s="13"/>
-      <c r="J69" s="9"/>
-      <c r="L69" s="35"/>
-    </row>
-    <row r="70" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="40" t="s">
+    <row r="69" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C69" s="51"/>
+      <c r="D69" s="52"/>
+      <c r="E69" s="53"/>
+      <c r="F69" s="53"/>
+      <c r="G69" s="54"/>
+      <c r="H69" s="158"/>
+      <c r="I69" s="158"/>
+      <c r="J69" s="158"/>
+      <c r="L69" s="57"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C70" s="214">
+        <v>43040</v>
+      </c>
+      <c r="D70" s="202" t="s">
+        <v>243</v>
+      </c>
+      <c r="E70" s="26">
+        <v>10</v>
+      </c>
+      <c r="F70" s="26">
+        <v>1</v>
+      </c>
+      <c r="G70" s="27">
+        <v>0.4</v>
+      </c>
+      <c r="H70" s="215">
+        <f>SUM(G70:G76)</f>
+        <v>3.5799999999999996</v>
+      </c>
+      <c r="I70" s="215">
+        <v>3.39</v>
+      </c>
+      <c r="J70" s="226">
+        <f>H70+I70+K71</f>
+        <v>7.2206000000000001</v>
+      </c>
+      <c r="K70" s="12" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C71" s="214"/>
+      <c r="D71" s="202" t="s">
+        <v>237</v>
+      </c>
+      <c r="E71" s="26">
+        <v>1</v>
+      </c>
+      <c r="F71" s="26">
+        <v>1</v>
+      </c>
+      <c r="G71" s="27">
+        <v>0.9</v>
+      </c>
+      <c r="H71" s="215"/>
+      <c r="I71" s="215"/>
+      <c r="J71" s="226"/>
+      <c r="K71" s="224">
+        <f>SUM(G70:G76)*0.07</f>
+        <v>0.25059999999999999</v>
+      </c>
+      <c r="L71" s="225"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C72" s="214"/>
+      <c r="D72" s="202" t="s">
+        <v>238</v>
+      </c>
+      <c r="E72" s="26">
+        <v>2</v>
+      </c>
+      <c r="F72" s="26">
+        <v>1</v>
+      </c>
+      <c r="G72" s="27">
+        <v>0.64</v>
+      </c>
+      <c r="H72" s="215"/>
+      <c r="I72" s="215"/>
+      <c r="J72" s="226"/>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C73" s="214"/>
+      <c r="D73" s="202" t="s">
+        <v>239</v>
+      </c>
+      <c r="E73" s="26">
+        <v>10</v>
+      </c>
+      <c r="F73" s="26">
+        <v>1</v>
+      </c>
+      <c r="G73" s="27">
+        <v>0.4</v>
+      </c>
+      <c r="H73" s="215"/>
+      <c r="I73" s="215"/>
+      <c r="J73" s="226"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C74" s="214"/>
+      <c r="D74" s="202" t="s">
+        <v>240</v>
+      </c>
+      <c r="E74" s="26">
+        <v>1</v>
+      </c>
+      <c r="F74" s="26">
+        <v>1</v>
+      </c>
+      <c r="G74" s="27">
+        <v>0.32</v>
+      </c>
+      <c r="H74" s="215"/>
+      <c r="I74" s="215"/>
+      <c r="J74" s="226"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C75" s="214"/>
+      <c r="D75" s="202" t="s">
+        <v>241</v>
+      </c>
+      <c r="E75" s="26">
+        <v>1</v>
+      </c>
+      <c r="F75" s="26">
+        <v>1</v>
+      </c>
+      <c r="G75" s="27">
+        <v>0.46</v>
+      </c>
+      <c r="H75" s="215"/>
+      <c r="I75" s="215"/>
+      <c r="J75" s="226"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C76" s="214"/>
+      <c r="D76" s="202" t="s">
+        <v>242</v>
+      </c>
+      <c r="E76" s="26">
+        <v>1</v>
+      </c>
+      <c r="F76" s="26">
+        <v>1</v>
+      </c>
+      <c r="G76" s="27">
+        <v>0.46</v>
+      </c>
+      <c r="H76" s="215"/>
+      <c r="I76" s="215"/>
+      <c r="J76" s="226"/>
+    </row>
+    <row r="77" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C77" s="7"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="24"/>
+      <c r="F77" s="24"/>
+      <c r="G77" s="25"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="9"/>
+      <c r="L77" s="35"/>
+    </row>
+    <row r="78" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C70" s="41">
+      <c r="C78" s="41">
         <f ca="1">TODAY()</f>
-        <v>43035</v>
-      </c>
-      <c r="E70" s="29"/>
-      <c r="F70" s="29"/>
-      <c r="G70" s="29"/>
-      <c r="H70" s="29"/>
-      <c r="I70" s="28" t="s">
+        <v>43041</v>
+      </c>
+      <c r="E78" s="29"/>
+      <c r="F78" s="29"/>
+      <c r="G78" s="29"/>
+      <c r="H78" s="29"/>
+      <c r="I78" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="J70" s="30">
-        <f>SUM(J4:J69)</f>
-        <v>293.11</v>
-      </c>
-      <c r="K70" s="24" t="s">
+      <c r="J78" s="30">
+        <f>SUM(J4:J77)</f>
+        <v>300.3306</v>
+      </c>
+      <c r="K78" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="L70" s="39">
-        <f ca="1">(C70-C4)*0.0328767</f>
-        <v>5.0301350999999999</v>
-      </c>
-      <c r="M70" s="24" t="s">
+      <c r="L78" s="39">
+        <f ca="1">(C78-C4)*0.0328767</f>
+        <v>5.2273953000000004</v>
+      </c>
+      <c r="M78" s="24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C71" s="7"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="24"/>
-      <c r="F71" s="24"/>
-      <c r="G71" s="25"/>
-      <c r="H71" s="31"/>
-      <c r="I71" s="34" t="s">
+    <row r="79" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C79" s="7"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="24"/>
+      <c r="G79" s="25"/>
+      <c r="H79" s="31"/>
+      <c r="I79" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="J71" s="22">
-        <f ca="1">J70/L70</f>
-        <v>58.270800718652673</v>
-      </c>
-      <c r="K71" s="32" t="s">
+      <c r="J79" s="22">
+        <f ca="1">J78/L78</f>
+        <v>57.453202362560944</v>
+      </c>
+      <c r="K79" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="L71" s="36"/>
-      <c r="M71" s="32" t="s">
+      <c r="L79" s="36"/>
+      <c r="M79" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="N71" s="33"/>
-    </row>
-    <row r="72" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="58"/>
-      <c r="B72" s="58"/>
-      <c r="C72" s="44"/>
-      <c r="D72" s="45"/>
-      <c r="E72" s="46"/>
-      <c r="F72" s="46"/>
-      <c r="G72" s="47"/>
-      <c r="H72" s="48"/>
-      <c r="I72" s="59"/>
-      <c r="J72" s="48"/>
-      <c r="K72" s="58"/>
-      <c r="L72" s="60"/>
-      <c r="M72" s="58"/>
-      <c r="N72" s="58"/>
-      <c r="O72" s="58"/>
-    </row>
-    <row r="73" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C73" s="7"/>
-      <c r="D73" s="63" t="s">
-        <v>75</v>
-      </c>
-      <c r="E73" s="203" t="s">
-        <v>227</v>
-      </c>
-      <c r="H73" s="10"/>
-      <c r="I73" s="11"/>
-      <c r="J73" s="10"/>
-      <c r="L73" s="35"/>
-    </row>
-    <row r="74" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C74" s="7"/>
-      <c r="D74" s="8"/>
-      <c r="E74" s="24"/>
-      <c r="F74" s="24"/>
-      <c r="G74" s="25"/>
-      <c r="H74" s="10"/>
-      <c r="I74" s="11"/>
-      <c r="J74" s="10"/>
-      <c r="L74" s="35"/>
-    </row>
-    <row r="75" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C75" s="7"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="24"/>
-      <c r="F75" s="24"/>
-      <c r="G75" s="25"/>
-      <c r="H75" s="10"/>
-      <c r="I75" s="11"/>
-      <c r="J75" s="10"/>
-      <c r="L75" s="35"/>
-    </row>
-    <row r="76" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C76" s="147" t="s">
-        <v>164</v>
-      </c>
-      <c r="D76" s="148"/>
-      <c r="E76" s="24"/>
-      <c r="F76" s="24"/>
-      <c r="G76" s="25"/>
-      <c r="H76" s="10"/>
-      <c r="I76" s="11"/>
-      <c r="J76" s="10"/>
-      <c r="L76" s="35"/>
-    </row>
-    <row r="77" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C77" s="49"/>
-      <c r="D77" s="95" t="s">
-        <v>0</v>
-      </c>
-      <c r="E77" s="98"/>
-      <c r="F77" s="98" t="s">
-        <v>160</v>
-      </c>
-      <c r="G77" s="99">
-        <v>2.19</v>
-      </c>
-      <c r="H77" s="10"/>
-      <c r="I77" s="11"/>
-      <c r="J77" s="10"/>
-      <c r="L77" s="35"/>
-    </row>
-    <row r="78" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C78" s="7"/>
-      <c r="D78" s="95" t="s">
-        <v>1</v>
-      </c>
-      <c r="E78" s="98"/>
-      <c r="F78" s="98" t="s">
-        <v>160</v>
-      </c>
-      <c r="G78" s="99">
-        <v>1.06</v>
-      </c>
-      <c r="H78" s="10"/>
-      <c r="I78" s="11"/>
-      <c r="J78" s="10"/>
-      <c r="L78" s="35"/>
-    </row>
-    <row r="79" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C79" s="7"/>
-      <c r="D79" s="95" t="str">
-        <f>D24</f>
-        <v>NOKIA 5110 LCD</v>
-      </c>
-      <c r="E79" s="98"/>
-      <c r="F79" s="98"/>
-      <c r="G79" s="99">
-        <f>G24</f>
-        <v>1.97</v>
-      </c>
-      <c r="H79" s="10"/>
-      <c r="I79" s="11"/>
-      <c r="J79" s="10"/>
-      <c r="L79" s="35"/>
+      <c r="N79" s="33"/>
     </row>
     <row r="80" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C80" s="7"/>
-      <c r="D80" s="95" t="s">
-        <v>5</v>
-      </c>
-      <c r="E80" s="98"/>
-      <c r="F80" s="98"/>
-      <c r="G80" s="99">
-        <v>0.2485</v>
-      </c>
-      <c r="H80" s="10"/>
-      <c r="I80" s="11"/>
-      <c r="J80" s="10"/>
-      <c r="L80" s="35"/>
+      <c r="A80" s="58"/>
+      <c r="B80" s="58"/>
+      <c r="C80" s="44"/>
+      <c r="D80" s="45"/>
+      <c r="E80" s="46"/>
+      <c r="F80" s="46"/>
+      <c r="G80" s="47"/>
+      <c r="H80" s="48"/>
+      <c r="I80" s="59"/>
+      <c r="J80" s="48"/>
+      <c r="K80" s="58"/>
+      <c r="L80" s="60"/>
+      <c r="M80" s="58"/>
+      <c r="N80" s="58"/>
+      <c r="O80" s="58"/>
     </row>
     <row r="81" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C81" s="7"/>
-      <c r="D81" s="95" t="s">
-        <v>156</v>
-      </c>
-      <c r="E81" s="98"/>
-      <c r="F81" s="98"/>
-      <c r="G81" s="99">
-        <v>0.29949999999999999</v>
+      <c r="D81" s="63" t="s">
+        <v>75</v>
+      </c>
+      <c r="E81" s="203" t="s">
+        <v>227</v>
       </c>
       <c r="H81" s="10"/>
       <c r="I81" s="11"/>
@@ -4511,14 +4581,10 @@
     </row>
     <row r="82" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C82" s="7"/>
-      <c r="D82" s="95" t="s">
-        <v>158</v>
-      </c>
-      <c r="E82" s="98"/>
-      <c r="F82" s="98"/>
-      <c r="G82" s="99">
-        <v>1</v>
-      </c>
+      <c r="D82" s="8"/>
+      <c r="E82" s="24"/>
+      <c r="F82" s="24"/>
+      <c r="G82" s="25"/>
       <c r="H82" s="10"/>
       <c r="I82" s="11"/>
       <c r="J82" s="10"/>
@@ -4526,43 +4592,39 @@
     </row>
     <row r="83" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C83" s="7"/>
-      <c r="D83" s="95" t="s">
-        <v>155</v>
-      </c>
-      <c r="E83" s="98"/>
-      <c r="F83" s="98"/>
-      <c r="G83" s="99">
-        <v>6.25</v>
-      </c>
+      <c r="D83" s="8"/>
+      <c r="E83" s="24"/>
+      <c r="F83" s="24"/>
+      <c r="G83" s="25"/>
       <c r="H83" s="10"/>
       <c r="I83" s="11"/>
       <c r="J83" s="10"/>
       <c r="L83" s="35"/>
     </row>
     <row r="84" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C84" s="7"/>
-      <c r="D84" s="95" t="s">
-        <v>157</v>
-      </c>
-      <c r="E84" s="98"/>
-      <c r="F84" s="98"/>
-      <c r="G84" s="99">
-        <v>0.57950000000000002</v>
-      </c>
+      <c r="C84" s="147" t="s">
+        <v>164</v>
+      </c>
+      <c r="D84" s="148"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="24"/>
+      <c r="G84" s="25"/>
       <c r="H84" s="10"/>
       <c r="I84" s="11"/>
       <c r="J84" s="10"/>
       <c r="L84" s="35"/>
     </row>
     <row r="85" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C85" s="7"/>
+      <c r="C85" s="49"/>
       <c r="D85" s="95" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E85" s="98"/>
-      <c r="F85" s="98"/>
+      <c r="F85" s="98" t="s">
+        <v>160</v>
+      </c>
       <c r="G85" s="99">
-        <v>1.0640000000000001</v>
+        <v>2.19</v>
       </c>
       <c r="H85" s="10"/>
       <c r="I85" s="11"/>
@@ -4572,12 +4634,14 @@
     <row r="86" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C86" s="7"/>
       <c r="D86" s="95" t="s">
-        <v>161</v>
+        <v>1</v>
       </c>
       <c r="E86" s="98"/>
-      <c r="F86" s="98"/>
+      <c r="F86" s="98" t="s">
+        <v>160</v>
+      </c>
       <c r="G86" s="99">
-        <v>0.5</v>
+        <v>1.06</v>
       </c>
       <c r="H86" s="10"/>
       <c r="I86" s="11"/>
@@ -4585,46 +4649,47 @@
       <c r="L86" s="35"/>
     </row>
     <row r="87" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C87" s="44"/>
-      <c r="D87" s="96" t="s">
-        <v>159</v>
-      </c>
-      <c r="E87" s="100"/>
-      <c r="F87" s="100"/>
-      <c r="G87" s="101">
-        <v>2</v>
-      </c>
-      <c r="H87" s="48"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="95" t="str">
+        <f>D24</f>
+        <v>NOKIA 5110 LCD</v>
+      </c>
+      <c r="E87" s="98"/>
+      <c r="F87" s="98"/>
+      <c r="G87" s="99">
+        <f>G24</f>
+        <v>1.97</v>
+      </c>
+      <c r="H87" s="10"/>
       <c r="I87" s="11"/>
       <c r="J87" s="10"/>
       <c r="L87" s="35"/>
     </row>
     <row r="88" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="58"/>
-      <c r="B88" s="58"/>
-      <c r="C88" s="44"/>
-      <c r="D88" s="45"/>
-      <c r="E88" s="46"/>
-      <c r="F88" s="46"/>
-      <c r="G88" s="97">
-        <f>SUM(G77:G87)</f>
-        <v>17.1615</v>
-      </c>
-      <c r="H88" s="48"/>
-      <c r="I88" s="59"/>
-      <c r="J88" s="48"/>
-      <c r="K88" s="58"/>
-      <c r="L88" s="60"/>
-      <c r="M88" s="58"/>
-      <c r="N88" s="58"/>
-      <c r="O88" s="58"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="95" t="s">
+        <v>5</v>
+      </c>
+      <c r="E88" s="98"/>
+      <c r="F88" s="98"/>
+      <c r="G88" s="99">
+        <v>0.2485</v>
+      </c>
+      <c r="H88" s="10"/>
+      <c r="I88" s="11"/>
+      <c r="J88" s="10"/>
+      <c r="L88" s="35"/>
     </row>
     <row r="89" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C89" s="7"/>
-      <c r="D89" s="8"/>
-      <c r="E89" s="24"/>
-      <c r="F89" s="24"/>
-      <c r="G89" s="25"/>
+      <c r="D89" s="95" t="s">
+        <v>156</v>
+      </c>
+      <c r="E89" s="98"/>
+      <c r="F89" s="98"/>
+      <c r="G89" s="99">
+        <v>0.29949999999999999</v>
+      </c>
       <c r="H89" s="10"/>
       <c r="I89" s="11"/>
       <c r="J89" s="10"/>
@@ -4632,10 +4697,14 @@
     </row>
     <row r="90" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C90" s="7"/>
-      <c r="D90" s="8"/>
-      <c r="E90" s="24"/>
-      <c r="F90" s="24"/>
-      <c r="G90" s="25"/>
+      <c r="D90" s="95" t="s">
+        <v>158</v>
+      </c>
+      <c r="E90" s="98"/>
+      <c r="F90" s="98"/>
+      <c r="G90" s="99">
+        <v>1</v>
+      </c>
       <c r="H90" s="10"/>
       <c r="I90" s="11"/>
       <c r="J90" s="10"/>
@@ -4643,10 +4712,14 @@
     </row>
     <row r="91" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C91" s="7"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="24"/>
-      <c r="F91" s="24"/>
-      <c r="G91" s="25"/>
+      <c r="D91" s="95" t="s">
+        <v>155</v>
+      </c>
+      <c r="E91" s="98"/>
+      <c r="F91" s="98"/>
+      <c r="G91" s="99">
+        <v>6.25</v>
+      </c>
       <c r="H91" s="10"/>
       <c r="I91" s="11"/>
       <c r="J91" s="10"/>
@@ -4654,521 +4727,553 @@
     </row>
     <row r="92" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C92" s="7"/>
-      <c r="D92" s="8"/>
-      <c r="E92" s="24"/>
-      <c r="F92" s="24"/>
-      <c r="G92" s="25"/>
+      <c r="D92" s="95" t="s">
+        <v>157</v>
+      </c>
+      <c r="E92" s="98"/>
+      <c r="F92" s="98"/>
+      <c r="G92" s="99">
+        <v>0.57950000000000002</v>
+      </c>
       <c r="H92" s="10"/>
       <c r="I92" s="11"/>
       <c r="J92" s="10"/>
       <c r="L92" s="35"/>
     </row>
-    <row r="93" spans="1:15" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C93" s="93" t="s">
-        <v>163</v>
-      </c>
-      <c r="D93" s="94"/>
-      <c r="E93" s="18"/>
-      <c r="H93" s="14"/>
-      <c r="I93" s="17"/>
-      <c r="J93" s="14"/>
-      <c r="K93" s="14"/>
-      <c r="L93" s="14"/>
-    </row>
-    <row r="94" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C94" s="144"/>
-      <c r="D94" s="151" t="s">
-        <v>226</v>
+    <row r="93" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C93" s="7"/>
+      <c r="D93" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="E93" s="98"/>
+      <c r="F93" s="98"/>
+      <c r="G93" s="99">
+        <v>1.0640000000000001</v>
+      </c>
+      <c r="H93" s="10"/>
+      <c r="I93" s="11"/>
+      <c r="J93" s="10"/>
+      <c r="L93" s="35"/>
+    </row>
+    <row r="94" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C94" s="7"/>
+      <c r="D94" s="95" t="s">
+        <v>161</v>
       </c>
       <c r="E94" s="98"/>
       <c r="F94" s="98"/>
       <c r="G94" s="99">
-        <v>1.53</v>
-      </c>
-      <c r="H94" s="157"/>
-      <c r="I94" s="158"/>
-      <c r="J94" s="157"/>
-      <c r="K94" s="157"/>
-      <c r="L94" s="159"/>
-    </row>
-    <row r="95" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C95" s="144"/>
-      <c r="D95" s="151" t="s">
-        <v>30</v>
-      </c>
-      <c r="E95" s="98"/>
-      <c r="F95" s="98"/>
-      <c r="G95" s="99">
-        <v>33.57</v>
-      </c>
-      <c r="H95" s="157"/>
-      <c r="I95" s="158"/>
-      <c r="J95" s="157"/>
-      <c r="K95" s="157"/>
-      <c r="L95" s="159"/>
-    </row>
-    <row r="96" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C96" s="144"/>
-      <c r="D96" s="151" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="H94" s="10"/>
+      <c r="I94" s="11"/>
+      <c r="J94" s="10"/>
+      <c r="L94" s="35"/>
+    </row>
+    <row r="95" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C95" s="44"/>
+      <c r="D95" s="96" t="s">
+        <v>159</v>
+      </c>
+      <c r="E95" s="100"/>
+      <c r="F95" s="100"/>
+      <c r="G95" s="101">
         <v>2</v>
       </c>
-      <c r="E96" s="98"/>
-      <c r="F96" s="98"/>
-      <c r="G96" s="99">
-        <v>6.56</v>
-      </c>
-      <c r="H96" s="157"/>
-      <c r="I96" s="158"/>
-      <c r="J96" s="157"/>
-      <c r="K96" s="157"/>
-      <c r="L96" s="159"/>
-    </row>
-    <row r="97" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C97" s="144"/>
-      <c r="D97" s="151" t="s">
-        <v>11</v>
-      </c>
-      <c r="E97" s="98"/>
-      <c r="F97" s="98"/>
-      <c r="G97" s="99">
-        <v>2.57</v>
-      </c>
-      <c r="H97" s="157"/>
-      <c r="I97" s="158"/>
-      <c r="J97" s="157"/>
-      <c r="K97" s="157"/>
-      <c r="L97" s="159"/>
-    </row>
-    <row r="98" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C98" s="144"/>
-      <c r="D98" s="151" t="s">
-        <v>61</v>
-      </c>
-      <c r="E98" s="98"/>
-      <c r="F98" s="98"/>
-      <c r="G98" s="99">
-        <v>5.22</v>
-      </c>
-      <c r="H98" s="157"/>
-      <c r="I98" s="158"/>
-      <c r="J98" s="157"/>
-      <c r="K98" s="157"/>
-      <c r="L98" s="159"/>
-    </row>
-    <row r="99" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C99" s="144"/>
-      <c r="D99" s="151" t="s">
-        <v>162</v>
-      </c>
-      <c r="E99" s="98"/>
-      <c r="F99" s="98"/>
-      <c r="G99" s="99">
-        <v>0.39900000000000002</v>
-      </c>
-      <c r="H99" s="157"/>
-      <c r="I99" s="158"/>
-      <c r="J99" s="157"/>
-      <c r="K99" s="157"/>
-      <c r="L99" s="159"/>
-    </row>
-    <row r="100" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C100" s="145"/>
-      <c r="D100" s="151" t="s">
-        <v>73</v>
-      </c>
-      <c r="E100" s="98"/>
-      <c r="F100" s="98"/>
-      <c r="G100" s="99">
-        <v>0.77</v>
-      </c>
-      <c r="H100" s="9"/>
-      <c r="I100" s="13"/>
-      <c r="J100" s="9"/>
-      <c r="K100" s="9"/>
-      <c r="L100" s="38"/>
-    </row>
-    <row r="101" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C101" s="145"/>
-      <c r="D101" s="151" t="s">
-        <v>6</v>
-      </c>
-      <c r="E101" s="98"/>
-      <c r="F101" s="98"/>
-      <c r="G101" s="99">
-        <v>0.02</v>
-      </c>
-      <c r="H101" s="9"/>
-      <c r="I101" s="13"/>
-      <c r="J101" s="9"/>
-      <c r="K101" s="9"/>
-      <c r="L101" s="38"/>
-    </row>
-    <row r="102" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C102" s="145"/>
-      <c r="D102" s="153" t="s">
-        <v>168</v>
+      <c r="H95" s="48"/>
+      <c r="I95" s="11"/>
+      <c r="J95" s="10"/>
+      <c r="L95" s="35"/>
+    </row>
+    <row r="96" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="58"/>
+      <c r="B96" s="58"/>
+      <c r="C96" s="44"/>
+      <c r="D96" s="45"/>
+      <c r="E96" s="46"/>
+      <c r="F96" s="46"/>
+      <c r="G96" s="97">
+        <f>SUM(G85:G95)</f>
+        <v>17.1615</v>
+      </c>
+      <c r="H96" s="48"/>
+      <c r="I96" s="59"/>
+      <c r="J96" s="48"/>
+      <c r="K96" s="58"/>
+      <c r="L96" s="60"/>
+      <c r="M96" s="58"/>
+      <c r="N96" s="58"/>
+      <c r="O96" s="58"/>
+    </row>
+    <row r="97" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C97" s="7"/>
+      <c r="D97" s="8"/>
+      <c r="E97" s="24"/>
+      <c r="F97" s="24"/>
+      <c r="G97" s="25"/>
+      <c r="H97" s="10"/>
+      <c r="I97" s="11"/>
+      <c r="J97" s="10"/>
+      <c r="L97" s="35"/>
+    </row>
+    <row r="98" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C98" s="7"/>
+      <c r="D98" s="8"/>
+      <c r="E98" s="24"/>
+      <c r="F98" s="24"/>
+      <c r="G98" s="25"/>
+      <c r="H98" s="10"/>
+      <c r="I98" s="11"/>
+      <c r="J98" s="10"/>
+      <c r="L98" s="35"/>
+    </row>
+    <row r="99" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C99" s="7"/>
+      <c r="D99" s="8"/>
+      <c r="E99" s="24"/>
+      <c r="F99" s="24"/>
+      <c r="G99" s="25"/>
+      <c r="H99" s="10"/>
+      <c r="I99" s="11"/>
+      <c r="J99" s="10"/>
+      <c r="L99" s="35"/>
+    </row>
+    <row r="100" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C100" s="7"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="24"/>
+      <c r="F100" s="24"/>
+      <c r="G100" s="25"/>
+      <c r="H100" s="10"/>
+      <c r="I100" s="11"/>
+      <c r="J100" s="10"/>
+      <c r="L100" s="35"/>
+    </row>
+    <row r="101" spans="3:12" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C101" s="93" t="s">
+        <v>163</v>
+      </c>
+      <c r="D101" s="94"/>
+      <c r="E101" s="18"/>
+      <c r="H101" s="14"/>
+      <c r="I101" s="17"/>
+      <c r="J101" s="14"/>
+      <c r="K101" s="14"/>
+      <c r="L101" s="14"/>
+    </row>
+    <row r="102" spans="3:12" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C102" s="144"/>
+      <c r="D102" s="151" t="s">
+        <v>226</v>
       </c>
       <c r="E102" s="98"/>
       <c r="F102" s="98"/>
       <c r="G102" s="99">
-        <f>5.72+(0.5*4.99)</f>
-        <v>8.2149999999999999</v>
-      </c>
-      <c r="H102" s="9"/>
-      <c r="I102" s="13"/>
-      <c r="J102" s="9"/>
-      <c r="K102" s="9"/>
-      <c r="L102" s="38"/>
-    </row>
-    <row r="103" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C103" s="145"/>
+        <v>1.53</v>
+      </c>
+      <c r="H102" s="157"/>
+      <c r="I102" s="158"/>
+      <c r="J102" s="157"/>
+      <c r="K102" s="157"/>
+      <c r="L102" s="159"/>
+    </row>
+    <row r="103" spans="3:12" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C103" s="144"/>
       <c r="D103" s="151" t="s">
-        <v>169</v>
+        <v>30</v>
       </c>
       <c r="E103" s="98"/>
       <c r="F103" s="98"/>
       <c r="G103" s="99">
-        <f>2.83+(0.5*4.99)</f>
-        <v>5.3250000000000002</v>
-      </c>
-      <c r="H103" s="9"/>
-      <c r="I103" s="13"/>
-      <c r="J103" s="9"/>
-      <c r="K103" s="9"/>
-      <c r="L103" s="38"/>
-    </row>
-    <row r="104" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C104" s="146"/>
-      <c r="D104" s="152" t="s">
-        <v>74</v>
-      </c>
-      <c r="E104" s="100"/>
-      <c r="F104" s="100"/>
-      <c r="G104" s="101">
-        <v>1.53</v>
-      </c>
-      <c r="H104" s="160"/>
-      <c r="I104" s="13"/>
-      <c r="J104" s="9"/>
-      <c r="K104" s="9"/>
-      <c r="L104" s="38"/>
-    </row>
-    <row r="105" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="67"/>
-      <c r="B105" s="67"/>
-      <c r="C105" s="68"/>
-      <c r="D105" s="69"/>
-      <c r="E105" s="70"/>
-      <c r="F105" s="70"/>
-      <c r="G105" s="97">
-        <f>SUM(G94:G104)</f>
-        <v>65.709000000000017</v>
-      </c>
-      <c r="H105" s="71"/>
-      <c r="I105" s="72"/>
-      <c r="J105" s="71"/>
-      <c r="K105" s="67"/>
-      <c r="L105" s="67"/>
-      <c r="M105" s="67"/>
-      <c r="N105" s="67"/>
-      <c r="O105" s="67"/>
-    </row>
-    <row r="106" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C106" s="51"/>
-      <c r="D106" s="73"/>
-      <c r="E106" s="74"/>
-      <c r="F106" s="74"/>
-      <c r="G106" s="75"/>
-      <c r="H106" s="55"/>
-      <c r="I106" s="56"/>
-      <c r="J106" s="55"/>
-      <c r="L106" s="57"/>
-    </row>
-    <row r="107" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="79"/>
-      <c r="B108" s="79"/>
-      <c r="C108" s="80"/>
-      <c r="D108" s="81"/>
-      <c r="E108" s="82"/>
-      <c r="F108" s="82"/>
-      <c r="G108" s="83"/>
-      <c r="H108" s="84"/>
-      <c r="I108" s="85"/>
-      <c r="J108" s="84"/>
-      <c r="K108" s="79"/>
-      <c r="L108" s="79"/>
-      <c r="M108" s="79"/>
-      <c r="N108" s="79"/>
-      <c r="O108" s="79"/>
-    </row>
-    <row r="109" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C109" s="87"/>
-      <c r="D109" s="88"/>
-      <c r="E109" s="61"/>
-      <c r="F109" s="61"/>
-      <c r="G109" s="89"/>
-      <c r="H109" s="90"/>
-      <c r="I109" s="91"/>
-      <c r="J109" s="90"/>
-      <c r="L109" s="92"/>
-    </row>
-    <row r="110" spans="1:15" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C110" s="93" t="s">
-        <v>165</v>
-      </c>
-      <c r="D110" s="94"/>
-      <c r="E110" s="18"/>
-      <c r="H110" s="64"/>
-      <c r="I110" s="65"/>
-      <c r="J110" s="64"/>
-    </row>
-    <row r="111" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C111" s="144"/>
+        <v>33.57</v>
+      </c>
+      <c r="H103" s="157"/>
+      <c r="I103" s="158"/>
+      <c r="J103" s="157"/>
+      <c r="K103" s="157"/>
+      <c r="L103" s="159"/>
+    </row>
+    <row r="104" spans="3:12" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C104" s="144"/>
+      <c r="D104" s="151" t="s">
+        <v>2</v>
+      </c>
+      <c r="E104" s="98"/>
+      <c r="F104" s="98"/>
+      <c r="G104" s="99">
+        <v>6.56</v>
+      </c>
+      <c r="H104" s="157"/>
+      <c r="I104" s="158"/>
+      <c r="J104" s="157"/>
+      <c r="K104" s="157"/>
+      <c r="L104" s="159"/>
+    </row>
+    <row r="105" spans="3:12" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C105" s="144"/>
+      <c r="D105" s="151" t="s">
+        <v>11</v>
+      </c>
+      <c r="E105" s="98"/>
+      <c r="F105" s="98"/>
+      <c r="G105" s="99">
+        <v>2.57</v>
+      </c>
+      <c r="H105" s="157"/>
+      <c r="I105" s="158"/>
+      <c r="J105" s="157"/>
+      <c r="K105" s="157"/>
+      <c r="L105" s="159"/>
+    </row>
+    <row r="106" spans="3:12" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C106" s="144"/>
+      <c r="D106" s="151" t="s">
+        <v>61</v>
+      </c>
+      <c r="E106" s="98"/>
+      <c r="F106" s="98"/>
+      <c r="G106" s="99">
+        <v>5.22</v>
+      </c>
+      <c r="H106" s="157"/>
+      <c r="I106" s="158"/>
+      <c r="J106" s="157"/>
+      <c r="K106" s="157"/>
+      <c r="L106" s="159"/>
+    </row>
+    <row r="107" spans="3:12" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C107" s="144"/>
+      <c r="D107" s="151" t="s">
+        <v>162</v>
+      </c>
+      <c r="E107" s="98"/>
+      <c r="F107" s="98"/>
+      <c r="G107" s="99">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="H107" s="157"/>
+      <c r="I107" s="158"/>
+      <c r="J107" s="157"/>
+      <c r="K107" s="157"/>
+      <c r="L107" s="159"/>
+    </row>
+    <row r="108" spans="3:12" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C108" s="145"/>
+      <c r="D108" s="151" t="s">
+        <v>73</v>
+      </c>
+      <c r="E108" s="98"/>
+      <c r="F108" s="98"/>
+      <c r="G108" s="99">
+        <v>0.77</v>
+      </c>
+      <c r="H108" s="9"/>
+      <c r="I108" s="13"/>
+      <c r="J108" s="9"/>
+      <c r="K108" s="9"/>
+      <c r="L108" s="38"/>
+    </row>
+    <row r="109" spans="3:12" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C109" s="145"/>
+      <c r="D109" s="151" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" s="98"/>
+      <c r="F109" s="98"/>
+      <c r="G109" s="99">
+        <v>0.02</v>
+      </c>
+      <c r="H109" s="9"/>
+      <c r="I109" s="13"/>
+      <c r="J109" s="9"/>
+      <c r="K109" s="9"/>
+      <c r="L109" s="38"/>
+    </row>
+    <row r="110" spans="3:12" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C110" s="145"/>
+      <c r="D110" s="153" t="s">
+        <v>168</v>
+      </c>
+      <c r="E110" s="98"/>
+      <c r="F110" s="98"/>
+      <c r="G110" s="99">
+        <f>5.72+(0.5*4.99)</f>
+        <v>8.2149999999999999</v>
+      </c>
+      <c r="H110" s="9"/>
+      <c r="I110" s="13"/>
+      <c r="J110" s="9"/>
+      <c r="K110" s="9"/>
+      <c r="L110" s="38"/>
+    </row>
+    <row r="111" spans="3:12" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C111" s="145"/>
       <c r="D111" s="151" t="s">
-        <v>225</v>
+        <v>169</v>
       </c>
       <c r="E111" s="98"/>
       <c r="F111" s="98"/>
       <c r="G111" s="99">
+        <f>2.83+(0.5*4.99)</f>
+        <v>5.3250000000000002</v>
+      </c>
+      <c r="H111" s="9"/>
+      <c r="I111" s="13"/>
+      <c r="J111" s="9"/>
+      <c r="K111" s="9"/>
+      <c r="L111" s="38"/>
+    </row>
+    <row r="112" spans="3:12" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C112" s="146"/>
+      <c r="D112" s="152" t="s">
+        <v>74</v>
+      </c>
+      <c r="E112" s="100"/>
+      <c r="F112" s="100"/>
+      <c r="G112" s="101">
         <v>1.53</v>
       </c>
-      <c r="H111" s="55"/>
-      <c r="I111" s="56"/>
-      <c r="J111" s="55"/>
-      <c r="L111" s="57"/>
-    </row>
-    <row r="112" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C112" s="144"/>
-      <c r="D112" s="151" t="s">
-        <v>166</v>
-      </c>
-      <c r="E112" s="98"/>
-      <c r="F112" s="98"/>
-      <c r="G112" s="99">
-        <v>33.57</v>
-      </c>
-      <c r="H112" s="55"/>
-      <c r="I112" s="56"/>
-      <c r="J112" s="55"/>
-      <c r="L112" s="57"/>
-    </row>
-    <row r="113" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C113" s="144"/>
-      <c r="D113" s="151" t="s">
-        <v>2</v>
-      </c>
-      <c r="E113" s="98"/>
-      <c r="F113" s="98"/>
-      <c r="G113" s="99">
-        <v>6.56</v>
-      </c>
-      <c r="H113" s="55"/>
-      <c r="I113" s="56"/>
-      <c r="J113" s="55"/>
-      <c r="L113" s="57"/>
-    </row>
-    <row r="114" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C114" s="144"/>
-      <c r="D114" s="151" t="s">
-        <v>61</v>
-      </c>
-      <c r="E114" s="98"/>
-      <c r="F114" s="98"/>
-      <c r="G114" s="99">
-        <v>6.91</v>
-      </c>
+      <c r="H112" s="160"/>
+      <c r="I112" s="13"/>
+      <c r="J112" s="9"/>
+      <c r="K112" s="9"/>
+      <c r="L112" s="38"/>
+    </row>
+    <row r="113" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="67"/>
+      <c r="B113" s="67"/>
+      <c r="C113" s="68"/>
+      <c r="D113" s="69"/>
+      <c r="E113" s="70"/>
+      <c r="F113" s="70"/>
+      <c r="G113" s="97">
+        <f>SUM(G102:G112)</f>
+        <v>65.709000000000017</v>
+      </c>
+      <c r="H113" s="71"/>
+      <c r="I113" s="72"/>
+      <c r="J113" s="71"/>
+      <c r="K113" s="67"/>
+      <c r="L113" s="67"/>
+      <c r="M113" s="67"/>
+      <c r="N113" s="67"/>
+      <c r="O113" s="67"/>
+    </row>
+    <row r="114" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C114" s="51"/>
+      <c r="D114" s="73"/>
+      <c r="E114" s="74"/>
+      <c r="F114" s="74"/>
+      <c r="G114" s="75"/>
       <c r="H114" s="55"/>
       <c r="I114" s="56"/>
       <c r="J114" s="55"/>
       <c r="L114" s="57"/>
     </row>
-    <row r="115" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C115" s="145"/>
-      <c r="D115" s="151" t="s">
-        <v>162</v>
-      </c>
-      <c r="E115" s="98"/>
-      <c r="F115" s="98"/>
-      <c r="G115" s="99">
-        <v>0.39900000000000002</v>
-      </c>
-      <c r="H115" s="10"/>
-      <c r="I115" s="11"/>
-      <c r="J115" s="10"/>
-      <c r="L115" s="35"/>
-    </row>
-    <row r="116" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C116" s="145"/>
-      <c r="D116" s="151" t="s">
-        <v>11</v>
-      </c>
-      <c r="E116" s="98"/>
-      <c r="F116" s="98"/>
-      <c r="G116" s="99">
-        <v>2.57</v>
-      </c>
-      <c r="H116" s="10"/>
-      <c r="I116" s="11"/>
-      <c r="J116" s="10"/>
-      <c r="L116" s="35"/>
-    </row>
-    <row r="117" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C117" s="145"/>
-      <c r="D117" s="151" t="s">
-        <v>6</v>
-      </c>
-      <c r="E117" s="98"/>
-      <c r="F117" s="98"/>
-      <c r="G117" s="99">
-        <v>0.02</v>
-      </c>
-      <c r="H117" s="10"/>
-      <c r="I117" s="11"/>
-      <c r="J117" s="10"/>
-      <c r="L117" s="35"/>
-    </row>
-    <row r="118" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D118" s="151" t="s">
-        <v>73</v>
-      </c>
-      <c r="E118" s="98"/>
-      <c r="F118" s="98"/>
-      <c r="G118" s="99">
-        <v>0.77</v>
-      </c>
+    <row r="115" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="79"/>
+      <c r="B116" s="79"/>
+      <c r="C116" s="80"/>
+      <c r="D116" s="81"/>
+      <c r="E116" s="82"/>
+      <c r="F116" s="82"/>
+      <c r="G116" s="83"/>
+      <c r="H116" s="84"/>
+      <c r="I116" s="85"/>
+      <c r="J116" s="84"/>
+      <c r="K116" s="79"/>
+      <c r="L116" s="79"/>
+      <c r="M116" s="79"/>
+      <c r="N116" s="79"/>
+      <c r="O116" s="79"/>
+    </row>
+    <row r="117" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C117" s="87"/>
+      <c r="D117" s="88"/>
+      <c r="E117" s="61"/>
+      <c r="F117" s="61"/>
+      <c r="G117" s="89"/>
+      <c r="H117" s="90"/>
+      <c r="I117" s="91"/>
+      <c r="J117" s="90"/>
+      <c r="L117" s="92"/>
+    </row>
+    <row r="118" spans="1:15" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C118" s="93" t="s">
+        <v>165</v>
+      </c>
+      <c r="D118" s="94"/>
+      <c r="E118" s="18"/>
+      <c r="H118" s="64"/>
+      <c r="I118" s="65"/>
+      <c r="J118" s="64"/>
     </row>
     <row r="119" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D119" s="154" t="s">
-        <v>74</v>
-      </c>
-      <c r="E119" s="155"/>
-      <c r="F119" s="155"/>
-      <c r="G119" s="156">
+      <c r="C119" s="144"/>
+      <c r="D119" s="151" t="s">
+        <v>225</v>
+      </c>
+      <c r="E119" s="98"/>
+      <c r="F119" s="98"/>
+      <c r="G119" s="99">
         <v>1.53</v>
       </c>
+      <c r="H119" s="55"/>
+      <c r="I119" s="56"/>
+      <c r="J119" s="55"/>
+      <c r="L119" s="57"/>
     </row>
     <row r="120" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C120" s="146"/>
-      <c r="D120" s="152" t="s">
-        <v>224</v>
-      </c>
-      <c r="E120" s="100"/>
-      <c r="F120" s="100"/>
-      <c r="G120" s="101">
-        <v>3.78</v>
-      </c>
-      <c r="H120" s="48"/>
-      <c r="I120" s="11"/>
-      <c r="J120" s="10"/>
-      <c r="K120" s="12"/>
-      <c r="L120" s="35"/>
-      <c r="M120" s="12"/>
-      <c r="N120" s="12"/>
-      <c r="O120" s="12"/>
-    </row>
-    <row r="121" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="67"/>
-      <c r="B121" s="67"/>
-      <c r="C121" s="68"/>
-      <c r="D121" s="69"/>
-      <c r="E121" s="70"/>
-      <c r="F121" s="70"/>
-      <c r="G121" s="97">
-        <f>SUM(G111:G120)</f>
-        <v>57.639000000000017</v>
-      </c>
-      <c r="H121" s="71"/>
-      <c r="I121" s="72"/>
-      <c r="J121" s="71"/>
-      <c r="K121" s="67"/>
-      <c r="L121" s="67"/>
-      <c r="M121" s="67"/>
-      <c r="N121" s="67"/>
-      <c r="O121" s="67"/>
-    </row>
-    <row r="122" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C122" s="51"/>
-      <c r="D122" s="52"/>
-      <c r="E122" s="53"/>
-      <c r="F122" s="53"/>
-      <c r="G122" s="54"/>
+      <c r="C120" s="144"/>
+      <c r="D120" s="151" t="s">
+        <v>166</v>
+      </c>
+      <c r="E120" s="98"/>
+      <c r="F120" s="98"/>
+      <c r="G120" s="99">
+        <v>33.57</v>
+      </c>
+      <c r="H120" s="55"/>
+      <c r="I120" s="56"/>
+      <c r="J120" s="55"/>
+      <c r="L120" s="57"/>
+    </row>
+    <row r="121" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C121" s="144"/>
+      <c r="D121" s="151" t="s">
+        <v>2</v>
+      </c>
+      <c r="E121" s="98"/>
+      <c r="F121" s="98"/>
+      <c r="G121" s="99">
+        <v>6.56</v>
+      </c>
+      <c r="H121" s="55"/>
+      <c r="I121" s="56"/>
+      <c r="J121" s="55"/>
+      <c r="L121" s="57"/>
+    </row>
+    <row r="122" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C122" s="144"/>
+      <c r="D122" s="151" t="s">
+        <v>61</v>
+      </c>
+      <c r="E122" s="98"/>
+      <c r="F122" s="98"/>
+      <c r="G122" s="99">
+        <v>6.91</v>
+      </c>
       <c r="H122" s="55"/>
       <c r="I122" s="56"/>
       <c r="J122" s="55"/>
       <c r="L122" s="57"/>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C123" s="51"/>
-      <c r="D123" s="52"/>
-      <c r="E123" s="53"/>
-      <c r="F123" s="53"/>
-      <c r="G123" s="54"/>
-      <c r="H123" s="55"/>
-      <c r="I123" s="56"/>
-      <c r="J123" s="55"/>
-    </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C124" s="51"/>
-      <c r="D124" s="52"/>
-      <c r="E124" s="53"/>
-      <c r="F124" s="53"/>
-      <c r="G124" s="54"/>
-      <c r="H124" s="55"/>
-      <c r="I124" s="56"/>
-      <c r="J124" s="55"/>
-    </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C125" s="51"/>
-      <c r="D125" s="52"/>
-      <c r="E125" s="53"/>
-      <c r="F125" s="53"/>
-      <c r="G125" s="54"/>
-      <c r="H125" s="55"/>
-      <c r="I125" s="56"/>
-      <c r="J125" s="55"/>
-    </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C126" s="51"/>
-      <c r="D126" s="52"/>
-      <c r="E126" s="53"/>
-      <c r="F126" s="53"/>
-      <c r="G126" s="54"/>
-      <c r="H126" s="55"/>
-      <c r="I126" s="56"/>
-      <c r="J126" s="55"/>
-    </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C127" s="51"/>
-      <c r="D127" s="52"/>
-      <c r="E127" s="53"/>
-      <c r="F127" s="53"/>
-      <c r="G127" s="54"/>
-      <c r="H127" s="55"/>
-      <c r="I127" s="56"/>
-      <c r="J127" s="55"/>
-    </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C128" s="51"/>
-      <c r="D128" s="52"/>
-      <c r="E128" s="53"/>
-      <c r="F128" s="53"/>
-      <c r="G128" s="54"/>
-      <c r="H128" s="55"/>
-      <c r="I128" s="56"/>
-      <c r="J128" s="55"/>
-    </row>
-    <row r="129" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C129" s="51"/>
-      <c r="D129" s="52"/>
-      <c r="E129" s="53"/>
-      <c r="F129" s="53"/>
-      <c r="G129" s="54"/>
-      <c r="H129" s="55"/>
-      <c r="I129" s="56"/>
-      <c r="J129" s="55"/>
-    </row>
-    <row r="130" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C123" s="145"/>
+      <c r="D123" s="151" t="s">
+        <v>162</v>
+      </c>
+      <c r="E123" s="98"/>
+      <c r="F123" s="98"/>
+      <c r="G123" s="99">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="H123" s="10"/>
+      <c r="I123" s="11"/>
+      <c r="J123" s="10"/>
+      <c r="L123" s="35"/>
+    </row>
+    <row r="124" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C124" s="145"/>
+      <c r="D124" s="151" t="s">
+        <v>11</v>
+      </c>
+      <c r="E124" s="98"/>
+      <c r="F124" s="98"/>
+      <c r="G124" s="99">
+        <v>2.57</v>
+      </c>
+      <c r="H124" s="10"/>
+      <c r="I124" s="11"/>
+      <c r="J124" s="10"/>
+      <c r="L124" s="35"/>
+    </row>
+    <row r="125" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C125" s="145"/>
+      <c r="D125" s="151" t="s">
+        <v>6</v>
+      </c>
+      <c r="E125" s="98"/>
+      <c r="F125" s="98"/>
+      <c r="G125" s="99">
+        <v>0.02</v>
+      </c>
+      <c r="H125" s="10"/>
+      <c r="I125" s="11"/>
+      <c r="J125" s="10"/>
+      <c r="L125" s="35"/>
+    </row>
+    <row r="126" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D126" s="151" t="s">
+        <v>73</v>
+      </c>
+      <c r="E126" s="98"/>
+      <c r="F126" s="98"/>
+      <c r="G126" s="99">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D127" s="154" t="s">
+        <v>74</v>
+      </c>
+      <c r="E127" s="155"/>
+      <c r="F127" s="155"/>
+      <c r="G127" s="156">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C128" s="146"/>
+      <c r="D128" s="152" t="s">
+        <v>224</v>
+      </c>
+      <c r="E128" s="100"/>
+      <c r="F128" s="100"/>
+      <c r="G128" s="101">
+        <v>3.78</v>
+      </c>
+      <c r="H128" s="48"/>
+      <c r="I128" s="11"/>
+      <c r="J128" s="10"/>
+      <c r="K128" s="12"/>
+      <c r="L128" s="35"/>
+      <c r="M128" s="12"/>
+      <c r="N128" s="12"/>
+      <c r="O128" s="12"/>
+    </row>
+    <row r="129" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="67"/>
+      <c r="B129" s="67"/>
+      <c r="C129" s="68"/>
+      <c r="D129" s="69"/>
+      <c r="E129" s="70"/>
+      <c r="F129" s="70"/>
+      <c r="G129" s="97">
+        <f>SUM(G119:G128)</f>
+        <v>57.639000000000017</v>
+      </c>
+      <c r="H129" s="71"/>
+      <c r="I129" s="72"/>
+      <c r="J129" s="71"/>
+      <c r="K129" s="67"/>
+      <c r="L129" s="67"/>
+      <c r="M129" s="67"/>
+      <c r="N129" s="67"/>
+      <c r="O129" s="67"/>
+    </row>
+    <row r="130" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C130" s="51"/>
       <c r="D130" s="52"/>
       <c r="E130" s="53"/>
@@ -5177,8 +5282,9 @@
       <c r="H130" s="55"/>
       <c r="I130" s="56"/>
       <c r="J130" s="55"/>
-    </row>
-    <row r="131" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="L130" s="57"/>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C131" s="51"/>
       <c r="D131" s="52"/>
       <c r="E131" s="53"/>
@@ -5188,7 +5294,7 @@
       <c r="I131" s="56"/>
       <c r="J131" s="55"/>
     </row>
-    <row r="132" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C132" s="51"/>
       <c r="D132" s="52"/>
       <c r="E132" s="53"/>
@@ -5198,7 +5304,7 @@
       <c r="I132" s="56"/>
       <c r="J132" s="55"/>
     </row>
-    <row r="133" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C133" s="51"/>
       <c r="D133" s="52"/>
       <c r="E133" s="53"/>
@@ -5208,7 +5314,7 @@
       <c r="I133" s="56"/>
       <c r="J133" s="55"/>
     </row>
-    <row r="134" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C134" s="51"/>
       <c r="D134" s="52"/>
       <c r="E134" s="53"/>
@@ -5218,7 +5324,7 @@
       <c r="I134" s="56"/>
       <c r="J134" s="55"/>
     </row>
-    <row r="135" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C135" s="51"/>
       <c r="D135" s="52"/>
       <c r="E135" s="53"/>
@@ -5228,7 +5334,7 @@
       <c r="I135" s="56"/>
       <c r="J135" s="55"/>
     </row>
-    <row r="136" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C136" s="51"/>
       <c r="D136" s="52"/>
       <c r="E136" s="53"/>
@@ -5238,7 +5344,7 @@
       <c r="I136" s="56"/>
       <c r="J136" s="55"/>
     </row>
-    <row r="137" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C137" s="51"/>
       <c r="D137" s="52"/>
       <c r="E137" s="53"/>
@@ -5248,7 +5354,7 @@
       <c r="I137" s="56"/>
       <c r="J137" s="55"/>
     </row>
-    <row r="138" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C138" s="51"/>
       <c r="D138" s="52"/>
       <c r="E138" s="53"/>
@@ -5258,7 +5364,7 @@
       <c r="I138" s="56"/>
       <c r="J138" s="55"/>
     </row>
-    <row r="139" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C139" s="51"/>
       <c r="D139" s="52"/>
       <c r="E139" s="53"/>
@@ -5268,7 +5374,7 @@
       <c r="I139" s="56"/>
       <c r="J139" s="55"/>
     </row>
-    <row r="140" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C140" s="51"/>
       <c r="D140" s="52"/>
       <c r="E140" s="53"/>
@@ -5278,7 +5384,7 @@
       <c r="I140" s="56"/>
       <c r="J140" s="55"/>
     </row>
-    <row r="141" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C141" s="51"/>
       <c r="D141" s="52"/>
       <c r="E141" s="53"/>
@@ -5288,7 +5394,7 @@
       <c r="I141" s="56"/>
       <c r="J141" s="55"/>
     </row>
-    <row r="142" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C142" s="51"/>
       <c r="D142" s="52"/>
       <c r="E142" s="53"/>
@@ -5298,7 +5404,7 @@
       <c r="I142" s="56"/>
       <c r="J142" s="55"/>
     </row>
-    <row r="143" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C143" s="51"/>
       <c r="D143" s="52"/>
       <c r="E143" s="53"/>
@@ -5308,7 +5414,7 @@
       <c r="I143" s="56"/>
       <c r="J143" s="55"/>
     </row>
-    <row r="144" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C144" s="51"/>
       <c r="D144" s="52"/>
       <c r="E144" s="53"/>
@@ -5769,22 +5875,105 @@
       <c r="J189" s="55"/>
     </row>
     <row r="190" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C190" s="51"/>
       <c r="D190" s="52"/>
       <c r="E190" s="53"/>
       <c r="F190" s="53"/>
       <c r="G190" s="54"/>
+      <c r="H190" s="55"/>
+      <c r="I190" s="56"/>
+      <c r="J190" s="55"/>
     </row>
     <row r="191" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C191" s="51"/>
       <c r="D191" s="52"/>
       <c r="E191" s="53"/>
       <c r="F191" s="53"/>
       <c r="G191" s="54"/>
+      <c r="H191" s="55"/>
+      <c r="I191" s="56"/>
+      <c r="J191" s="55"/>
+    </row>
+    <row r="192" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C192" s="51"/>
+      <c r="D192" s="52"/>
+      <c r="E192" s="53"/>
+      <c r="F192" s="53"/>
+      <c r="G192" s="54"/>
+      <c r="H192" s="55"/>
+      <c r="I192" s="56"/>
+      <c r="J192" s="55"/>
+    </row>
+    <row r="193" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C193" s="51"/>
+      <c r="D193" s="52"/>
+      <c r="E193" s="53"/>
+      <c r="F193" s="53"/>
+      <c r="G193" s="54"/>
+      <c r="H193" s="55"/>
+      <c r="I193" s="56"/>
+      <c r="J193" s="55"/>
+    </row>
+    <row r="194" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C194" s="51"/>
+      <c r="D194" s="52"/>
+      <c r="E194" s="53"/>
+      <c r="F194" s="53"/>
+      <c r="G194" s="54"/>
+      <c r="H194" s="55"/>
+      <c r="I194" s="56"/>
+      <c r="J194" s="55"/>
+    </row>
+    <row r="195" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C195" s="51"/>
+      <c r="D195" s="52"/>
+      <c r="E195" s="53"/>
+      <c r="F195" s="53"/>
+      <c r="G195" s="54"/>
+      <c r="H195" s="55"/>
+      <c r="I195" s="56"/>
+      <c r="J195" s="55"/>
+    </row>
+    <row r="196" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C196" s="51"/>
+      <c r="D196" s="52"/>
+      <c r="E196" s="53"/>
+      <c r="F196" s="53"/>
+      <c r="G196" s="54"/>
+      <c r="H196" s="55"/>
+      <c r="I196" s="56"/>
+      <c r="J196" s="55"/>
+    </row>
+    <row r="197" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C197" s="51"/>
+      <c r="D197" s="52"/>
+      <c r="E197" s="53"/>
+      <c r="F197" s="53"/>
+      <c r="G197" s="54"/>
+      <c r="H197" s="55"/>
+      <c r="I197" s="56"/>
+      <c r="J197" s="55"/>
+    </row>
+    <row r="198" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D198" s="52"/>
+      <c r="E198" s="53"/>
+      <c r="F198" s="53"/>
+      <c r="G198" s="54"/>
+    </row>
+    <row r="199" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D199" s="52"/>
+      <c r="E199" s="53"/>
+      <c r="F199" s="53"/>
+      <c r="G199" s="54"/>
     </row>
   </sheetData>
   <sortState ref="C4:H19">
     <sortCondition ref="C4:C19"/>
   </sortState>
-  <mergeCells count="42">
+  <mergeCells count="46">
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="I38:I39"/>
     <mergeCell ref="J38:J39"/>
     <mergeCell ref="C4:C10"/>
     <mergeCell ref="J4:J10"/>
@@ -5798,6 +5987,21 @@
     <mergeCell ref="I27:I29"/>
     <mergeCell ref="I21:I25"/>
     <mergeCell ref="H16:H17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="J27:J29"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="H51:H53"/>
+    <mergeCell ref="I51:I53"/>
+    <mergeCell ref="J51:J53"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
     <mergeCell ref="C41:C45"/>
     <mergeCell ref="H41:H45"/>
     <mergeCell ref="I41:I45"/>
@@ -5805,28 +6009,14 @@
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="K10:M10"/>
     <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="J27:J29"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="C70:C76"/>
+    <mergeCell ref="H70:H76"/>
+    <mergeCell ref="I70:I76"/>
+    <mergeCell ref="J70:J76"/>
     <mergeCell ref="C63:C66"/>
     <mergeCell ref="H63:H66"/>
     <mergeCell ref="I63:I66"/>
     <mergeCell ref="J63:J66"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="H51:H53"/>
-    <mergeCell ref="I51:I53"/>
-    <mergeCell ref="J51:J53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6778,7 +6968,7 @@
         <v>216</v>
       </c>
       <c r="AQ19" s="117">
-        <f>INVENTORY!G105</f>
+        <f>INVENTORY!G113</f>
         <v>65.709000000000017</v>
       </c>
       <c r="AS19" s="196" t="s">

</xml_diff>

<commit_message>
FIGURING OUT POWER/CONTROL BUTTON
</commit_message>
<xml_diff>
--- a/BillOfMaterials/INVENTORY.xlsx
+++ b/BillOfMaterials/INVENTORY.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="254">
   <si>
     <t>Arduino Nano</t>
   </si>
@@ -1363,6 +1363,33 @@
   </si>
   <si>
     <t>TAX</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO (DIGIKEY)</t>
+  </si>
+  <si>
+    <t>RES 1K OHM 1/4W 5% AXIAL</t>
+  </si>
+  <si>
+    <t>RES 10K OHM 1/4W 5% AXIAL</t>
+  </si>
+  <si>
+    <t>RES 200K OHM 1/4W 5% AXIAL</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 25V X7R RADIAL</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 100V 1A DO41</t>
+  </si>
+  <si>
+    <t>ZVNL120A MOSFET N-CH</t>
+  </si>
+  <si>
+    <t>TP2104N3-G MOSFET P-CH</t>
+  </si>
+  <si>
+    <t>2N3904BU TRANSISTOR NPN</t>
   </si>
 </sst>
 </file>
@@ -1927,7 +1954,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="227">
+  <cellXfs count="228">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2412,19 +2439,26 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2442,11 +2476,7 @@
     <xf numFmtId="44" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2967,11 +2997,11 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:AB199"/>
+  <dimension ref="A1:AB209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L68" sqref="L68"/>
+      <selection pane="bottomLeft" activeCell="L84" sqref="L84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3058,7 +3088,7 @@
       <c r="L3" s="35"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C4" s="214">
+      <c r="C4" s="216">
         <v>42882</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -3073,26 +3103,26 @@
       <c r="G4" s="27">
         <v>6.99</v>
       </c>
-      <c r="H4" s="217">
+      <c r="H4" s="218">
         <f>SUM(G4:G10)</f>
         <v>48.1</v>
       </c>
-      <c r="I4" s="215">
+      <c r="I4" s="217">
         <v>0</v>
       </c>
-      <c r="J4" s="217">
+      <c r="J4" s="218">
         <f>H4+I4</f>
         <v>48.1</v>
       </c>
-      <c r="K4" s="216">
+      <c r="K4" s="220">
         <f>G4/E4</f>
         <v>6.99</v>
       </c>
-      <c r="L4" s="216"/>
-      <c r="M4" s="216"/>
+      <c r="L4" s="220"/>
+      <c r="M4" s="220"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C5" s="214"/>
+      <c r="C5" s="216"/>
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
@@ -3105,18 +3135,18 @@
       <c r="G5" s="27">
         <v>6.99</v>
       </c>
-      <c r="H5" s="218"/>
-      <c r="I5" s="215"/>
-      <c r="J5" s="218"/>
-      <c r="K5" s="216">
+      <c r="H5" s="219"/>
+      <c r="I5" s="217"/>
+      <c r="J5" s="219"/>
+      <c r="K5" s="220">
         <f t="shared" ref="K5:K10" si="0">G5/E5</f>
         <v>6.99</v>
       </c>
-      <c r="L5" s="216"/>
-      <c r="M5" s="216"/>
+      <c r="L5" s="220"/>
+      <c r="M5" s="220"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C6" s="214"/>
+      <c r="C6" s="216"/>
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
@@ -3129,18 +3159,18 @@
       <c r="G6" s="27">
         <v>4.97</v>
       </c>
-      <c r="H6" s="218"/>
-      <c r="I6" s="215"/>
-      <c r="J6" s="218"/>
-      <c r="K6" s="216">
+      <c r="H6" s="219"/>
+      <c r="I6" s="217"/>
+      <c r="J6" s="219"/>
+      <c r="K6" s="220">
         <f t="shared" si="0"/>
         <v>0.2485</v>
       </c>
-      <c r="L6" s="216"/>
-      <c r="M6" s="216"/>
+      <c r="L6" s="220"/>
+      <c r="M6" s="220"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C7" s="214"/>
+      <c r="C7" s="216"/>
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
@@ -3153,18 +3183,18 @@
       <c r="G7" s="27">
         <v>5.99</v>
       </c>
-      <c r="H7" s="218"/>
-      <c r="I7" s="215"/>
-      <c r="J7" s="218"/>
-      <c r="K7" s="216">
+      <c r="H7" s="219"/>
+      <c r="I7" s="217"/>
+      <c r="J7" s="219"/>
+      <c r="K7" s="220">
         <f t="shared" si="0"/>
         <v>0.29949999999999999</v>
       </c>
-      <c r="L7" s="216"/>
-      <c r="M7" s="216"/>
+      <c r="L7" s="220"/>
+      <c r="M7" s="220"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C8" s="214"/>
+      <c r="C8" s="216"/>
       <c r="D8" s="1" t="s">
         <v>155</v>
       </c>
@@ -3177,18 +3207,18 @@
       <c r="G8" s="27">
         <v>6.25</v>
       </c>
-      <c r="H8" s="218"/>
-      <c r="I8" s="215"/>
-      <c r="J8" s="218"/>
-      <c r="K8" s="216">
+      <c r="H8" s="219"/>
+      <c r="I8" s="217"/>
+      <c r="J8" s="219"/>
+      <c r="K8" s="220">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
-      <c r="L8" s="216"/>
-      <c r="M8" s="216"/>
+      <c r="L8" s="220"/>
+      <c r="M8" s="220"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C9" s="214"/>
+      <c r="C9" s="216"/>
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3201,18 +3231,18 @@
       <c r="G9" s="27">
         <v>11.59</v>
       </c>
-      <c r="H9" s="218"/>
-      <c r="I9" s="215"/>
-      <c r="J9" s="218"/>
-      <c r="K9" s="216">
+      <c r="H9" s="219"/>
+      <c r="I9" s="217"/>
+      <c r="J9" s="219"/>
+      <c r="K9" s="220">
         <f t="shared" si="0"/>
         <v>0.57950000000000002</v>
       </c>
-      <c r="L9" s="216"/>
-      <c r="M9" s="216"/>
+      <c r="L9" s="220"/>
+      <c r="M9" s="220"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C10" s="214"/>
+      <c r="C10" s="216"/>
       <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
@@ -3225,15 +3255,15 @@
       <c r="G10" s="27">
         <v>5.32</v>
       </c>
-      <c r="H10" s="218"/>
-      <c r="I10" s="215"/>
-      <c r="J10" s="218"/>
-      <c r="K10" s="216">
+      <c r="H10" s="219"/>
+      <c r="I10" s="217"/>
+      <c r="J10" s="219"/>
+      <c r="K10" s="220">
         <f t="shared" si="0"/>
         <v>1.0640000000000001</v>
       </c>
-      <c r="L10" s="216"/>
-      <c r="M10" s="216"/>
+      <c r="L10" s="220"/>
+      <c r="M10" s="220"/>
     </row>
     <row r="11" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C11" s="7"/>
@@ -3340,14 +3370,14 @@
       <c r="G16" s="27">
         <v>6.56</v>
       </c>
-      <c r="H16" s="217">
+      <c r="H16" s="218">
         <f>SUM(G16:G17)</f>
         <v>7.55</v>
       </c>
-      <c r="I16" s="215">
+      <c r="I16" s="217">
         <v>0</v>
       </c>
-      <c r="J16" s="217">
+      <c r="J16" s="218">
         <f>H16+I16</f>
         <v>7.55</v>
       </c>
@@ -3368,9 +3398,9 @@
       <c r="G17" s="27">
         <v>0.99</v>
       </c>
-      <c r="H17" s="217"/>
-      <c r="I17" s="215"/>
-      <c r="J17" s="217"/>
+      <c r="H17" s="218"/>
+      <c r="I17" s="217"/>
+      <c r="J17" s="218"/>
     </row>
     <row r="18" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
@@ -3422,7 +3452,7 @@
       <c r="L20" s="35"/>
     </row>
     <row r="21" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C21" s="214">
+      <c r="C21" s="216">
         <v>42925</v>
       </c>
       <c r="D21" s="149" t="s">
@@ -3437,20 +3467,20 @@
       <c r="G21" s="27">
         <v>2.56</v>
       </c>
-      <c r="H21" s="217">
+      <c r="H21" s="218">
         <f>SUM(G21:G25)</f>
         <v>17.230000000000004</v>
       </c>
-      <c r="I21" s="215">
+      <c r="I21" s="217">
         <v>5.65</v>
       </c>
-      <c r="J21" s="217">
+      <c r="J21" s="218">
         <f>H21+I21</f>
         <v>22.880000000000003</v>
       </c>
     </row>
     <row r="22" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C22" s="214"/>
+      <c r="C22" s="216"/>
       <c r="D22" s="149" t="s">
         <v>21</v>
       </c>
@@ -3463,12 +3493,12 @@
       <c r="G22" s="27">
         <v>1.8</v>
       </c>
-      <c r="H22" s="218"/>
-      <c r="I22" s="215"/>
-      <c r="J22" s="218"/>
+      <c r="H22" s="219"/>
+      <c r="I22" s="217"/>
+      <c r="J22" s="219"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C23" s="214"/>
+      <c r="C23" s="216"/>
       <c r="D23" s="1" t="s">
         <v>20</v>
       </c>
@@ -3481,12 +3511,12 @@
       <c r="G23" s="27">
         <v>3.99</v>
       </c>
-      <c r="H23" s="218"/>
-      <c r="I23" s="215"/>
-      <c r="J23" s="218"/>
+      <c r="H23" s="219"/>
+      <c r="I23" s="217"/>
+      <c r="J23" s="219"/>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C24" s="214"/>
+      <c r="C24" s="216"/>
       <c r="D24" s="149" t="s">
         <v>13</v>
       </c>
@@ -3499,12 +3529,12 @@
       <c r="G24" s="27">
         <v>1.97</v>
       </c>
-      <c r="H24" s="218"/>
-      <c r="I24" s="215"/>
-      <c r="J24" s="218"/>
+      <c r="H24" s="219"/>
+      <c r="I24" s="217"/>
+      <c r="J24" s="219"/>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C25" s="214"/>
+      <c r="C25" s="216"/>
       <c r="D25" s="1" t="s">
         <v>2</v>
       </c>
@@ -3517,9 +3547,9 @@
       <c r="G25" s="27">
         <v>6.91</v>
       </c>
-      <c r="H25" s="218"/>
-      <c r="I25" s="215"/>
-      <c r="J25" s="218"/>
+      <c r="H25" s="219"/>
+      <c r="I25" s="217"/>
+      <c r="J25" s="219"/>
     </row>
     <row r="26" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
@@ -3533,7 +3563,7 @@
       <c r="L26" s="35"/>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C27" s="214">
+      <c r="C27" s="216">
         <v>42927</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -3548,20 +3578,20 @@
       <c r="G27" s="27">
         <v>0.75</v>
       </c>
-      <c r="H27" s="217">
+      <c r="H27" s="218">
         <f>SUM(G27:G29)</f>
         <v>3.44</v>
       </c>
-      <c r="I27" s="215">
+      <c r="I27" s="217">
         <v>4.99</v>
       </c>
-      <c r="J27" s="217">
+      <c r="J27" s="218">
         <f>H27+I27</f>
         <v>8.43</v>
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C28" s="214"/>
+      <c r="C28" s="216"/>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
@@ -3574,12 +3604,12 @@
       <c r="G28" s="27">
         <v>0.75</v>
       </c>
-      <c r="H28" s="218"/>
-      <c r="I28" s="215"/>
-      <c r="J28" s="218"/>
+      <c r="H28" s="219"/>
+      <c r="I28" s="217"/>
+      <c r="J28" s="219"/>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C29" s="214"/>
+      <c r="C29" s="216"/>
       <c r="D29" s="1" t="s">
         <v>154</v>
       </c>
@@ -3592,9 +3622,9 @@
       <c r="G29" s="27">
         <v>1.94</v>
       </c>
-      <c r="H29" s="218"/>
-      <c r="I29" s="215"/>
-      <c r="J29" s="218"/>
+      <c r="H29" s="219"/>
+      <c r="I29" s="217"/>
+      <c r="J29" s="219"/>
     </row>
     <row r="30" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="7"/>
@@ -3646,7 +3676,7 @@
       <c r="L32" s="35"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C33" s="214">
+      <c r="C33" s="216">
         <v>42929</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -3661,20 +3691,20 @@
       <c r="G33" s="27">
         <v>0.77</v>
       </c>
-      <c r="H33" s="217">
+      <c r="H33" s="218">
         <f>SUM(G33:G34)</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="I33" s="215">
+      <c r="I33" s="217">
         <v>3.39</v>
       </c>
-      <c r="J33" s="215">
+      <c r="J33" s="217">
         <f>SUM(H33:I34)</f>
         <v>5.6899999999999995</v>
       </c>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C34" s="214"/>
+      <c r="C34" s="216"/>
       <c r="D34" s="1" t="s">
         <v>76</v>
       </c>
@@ -3687,9 +3717,9 @@
       <c r="G34" s="27">
         <v>1.53</v>
       </c>
-      <c r="H34" s="218"/>
-      <c r="I34" s="215"/>
-      <c r="J34" s="215"/>
+      <c r="H34" s="219"/>
+      <c r="I34" s="217"/>
+      <c r="J34" s="217"/>
     </row>
     <row r="35" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="7"/>
@@ -3741,7 +3771,7 @@
       <c r="L37" s="35"/>
     </row>
     <row r="38" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C38" s="214">
+      <c r="C38" s="216">
         <v>42931</v>
       </c>
       <c r="D38" s="149" t="s">
@@ -3756,20 +3786,20 @@
       <c r="G38" s="27">
         <v>5.72</v>
       </c>
-      <c r="H38" s="215">
+      <c r="H38" s="217">
         <f>SUM(G38:G39)</f>
         <v>8.5500000000000007</v>
       </c>
-      <c r="I38" s="215">
+      <c r="I38" s="217">
         <v>4.99</v>
       </c>
-      <c r="J38" s="215">
+      <c r="J38" s="217">
         <f>SUM(H38:I39)</f>
         <v>13.540000000000001</v>
       </c>
     </row>
     <row r="39" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C39" s="214"/>
+      <c r="C39" s="216"/>
       <c r="D39" s="149" t="s">
         <v>122</v>
       </c>
@@ -3782,9 +3812,9 @@
       <c r="G39" s="27">
         <v>2.83</v>
       </c>
-      <c r="H39" s="215"/>
-      <c r="I39" s="215"/>
-      <c r="J39" s="215"/>
+      <c r="H39" s="217"/>
+      <c r="I39" s="217"/>
+      <c r="J39" s="217"/>
     </row>
     <row r="40" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="7"/>
@@ -3798,7 +3828,7 @@
       <c r="L40" s="35"/>
     </row>
     <row r="41" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C41" s="214">
+      <c r="C41" s="216">
         <v>42936</v>
       </c>
       <c r="D41" s="149" t="s">
@@ -3813,20 +3843,20 @@
       <c r="G41" s="27">
         <v>10.58</v>
       </c>
-      <c r="H41" s="215">
+      <c r="H41" s="217">
         <f>SUM(G41:G45)</f>
         <v>18.649999999999999</v>
       </c>
-      <c r="I41" s="215">
+      <c r="I41" s="217">
         <v>0.25</v>
       </c>
-      <c r="J41" s="215">
+      <c r="J41" s="217">
         <f>H41+I41</f>
         <v>18.899999999999999</v>
       </c>
     </row>
     <row r="42" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C42" s="214"/>
+      <c r="C42" s="216"/>
       <c r="D42" s="149" t="s">
         <v>150</v>
       </c>
@@ -3839,12 +3869,12 @@
       <c r="G42" s="27">
         <v>3.86</v>
       </c>
-      <c r="H42" s="215"/>
-      <c r="I42" s="215"/>
-      <c r="J42" s="215"/>
+      <c r="H42" s="217"/>
+      <c r="I42" s="217"/>
+      <c r="J42" s="217"/>
     </row>
     <row r="43" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C43" s="214"/>
+      <c r="C43" s="216"/>
       <c r="D43" s="149" t="s">
         <v>151</v>
       </c>
@@ -3858,12 +3888,12 @@
         <f>1.99-0.1</f>
         <v>1.89</v>
       </c>
-      <c r="H43" s="215"/>
-      <c r="I43" s="215"/>
-      <c r="J43" s="215"/>
+      <c r="H43" s="217"/>
+      <c r="I43" s="217"/>
+      <c r="J43" s="217"/>
     </row>
     <row r="44" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C44" s="214"/>
+      <c r="C44" s="216"/>
       <c r="D44" s="149" t="s">
         <v>152</v>
       </c>
@@ -3877,12 +3907,12 @@
         <f>0.99-0.05</f>
         <v>0.94</v>
       </c>
-      <c r="H44" s="215"/>
-      <c r="I44" s="215"/>
-      <c r="J44" s="215"/>
+      <c r="H44" s="217"/>
+      <c r="I44" s="217"/>
+      <c r="J44" s="217"/>
     </row>
     <row r="45" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C45" s="214"/>
+      <c r="C45" s="216"/>
       <c r="D45" s="149" t="s">
         <v>153</v>
       </c>
@@ -3896,9 +3926,9 @@
         <f>1.45-0.07</f>
         <v>1.38</v>
       </c>
-      <c r="H45" s="215"/>
-      <c r="I45" s="215"/>
-      <c r="J45" s="215"/>
+      <c r="H45" s="217"/>
+      <c r="I45" s="217"/>
+      <c r="J45" s="217"/>
     </row>
     <row r="46" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="51"/>
@@ -3987,7 +4017,7 @@
       <c r="L50" s="57"/>
     </row>
     <row r="51" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C51" s="214">
+      <c r="C51" s="216">
         <v>42986</v>
       </c>
       <c r="D51" s="149" t="s">
@@ -4002,20 +4032,20 @@
       <c r="G51" s="27">
         <v>29.95</v>
       </c>
-      <c r="H51" s="215">
+      <c r="H51" s="217">
         <f>G51+G52+G53+2.13</f>
         <v>34.380000000000003</v>
       </c>
-      <c r="I51" s="215">
+      <c r="I51" s="217">
         <v>3.03</v>
       </c>
-      <c r="J51" s="215">
+      <c r="J51" s="217">
         <f>H51+I51</f>
         <v>37.410000000000004</v>
       </c>
     </row>
     <row r="52" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C52" s="214"/>
+      <c r="C52" s="216"/>
       <c r="D52" s="149" t="s">
         <v>222</v>
       </c>
@@ -4028,12 +4058,12 @@
       <c r="G52" s="27">
         <v>0.77</v>
       </c>
-      <c r="H52" s="215"/>
-      <c r="I52" s="215"/>
-      <c r="J52" s="215"/>
+      <c r="H52" s="217"/>
+      <c r="I52" s="217"/>
+      <c r="J52" s="217"/>
     </row>
     <row r="53" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C53" s="214"/>
+      <c r="C53" s="216"/>
       <c r="D53" s="149" t="s">
         <v>223</v>
       </c>
@@ -4046,9 +4076,9 @@
       <c r="G53" s="27">
         <v>1.53</v>
       </c>
-      <c r="H53" s="215"/>
-      <c r="I53" s="215"/>
-      <c r="J53" s="215"/>
+      <c r="H53" s="217"/>
+      <c r="I53" s="217"/>
+      <c r="J53" s="217"/>
     </row>
     <row r="54" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="51"/>
@@ -4211,7 +4241,7 @@
       <c r="L62" s="57"/>
     </row>
     <row r="63" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C63" s="214">
+      <c r="C63" s="216">
         <v>43027</v>
       </c>
       <c r="D63" s="149" t="s">
@@ -4226,20 +4256,20 @@
       <c r="G63" s="27">
         <v>2.66</v>
       </c>
-      <c r="H63" s="215">
+      <c r="H63" s="217">
         <f>SUM(G63:G66)</f>
         <v>10.18</v>
       </c>
-      <c r="I63" s="215">
+      <c r="I63" s="217">
         <v>3.75</v>
       </c>
-      <c r="J63" s="215">
+      <c r="J63" s="217">
         <f>H63+I63</f>
         <v>13.93</v>
       </c>
     </row>
     <row r="64" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C64" s="214"/>
+      <c r="C64" s="216"/>
       <c r="D64" s="149" t="s">
         <v>234</v>
       </c>
@@ -4252,12 +4282,12 @@
       <c r="G64" s="27">
         <v>1.53</v>
       </c>
-      <c r="H64" s="215"/>
-      <c r="I64" s="215"/>
-      <c r="J64" s="215"/>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C65" s="214"/>
+      <c r="H64" s="217"/>
+      <c r="I64" s="217"/>
+      <c r="J64" s="217"/>
+    </row>
+    <row r="65" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C65" s="216"/>
       <c r="D65" s="149" t="s">
         <v>222</v>
       </c>
@@ -4270,12 +4300,12 @@
       <c r="G65" s="27">
         <v>0.77</v>
       </c>
-      <c r="H65" s="215"/>
-      <c r="I65" s="215"/>
-      <c r="J65" s="215"/>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C66" s="214"/>
+      <c r="H65" s="217"/>
+      <c r="I65" s="217"/>
+      <c r="J65" s="217"/>
+    </row>
+    <row r="66" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C66" s="216"/>
       <c r="D66" s="149" t="s">
         <v>235</v>
       </c>
@@ -4288,11 +4318,11 @@
       <c r="G66" s="27">
         <v>5.22</v>
       </c>
-      <c r="H66" s="215"/>
-      <c r="I66" s="215"/>
-      <c r="J66" s="215"/>
-    </row>
-    <row r="67" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H66" s="217"/>
+      <c r="I66" s="217"/>
+      <c r="J66" s="217"/>
+    </row>
+    <row r="67" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C67" s="51"/>
       <c r="D67" s="52"/>
       <c r="E67" s="53"/>
@@ -4303,7 +4333,7 @@
       <c r="J67" s="158"/>
       <c r="L67" s="57"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C68" s="213">
         <v>43036</v>
       </c>
@@ -4330,7 +4360,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="69" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C69" s="51"/>
       <c r="D69" s="52"/>
       <c r="E69" s="53"/>
@@ -4341,11 +4371,11 @@
       <c r="J69" s="158"/>
       <c r="L69" s="57"/>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C70" s="214">
+    <row r="70" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C70" s="216">
         <v>43040</v>
       </c>
-      <c r="D70" s="202" t="s">
+      <c r="D70" s="149" t="s">
         <v>243</v>
       </c>
       <c r="E70" s="26">
@@ -4357,14 +4387,14 @@
       <c r="G70" s="27">
         <v>0.4</v>
       </c>
-      <c r="H70" s="215">
+      <c r="H70" s="217">
         <f>SUM(G70:G76)</f>
         <v>3.5799999999999996</v>
       </c>
-      <c r="I70" s="215">
+      <c r="I70" s="217">
         <v>3.39</v>
       </c>
-      <c r="J70" s="226">
+      <c r="J70" s="221">
         <f>H70+I70+K71</f>
         <v>7.2206000000000001</v>
       </c>
@@ -4372,9 +4402,9 @@
         <v>244</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C71" s="214"/>
-      <c r="D71" s="202" t="s">
+    <row r="71" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C71" s="216"/>
+      <c r="D71" s="149" t="s">
         <v>237</v>
       </c>
       <c r="E71" s="26">
@@ -4386,18 +4416,18 @@
       <c r="G71" s="27">
         <v>0.9</v>
       </c>
-      <c r="H71" s="215"/>
-      <c r="I71" s="215"/>
-      <c r="J71" s="226"/>
-      <c r="K71" s="224">
+      <c r="H71" s="217"/>
+      <c r="I71" s="217"/>
+      <c r="J71" s="221"/>
+      <c r="K71" s="214">
         <f>SUM(G70:G76)*0.07</f>
         <v>0.25059999999999999</v>
       </c>
-      <c r="L71" s="225"/>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C72" s="214"/>
-      <c r="D72" s="202" t="s">
+      <c r="L71" s="215"/>
+    </row>
+    <row r="72" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C72" s="216"/>
+      <c r="D72" s="149" t="s">
         <v>238</v>
       </c>
       <c r="E72" s="26">
@@ -4409,13 +4439,13 @@
       <c r="G72" s="27">
         <v>0.64</v>
       </c>
-      <c r="H72" s="215"/>
-      <c r="I72" s="215"/>
-      <c r="J72" s="226"/>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C73" s="214"/>
-      <c r="D73" s="202" t="s">
+      <c r="H72" s="217"/>
+      <c r="I72" s="217"/>
+      <c r="J72" s="221"/>
+    </row>
+    <row r="73" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C73" s="216"/>
+      <c r="D73" s="149" t="s">
         <v>239</v>
       </c>
       <c r="E73" s="26">
@@ -4427,13 +4457,13 @@
       <c r="G73" s="27">
         <v>0.4</v>
       </c>
-      <c r="H73" s="215"/>
-      <c r="I73" s="215"/>
-      <c r="J73" s="226"/>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C74" s="214"/>
-      <c r="D74" s="202" t="s">
+      <c r="H73" s="217"/>
+      <c r="I73" s="217"/>
+      <c r="J73" s="221"/>
+    </row>
+    <row r="74" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C74" s="216"/>
+      <c r="D74" s="149" t="s">
         <v>240</v>
       </c>
       <c r="E74" s="26">
@@ -4445,13 +4475,13 @@
       <c r="G74" s="27">
         <v>0.32</v>
       </c>
-      <c r="H74" s="215"/>
-      <c r="I74" s="215"/>
-      <c r="J74" s="226"/>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C75" s="214"/>
-      <c r="D75" s="202" t="s">
+      <c r="H74" s="217"/>
+      <c r="I74" s="217"/>
+      <c r="J74" s="221"/>
+    </row>
+    <row r="75" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C75" s="216"/>
+      <c r="D75" s="149" t="s">
         <v>241</v>
       </c>
       <c r="E75" s="26">
@@ -4463,13 +4493,13 @@
       <c r="G75" s="27">
         <v>0.46</v>
       </c>
-      <c r="H75" s="215"/>
-      <c r="I75" s="215"/>
-      <c r="J75" s="226"/>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C76" s="214"/>
-      <c r="D76" s="202" t="s">
+      <c r="H75" s="217"/>
+      <c r="I75" s="217"/>
+      <c r="J75" s="221"/>
+    </row>
+    <row r="76" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C76" s="216"/>
+      <c r="D76" s="149" t="s">
         <v>242</v>
       </c>
       <c r="E76" s="26">
@@ -4481,244 +4511,288 @@
       <c r="G76" s="27">
         <v>0.46</v>
       </c>
-      <c r="H76" s="215"/>
-      <c r="I76" s="215"/>
-      <c r="J76" s="226"/>
-    </row>
-    <row r="77" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C77" s="7"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="24"/>
-      <c r="F77" s="24"/>
-      <c r="G77" s="25"/>
-      <c r="H77" s="9"/>
-      <c r="I77" s="13"/>
-      <c r="J77" s="9"/>
-      <c r="L77" s="35"/>
-    </row>
-    <row r="78" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="40" t="s">
+      <c r="H76" s="217"/>
+      <c r="I76" s="217"/>
+      <c r="J76" s="221"/>
+    </row>
+    <row r="77" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C77" s="51"/>
+      <c r="D77" s="52"/>
+      <c r="E77" s="53"/>
+      <c r="F77" s="53"/>
+      <c r="G77" s="54"/>
+      <c r="H77" s="158"/>
+      <c r="I77" s="158"/>
+      <c r="J77" s="227"/>
+      <c r="L77" s="57"/>
+    </row>
+    <row r="78" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C78" s="216">
+        <v>43045</v>
+      </c>
+      <c r="D78" s="149" t="s">
+        <v>245</v>
+      </c>
+      <c r="E78" s="26">
+        <v>1</v>
+      </c>
+      <c r="F78" s="26">
+        <v>1</v>
+      </c>
+      <c r="G78" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="H78" s="217">
+        <f>SUM(G78:G86)</f>
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="I78" s="217">
+        <v>3.39</v>
+      </c>
+      <c r="J78" s="221">
+        <f>H78+I78+K79</f>
+        <v>7.8305000000000007</v>
+      </c>
+      <c r="K78" s="12" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="79" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C79" s="216"/>
+      <c r="D79" s="149" t="s">
+        <v>246</v>
+      </c>
+      <c r="E79" s="26">
+        <v>10</v>
+      </c>
+      <c r="F79" s="26">
+        <v>1</v>
+      </c>
+      <c r="G79" s="27">
+        <v>0.4</v>
+      </c>
+      <c r="H79" s="217"/>
+      <c r="I79" s="217"/>
+      <c r="J79" s="221"/>
+      <c r="K79" s="214">
+        <f>SUM(G78:G86)*0.07</f>
+        <v>0.29050000000000004</v>
+      </c>
+    </row>
+    <row r="80" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C80" s="216"/>
+      <c r="D80" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="E80" s="26">
+        <v>10</v>
+      </c>
+      <c r="F80" s="26">
+        <v>1</v>
+      </c>
+      <c r="G80" s="27">
+        <v>0.4</v>
+      </c>
+      <c r="H80" s="217"/>
+      <c r="I80" s="217"/>
+      <c r="J80" s="221"/>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C81" s="216"/>
+      <c r="D81" s="149" t="s">
+        <v>248</v>
+      </c>
+      <c r="E81" s="26">
+        <v>10</v>
+      </c>
+      <c r="F81" s="26">
+        <v>1</v>
+      </c>
+      <c r="G81" s="27">
+        <v>0.4</v>
+      </c>
+      <c r="H81" s="217"/>
+      <c r="I81" s="217"/>
+      <c r="J81" s="221"/>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C82" s="216"/>
+      <c r="D82" s="149" t="s">
+        <v>249</v>
+      </c>
+      <c r="E82" s="26">
+        <v>1</v>
+      </c>
+      <c r="F82" s="26">
+        <v>1</v>
+      </c>
+      <c r="G82" s="27">
+        <v>0.63</v>
+      </c>
+      <c r="H82" s="217"/>
+      <c r="I82" s="217"/>
+      <c r="J82" s="221"/>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C83" s="216"/>
+      <c r="D83" s="149" t="s">
+        <v>250</v>
+      </c>
+      <c r="E83" s="26">
+        <v>1</v>
+      </c>
+      <c r="F83" s="26">
+        <v>1</v>
+      </c>
+      <c r="G83" s="27">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H83" s="217"/>
+      <c r="I83" s="217"/>
+      <c r="J83" s="221"/>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C84" s="216"/>
+      <c r="D84" s="149" t="s">
+        <v>251</v>
+      </c>
+      <c r="E84" s="26">
+        <v>1</v>
+      </c>
+      <c r="F84" s="26">
+        <v>1</v>
+      </c>
+      <c r="G84" s="27">
+        <v>0.86</v>
+      </c>
+      <c r="H84" s="217"/>
+      <c r="I84" s="217"/>
+      <c r="J84" s="221"/>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C85" s="216"/>
+      <c r="D85" s="149" t="s">
+        <v>252</v>
+      </c>
+      <c r="E85" s="26">
+        <v>1</v>
+      </c>
+      <c r="F85" s="26">
+        <v>1</v>
+      </c>
+      <c r="G85" s="27">
+        <v>0.61</v>
+      </c>
+      <c r="H85" s="217"/>
+      <c r="I85" s="217"/>
+      <c r="J85" s="221"/>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C86" s="216"/>
+      <c r="D86" s="149" t="s">
+        <v>253</v>
+      </c>
+      <c r="E86" s="26">
+        <v>1</v>
+      </c>
+      <c r="F86" s="26">
+        <v>1</v>
+      </c>
+      <c r="G86" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="H86" s="217"/>
+      <c r="I86" s="217"/>
+      <c r="J86" s="221"/>
+    </row>
+    <row r="87" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C87" s="7"/>
+      <c r="D87" s="8"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="25"/>
+      <c r="H87" s="9"/>
+      <c r="I87" s="13"/>
+      <c r="J87" s="9"/>
+      <c r="L87" s="35"/>
+    </row>
+    <row r="88" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C78" s="41">
+      <c r="C88" s="41">
         <f ca="1">TODAY()</f>
-        <v>43041</v>
-      </c>
-      <c r="E78" s="29"/>
-      <c r="F78" s="29"/>
-      <c r="G78" s="29"/>
-      <c r="H78" s="29"/>
-      <c r="I78" s="28" t="s">
+        <v>43045</v>
+      </c>
+      <c r="E88" s="29"/>
+      <c r="F88" s="29"/>
+      <c r="G88" s="29"/>
+      <c r="H88" s="29"/>
+      <c r="I88" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="J78" s="30">
-        <f>SUM(J4:J77)</f>
-        <v>300.3306</v>
-      </c>
-      <c r="K78" s="24" t="s">
+      <c r="J88" s="30">
+        <f>SUM(J4:J87)</f>
+        <v>308.16110000000003</v>
+      </c>
+      <c r="K88" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="L78" s="39">
-        <f ca="1">(C78-C4)*0.0328767</f>
-        <v>5.2273953000000004</v>
-      </c>
-      <c r="M78" s="24" t="s">
+      <c r="L88" s="39">
+        <f ca="1">(C88-C4)*0.0328767</f>
+        <v>5.3589020999999999</v>
+      </c>
+      <c r="M88" s="24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="79" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C79" s="7"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="24"/>
-      <c r="F79" s="24"/>
-      <c r="G79" s="25"/>
-      <c r="H79" s="31"/>
-      <c r="I79" s="34" t="s">
+    <row r="89" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C89" s="7"/>
+      <c r="D89" s="8"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="24"/>
+      <c r="G89" s="25"/>
+      <c r="H89" s="31"/>
+      <c r="I89" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="J79" s="22">
-        <f ca="1">J78/L78</f>
-        <v>57.453202362560944</v>
-      </c>
-      <c r="K79" s="32" t="s">
+      <c r="J89" s="22">
+        <f ca="1">J88/L88</f>
+        <v>57.504521308571775</v>
+      </c>
+      <c r="K89" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="L79" s="36"/>
-      <c r="M79" s="32" t="s">
+      <c r="L89" s="36"/>
+      <c r="M89" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="N79" s="33"/>
-    </row>
-    <row r="80" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="58"/>
-      <c r="B80" s="58"/>
-      <c r="C80" s="44"/>
-      <c r="D80" s="45"/>
-      <c r="E80" s="46"/>
-      <c r="F80" s="46"/>
-      <c r="G80" s="47"/>
-      <c r="H80" s="48"/>
-      <c r="I80" s="59"/>
-      <c r="J80" s="48"/>
-      <c r="K80" s="58"/>
-      <c r="L80" s="60"/>
-      <c r="M80" s="58"/>
-      <c r="N80" s="58"/>
-      <c r="O80" s="58"/>
-    </row>
-    <row r="81" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C81" s="7"/>
-      <c r="D81" s="63" t="s">
-        <v>75</v>
-      </c>
-      <c r="E81" s="203" t="s">
-        <v>227</v>
-      </c>
-      <c r="H81" s="10"/>
-      <c r="I81" s="11"/>
-      <c r="J81" s="10"/>
-      <c r="L81" s="35"/>
-    </row>
-    <row r="82" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C82" s="7"/>
-      <c r="D82" s="8"/>
-      <c r="E82" s="24"/>
-      <c r="F82" s="24"/>
-      <c r="G82" s="25"/>
-      <c r="H82" s="10"/>
-      <c r="I82" s="11"/>
-      <c r="J82" s="10"/>
-      <c r="L82" s="35"/>
-    </row>
-    <row r="83" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C83" s="7"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="24"/>
-      <c r="F83" s="24"/>
-      <c r="G83" s="25"/>
-      <c r="H83" s="10"/>
-      <c r="I83" s="11"/>
-      <c r="J83" s="10"/>
-      <c r="L83" s="35"/>
-    </row>
-    <row r="84" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C84" s="147" t="s">
-        <v>164</v>
-      </c>
-      <c r="D84" s="148"/>
-      <c r="E84" s="24"/>
-      <c r="F84" s="24"/>
-      <c r="G84" s="25"/>
-      <c r="H84" s="10"/>
-      <c r="I84" s="11"/>
-      <c r="J84" s="10"/>
-      <c r="L84" s="35"/>
-    </row>
-    <row r="85" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C85" s="49"/>
-      <c r="D85" s="95" t="s">
-        <v>0</v>
-      </c>
-      <c r="E85" s="98"/>
-      <c r="F85" s="98" t="s">
-        <v>160</v>
-      </c>
-      <c r="G85" s="99">
-        <v>2.19</v>
-      </c>
-      <c r="H85" s="10"/>
-      <c r="I85" s="11"/>
-      <c r="J85" s="10"/>
-      <c r="L85" s="35"/>
-    </row>
-    <row r="86" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C86" s="7"/>
-      <c r="D86" s="95" t="s">
-        <v>1</v>
-      </c>
-      <c r="E86" s="98"/>
-      <c r="F86" s="98" t="s">
-        <v>160</v>
-      </c>
-      <c r="G86" s="99">
-        <v>1.06</v>
-      </c>
-      <c r="H86" s="10"/>
-      <c r="I86" s="11"/>
-      <c r="J86" s="10"/>
-      <c r="L86" s="35"/>
-    </row>
-    <row r="87" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C87" s="7"/>
-      <c r="D87" s="95" t="str">
-        <f>D24</f>
-        <v>NOKIA 5110 LCD</v>
-      </c>
-      <c r="E87" s="98"/>
-      <c r="F87" s="98"/>
-      <c r="G87" s="99">
-        <f>G24</f>
-        <v>1.97</v>
-      </c>
-      <c r="H87" s="10"/>
-      <c r="I87" s="11"/>
-      <c r="J87" s="10"/>
-      <c r="L87" s="35"/>
-    </row>
-    <row r="88" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C88" s="7"/>
-      <c r="D88" s="95" t="s">
-        <v>5</v>
-      </c>
-      <c r="E88" s="98"/>
-      <c r="F88" s="98"/>
-      <c r="G88" s="99">
-        <v>0.2485</v>
-      </c>
-      <c r="H88" s="10"/>
-      <c r="I88" s="11"/>
-      <c r="J88" s="10"/>
-      <c r="L88" s="35"/>
-    </row>
-    <row r="89" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C89" s="7"/>
-      <c r="D89" s="95" t="s">
-        <v>156</v>
-      </c>
-      <c r="E89" s="98"/>
-      <c r="F89" s="98"/>
-      <c r="G89" s="99">
-        <v>0.29949999999999999</v>
-      </c>
-      <c r="H89" s="10"/>
-      <c r="I89" s="11"/>
-      <c r="J89" s="10"/>
-      <c r="L89" s="35"/>
+      <c r="N89" s="33"/>
     </row>
     <row r="90" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C90" s="7"/>
-      <c r="D90" s="95" t="s">
-        <v>158</v>
-      </c>
-      <c r="E90" s="98"/>
-      <c r="F90" s="98"/>
-      <c r="G90" s="99">
-        <v>1</v>
-      </c>
-      <c r="H90" s="10"/>
-      <c r="I90" s="11"/>
-      <c r="J90" s="10"/>
-      <c r="L90" s="35"/>
+      <c r="A90" s="58"/>
+      <c r="B90" s="58"/>
+      <c r="C90" s="44"/>
+      <c r="D90" s="45"/>
+      <c r="E90" s="46"/>
+      <c r="F90" s="46"/>
+      <c r="G90" s="47"/>
+      <c r="H90" s="48"/>
+      <c r="I90" s="59"/>
+      <c r="J90" s="48"/>
+      <c r="K90" s="58"/>
+      <c r="L90" s="60"/>
+      <c r="M90" s="58"/>
+      <c r="N90" s="58"/>
+      <c r="O90" s="58"/>
     </row>
     <row r="91" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C91" s="7"/>
-      <c r="D91" s="95" t="s">
-        <v>155</v>
-      </c>
-      <c r="E91" s="98"/>
-      <c r="F91" s="98"/>
-      <c r="G91" s="99">
-        <v>6.25</v>
+      <c r="D91" s="63" t="s">
+        <v>75</v>
+      </c>
+      <c r="E91" s="203" t="s">
+        <v>227</v>
       </c>
       <c r="H91" s="10"/>
       <c r="I91" s="11"/>
@@ -4727,14 +4801,10 @@
     </row>
     <row r="92" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C92" s="7"/>
-      <c r="D92" s="95" t="s">
-        <v>157</v>
-      </c>
-      <c r="E92" s="98"/>
-      <c r="F92" s="98"/>
-      <c r="G92" s="99">
-        <v>0.57950000000000002</v>
-      </c>
+      <c r="D92" s="8"/>
+      <c r="E92" s="24"/>
+      <c r="F92" s="24"/>
+      <c r="G92" s="25"/>
       <c r="H92" s="10"/>
       <c r="I92" s="11"/>
       <c r="J92" s="10"/>
@@ -4742,639 +4812,688 @@
     </row>
     <row r="93" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C93" s="7"/>
-      <c r="D93" s="95" t="s">
-        <v>17</v>
-      </c>
-      <c r="E93" s="98"/>
-      <c r="F93" s="98"/>
-      <c r="G93" s="99">
-        <v>1.0640000000000001</v>
-      </c>
+      <c r="D93" s="8"/>
+      <c r="E93" s="24"/>
+      <c r="F93" s="24"/>
+      <c r="G93" s="25"/>
       <c r="H93" s="10"/>
       <c r="I93" s="11"/>
       <c r="J93" s="10"/>
       <c r="L93" s="35"/>
     </row>
     <row r="94" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C94" s="7"/>
-      <c r="D94" s="95" t="s">
-        <v>161</v>
-      </c>
-      <c r="E94" s="98"/>
-      <c r="F94" s="98"/>
-      <c r="G94" s="99">
-        <v>0.5</v>
-      </c>
+      <c r="C94" s="147" t="s">
+        <v>164</v>
+      </c>
+      <c r="D94" s="148"/>
+      <c r="E94" s="24"/>
+      <c r="F94" s="24"/>
+      <c r="G94" s="25"/>
       <c r="H94" s="10"/>
       <c r="I94" s="11"/>
       <c r="J94" s="10"/>
       <c r="L94" s="35"/>
     </row>
     <row r="95" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C95" s="44"/>
-      <c r="D95" s="96" t="s">
-        <v>159</v>
-      </c>
-      <c r="E95" s="100"/>
-      <c r="F95" s="100"/>
-      <c r="G95" s="101">
-        <v>2</v>
-      </c>
-      <c r="H95" s="48"/>
+      <c r="C95" s="49"/>
+      <c r="D95" s="95" t="s">
+        <v>0</v>
+      </c>
+      <c r="E95" s="98"/>
+      <c r="F95" s="98" t="s">
+        <v>160</v>
+      </c>
+      <c r="G95" s="99">
+        <v>2.19</v>
+      </c>
+      <c r="H95" s="10"/>
       <c r="I95" s="11"/>
       <c r="J95" s="10"/>
       <c r="L95" s="35"/>
     </row>
     <row r="96" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="58"/>
-      <c r="B96" s="58"/>
-      <c r="C96" s="44"/>
-      <c r="D96" s="45"/>
-      <c r="E96" s="46"/>
-      <c r="F96" s="46"/>
-      <c r="G96" s="97">
-        <f>SUM(G85:G95)</f>
-        <v>17.1615</v>
-      </c>
-      <c r="H96" s="48"/>
-      <c r="I96" s="59"/>
-      <c r="J96" s="48"/>
-      <c r="K96" s="58"/>
-      <c r="L96" s="60"/>
-      <c r="M96" s="58"/>
-      <c r="N96" s="58"/>
-      <c r="O96" s="58"/>
-    </row>
-    <row r="97" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C96" s="7"/>
+      <c r="D96" s="95" t="s">
+        <v>1</v>
+      </c>
+      <c r="E96" s="98"/>
+      <c r="F96" s="98" t="s">
+        <v>160</v>
+      </c>
+      <c r="G96" s="99">
+        <v>1.06</v>
+      </c>
+      <c r="H96" s="10"/>
+      <c r="I96" s="11"/>
+      <c r="J96" s="10"/>
+      <c r="L96" s="35"/>
+    </row>
+    <row r="97" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C97" s="7"/>
-      <c r="D97" s="8"/>
-      <c r="E97" s="24"/>
-      <c r="F97" s="24"/>
-      <c r="G97" s="25"/>
+      <c r="D97" s="95" t="str">
+        <f>D24</f>
+        <v>NOKIA 5110 LCD</v>
+      </c>
+      <c r="E97" s="98"/>
+      <c r="F97" s="98"/>
+      <c r="G97" s="99">
+        <f>G24</f>
+        <v>1.97</v>
+      </c>
       <c r="H97" s="10"/>
       <c r="I97" s="11"/>
       <c r="J97" s="10"/>
       <c r="L97" s="35"/>
     </row>
-    <row r="98" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C98" s="7"/>
-      <c r="D98" s="8"/>
-      <c r="E98" s="24"/>
-      <c r="F98" s="24"/>
-      <c r="G98" s="25"/>
+      <c r="D98" s="95" t="s">
+        <v>5</v>
+      </c>
+      <c r="E98" s="98"/>
+      <c r="F98" s="98"/>
+      <c r="G98" s="99">
+        <v>0.2485</v>
+      </c>
       <c r="H98" s="10"/>
       <c r="I98" s="11"/>
       <c r="J98" s="10"/>
       <c r="L98" s="35"/>
     </row>
-    <row r="99" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C99" s="7"/>
-      <c r="D99" s="8"/>
-      <c r="E99" s="24"/>
-      <c r="F99" s="24"/>
-      <c r="G99" s="25"/>
+      <c r="D99" s="95" t="s">
+        <v>156</v>
+      </c>
+      <c r="E99" s="98"/>
+      <c r="F99" s="98"/>
+      <c r="G99" s="99">
+        <v>0.29949999999999999</v>
+      </c>
       <c r="H99" s="10"/>
       <c r="I99" s="11"/>
       <c r="J99" s="10"/>
       <c r="L99" s="35"/>
     </row>
-    <row r="100" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C100" s="7"/>
-      <c r="D100" s="8"/>
-      <c r="E100" s="24"/>
-      <c r="F100" s="24"/>
-      <c r="G100" s="25"/>
+      <c r="D100" s="95" t="s">
+        <v>158</v>
+      </c>
+      <c r="E100" s="98"/>
+      <c r="F100" s="98"/>
+      <c r="G100" s="99">
+        <v>1</v>
+      </c>
       <c r="H100" s="10"/>
       <c r="I100" s="11"/>
       <c r="J100" s="10"/>
       <c r="L100" s="35"/>
     </row>
-    <row r="101" spans="3:12" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C101" s="93" t="s">
-        <v>163</v>
-      </c>
-      <c r="D101" s="94"/>
-      <c r="E101" s="18"/>
-      <c r="H101" s="14"/>
-      <c r="I101" s="17"/>
-      <c r="J101" s="14"/>
-      <c r="K101" s="14"/>
-      <c r="L101" s="14"/>
-    </row>
-    <row r="102" spans="3:12" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C102" s="144"/>
-      <c r="D102" s="151" t="s">
-        <v>226</v>
+    <row r="101" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C101" s="7"/>
+      <c r="D101" s="95" t="s">
+        <v>155</v>
+      </c>
+      <c r="E101" s="98"/>
+      <c r="F101" s="98"/>
+      <c r="G101" s="99">
+        <v>6.25</v>
+      </c>
+      <c r="H101" s="10"/>
+      <c r="I101" s="11"/>
+      <c r="J101" s="10"/>
+      <c r="L101" s="35"/>
+    </row>
+    <row r="102" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C102" s="7"/>
+      <c r="D102" s="95" t="s">
+        <v>157</v>
       </c>
       <c r="E102" s="98"/>
       <c r="F102" s="98"/>
       <c r="G102" s="99">
-        <v>1.53</v>
-      </c>
-      <c r="H102" s="157"/>
-      <c r="I102" s="158"/>
-      <c r="J102" s="157"/>
-      <c r="K102" s="157"/>
-      <c r="L102" s="159"/>
-    </row>
-    <row r="103" spans="3:12" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C103" s="144"/>
-      <c r="D103" s="151" t="s">
-        <v>30</v>
+        <v>0.57950000000000002</v>
+      </c>
+      <c r="H102" s="10"/>
+      <c r="I102" s="11"/>
+      <c r="J102" s="10"/>
+      <c r="L102" s="35"/>
+    </row>
+    <row r="103" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C103" s="7"/>
+      <c r="D103" s="95" t="s">
+        <v>17</v>
       </c>
       <c r="E103" s="98"/>
       <c r="F103" s="98"/>
       <c r="G103" s="99">
-        <v>33.57</v>
-      </c>
-      <c r="H103" s="157"/>
-      <c r="I103" s="158"/>
-      <c r="J103" s="157"/>
-      <c r="K103" s="157"/>
-      <c r="L103" s="159"/>
-    </row>
-    <row r="104" spans="3:12" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C104" s="144"/>
-      <c r="D104" s="151" t="s">
-        <v>2</v>
+        <v>1.0640000000000001</v>
+      </c>
+      <c r="H103" s="10"/>
+      <c r="I103" s="11"/>
+      <c r="J103" s="10"/>
+      <c r="L103" s="35"/>
+    </row>
+    <row r="104" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C104" s="7"/>
+      <c r="D104" s="95" t="s">
+        <v>161</v>
       </c>
       <c r="E104" s="98"/>
       <c r="F104" s="98"/>
       <c r="G104" s="99">
+        <v>0.5</v>
+      </c>
+      <c r="H104" s="10"/>
+      <c r="I104" s="11"/>
+      <c r="J104" s="10"/>
+      <c r="L104" s="35"/>
+    </row>
+    <row r="105" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C105" s="44"/>
+      <c r="D105" s="96" t="s">
+        <v>159</v>
+      </c>
+      <c r="E105" s="100"/>
+      <c r="F105" s="100"/>
+      <c r="G105" s="101">
+        <v>2</v>
+      </c>
+      <c r="H105" s="48"/>
+      <c r="I105" s="11"/>
+      <c r="J105" s="10"/>
+      <c r="L105" s="35"/>
+    </row>
+    <row r="106" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="58"/>
+      <c r="B106" s="58"/>
+      <c r="C106" s="44"/>
+      <c r="D106" s="45"/>
+      <c r="E106" s="46"/>
+      <c r="F106" s="46"/>
+      <c r="G106" s="97">
+        <f>SUM(G95:G105)</f>
+        <v>17.1615</v>
+      </c>
+      <c r="H106" s="48"/>
+      <c r="I106" s="59"/>
+      <c r="J106" s="48"/>
+      <c r="K106" s="58"/>
+      <c r="L106" s="60"/>
+      <c r="M106" s="58"/>
+      <c r="N106" s="58"/>
+      <c r="O106" s="58"/>
+    </row>
+    <row r="107" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C107" s="7"/>
+      <c r="D107" s="8"/>
+      <c r="E107" s="24"/>
+      <c r="F107" s="24"/>
+      <c r="G107" s="25"/>
+      <c r="H107" s="10"/>
+      <c r="I107" s="11"/>
+      <c r="J107" s="10"/>
+      <c r="L107" s="35"/>
+    </row>
+    <row r="108" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C108" s="7"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="24"/>
+      <c r="F108" s="24"/>
+      <c r="G108" s="25"/>
+      <c r="H108" s="10"/>
+      <c r="I108" s="11"/>
+      <c r="J108" s="10"/>
+      <c r="L108" s="35"/>
+    </row>
+    <row r="109" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C109" s="7"/>
+      <c r="D109" s="8"/>
+      <c r="E109" s="24"/>
+      <c r="F109" s="24"/>
+      <c r="G109" s="25"/>
+      <c r="H109" s="10"/>
+      <c r="I109" s="11"/>
+      <c r="J109" s="10"/>
+      <c r="L109" s="35"/>
+    </row>
+    <row r="110" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C110" s="7"/>
+      <c r="D110" s="8"/>
+      <c r="E110" s="24"/>
+      <c r="F110" s="24"/>
+      <c r="G110" s="25"/>
+      <c r="H110" s="10"/>
+      <c r="I110" s="11"/>
+      <c r="J110" s="10"/>
+      <c r="L110" s="35"/>
+    </row>
+    <row r="111" spans="1:15" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C111" s="93" t="s">
+        <v>163</v>
+      </c>
+      <c r="D111" s="94"/>
+      <c r="E111" s="18"/>
+      <c r="H111" s="14"/>
+      <c r="I111" s="17"/>
+      <c r="J111" s="14"/>
+      <c r="K111" s="14"/>
+      <c r="L111" s="14"/>
+    </row>
+    <row r="112" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C112" s="144"/>
+      <c r="D112" s="151" t="s">
+        <v>226</v>
+      </c>
+      <c r="E112" s="98"/>
+      <c r="F112" s="98"/>
+      <c r="G112" s="99">
+        <v>1.53</v>
+      </c>
+      <c r="H112" s="157"/>
+      <c r="I112" s="158"/>
+      <c r="J112" s="157"/>
+      <c r="K112" s="157"/>
+      <c r="L112" s="159"/>
+    </row>
+    <row r="113" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C113" s="144"/>
+      <c r="D113" s="151" t="s">
+        <v>30</v>
+      </c>
+      <c r="E113" s="98"/>
+      <c r="F113" s="98"/>
+      <c r="G113" s="99">
+        <v>33.57</v>
+      </c>
+      <c r="H113" s="157"/>
+      <c r="I113" s="158"/>
+      <c r="J113" s="157"/>
+      <c r="K113" s="157"/>
+      <c r="L113" s="159"/>
+    </row>
+    <row r="114" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C114" s="144"/>
+      <c r="D114" s="151" t="s">
+        <v>2</v>
+      </c>
+      <c r="E114" s="98"/>
+      <c r="F114" s="98"/>
+      <c r="G114" s="99">
         <v>6.56</v>
       </c>
-      <c r="H104" s="157"/>
-      <c r="I104" s="158"/>
-      <c r="J104" s="157"/>
-      <c r="K104" s="157"/>
-      <c r="L104" s="159"/>
-    </row>
-    <row r="105" spans="3:12" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C105" s="144"/>
-      <c r="D105" s="151" t="s">
+      <c r="H114" s="157"/>
+      <c r="I114" s="158"/>
+      <c r="J114" s="157"/>
+      <c r="K114" s="157"/>
+      <c r="L114" s="159"/>
+    </row>
+    <row r="115" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C115" s="144"/>
+      <c r="D115" s="151" t="s">
         <v>11</v>
       </c>
-      <c r="E105" s="98"/>
-      <c r="F105" s="98"/>
-      <c r="G105" s="99">
+      <c r="E115" s="98"/>
+      <c r="F115" s="98"/>
+      <c r="G115" s="99">
         <v>2.57</v>
       </c>
-      <c r="H105" s="157"/>
-      <c r="I105" s="158"/>
-      <c r="J105" s="157"/>
-      <c r="K105" s="157"/>
-      <c r="L105" s="159"/>
-    </row>
-    <row r="106" spans="3:12" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C106" s="144"/>
-      <c r="D106" s="151" t="s">
+      <c r="H115" s="157"/>
+      <c r="I115" s="158"/>
+      <c r="J115" s="157"/>
+      <c r="K115" s="157"/>
+      <c r="L115" s="159"/>
+    </row>
+    <row r="116" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C116" s="144"/>
+      <c r="D116" s="151" t="s">
         <v>61</v>
       </c>
-      <c r="E106" s="98"/>
-      <c r="F106" s="98"/>
-      <c r="G106" s="99">
+      <c r="E116" s="98"/>
+      <c r="F116" s="98"/>
+      <c r="G116" s="99">
         <v>5.22</v>
       </c>
-      <c r="H106" s="157"/>
-      <c r="I106" s="158"/>
-      <c r="J106" s="157"/>
-      <c r="K106" s="157"/>
-      <c r="L106" s="159"/>
-    </row>
-    <row r="107" spans="3:12" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C107" s="144"/>
-      <c r="D107" s="151" t="s">
+      <c r="H116" s="157"/>
+      <c r="I116" s="158"/>
+      <c r="J116" s="157"/>
+      <c r="K116" s="157"/>
+      <c r="L116" s="159"/>
+    </row>
+    <row r="117" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C117" s="144"/>
+      <c r="D117" s="151" t="s">
         <v>162</v>
       </c>
-      <c r="E107" s="98"/>
-      <c r="F107" s="98"/>
-      <c r="G107" s="99">
+      <c r="E117" s="98"/>
+      <c r="F117" s="98"/>
+      <c r="G117" s="99">
         <v>0.39900000000000002</v>
       </c>
-      <c r="H107" s="157"/>
-      <c r="I107" s="158"/>
-      <c r="J107" s="157"/>
-      <c r="K107" s="157"/>
-      <c r="L107" s="159"/>
-    </row>
-    <row r="108" spans="3:12" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C108" s="145"/>
-      <c r="D108" s="151" t="s">
+      <c r="H117" s="157"/>
+      <c r="I117" s="158"/>
+      <c r="J117" s="157"/>
+      <c r="K117" s="157"/>
+      <c r="L117" s="159"/>
+    </row>
+    <row r="118" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C118" s="145"/>
+      <c r="D118" s="151" t="s">
         <v>73</v>
       </c>
-      <c r="E108" s="98"/>
-      <c r="F108" s="98"/>
-      <c r="G108" s="99">
+      <c r="E118" s="98"/>
+      <c r="F118" s="98"/>
+      <c r="G118" s="99">
         <v>0.77</v>
       </c>
-      <c r="H108" s="9"/>
-      <c r="I108" s="13"/>
-      <c r="J108" s="9"/>
-      <c r="K108" s="9"/>
-      <c r="L108" s="38"/>
-    </row>
-    <row r="109" spans="3:12" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C109" s="145"/>
-      <c r="D109" s="151" t="s">
+      <c r="H118" s="9"/>
+      <c r="I118" s="13"/>
+      <c r="J118" s="9"/>
+      <c r="K118" s="9"/>
+      <c r="L118" s="38"/>
+    </row>
+    <row r="119" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C119" s="145"/>
+      <c r="D119" s="151" t="s">
         <v>6</v>
-      </c>
-      <c r="E109" s="98"/>
-      <c r="F109" s="98"/>
-      <c r="G109" s="99">
-        <v>0.02</v>
-      </c>
-      <c r="H109" s="9"/>
-      <c r="I109" s="13"/>
-      <c r="J109" s="9"/>
-      <c r="K109" s="9"/>
-      <c r="L109" s="38"/>
-    </row>
-    <row r="110" spans="3:12" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C110" s="145"/>
-      <c r="D110" s="153" t="s">
-        <v>168</v>
-      </c>
-      <c r="E110" s="98"/>
-      <c r="F110" s="98"/>
-      <c r="G110" s="99">
-        <f>5.72+(0.5*4.99)</f>
-        <v>8.2149999999999999</v>
-      </c>
-      <c r="H110" s="9"/>
-      <c r="I110" s="13"/>
-      <c r="J110" s="9"/>
-      <c r="K110" s="9"/>
-      <c r="L110" s="38"/>
-    </row>
-    <row r="111" spans="3:12" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C111" s="145"/>
-      <c r="D111" s="151" t="s">
-        <v>169</v>
-      </c>
-      <c r="E111" s="98"/>
-      <c r="F111" s="98"/>
-      <c r="G111" s="99">
-        <f>2.83+(0.5*4.99)</f>
-        <v>5.3250000000000002</v>
-      </c>
-      <c r="H111" s="9"/>
-      <c r="I111" s="13"/>
-      <c r="J111" s="9"/>
-      <c r="K111" s="9"/>
-      <c r="L111" s="38"/>
-    </row>
-    <row r="112" spans="3:12" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C112" s="146"/>
-      <c r="D112" s="152" t="s">
-        <v>74</v>
-      </c>
-      <c r="E112" s="100"/>
-      <c r="F112" s="100"/>
-      <c r="G112" s="101">
-        <v>1.53</v>
-      </c>
-      <c r="H112" s="160"/>
-      <c r="I112" s="13"/>
-      <c r="J112" s="9"/>
-      <c r="K112" s="9"/>
-      <c r="L112" s="38"/>
-    </row>
-    <row r="113" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="67"/>
-      <c r="B113" s="67"/>
-      <c r="C113" s="68"/>
-      <c r="D113" s="69"/>
-      <c r="E113" s="70"/>
-      <c r="F113" s="70"/>
-      <c r="G113" s="97">
-        <f>SUM(G102:G112)</f>
-        <v>65.709000000000017</v>
-      </c>
-      <c r="H113" s="71"/>
-      <c r="I113" s="72"/>
-      <c r="J113" s="71"/>
-      <c r="K113" s="67"/>
-      <c r="L113" s="67"/>
-      <c r="M113" s="67"/>
-      <c r="N113" s="67"/>
-      <c r="O113" s="67"/>
-    </row>
-    <row r="114" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C114" s="51"/>
-      <c r="D114" s="73"/>
-      <c r="E114" s="74"/>
-      <c r="F114" s="74"/>
-      <c r="G114" s="75"/>
-      <c r="H114" s="55"/>
-      <c r="I114" s="56"/>
-      <c r="J114" s="55"/>
-      <c r="L114" s="57"/>
-    </row>
-    <row r="115" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="116" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="79"/>
-      <c r="B116" s="79"/>
-      <c r="C116" s="80"/>
-      <c r="D116" s="81"/>
-      <c r="E116" s="82"/>
-      <c r="F116" s="82"/>
-      <c r="G116" s="83"/>
-      <c r="H116" s="84"/>
-      <c r="I116" s="85"/>
-      <c r="J116" s="84"/>
-      <c r="K116" s="79"/>
-      <c r="L116" s="79"/>
-      <c r="M116" s="79"/>
-      <c r="N116" s="79"/>
-      <c r="O116" s="79"/>
-    </row>
-    <row r="117" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C117" s="87"/>
-      <c r="D117" s="88"/>
-      <c r="E117" s="61"/>
-      <c r="F117" s="61"/>
-      <c r="G117" s="89"/>
-      <c r="H117" s="90"/>
-      <c r="I117" s="91"/>
-      <c r="J117" s="90"/>
-      <c r="L117" s="92"/>
-    </row>
-    <row r="118" spans="1:15" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C118" s="93" t="s">
-        <v>165</v>
-      </c>
-      <c r="D118" s="94"/>
-      <c r="E118" s="18"/>
-      <c r="H118" s="64"/>
-      <c r="I118" s="65"/>
-      <c r="J118" s="64"/>
-    </row>
-    <row r="119" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C119" s="144"/>
-      <c r="D119" s="151" t="s">
-        <v>225</v>
       </c>
       <c r="E119" s="98"/>
       <c r="F119" s="98"/>
       <c r="G119" s="99">
-        <v>1.53</v>
-      </c>
-      <c r="H119" s="55"/>
-      <c r="I119" s="56"/>
-      <c r="J119" s="55"/>
-      <c r="L119" s="57"/>
-    </row>
-    <row r="120" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C120" s="144"/>
-      <c r="D120" s="151" t="s">
-        <v>166</v>
+        <v>0.02</v>
+      </c>
+      <c r="H119" s="9"/>
+      <c r="I119" s="13"/>
+      <c r="J119" s="9"/>
+      <c r="K119" s="9"/>
+      <c r="L119" s="38"/>
+    </row>
+    <row r="120" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C120" s="145"/>
+      <c r="D120" s="153" t="s">
+        <v>168</v>
       </c>
       <c r="E120" s="98"/>
       <c r="F120" s="98"/>
       <c r="G120" s="99">
-        <v>33.57</v>
-      </c>
-      <c r="H120" s="55"/>
-      <c r="I120" s="56"/>
-      <c r="J120" s="55"/>
-      <c r="L120" s="57"/>
-    </row>
-    <row r="121" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C121" s="144"/>
+        <f>5.72+(0.5*4.99)</f>
+        <v>8.2149999999999999</v>
+      </c>
+      <c r="H120" s="9"/>
+      <c r="I120" s="13"/>
+      <c r="J120" s="9"/>
+      <c r="K120" s="9"/>
+      <c r="L120" s="38"/>
+    </row>
+    <row r="121" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C121" s="145"/>
       <c r="D121" s="151" t="s">
-        <v>2</v>
+        <v>169</v>
       </c>
       <c r="E121" s="98"/>
       <c r="F121" s="98"/>
       <c r="G121" s="99">
-        <v>6.56</v>
-      </c>
-      <c r="H121" s="55"/>
-      <c r="I121" s="56"/>
-      <c r="J121" s="55"/>
-      <c r="L121" s="57"/>
-    </row>
-    <row r="122" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C122" s="144"/>
-      <c r="D122" s="151" t="s">
-        <v>61</v>
-      </c>
-      <c r="E122" s="98"/>
-      <c r="F122" s="98"/>
-      <c r="G122" s="99">
-        <v>6.91</v>
-      </c>
-      <c r="H122" s="55"/>
-      <c r="I122" s="56"/>
-      <c r="J122" s="55"/>
-      <c r="L122" s="57"/>
-    </row>
-    <row r="123" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C123" s="145"/>
-      <c r="D123" s="151" t="s">
-        <v>162</v>
-      </c>
-      <c r="E123" s="98"/>
-      <c r="F123" s="98"/>
-      <c r="G123" s="99">
-        <v>0.39900000000000002</v>
-      </c>
-      <c r="H123" s="10"/>
-      <c r="I123" s="11"/>
-      <c r="J123" s="10"/>
-      <c r="L123" s="35"/>
-    </row>
-    <row r="124" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C124" s="145"/>
-      <c r="D124" s="151" t="s">
-        <v>11</v>
-      </c>
-      <c r="E124" s="98"/>
-      <c r="F124" s="98"/>
-      <c r="G124" s="99">
-        <v>2.57</v>
-      </c>
-      <c r="H124" s="10"/>
-      <c r="I124" s="11"/>
-      <c r="J124" s="10"/>
-      <c r="L124" s="35"/>
-    </row>
-    <row r="125" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C125" s="145"/>
-      <c r="D125" s="151" t="s">
-        <v>6</v>
-      </c>
-      <c r="E125" s="98"/>
-      <c r="F125" s="98"/>
-      <c r="G125" s="99">
-        <v>0.02</v>
-      </c>
-      <c r="H125" s="10"/>
-      <c r="I125" s="11"/>
-      <c r="J125" s="10"/>
-      <c r="L125" s="35"/>
-    </row>
-    <row r="126" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D126" s="151" t="s">
-        <v>73</v>
-      </c>
-      <c r="E126" s="98"/>
-      <c r="F126" s="98"/>
-      <c r="G126" s="99">
-        <v>0.77</v>
-      </c>
-    </row>
-    <row r="127" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D127" s="154" t="s">
+        <f>2.83+(0.5*4.99)</f>
+        <v>5.3250000000000002</v>
+      </c>
+      <c r="H121" s="9"/>
+      <c r="I121" s="13"/>
+      <c r="J121" s="9"/>
+      <c r="K121" s="9"/>
+      <c r="L121" s="38"/>
+    </row>
+    <row r="122" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C122" s="146"/>
+      <c r="D122" s="152" t="s">
         <v>74</v>
       </c>
-      <c r="E127" s="155"/>
-      <c r="F127" s="155"/>
-      <c r="G127" s="156">
+      <c r="E122" s="100"/>
+      <c r="F122" s="100"/>
+      <c r="G122" s="101">
         <v>1.53</v>
       </c>
-    </row>
-    <row r="128" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C128" s="146"/>
-      <c r="D128" s="152" t="s">
-        <v>224</v>
-      </c>
-      <c r="E128" s="100"/>
-      <c r="F128" s="100"/>
-      <c r="G128" s="101">
-        <v>3.78</v>
-      </c>
-      <c r="H128" s="48"/>
-      <c r="I128" s="11"/>
-      <c r="J128" s="10"/>
-      <c r="K128" s="12"/>
-      <c r="L128" s="35"/>
-      <c r="M128" s="12"/>
-      <c r="N128" s="12"/>
-      <c r="O128" s="12"/>
-    </row>
-    <row r="129" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="67"/>
-      <c r="B129" s="67"/>
-      <c r="C129" s="68"/>
-      <c r="D129" s="69"/>
-      <c r="E129" s="70"/>
-      <c r="F129" s="70"/>
-      <c r="G129" s="97">
-        <f>SUM(G119:G128)</f>
-        <v>57.639000000000017</v>
-      </c>
-      <c r="H129" s="71"/>
-      <c r="I129" s="72"/>
-      <c r="J129" s="71"/>
-      <c r="K129" s="67"/>
-      <c r="L129" s="67"/>
-      <c r="M129" s="67"/>
-      <c r="N129" s="67"/>
-      <c r="O129" s="67"/>
-    </row>
-    <row r="130" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C130" s="51"/>
-      <c r="D130" s="52"/>
-      <c r="E130" s="53"/>
-      <c r="F130" s="53"/>
-      <c r="G130" s="54"/>
+      <c r="H122" s="160"/>
+      <c r="I122" s="13"/>
+      <c r="J122" s="9"/>
+      <c r="K122" s="9"/>
+      <c r="L122" s="38"/>
+    </row>
+    <row r="123" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="67"/>
+      <c r="B123" s="67"/>
+      <c r="C123" s="68"/>
+      <c r="D123" s="69"/>
+      <c r="E123" s="70"/>
+      <c r="F123" s="70"/>
+      <c r="G123" s="97">
+        <f>SUM(G112:G122)</f>
+        <v>65.709000000000017</v>
+      </c>
+      <c r="H123" s="71"/>
+      <c r="I123" s="72"/>
+      <c r="J123" s="71"/>
+      <c r="K123" s="67"/>
+      <c r="L123" s="67"/>
+      <c r="M123" s="67"/>
+      <c r="N123" s="67"/>
+      <c r="O123" s="67"/>
+    </row>
+    <row r="124" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C124" s="51"/>
+      <c r="D124" s="73"/>
+      <c r="E124" s="74"/>
+      <c r="F124" s="74"/>
+      <c r="G124" s="75"/>
+      <c r="H124" s="55"/>
+      <c r="I124" s="56"/>
+      <c r="J124" s="55"/>
+      <c r="L124" s="57"/>
+    </row>
+    <row r="125" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="79"/>
+      <c r="B126" s="79"/>
+      <c r="C126" s="80"/>
+      <c r="D126" s="81"/>
+      <c r="E126" s="82"/>
+      <c r="F126" s="82"/>
+      <c r="G126" s="83"/>
+      <c r="H126" s="84"/>
+      <c r="I126" s="85"/>
+      <c r="J126" s="84"/>
+      <c r="K126" s="79"/>
+      <c r="L126" s="79"/>
+      <c r="M126" s="79"/>
+      <c r="N126" s="79"/>
+      <c r="O126" s="79"/>
+    </row>
+    <row r="127" spans="1:15" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C127" s="87"/>
+      <c r="D127" s="88"/>
+      <c r="E127" s="61"/>
+      <c r="F127" s="61"/>
+      <c r="G127" s="89"/>
+      <c r="H127" s="90"/>
+      <c r="I127" s="91"/>
+      <c r="J127" s="90"/>
+      <c r="L127" s="92"/>
+    </row>
+    <row r="128" spans="1:15" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C128" s="93" t="s">
+        <v>165</v>
+      </c>
+      <c r="D128" s="94"/>
+      <c r="E128" s="18"/>
+      <c r="H128" s="64"/>
+      <c r="I128" s="65"/>
+      <c r="J128" s="64"/>
+    </row>
+    <row r="129" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C129" s="144"/>
+      <c r="D129" s="151" t="s">
+        <v>225</v>
+      </c>
+      <c r="E129" s="98"/>
+      <c r="F129" s="98"/>
+      <c r="G129" s="99">
+        <v>1.53</v>
+      </c>
+      <c r="H129" s="55"/>
+      <c r="I129" s="56"/>
+      <c r="J129" s="55"/>
+      <c r="L129" s="57"/>
+    </row>
+    <row r="130" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C130" s="144"/>
+      <c r="D130" s="151" t="s">
+        <v>166</v>
+      </c>
+      <c r="E130" s="98"/>
+      <c r="F130" s="98"/>
+      <c r="G130" s="99">
+        <v>33.57</v>
+      </c>
       <c r="H130" s="55"/>
       <c r="I130" s="56"/>
       <c r="J130" s="55"/>
       <c r="L130" s="57"/>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C131" s="51"/>
-      <c r="D131" s="52"/>
-      <c r="E131" s="53"/>
-      <c r="F131" s="53"/>
-      <c r="G131" s="54"/>
+    <row r="131" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C131" s="144"/>
+      <c r="D131" s="151" t="s">
+        <v>2</v>
+      </c>
+      <c r="E131" s="98"/>
+      <c r="F131" s="98"/>
+      <c r="G131" s="99">
+        <v>6.56</v>
+      </c>
       <c r="H131" s="55"/>
       <c r="I131" s="56"/>
       <c r="J131" s="55"/>
-    </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C132" s="51"/>
-      <c r="D132" s="52"/>
-      <c r="E132" s="53"/>
-      <c r="F132" s="53"/>
-      <c r="G132" s="54"/>
+      <c r="L131" s="57"/>
+    </row>
+    <row r="132" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C132" s="144"/>
+      <c r="D132" s="151" t="s">
+        <v>61</v>
+      </c>
+      <c r="E132" s="98"/>
+      <c r="F132" s="98"/>
+      <c r="G132" s="99">
+        <v>6.91</v>
+      </c>
       <c r="H132" s="55"/>
       <c r="I132" s="56"/>
       <c r="J132" s="55"/>
-    </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C133" s="51"/>
-      <c r="D133" s="52"/>
-      <c r="E133" s="53"/>
-      <c r="F133" s="53"/>
-      <c r="G133" s="54"/>
-      <c r="H133" s="55"/>
-      <c r="I133" s="56"/>
-      <c r="J133" s="55"/>
-    </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C134" s="51"/>
-      <c r="D134" s="52"/>
-      <c r="E134" s="53"/>
-      <c r="F134" s="53"/>
-      <c r="G134" s="54"/>
-      <c r="H134" s="55"/>
-      <c r="I134" s="56"/>
-      <c r="J134" s="55"/>
-    </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C135" s="51"/>
-      <c r="D135" s="52"/>
-      <c r="E135" s="53"/>
-      <c r="F135" s="53"/>
-      <c r="G135" s="54"/>
-      <c r="H135" s="55"/>
-      <c r="I135" s="56"/>
-      <c r="J135" s="55"/>
-    </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C136" s="51"/>
-      <c r="D136" s="52"/>
-      <c r="E136" s="53"/>
-      <c r="F136" s="53"/>
-      <c r="G136" s="54"/>
-      <c r="H136" s="55"/>
-      <c r="I136" s="56"/>
-      <c r="J136" s="55"/>
-    </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C137" s="51"/>
-      <c r="D137" s="52"/>
-      <c r="E137" s="53"/>
-      <c r="F137" s="53"/>
-      <c r="G137" s="54"/>
-      <c r="H137" s="55"/>
-      <c r="I137" s="56"/>
-      <c r="J137" s="55"/>
-    </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C138" s="51"/>
-      <c r="D138" s="52"/>
-      <c r="E138" s="53"/>
-      <c r="F138" s="53"/>
-      <c r="G138" s="54"/>
-      <c r="H138" s="55"/>
-      <c r="I138" s="56"/>
-      <c r="J138" s="55"/>
-    </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C139" s="51"/>
-      <c r="D139" s="52"/>
-      <c r="E139" s="53"/>
-      <c r="F139" s="53"/>
-      <c r="G139" s="54"/>
-      <c r="H139" s="55"/>
-      <c r="I139" s="56"/>
-      <c r="J139" s="55"/>
-    </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L132" s="57"/>
+    </row>
+    <row r="133" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C133" s="145"/>
+      <c r="D133" s="151" t="s">
+        <v>162</v>
+      </c>
+      <c r="E133" s="98"/>
+      <c r="F133" s="98"/>
+      <c r="G133" s="99">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="H133" s="10"/>
+      <c r="I133" s="11"/>
+      <c r="J133" s="10"/>
+      <c r="L133" s="35"/>
+    </row>
+    <row r="134" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C134" s="145"/>
+      <c r="D134" s="151" t="s">
+        <v>11</v>
+      </c>
+      <c r="E134" s="98"/>
+      <c r="F134" s="98"/>
+      <c r="G134" s="99">
+        <v>2.57</v>
+      </c>
+      <c r="H134" s="10"/>
+      <c r="I134" s="11"/>
+      <c r="J134" s="10"/>
+      <c r="L134" s="35"/>
+    </row>
+    <row r="135" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C135" s="145"/>
+      <c r="D135" s="151" t="s">
+        <v>6</v>
+      </c>
+      <c r="E135" s="98"/>
+      <c r="F135" s="98"/>
+      <c r="G135" s="99">
+        <v>0.02</v>
+      </c>
+      <c r="H135" s="10"/>
+      <c r="I135" s="11"/>
+      <c r="J135" s="10"/>
+      <c r="L135" s="35"/>
+    </row>
+    <row r="136" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D136" s="151" t="s">
+        <v>73</v>
+      </c>
+      <c r="E136" s="98"/>
+      <c r="F136" s="98"/>
+      <c r="G136" s="99">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D137" s="154" t="s">
+        <v>74</v>
+      </c>
+      <c r="E137" s="155"/>
+      <c r="F137" s="155"/>
+      <c r="G137" s="156">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C138" s="146"/>
+      <c r="D138" s="152" t="s">
+        <v>224</v>
+      </c>
+      <c r="E138" s="100"/>
+      <c r="F138" s="100"/>
+      <c r="G138" s="101">
+        <v>3.78</v>
+      </c>
+      <c r="H138" s="48"/>
+      <c r="I138" s="11"/>
+      <c r="J138" s="10"/>
+      <c r="K138" s="12"/>
+      <c r="L138" s="35"/>
+      <c r="M138" s="12"/>
+      <c r="N138" s="12"/>
+      <c r="O138" s="12"/>
+    </row>
+    <row r="139" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="67"/>
+      <c r="B139" s="67"/>
+      <c r="C139" s="68"/>
+      <c r="D139" s="69"/>
+      <c r="E139" s="70"/>
+      <c r="F139" s="70"/>
+      <c r="G139" s="97">
+        <f>SUM(G129:G138)</f>
+        <v>57.639000000000017</v>
+      </c>
+      <c r="H139" s="71"/>
+      <c r="I139" s="72"/>
+      <c r="J139" s="71"/>
+      <c r="K139" s="67"/>
+      <c r="L139" s="67"/>
+      <c r="M139" s="67"/>
+      <c r="N139" s="67"/>
+      <c r="O139" s="67"/>
+    </row>
+    <row r="140" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C140" s="51"/>
       <c r="D140" s="52"/>
       <c r="E140" s="53"/>
@@ -5383,6 +5502,7 @@
       <c r="H140" s="55"/>
       <c r="I140" s="56"/>
       <c r="J140" s="55"/>
+      <c r="L140" s="57"/>
     </row>
     <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C141" s="51"/>
@@ -5955,22 +6075,156 @@
       <c r="J197" s="55"/>
     </row>
     <row r="198" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C198" s="51"/>
       <c r="D198" s="52"/>
       <c r="E198" s="53"/>
       <c r="F198" s="53"/>
       <c r="G198" s="54"/>
+      <c r="H198" s="55"/>
+      <c r="I198" s="56"/>
+      <c r="J198" s="55"/>
     </row>
     <row r="199" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C199" s="51"/>
       <c r="D199" s="52"/>
       <c r="E199" s="53"/>
       <c r="F199" s="53"/>
       <c r="G199" s="54"/>
+      <c r="H199" s="55"/>
+      <c r="I199" s="56"/>
+      <c r="J199" s="55"/>
+    </row>
+    <row r="200" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C200" s="51"/>
+      <c r="D200" s="52"/>
+      <c r="E200" s="53"/>
+      <c r="F200" s="53"/>
+      <c r="G200" s="54"/>
+      <c r="H200" s="55"/>
+      <c r="I200" s="56"/>
+      <c r="J200" s="55"/>
+    </row>
+    <row r="201" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C201" s="51"/>
+      <c r="D201" s="52"/>
+      <c r="E201" s="53"/>
+      <c r="F201" s="53"/>
+      <c r="G201" s="54"/>
+      <c r="H201" s="55"/>
+      <c r="I201" s="56"/>
+      <c r="J201" s="55"/>
+    </row>
+    <row r="202" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C202" s="51"/>
+      <c r="D202" s="52"/>
+      <c r="E202" s="53"/>
+      <c r="F202" s="53"/>
+      <c r="G202" s="54"/>
+      <c r="H202" s="55"/>
+      <c r="I202" s="56"/>
+      <c r="J202" s="55"/>
+    </row>
+    <row r="203" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C203" s="51"/>
+      <c r="D203" s="52"/>
+      <c r="E203" s="53"/>
+      <c r="F203" s="53"/>
+      <c r="G203" s="54"/>
+      <c r="H203" s="55"/>
+      <c r="I203" s="56"/>
+      <c r="J203" s="55"/>
+    </row>
+    <row r="204" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C204" s="51"/>
+      <c r="D204" s="52"/>
+      <c r="E204" s="53"/>
+      <c r="F204" s="53"/>
+      <c r="G204" s="54"/>
+      <c r="H204" s="55"/>
+      <c r="I204" s="56"/>
+      <c r="J204" s="55"/>
+    </row>
+    <row r="205" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C205" s="51"/>
+      <c r="D205" s="52"/>
+      <c r="E205" s="53"/>
+      <c r="F205" s="53"/>
+      <c r="G205" s="54"/>
+      <c r="H205" s="55"/>
+      <c r="I205" s="56"/>
+      <c r="J205" s="55"/>
+    </row>
+    <row r="206" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C206" s="51"/>
+      <c r="D206" s="52"/>
+      <c r="E206" s="53"/>
+      <c r="F206" s="53"/>
+      <c r="G206" s="54"/>
+      <c r="H206" s="55"/>
+      <c r="I206" s="56"/>
+      <c r="J206" s="55"/>
+    </row>
+    <row r="207" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C207" s="51"/>
+      <c r="D207" s="52"/>
+      <c r="E207" s="53"/>
+      <c r="F207" s="53"/>
+      <c r="G207" s="54"/>
+      <c r="H207" s="55"/>
+      <c r="I207" s="56"/>
+      <c r="J207" s="55"/>
+    </row>
+    <row r="208" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D208" s="52"/>
+      <c r="E208" s="53"/>
+      <c r="F208" s="53"/>
+      <c r="G208" s="54"/>
+    </row>
+    <row r="209" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D209" s="52"/>
+      <c r="E209" s="53"/>
+      <c r="F209" s="53"/>
+      <c r="G209" s="54"/>
     </row>
   </sheetData>
   <sortState ref="C4:H19">
     <sortCondition ref="C4:C19"/>
   </sortState>
-  <mergeCells count="46">
+  <mergeCells count="50">
+    <mergeCell ref="C78:C86"/>
+    <mergeCell ref="H78:H86"/>
+    <mergeCell ref="I78:I86"/>
+    <mergeCell ref="J78:J86"/>
+    <mergeCell ref="C70:C76"/>
+    <mergeCell ref="H70:H76"/>
+    <mergeCell ref="I70:I76"/>
+    <mergeCell ref="J70:J76"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="H63:H66"/>
+    <mergeCell ref="I63:I66"/>
+    <mergeCell ref="J63:J66"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="H51:H53"/>
+    <mergeCell ref="I51:I53"/>
+    <mergeCell ref="J51:J53"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="C41:C45"/>
+    <mergeCell ref="H41:H45"/>
+    <mergeCell ref="I41:I45"/>
+    <mergeCell ref="J41:J45"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="J27:J29"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="H33:H34"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="H38:H39"/>
     <mergeCell ref="I38:I39"/>
@@ -5987,36 +6241,6 @@
     <mergeCell ref="I27:I29"/>
     <mergeCell ref="I21:I25"/>
     <mergeCell ref="H16:H17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="J27:J29"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="H51:H53"/>
-    <mergeCell ref="I51:I53"/>
-    <mergeCell ref="J51:J53"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="C41:C45"/>
-    <mergeCell ref="H41:H45"/>
-    <mergeCell ref="I41:I45"/>
-    <mergeCell ref="J41:J45"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="C70:C76"/>
-    <mergeCell ref="H70:H76"/>
-    <mergeCell ref="I70:I76"/>
-    <mergeCell ref="J70:J76"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="H63:H66"/>
-    <mergeCell ref="I63:I66"/>
-    <mergeCell ref="J63:J66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6924,21 +7148,21 @@
       <c r="AB16" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="AN16" s="219" t="s">
+      <c r="AN16" s="222" t="s">
         <v>123</v>
       </c>
-      <c r="AO16" s="219"/>
-      <c r="AP16" s="219"/>
-      <c r="AQ16" s="219"/>
-      <c r="AT16" s="218" t="s">
+      <c r="AO16" s="222"/>
+      <c r="AP16" s="222"/>
+      <c r="AQ16" s="222"/>
+      <c r="AT16" s="219" t="s">
         <v>119</v>
       </c>
-      <c r="AU16" s="218"/>
-      <c r="AV16" s="218"/>
-      <c r="AW16" s="218"/>
-      <c r="AX16" s="218"/>
-      <c r="AY16" s="218"/>
-      <c r="AZ16" s="218"/>
+      <c r="AU16" s="219"/>
+      <c r="AV16" s="219"/>
+      <c r="AW16" s="219"/>
+      <c r="AX16" s="219"/>
+      <c r="AY16" s="219"/>
+      <c r="AZ16" s="219"/>
     </row>
     <row r="17" spans="25:59" x14ac:dyDescent="0.25">
       <c r="Y17" s="108" t="s">
@@ -6953,22 +7177,22 @@
       <c r="AB17" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="AJ17" s="218" t="s">
+      <c r="AJ17" s="219" t="s">
         <v>117</v>
       </c>
-      <c r="AK17" s="218"/>
-      <c r="AL17" s="218"/>
-      <c r="AN17" s="219"/>
-      <c r="AO17" s="219"/>
-      <c r="AP17" s="219"/>
-      <c r="AQ17" s="219"/>
+      <c r="AK17" s="219"/>
+      <c r="AL17" s="219"/>
+      <c r="AN17" s="222"/>
+      <c r="AO17" s="222"/>
+      <c r="AP17" s="222"/>
+      <c r="AQ17" s="222"/>
     </row>
     <row r="19" spans="25:59" x14ac:dyDescent="0.25">
       <c r="AP19" s="195" t="s">
         <v>216</v>
       </c>
       <c r="AQ19" s="117">
-        <f>INVENTORY!G113</f>
+        <f>INVENTORY!G123</f>
         <v>65.709000000000017</v>
       </c>
       <c r="AS19" s="196" t="s">
@@ -6976,11 +7200,11 @@
       </c>
     </row>
     <row r="20" spans="25:59" x14ac:dyDescent="0.25">
-      <c r="AK20" s="220" t="s">
+      <c r="AK20" s="223" t="s">
         <v>120</v>
       </c>
-      <c r="AL20" s="220"/>
-      <c r="AM20" s="220"/>
+      <c r="AL20" s="223"/>
+      <c r="AM20" s="223"/>
       <c r="AP20" s="195" t="s">
         <v>217</v>
       </c>
@@ -7275,7 +7499,7 @@
         <f t="shared" si="1"/>
         <v>6.6300000000000008</v>
       </c>
-      <c r="H11" s="221">
+      <c r="H11" s="224">
         <v>3.39</v>
       </c>
       <c r="I11" s="172" t="s">
@@ -7305,7 +7529,7 @@
         <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
-      <c r="H12" s="221"/>
+      <c r="H12" s="224"/>
       <c r="I12" s="172" t="s">
         <v>186</v>
       </c>
@@ -7361,7 +7585,7 @@
         <f t="shared" si="1"/>
         <v>57.199999999999996</v>
       </c>
-      <c r="H14" s="222">
+      <c r="H14" s="225">
         <v>4.99</v>
       </c>
       <c r="I14" s="172" t="s">
@@ -7390,7 +7614,7 @@
         <f t="shared" si="1"/>
         <v>28.3</v>
       </c>
-      <c r="H15" s="223"/>
+      <c r="H15" s="226"/>
       <c r="I15" s="182" t="s">
         <v>228</v>
       </c>

</xml_diff>

<commit_message>
PARTS TO TRY AND BUILD A POWER BUTTON FOR THE ADAFRUIT FEATHER
</commit_message>
<xml_diff>
--- a/BillOfMaterials/INVENTORY.xlsx
+++ b/BillOfMaterials/INVENTORY.xlsx
@@ -2443,24 +2443,27 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2475,9 +2478,6 @@
     </xf>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2999,9 +2999,9 @@
   </sheetPr>
   <dimension ref="A1:AB209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L84" sqref="L84"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3088,7 +3088,7 @@
       <c r="L3" s="35"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C4" s="216">
+      <c r="C4" s="217">
         <v>42882</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -3103,14 +3103,14 @@
       <c r="G4" s="27">
         <v>6.99</v>
       </c>
-      <c r="H4" s="218">
+      <c r="H4" s="221">
         <f>SUM(G4:G10)</f>
         <v>48.1</v>
       </c>
-      <c r="I4" s="217">
+      <c r="I4" s="218">
         <v>0</v>
       </c>
-      <c r="J4" s="218">
+      <c r="J4" s="221">
         <f>H4+I4</f>
         <v>48.1</v>
       </c>
@@ -3122,7 +3122,7 @@
       <c r="M4" s="220"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C5" s="216"/>
+      <c r="C5" s="217"/>
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
@@ -3135,9 +3135,9 @@
       <c r="G5" s="27">
         <v>6.99</v>
       </c>
-      <c r="H5" s="219"/>
-      <c r="I5" s="217"/>
-      <c r="J5" s="219"/>
+      <c r="H5" s="222"/>
+      <c r="I5" s="218"/>
+      <c r="J5" s="222"/>
       <c r="K5" s="220">
         <f t="shared" ref="K5:K10" si="0">G5/E5</f>
         <v>6.99</v>
@@ -3146,7 +3146,7 @@
       <c r="M5" s="220"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C6" s="216"/>
+      <c r="C6" s="217"/>
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
@@ -3159,9 +3159,9 @@
       <c r="G6" s="27">
         <v>4.97</v>
       </c>
-      <c r="H6" s="219"/>
-      <c r="I6" s="217"/>
-      <c r="J6" s="219"/>
+      <c r="H6" s="222"/>
+      <c r="I6" s="218"/>
+      <c r="J6" s="222"/>
       <c r="K6" s="220">
         <f t="shared" si="0"/>
         <v>0.2485</v>
@@ -3170,7 +3170,7 @@
       <c r="M6" s="220"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C7" s="216"/>
+      <c r="C7" s="217"/>
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
@@ -3183,9 +3183,9 @@
       <c r="G7" s="27">
         <v>5.99</v>
       </c>
-      <c r="H7" s="219"/>
-      <c r="I7" s="217"/>
-      <c r="J7" s="219"/>
+      <c r="H7" s="222"/>
+      <c r="I7" s="218"/>
+      <c r="J7" s="222"/>
       <c r="K7" s="220">
         <f t="shared" si="0"/>
         <v>0.29949999999999999</v>
@@ -3194,7 +3194,7 @@
       <c r="M7" s="220"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C8" s="216"/>
+      <c r="C8" s="217"/>
       <c r="D8" s="1" t="s">
         <v>155</v>
       </c>
@@ -3207,9 +3207,9 @@
       <c r="G8" s="27">
         <v>6.25</v>
       </c>
-      <c r="H8" s="219"/>
-      <c r="I8" s="217"/>
-      <c r="J8" s="219"/>
+      <c r="H8" s="222"/>
+      <c r="I8" s="218"/>
+      <c r="J8" s="222"/>
       <c r="K8" s="220">
         <f t="shared" si="0"/>
         <v>6.25</v>
@@ -3218,7 +3218,7 @@
       <c r="M8" s="220"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C9" s="216"/>
+      <c r="C9" s="217"/>
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3231,9 +3231,9 @@
       <c r="G9" s="27">
         <v>11.59</v>
       </c>
-      <c r="H9" s="219"/>
-      <c r="I9" s="217"/>
-      <c r="J9" s="219"/>
+      <c r="H9" s="222"/>
+      <c r="I9" s="218"/>
+      <c r="J9" s="222"/>
       <c r="K9" s="220">
         <f t="shared" si="0"/>
         <v>0.57950000000000002</v>
@@ -3242,7 +3242,7 @@
       <c r="M9" s="220"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C10" s="216"/>
+      <c r="C10" s="217"/>
       <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
@@ -3255,9 +3255,9 @@
       <c r="G10" s="27">
         <v>5.32</v>
       </c>
-      <c r="H10" s="219"/>
-      <c r="I10" s="217"/>
-      <c r="J10" s="219"/>
+      <c r="H10" s="222"/>
+      <c r="I10" s="218"/>
+      <c r="J10" s="222"/>
       <c r="K10" s="220">
         <f t="shared" si="0"/>
         <v>1.0640000000000001</v>
@@ -3370,14 +3370,14 @@
       <c r="G16" s="27">
         <v>6.56</v>
       </c>
-      <c r="H16" s="218">
+      <c r="H16" s="221">
         <f>SUM(G16:G17)</f>
         <v>7.55</v>
       </c>
-      <c r="I16" s="217">
+      <c r="I16" s="218">
         <v>0</v>
       </c>
-      <c r="J16" s="218">
+      <c r="J16" s="221">
         <f>H16+I16</f>
         <v>7.55</v>
       </c>
@@ -3398,9 +3398,9 @@
       <c r="G17" s="27">
         <v>0.99</v>
       </c>
-      <c r="H17" s="218"/>
-      <c r="I17" s="217"/>
-      <c r="J17" s="218"/>
+      <c r="H17" s="221"/>
+      <c r="I17" s="218"/>
+      <c r="J17" s="221"/>
     </row>
     <row r="18" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
@@ -3452,7 +3452,7 @@
       <c r="L20" s="35"/>
     </row>
     <row r="21" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C21" s="216">
+      <c r="C21" s="217">
         <v>42925</v>
       </c>
       <c r="D21" s="149" t="s">
@@ -3467,20 +3467,20 @@
       <c r="G21" s="27">
         <v>2.56</v>
       </c>
-      <c r="H21" s="218">
+      <c r="H21" s="221">
         <f>SUM(G21:G25)</f>
         <v>17.230000000000004</v>
       </c>
-      <c r="I21" s="217">
+      <c r="I21" s="218">
         <v>5.65</v>
       </c>
-      <c r="J21" s="218">
+      <c r="J21" s="221">
         <f>H21+I21</f>
         <v>22.880000000000003</v>
       </c>
     </row>
     <row r="22" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C22" s="216"/>
+      <c r="C22" s="217"/>
       <c r="D22" s="149" t="s">
         <v>21</v>
       </c>
@@ -3493,12 +3493,12 @@
       <c r="G22" s="27">
         <v>1.8</v>
       </c>
-      <c r="H22" s="219"/>
-      <c r="I22" s="217"/>
-      <c r="J22" s="219"/>
+      <c r="H22" s="222"/>
+      <c r="I22" s="218"/>
+      <c r="J22" s="222"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C23" s="216"/>
+      <c r="C23" s="217"/>
       <c r="D23" s="1" t="s">
         <v>20</v>
       </c>
@@ -3511,12 +3511,12 @@
       <c r="G23" s="27">
         <v>3.99</v>
       </c>
-      <c r="H23" s="219"/>
-      <c r="I23" s="217"/>
-      <c r="J23" s="219"/>
+      <c r="H23" s="222"/>
+      <c r="I23" s="218"/>
+      <c r="J23" s="222"/>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C24" s="216"/>
+      <c r="C24" s="217"/>
       <c r="D24" s="149" t="s">
         <v>13</v>
       </c>
@@ -3529,12 +3529,12 @@
       <c r="G24" s="27">
         <v>1.97</v>
       </c>
-      <c r="H24" s="219"/>
-      <c r="I24" s="217"/>
-      <c r="J24" s="219"/>
+      <c r="H24" s="222"/>
+      <c r="I24" s="218"/>
+      <c r="J24" s="222"/>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C25" s="216"/>
+      <c r="C25" s="217"/>
       <c r="D25" s="1" t="s">
         <v>2</v>
       </c>
@@ -3547,9 +3547,9 @@
       <c r="G25" s="27">
         <v>6.91</v>
       </c>
-      <c r="H25" s="219"/>
-      <c r="I25" s="217"/>
-      <c r="J25" s="219"/>
+      <c r="H25" s="222"/>
+      <c r="I25" s="218"/>
+      <c r="J25" s="222"/>
     </row>
     <row r="26" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
@@ -3563,7 +3563,7 @@
       <c r="L26" s="35"/>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C27" s="216">
+      <c r="C27" s="217">
         <v>42927</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -3578,20 +3578,20 @@
       <c r="G27" s="27">
         <v>0.75</v>
       </c>
-      <c r="H27" s="218">
+      <c r="H27" s="221">
         <f>SUM(G27:G29)</f>
         <v>3.44</v>
       </c>
-      <c r="I27" s="217">
+      <c r="I27" s="218">
         <v>4.99</v>
       </c>
-      <c r="J27" s="218">
+      <c r="J27" s="221">
         <f>H27+I27</f>
         <v>8.43</v>
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C28" s="216"/>
+      <c r="C28" s="217"/>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
@@ -3604,12 +3604,12 @@
       <c r="G28" s="27">
         <v>0.75</v>
       </c>
-      <c r="H28" s="219"/>
-      <c r="I28" s="217"/>
-      <c r="J28" s="219"/>
+      <c r="H28" s="222"/>
+      <c r="I28" s="218"/>
+      <c r="J28" s="222"/>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C29" s="216"/>
+      <c r="C29" s="217"/>
       <c r="D29" s="1" t="s">
         <v>154</v>
       </c>
@@ -3622,9 +3622,9 @@
       <c r="G29" s="27">
         <v>1.94</v>
       </c>
-      <c r="H29" s="219"/>
-      <c r="I29" s="217"/>
-      <c r="J29" s="219"/>
+      <c r="H29" s="222"/>
+      <c r="I29" s="218"/>
+      <c r="J29" s="222"/>
     </row>
     <row r="30" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="7"/>
@@ -3676,7 +3676,7 @@
       <c r="L32" s="35"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C33" s="216">
+      <c r="C33" s="217">
         <v>42929</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -3691,20 +3691,20 @@
       <c r="G33" s="27">
         <v>0.77</v>
       </c>
-      <c r="H33" s="218">
+      <c r="H33" s="221">
         <f>SUM(G33:G34)</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="I33" s="217">
+      <c r="I33" s="218">
         <v>3.39</v>
       </c>
-      <c r="J33" s="217">
+      <c r="J33" s="218">
         <f>SUM(H33:I34)</f>
         <v>5.6899999999999995</v>
       </c>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C34" s="216"/>
+      <c r="C34" s="217"/>
       <c r="D34" s="1" t="s">
         <v>76</v>
       </c>
@@ -3717,9 +3717,9 @@
       <c r="G34" s="27">
         <v>1.53</v>
       </c>
-      <c r="H34" s="219"/>
-      <c r="I34" s="217"/>
-      <c r="J34" s="217"/>
+      <c r="H34" s="222"/>
+      <c r="I34" s="218"/>
+      <c r="J34" s="218"/>
     </row>
     <row r="35" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="7"/>
@@ -3771,7 +3771,7 @@
       <c r="L37" s="35"/>
     </row>
     <row r="38" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C38" s="216">
+      <c r="C38" s="217">
         <v>42931</v>
       </c>
       <c r="D38" s="149" t="s">
@@ -3786,20 +3786,20 @@
       <c r="G38" s="27">
         <v>5.72</v>
       </c>
-      <c r="H38" s="217">
+      <c r="H38" s="218">
         <f>SUM(G38:G39)</f>
         <v>8.5500000000000007</v>
       </c>
-      <c r="I38" s="217">
+      <c r="I38" s="218">
         <v>4.99</v>
       </c>
-      <c r="J38" s="217">
+      <c r="J38" s="218">
         <f>SUM(H38:I39)</f>
         <v>13.540000000000001</v>
       </c>
     </row>
     <row r="39" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C39" s="216"/>
+      <c r="C39" s="217"/>
       <c r="D39" s="149" t="s">
         <v>122</v>
       </c>
@@ -3812,9 +3812,9 @@
       <c r="G39" s="27">
         <v>2.83</v>
       </c>
-      <c r="H39" s="217"/>
-      <c r="I39" s="217"/>
-      <c r="J39" s="217"/>
+      <c r="H39" s="218"/>
+      <c r="I39" s="218"/>
+      <c r="J39" s="218"/>
     </row>
     <row r="40" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="7"/>
@@ -3828,7 +3828,7 @@
       <c r="L40" s="35"/>
     </row>
     <row r="41" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C41" s="216">
+      <c r="C41" s="217">
         <v>42936</v>
       </c>
       <c r="D41" s="149" t="s">
@@ -3843,20 +3843,20 @@
       <c r="G41" s="27">
         <v>10.58</v>
       </c>
-      <c r="H41" s="217">
+      <c r="H41" s="218">
         <f>SUM(G41:G45)</f>
         <v>18.649999999999999</v>
       </c>
-      <c r="I41" s="217">
+      <c r="I41" s="218">
         <v>0.25</v>
       </c>
-      <c r="J41" s="217">
+      <c r="J41" s="218">
         <f>H41+I41</f>
         <v>18.899999999999999</v>
       </c>
     </row>
     <row r="42" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C42" s="216"/>
+      <c r="C42" s="217"/>
       <c r="D42" s="149" t="s">
         <v>150</v>
       </c>
@@ -3869,12 +3869,12 @@
       <c r="G42" s="27">
         <v>3.86</v>
       </c>
-      <c r="H42" s="217"/>
-      <c r="I42" s="217"/>
-      <c r="J42" s="217"/>
+      <c r="H42" s="218"/>
+      <c r="I42" s="218"/>
+      <c r="J42" s="218"/>
     </row>
     <row r="43" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C43" s="216"/>
+      <c r="C43" s="217"/>
       <c r="D43" s="149" t="s">
         <v>151</v>
       </c>
@@ -3888,12 +3888,12 @@
         <f>1.99-0.1</f>
         <v>1.89</v>
       </c>
-      <c r="H43" s="217"/>
-      <c r="I43" s="217"/>
-      <c r="J43" s="217"/>
+      <c r="H43" s="218"/>
+      <c r="I43" s="218"/>
+      <c r="J43" s="218"/>
     </row>
     <row r="44" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C44" s="216"/>
+      <c r="C44" s="217"/>
       <c r="D44" s="149" t="s">
         <v>152</v>
       </c>
@@ -3907,12 +3907,12 @@
         <f>0.99-0.05</f>
         <v>0.94</v>
       </c>
-      <c r="H44" s="217"/>
-      <c r="I44" s="217"/>
-      <c r="J44" s="217"/>
+      <c r="H44" s="218"/>
+      <c r="I44" s="218"/>
+      <c r="J44" s="218"/>
     </row>
     <row r="45" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C45" s="216"/>
+      <c r="C45" s="217"/>
       <c r="D45" s="149" t="s">
         <v>153</v>
       </c>
@@ -3926,9 +3926,9 @@
         <f>1.45-0.07</f>
         <v>1.38</v>
       </c>
-      <c r="H45" s="217"/>
-      <c r="I45" s="217"/>
-      <c r="J45" s="217"/>
+      <c r="H45" s="218"/>
+      <c r="I45" s="218"/>
+      <c r="J45" s="218"/>
     </row>
     <row r="46" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="51"/>
@@ -4017,7 +4017,7 @@
       <c r="L50" s="57"/>
     </row>
     <row r="51" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C51" s="216">
+      <c r="C51" s="217">
         <v>42986</v>
       </c>
       <c r="D51" s="149" t="s">
@@ -4032,20 +4032,20 @@
       <c r="G51" s="27">
         <v>29.95</v>
       </c>
-      <c r="H51" s="217">
+      <c r="H51" s="218">
         <f>G51+G52+G53+2.13</f>
         <v>34.380000000000003</v>
       </c>
-      <c r="I51" s="217">
+      <c r="I51" s="218">
         <v>3.03</v>
       </c>
-      <c r="J51" s="217">
+      <c r="J51" s="218">
         <f>H51+I51</f>
         <v>37.410000000000004</v>
       </c>
     </row>
     <row r="52" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C52" s="216"/>
+      <c r="C52" s="217"/>
       <c r="D52" s="149" t="s">
         <v>222</v>
       </c>
@@ -4058,12 +4058,12 @@
       <c r="G52" s="27">
         <v>0.77</v>
       </c>
-      <c r="H52" s="217"/>
-      <c r="I52" s="217"/>
-      <c r="J52" s="217"/>
+      <c r="H52" s="218"/>
+      <c r="I52" s="218"/>
+      <c r="J52" s="218"/>
     </row>
     <row r="53" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C53" s="216"/>
+      <c r="C53" s="217"/>
       <c r="D53" s="149" t="s">
         <v>223</v>
       </c>
@@ -4076,9 +4076,9 @@
       <c r="G53" s="27">
         <v>1.53</v>
       </c>
-      <c r="H53" s="217"/>
-      <c r="I53" s="217"/>
-      <c r="J53" s="217"/>
+      <c r="H53" s="218"/>
+      <c r="I53" s="218"/>
+      <c r="J53" s="218"/>
     </row>
     <row r="54" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="51"/>
@@ -4241,7 +4241,7 @@
       <c r="L62" s="57"/>
     </row>
     <row r="63" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C63" s="216">
+      <c r="C63" s="217">
         <v>43027</v>
       </c>
       <c r="D63" s="149" t="s">
@@ -4256,20 +4256,20 @@
       <c r="G63" s="27">
         <v>2.66</v>
       </c>
-      <c r="H63" s="217">
+      <c r="H63" s="218">
         <f>SUM(G63:G66)</f>
         <v>10.18</v>
       </c>
-      <c r="I63" s="217">
+      <c r="I63" s="218">
         <v>3.75</v>
       </c>
-      <c r="J63" s="217">
+      <c r="J63" s="218">
         <f>H63+I63</f>
         <v>13.93</v>
       </c>
     </row>
     <row r="64" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C64" s="216"/>
+      <c r="C64" s="217"/>
       <c r="D64" s="149" t="s">
         <v>234</v>
       </c>
@@ -4282,12 +4282,12 @@
       <c r="G64" s="27">
         <v>1.53</v>
       </c>
-      <c r="H64" s="217"/>
-      <c r="I64" s="217"/>
-      <c r="J64" s="217"/>
+      <c r="H64" s="218"/>
+      <c r="I64" s="218"/>
+      <c r="J64" s="218"/>
     </row>
     <row r="65" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C65" s="216"/>
+      <c r="C65" s="217"/>
       <c r="D65" s="149" t="s">
         <v>222</v>
       </c>
@@ -4300,12 +4300,12 @@
       <c r="G65" s="27">
         <v>0.77</v>
       </c>
-      <c r="H65" s="217"/>
-      <c r="I65" s="217"/>
-      <c r="J65" s="217"/>
+      <c r="H65" s="218"/>
+      <c r="I65" s="218"/>
+      <c r="J65" s="218"/>
     </row>
     <row r="66" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C66" s="216"/>
+      <c r="C66" s="217"/>
       <c r="D66" s="149" t="s">
         <v>235</v>
       </c>
@@ -4318,9 +4318,9 @@
       <c r="G66" s="27">
         <v>5.22</v>
       </c>
-      <c r="H66" s="217"/>
-      <c r="I66" s="217"/>
-      <c r="J66" s="217"/>
+      <c r="H66" s="218"/>
+      <c r="I66" s="218"/>
+      <c r="J66" s="218"/>
     </row>
     <row r="67" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C67" s="51"/>
@@ -4372,7 +4372,7 @@
       <c r="L69" s="57"/>
     </row>
     <row r="70" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C70" s="216">
+      <c r="C70" s="217">
         <v>43040</v>
       </c>
       <c r="D70" s="149" t="s">
@@ -4387,14 +4387,14 @@
       <c r="G70" s="27">
         <v>0.4</v>
       </c>
-      <c r="H70" s="217">
+      <c r="H70" s="218">
         <f>SUM(G70:G76)</f>
         <v>3.5799999999999996</v>
       </c>
-      <c r="I70" s="217">
+      <c r="I70" s="218">
         <v>3.39</v>
       </c>
-      <c r="J70" s="221">
+      <c r="J70" s="219">
         <f>H70+I70+K71</f>
         <v>7.2206000000000001</v>
       </c>
@@ -4403,7 +4403,7 @@
       </c>
     </row>
     <row r="71" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C71" s="216"/>
+      <c r="C71" s="217"/>
       <c r="D71" s="149" t="s">
         <v>237</v>
       </c>
@@ -4416,9 +4416,9 @@
       <c r="G71" s="27">
         <v>0.9</v>
       </c>
-      <c r="H71" s="217"/>
-      <c r="I71" s="217"/>
-      <c r="J71" s="221"/>
+      <c r="H71" s="218"/>
+      <c r="I71" s="218"/>
+      <c r="J71" s="219"/>
       <c r="K71" s="214">
         <f>SUM(G70:G76)*0.07</f>
         <v>0.25059999999999999</v>
@@ -4426,7 +4426,7 @@
       <c r="L71" s="215"/>
     </row>
     <row r="72" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C72" s="216"/>
+      <c r="C72" s="217"/>
       <c r="D72" s="149" t="s">
         <v>238</v>
       </c>
@@ -4439,12 +4439,12 @@
       <c r="G72" s="27">
         <v>0.64</v>
       </c>
-      <c r="H72" s="217"/>
-      <c r="I72" s="217"/>
-      <c r="J72" s="221"/>
+      <c r="H72" s="218"/>
+      <c r="I72" s="218"/>
+      <c r="J72" s="219"/>
     </row>
     <row r="73" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C73" s="216"/>
+      <c r="C73" s="217"/>
       <c r="D73" s="149" t="s">
         <v>239</v>
       </c>
@@ -4457,12 +4457,12 @@
       <c r="G73" s="27">
         <v>0.4</v>
       </c>
-      <c r="H73" s="217"/>
-      <c r="I73" s="217"/>
-      <c r="J73" s="221"/>
+      <c r="H73" s="218"/>
+      <c r="I73" s="218"/>
+      <c r="J73" s="219"/>
     </row>
     <row r="74" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C74" s="216"/>
+      <c r="C74" s="217"/>
       <c r="D74" s="149" t="s">
         <v>240</v>
       </c>
@@ -4475,12 +4475,12 @@
       <c r="G74" s="27">
         <v>0.32</v>
       </c>
-      <c r="H74" s="217"/>
-      <c r="I74" s="217"/>
-      <c r="J74" s="221"/>
+      <c r="H74" s="218"/>
+      <c r="I74" s="218"/>
+      <c r="J74" s="219"/>
     </row>
     <row r="75" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C75" s="216"/>
+      <c r="C75" s="217"/>
       <c r="D75" s="149" t="s">
         <v>241</v>
       </c>
@@ -4493,12 +4493,12 @@
       <c r="G75" s="27">
         <v>0.46</v>
       </c>
-      <c r="H75" s="217"/>
-      <c r="I75" s="217"/>
-      <c r="J75" s="221"/>
+      <c r="H75" s="218"/>
+      <c r="I75" s="218"/>
+      <c r="J75" s="219"/>
     </row>
     <row r="76" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C76" s="216"/>
+      <c r="C76" s="217"/>
       <c r="D76" s="149" t="s">
         <v>242</v>
       </c>
@@ -4511,9 +4511,9 @@
       <c r="G76" s="27">
         <v>0.46</v>
       </c>
-      <c r="H76" s="217"/>
-      <c r="I76" s="217"/>
-      <c r="J76" s="221"/>
+      <c r="H76" s="218"/>
+      <c r="I76" s="218"/>
+      <c r="J76" s="219"/>
     </row>
     <row r="77" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C77" s="51"/>
@@ -4523,14 +4523,14 @@
       <c r="G77" s="54"/>
       <c r="H77" s="158"/>
       <c r="I77" s="158"/>
-      <c r="J77" s="227"/>
+      <c r="J77" s="216"/>
       <c r="L77" s="57"/>
     </row>
     <row r="78" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C78" s="216">
+      <c r="C78" s="217">
         <v>43045</v>
       </c>
-      <c r="D78" s="149" t="s">
+      <c r="D78" s="202" t="s">
         <v>245</v>
       </c>
       <c r="E78" s="26">
@@ -4542,24 +4542,24 @@
       <c r="G78" s="27">
         <v>0.1</v>
       </c>
-      <c r="H78" s="217">
+      <c r="H78" s="218">
         <f>SUM(G78:G86)</f>
         <v>4.1500000000000004</v>
       </c>
-      <c r="I78" s="217">
-        <v>3.39</v>
-      </c>
-      <c r="J78" s="221">
+      <c r="I78" s="218">
+        <v>3.93</v>
+      </c>
+      <c r="J78" s="219">
         <f>H78+I78+K79</f>
-        <v>7.8305000000000007</v>
+        <v>8.3497500000000002</v>
       </c>
       <c r="K78" s="12" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="79" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C79" s="216"/>
-      <c r="D79" s="149" t="s">
+      <c r="C79" s="217"/>
+      <c r="D79" s="202" t="s">
         <v>246</v>
       </c>
       <c r="E79" s="26">
@@ -4571,17 +4571,17 @@
       <c r="G79" s="27">
         <v>0.4</v>
       </c>
-      <c r="H79" s="217"/>
-      <c r="I79" s="217"/>
-      <c r="J79" s="221"/>
+      <c r="H79" s="218"/>
+      <c r="I79" s="218"/>
+      <c r="J79" s="219"/>
       <c r="K79" s="214">
-        <f>SUM(G78:G86)*0.07</f>
-        <v>0.29050000000000004</v>
+        <f>SUM(G78:G86)*0.065</f>
+        <v>0.26975000000000005</v>
       </c>
     </row>
     <row r="80" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C80" s="216"/>
-      <c r="D80" s="149" t="s">
+      <c r="C80" s="217"/>
+      <c r="D80" s="202" t="s">
         <v>247</v>
       </c>
       <c r="E80" s="26">
@@ -4593,13 +4593,13 @@
       <c r="G80" s="27">
         <v>0.4</v>
       </c>
-      <c r="H80" s="217"/>
-      <c r="I80" s="217"/>
-      <c r="J80" s="221"/>
+      <c r="H80" s="218"/>
+      <c r="I80" s="218"/>
+      <c r="J80" s="219"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C81" s="216"/>
-      <c r="D81" s="149" t="s">
+      <c r="C81" s="217"/>
+      <c r="D81" s="202" t="s">
         <v>248</v>
       </c>
       <c r="E81" s="26">
@@ -4611,13 +4611,13 @@
       <c r="G81" s="27">
         <v>0.4</v>
       </c>
-      <c r="H81" s="217"/>
-      <c r="I81" s="217"/>
-      <c r="J81" s="221"/>
+      <c r="H81" s="218"/>
+      <c r="I81" s="218"/>
+      <c r="J81" s="219"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C82" s="216"/>
-      <c r="D82" s="149" t="s">
+      <c r="C82" s="217"/>
+      <c r="D82" s="202" t="s">
         <v>249</v>
       </c>
       <c r="E82" s="26">
@@ -4629,13 +4629,13 @@
       <c r="G82" s="27">
         <v>0.63</v>
       </c>
-      <c r="H82" s="217"/>
-      <c r="I82" s="217"/>
-      <c r="J82" s="221"/>
+      <c r="H82" s="218"/>
+      <c r="I82" s="218"/>
+      <c r="J82" s="219"/>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C83" s="216"/>
-      <c r="D83" s="149" t="s">
+      <c r="C83" s="217"/>
+      <c r="D83" s="202" t="s">
         <v>250</v>
       </c>
       <c r="E83" s="26">
@@ -4647,13 +4647,13 @@
       <c r="G83" s="27">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H83" s="217"/>
-      <c r="I83" s="217"/>
-      <c r="J83" s="221"/>
+      <c r="H83" s="218"/>
+      <c r="I83" s="218"/>
+      <c r="J83" s="219"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C84" s="216"/>
-      <c r="D84" s="149" t="s">
+      <c r="C84" s="217"/>
+      <c r="D84" s="202" t="s">
         <v>251</v>
       </c>
       <c r="E84" s="26">
@@ -4665,13 +4665,13 @@
       <c r="G84" s="27">
         <v>0.86</v>
       </c>
-      <c r="H84" s="217"/>
-      <c r="I84" s="217"/>
-      <c r="J84" s="221"/>
+      <c r="H84" s="218"/>
+      <c r="I84" s="218"/>
+      <c r="J84" s="219"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C85" s="216"/>
-      <c r="D85" s="149" t="s">
+      <c r="C85" s="217"/>
+      <c r="D85" s="202" t="s">
         <v>252</v>
       </c>
       <c r="E85" s="26">
@@ -4683,13 +4683,13 @@
       <c r="G85" s="27">
         <v>0.61</v>
       </c>
-      <c r="H85" s="217"/>
-      <c r="I85" s="217"/>
-      <c r="J85" s="221"/>
+      <c r="H85" s="218"/>
+      <c r="I85" s="218"/>
+      <c r="J85" s="219"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C86" s="216"/>
-      <c r="D86" s="149" t="s">
+      <c r="C86" s="217"/>
+      <c r="D86" s="202" t="s">
         <v>253</v>
       </c>
       <c r="E86" s="26">
@@ -4701,9 +4701,9 @@
       <c r="G86" s="27">
         <v>0.2</v>
       </c>
-      <c r="H86" s="217"/>
-      <c r="I86" s="217"/>
-      <c r="J86" s="221"/>
+      <c r="H86" s="218"/>
+      <c r="I86" s="218"/>
+      <c r="J86" s="219"/>
     </row>
     <row r="87" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C87" s="7"/>
@@ -4733,7 +4733,7 @@
       </c>
       <c r="J88" s="30">
         <f>SUM(J4:J87)</f>
-        <v>308.16110000000003</v>
+        <v>308.68034999999998</v>
       </c>
       <c r="K88" s="24" t="s">
         <v>24</v>
@@ -4758,7 +4758,7 @@
       </c>
       <c r="J89" s="22">
         <f ca="1">J88/L88</f>
-        <v>57.504521308571775</v>
+        <v>57.601416155745781</v>
       </c>
       <c r="K89" s="32" t="s">
         <v>27</v>
@@ -6191,27 +6191,19 @@
     <sortCondition ref="C4:C19"/>
   </sortState>
   <mergeCells count="50">
-    <mergeCell ref="C78:C86"/>
-    <mergeCell ref="H78:H86"/>
-    <mergeCell ref="I78:I86"/>
-    <mergeCell ref="J78:J86"/>
-    <mergeCell ref="C70:C76"/>
-    <mergeCell ref="H70:H76"/>
-    <mergeCell ref="I70:I76"/>
-    <mergeCell ref="J70:J76"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="H63:H66"/>
-    <mergeCell ref="I63:I66"/>
-    <mergeCell ref="J63:J66"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="H51:H53"/>
-    <mergeCell ref="I51:I53"/>
-    <mergeCell ref="J51:J53"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="C4:C10"/>
+    <mergeCell ref="J4:J10"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="H4:H10"/>
+    <mergeCell ref="I4:I10"/>
+    <mergeCell ref="J21:J25"/>
+    <mergeCell ref="H21:H25"/>
+    <mergeCell ref="H27:H29"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="I21:I25"/>
+    <mergeCell ref="H16:H17"/>
     <mergeCell ref="C41:C45"/>
     <mergeCell ref="H41:H45"/>
     <mergeCell ref="I41:I45"/>
@@ -6228,19 +6220,27 @@
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="H38:H39"/>
     <mergeCell ref="I38:I39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="C4:C10"/>
-    <mergeCell ref="J4:J10"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="H4:H10"/>
-    <mergeCell ref="I4:I10"/>
-    <mergeCell ref="J21:J25"/>
-    <mergeCell ref="H21:H25"/>
-    <mergeCell ref="H27:H29"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="I21:I25"/>
-    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="H63:H66"/>
+    <mergeCell ref="I63:I66"/>
+    <mergeCell ref="J63:J66"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="H51:H53"/>
+    <mergeCell ref="I51:I53"/>
+    <mergeCell ref="J51:J53"/>
+    <mergeCell ref="C78:C86"/>
+    <mergeCell ref="H78:H86"/>
+    <mergeCell ref="I78:I86"/>
+    <mergeCell ref="J78:J86"/>
+    <mergeCell ref="C70:C76"/>
+    <mergeCell ref="H70:H76"/>
+    <mergeCell ref="I70:I76"/>
+    <mergeCell ref="J70:J76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7148,21 +7148,21 @@
       <c r="AB16" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="AN16" s="222" t="s">
+      <c r="AN16" s="223" t="s">
         <v>123</v>
       </c>
-      <c r="AO16" s="222"/>
-      <c r="AP16" s="222"/>
-      <c r="AQ16" s="222"/>
-      <c r="AT16" s="219" t="s">
+      <c r="AO16" s="223"/>
+      <c r="AP16" s="223"/>
+      <c r="AQ16" s="223"/>
+      <c r="AT16" s="222" t="s">
         <v>119</v>
       </c>
-      <c r="AU16" s="219"/>
-      <c r="AV16" s="219"/>
-      <c r="AW16" s="219"/>
-      <c r="AX16" s="219"/>
-      <c r="AY16" s="219"/>
-      <c r="AZ16" s="219"/>
+      <c r="AU16" s="222"/>
+      <c r="AV16" s="222"/>
+      <c r="AW16" s="222"/>
+      <c r="AX16" s="222"/>
+      <c r="AY16" s="222"/>
+      <c r="AZ16" s="222"/>
     </row>
     <row r="17" spans="25:59" x14ac:dyDescent="0.25">
       <c r="Y17" s="108" t="s">
@@ -7177,15 +7177,15 @@
       <c r="AB17" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="AJ17" s="219" t="s">
+      <c r="AJ17" s="222" t="s">
         <v>117</v>
       </c>
-      <c r="AK17" s="219"/>
-      <c r="AL17" s="219"/>
-      <c r="AN17" s="222"/>
-      <c r="AO17" s="222"/>
-      <c r="AP17" s="222"/>
-      <c r="AQ17" s="222"/>
+      <c r="AK17" s="222"/>
+      <c r="AL17" s="222"/>
+      <c r="AN17" s="223"/>
+      <c r="AO17" s="223"/>
+      <c r="AP17" s="223"/>
+      <c r="AQ17" s="223"/>
     </row>
     <row r="19" spans="25:59" x14ac:dyDescent="0.25">
       <c r="AP19" s="195" t="s">
@@ -7200,11 +7200,11 @@
       </c>
     </row>
     <row r="20" spans="25:59" x14ac:dyDescent="0.25">
-      <c r="AK20" s="223" t="s">
+      <c r="AK20" s="224" t="s">
         <v>120</v>
       </c>
-      <c r="AL20" s="223"/>
-      <c r="AM20" s="223"/>
+      <c r="AL20" s="224"/>
+      <c r="AM20" s="224"/>
       <c r="AP20" s="195" t="s">
         <v>217</v>
       </c>
@@ -7499,7 +7499,7 @@
         <f t="shared" si="1"/>
         <v>6.6300000000000008</v>
       </c>
-      <c r="H11" s="224">
+      <c r="H11" s="225">
         <v>3.39</v>
       </c>
       <c r="I11" s="172" t="s">
@@ -7529,7 +7529,7 @@
         <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
-      <c r="H12" s="224"/>
+      <c r="H12" s="225"/>
       <c r="I12" s="172" t="s">
         <v>186</v>
       </c>
@@ -7585,7 +7585,7 @@
         <f t="shared" si="1"/>
         <v>57.199999999999996</v>
       </c>
-      <c r="H14" s="225">
+      <c r="H14" s="226">
         <v>4.99</v>
       </c>
       <c r="I14" s="172" t="s">
@@ -7614,7 +7614,7 @@
         <f t="shared" si="1"/>
         <v>28.3</v>
       </c>
-      <c r="H15" s="226"/>
+      <c r="H15" s="227"/>
       <c r="I15" s="182" t="s">
         <v>228</v>
       </c>

</xml_diff>

<commit_message>
Controlling a digital volume control with the menu... SUCCESSFULLY!
TODO-- IMPLEMENT WITH MICRO SD
TODO-- FINISH IMPLEMENTING WITH THE REMAINING TASKS (MS5611, BLE, FLITER, etc...)
</commit_message>
<xml_diff>
--- a/BillOfMaterials/INVENTORY.xlsx
+++ b/BillOfMaterials/INVENTORY.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INVENTORY" sheetId="1" r:id="rId1"/>
@@ -2446,22 +2446,22 @@
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2999,7 +2999,7 @@
   </sheetPr>
   <dimension ref="A1:AB209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
     </sheetView>
@@ -3088,7 +3088,7 @@
       <c r="L3" s="35"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C4" s="217">
+      <c r="C4" s="218">
         <v>42882</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -3103,26 +3103,26 @@
       <c r="G4" s="27">
         <v>6.99</v>
       </c>
-      <c r="H4" s="221">
+      <c r="H4" s="219">
         <f>SUM(G4:G10)</f>
         <v>48.1</v>
       </c>
-      <c r="I4" s="218">
+      <c r="I4" s="217">
         <v>0</v>
       </c>
-      <c r="J4" s="221">
+      <c r="J4" s="219">
         <f>H4+I4</f>
         <v>48.1</v>
       </c>
-      <c r="K4" s="220">
+      <c r="K4" s="221">
         <f>G4/E4</f>
         <v>6.99</v>
       </c>
-      <c r="L4" s="220"/>
-      <c r="M4" s="220"/>
+      <c r="L4" s="221"/>
+      <c r="M4" s="221"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C5" s="217"/>
+      <c r="C5" s="218"/>
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
@@ -3135,18 +3135,18 @@
       <c r="G5" s="27">
         <v>6.99</v>
       </c>
-      <c r="H5" s="222"/>
-      <c r="I5" s="218"/>
-      <c r="J5" s="222"/>
-      <c r="K5" s="220">
+      <c r="H5" s="220"/>
+      <c r="I5" s="217"/>
+      <c r="J5" s="220"/>
+      <c r="K5" s="221">
         <f t="shared" ref="K5:K10" si="0">G5/E5</f>
         <v>6.99</v>
       </c>
-      <c r="L5" s="220"/>
-      <c r="M5" s="220"/>
+      <c r="L5" s="221"/>
+      <c r="M5" s="221"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C6" s="217"/>
+      <c r="C6" s="218"/>
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
@@ -3159,18 +3159,18 @@
       <c r="G6" s="27">
         <v>4.97</v>
       </c>
-      <c r="H6" s="222"/>
-      <c r="I6" s="218"/>
-      <c r="J6" s="222"/>
-      <c r="K6" s="220">
+      <c r="H6" s="220"/>
+      <c r="I6" s="217"/>
+      <c r="J6" s="220"/>
+      <c r="K6" s="221">
         <f t="shared" si="0"/>
         <v>0.2485</v>
       </c>
-      <c r="L6" s="220"/>
-      <c r="M6" s="220"/>
+      <c r="L6" s="221"/>
+      <c r="M6" s="221"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C7" s="217"/>
+      <c r="C7" s="218"/>
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
@@ -3183,18 +3183,18 @@
       <c r="G7" s="27">
         <v>5.99</v>
       </c>
-      <c r="H7" s="222"/>
-      <c r="I7" s="218"/>
-      <c r="J7" s="222"/>
-      <c r="K7" s="220">
+      <c r="H7" s="220"/>
+      <c r="I7" s="217"/>
+      <c r="J7" s="220"/>
+      <c r="K7" s="221">
         <f t="shared" si="0"/>
         <v>0.29949999999999999</v>
       </c>
-      <c r="L7" s="220"/>
-      <c r="M7" s="220"/>
+      <c r="L7" s="221"/>
+      <c r="M7" s="221"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C8" s="217"/>
+      <c r="C8" s="218"/>
       <c r="D8" s="1" t="s">
         <v>155</v>
       </c>
@@ -3207,18 +3207,18 @@
       <c r="G8" s="27">
         <v>6.25</v>
       </c>
-      <c r="H8" s="222"/>
-      <c r="I8" s="218"/>
-      <c r="J8" s="222"/>
-      <c r="K8" s="220">
+      <c r="H8" s="220"/>
+      <c r="I8" s="217"/>
+      <c r="J8" s="220"/>
+      <c r="K8" s="221">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
-      <c r="L8" s="220"/>
-      <c r="M8" s="220"/>
+      <c r="L8" s="221"/>
+      <c r="M8" s="221"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C9" s="217"/>
+      <c r="C9" s="218"/>
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3231,18 +3231,18 @@
       <c r="G9" s="27">
         <v>11.59</v>
       </c>
-      <c r="H9" s="222"/>
-      <c r="I9" s="218"/>
-      <c r="J9" s="222"/>
-      <c r="K9" s="220">
+      <c r="H9" s="220"/>
+      <c r="I9" s="217"/>
+      <c r="J9" s="220"/>
+      <c r="K9" s="221">
         <f t="shared" si="0"/>
         <v>0.57950000000000002</v>
       </c>
-      <c r="L9" s="220"/>
-      <c r="M9" s="220"/>
+      <c r="L9" s="221"/>
+      <c r="M9" s="221"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C10" s="217"/>
+      <c r="C10" s="218"/>
       <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
@@ -3255,15 +3255,15 @@
       <c r="G10" s="27">
         <v>5.32</v>
       </c>
-      <c r="H10" s="222"/>
-      <c r="I10" s="218"/>
-      <c r="J10" s="222"/>
-      <c r="K10" s="220">
+      <c r="H10" s="220"/>
+      <c r="I10" s="217"/>
+      <c r="J10" s="220"/>
+      <c r="K10" s="221">
         <f t="shared" si="0"/>
         <v>1.0640000000000001</v>
       </c>
-      <c r="L10" s="220"/>
-      <c r="M10" s="220"/>
+      <c r="L10" s="221"/>
+      <c r="M10" s="221"/>
     </row>
     <row r="11" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C11" s="7"/>
@@ -3370,14 +3370,14 @@
       <c r="G16" s="27">
         <v>6.56</v>
       </c>
-      <c r="H16" s="221">
+      <c r="H16" s="219">
         <f>SUM(G16:G17)</f>
         <v>7.55</v>
       </c>
-      <c r="I16" s="218">
+      <c r="I16" s="217">
         <v>0</v>
       </c>
-      <c r="J16" s="221">
+      <c r="J16" s="219">
         <f>H16+I16</f>
         <v>7.55</v>
       </c>
@@ -3398,9 +3398,9 @@
       <c r="G17" s="27">
         <v>0.99</v>
       </c>
-      <c r="H17" s="221"/>
-      <c r="I17" s="218"/>
-      <c r="J17" s="221"/>
+      <c r="H17" s="219"/>
+      <c r="I17" s="217"/>
+      <c r="J17" s="219"/>
     </row>
     <row r="18" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
@@ -3452,7 +3452,7 @@
       <c r="L20" s="35"/>
     </row>
     <row r="21" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C21" s="217">
+      <c r="C21" s="218">
         <v>42925</v>
       </c>
       <c r="D21" s="149" t="s">
@@ -3467,20 +3467,20 @@
       <c r="G21" s="27">
         <v>2.56</v>
       </c>
-      <c r="H21" s="221">
+      <c r="H21" s="219">
         <f>SUM(G21:G25)</f>
         <v>17.230000000000004</v>
       </c>
-      <c r="I21" s="218">
+      <c r="I21" s="217">
         <v>5.65</v>
       </c>
-      <c r="J21" s="221">
+      <c r="J21" s="219">
         <f>H21+I21</f>
         <v>22.880000000000003</v>
       </c>
     </row>
     <row r="22" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C22" s="217"/>
+      <c r="C22" s="218"/>
       <c r="D22" s="149" t="s">
         <v>21</v>
       </c>
@@ -3493,12 +3493,12 @@
       <c r="G22" s="27">
         <v>1.8</v>
       </c>
-      <c r="H22" s="222"/>
-      <c r="I22" s="218"/>
-      <c r="J22" s="222"/>
+      <c r="H22" s="220"/>
+      <c r="I22" s="217"/>
+      <c r="J22" s="220"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C23" s="217"/>
+      <c r="C23" s="218"/>
       <c r="D23" s="1" t="s">
         <v>20</v>
       </c>
@@ -3511,12 +3511,12 @@
       <c r="G23" s="27">
         <v>3.99</v>
       </c>
-      <c r="H23" s="222"/>
-      <c r="I23" s="218"/>
-      <c r="J23" s="222"/>
+      <c r="H23" s="220"/>
+      <c r="I23" s="217"/>
+      <c r="J23" s="220"/>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C24" s="217"/>
+      <c r="C24" s="218"/>
       <c r="D24" s="149" t="s">
         <v>13</v>
       </c>
@@ -3529,12 +3529,12 @@
       <c r="G24" s="27">
         <v>1.97</v>
       </c>
-      <c r="H24" s="222"/>
-      <c r="I24" s="218"/>
-      <c r="J24" s="222"/>
+      <c r="H24" s="220"/>
+      <c r="I24" s="217"/>
+      <c r="J24" s="220"/>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C25" s="217"/>
+      <c r="C25" s="218"/>
       <c r="D25" s="1" t="s">
         <v>2</v>
       </c>
@@ -3547,9 +3547,9 @@
       <c r="G25" s="27">
         <v>6.91</v>
       </c>
-      <c r="H25" s="222"/>
-      <c r="I25" s="218"/>
-      <c r="J25" s="222"/>
+      <c r="H25" s="220"/>
+      <c r="I25" s="217"/>
+      <c r="J25" s="220"/>
     </row>
     <row r="26" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
@@ -3563,7 +3563,7 @@
       <c r="L26" s="35"/>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C27" s="217">
+      <c r="C27" s="218">
         <v>42927</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -3578,20 +3578,20 @@
       <c r="G27" s="27">
         <v>0.75</v>
       </c>
-      <c r="H27" s="221">
+      <c r="H27" s="219">
         <f>SUM(G27:G29)</f>
         <v>3.44</v>
       </c>
-      <c r="I27" s="218">
+      <c r="I27" s="217">
         <v>4.99</v>
       </c>
-      <c r="J27" s="221">
+      <c r="J27" s="219">
         <f>H27+I27</f>
         <v>8.43</v>
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C28" s="217"/>
+      <c r="C28" s="218"/>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
@@ -3604,12 +3604,12 @@
       <c r="G28" s="27">
         <v>0.75</v>
       </c>
-      <c r="H28" s="222"/>
-      <c r="I28" s="218"/>
-      <c r="J28" s="222"/>
+      <c r="H28" s="220"/>
+      <c r="I28" s="217"/>
+      <c r="J28" s="220"/>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C29" s="217"/>
+      <c r="C29" s="218"/>
       <c r="D29" s="1" t="s">
         <v>154</v>
       </c>
@@ -3622,9 +3622,9 @@
       <c r="G29" s="27">
         <v>1.94</v>
       </c>
-      <c r="H29" s="222"/>
-      <c r="I29" s="218"/>
-      <c r="J29" s="222"/>
+      <c r="H29" s="220"/>
+      <c r="I29" s="217"/>
+      <c r="J29" s="220"/>
     </row>
     <row r="30" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="7"/>
@@ -3676,7 +3676,7 @@
       <c r="L32" s="35"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C33" s="217">
+      <c r="C33" s="218">
         <v>42929</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -3691,20 +3691,20 @@
       <c r="G33" s="27">
         <v>0.77</v>
       </c>
-      <c r="H33" s="221">
+      <c r="H33" s="219">
         <f>SUM(G33:G34)</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="I33" s="218">
+      <c r="I33" s="217">
         <v>3.39</v>
       </c>
-      <c r="J33" s="218">
+      <c r="J33" s="217">
         <f>SUM(H33:I34)</f>
         <v>5.6899999999999995</v>
       </c>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C34" s="217"/>
+      <c r="C34" s="218"/>
       <c r="D34" s="1" t="s">
         <v>76</v>
       </c>
@@ -3717,9 +3717,9 @@
       <c r="G34" s="27">
         <v>1.53</v>
       </c>
-      <c r="H34" s="222"/>
-      <c r="I34" s="218"/>
-      <c r="J34" s="218"/>
+      <c r="H34" s="220"/>
+      <c r="I34" s="217"/>
+      <c r="J34" s="217"/>
     </row>
     <row r="35" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="7"/>
@@ -3771,7 +3771,7 @@
       <c r="L37" s="35"/>
     </row>
     <row r="38" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C38" s="217">
+      <c r="C38" s="218">
         <v>42931</v>
       </c>
       <c r="D38" s="149" t="s">
@@ -3786,20 +3786,20 @@
       <c r="G38" s="27">
         <v>5.72</v>
       </c>
-      <c r="H38" s="218">
+      <c r="H38" s="217">
         <f>SUM(G38:G39)</f>
         <v>8.5500000000000007</v>
       </c>
-      <c r="I38" s="218">
+      <c r="I38" s="217">
         <v>4.99</v>
       </c>
-      <c r="J38" s="218">
+      <c r="J38" s="217">
         <f>SUM(H38:I39)</f>
         <v>13.540000000000001</v>
       </c>
     </row>
     <row r="39" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C39" s="217"/>
+      <c r="C39" s="218"/>
       <c r="D39" s="149" t="s">
         <v>122</v>
       </c>
@@ -3812,9 +3812,9 @@
       <c r="G39" s="27">
         <v>2.83</v>
       </c>
-      <c r="H39" s="218"/>
-      <c r="I39" s="218"/>
-      <c r="J39" s="218"/>
+      <c r="H39" s="217"/>
+      <c r="I39" s="217"/>
+      <c r="J39" s="217"/>
     </row>
     <row r="40" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="7"/>
@@ -3828,7 +3828,7 @@
       <c r="L40" s="35"/>
     </row>
     <row r="41" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C41" s="217">
+      <c r="C41" s="218">
         <v>42936</v>
       </c>
       <c r="D41" s="149" t="s">
@@ -3843,20 +3843,20 @@
       <c r="G41" s="27">
         <v>10.58</v>
       </c>
-      <c r="H41" s="218">
+      <c r="H41" s="217">
         <f>SUM(G41:G45)</f>
         <v>18.649999999999999</v>
       </c>
-      <c r="I41" s="218">
+      <c r="I41" s="217">
         <v>0.25</v>
       </c>
-      <c r="J41" s="218">
+      <c r="J41" s="217">
         <f>H41+I41</f>
         <v>18.899999999999999</v>
       </c>
     </row>
     <row r="42" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C42" s="217"/>
+      <c r="C42" s="218"/>
       <c r="D42" s="149" t="s">
         <v>150</v>
       </c>
@@ -3869,12 +3869,12 @@
       <c r="G42" s="27">
         <v>3.86</v>
       </c>
-      <c r="H42" s="218"/>
-      <c r="I42" s="218"/>
-      <c r="J42" s="218"/>
+      <c r="H42" s="217"/>
+      <c r="I42" s="217"/>
+      <c r="J42" s="217"/>
     </row>
     <row r="43" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C43" s="217"/>
+      <c r="C43" s="218"/>
       <c r="D43" s="149" t="s">
         <v>151</v>
       </c>
@@ -3888,12 +3888,12 @@
         <f>1.99-0.1</f>
         <v>1.89</v>
       </c>
-      <c r="H43" s="218"/>
-      <c r="I43" s="218"/>
-      <c r="J43" s="218"/>
+      <c r="H43" s="217"/>
+      <c r="I43" s="217"/>
+      <c r="J43" s="217"/>
     </row>
     <row r="44" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C44" s="217"/>
+      <c r="C44" s="218"/>
       <c r="D44" s="149" t="s">
         <v>152</v>
       </c>
@@ -3907,12 +3907,12 @@
         <f>0.99-0.05</f>
         <v>0.94</v>
       </c>
-      <c r="H44" s="218"/>
-      <c r="I44" s="218"/>
-      <c r="J44" s="218"/>
+      <c r="H44" s="217"/>
+      <c r="I44" s="217"/>
+      <c r="J44" s="217"/>
     </row>
     <row r="45" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C45" s="217"/>
+      <c r="C45" s="218"/>
       <c r="D45" s="149" t="s">
         <v>153</v>
       </c>
@@ -3926,9 +3926,9 @@
         <f>1.45-0.07</f>
         <v>1.38</v>
       </c>
-      <c r="H45" s="218"/>
-      <c r="I45" s="218"/>
-      <c r="J45" s="218"/>
+      <c r="H45" s="217"/>
+      <c r="I45" s="217"/>
+      <c r="J45" s="217"/>
     </row>
     <row r="46" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="51"/>
@@ -4017,7 +4017,7 @@
       <c r="L50" s="57"/>
     </row>
     <row r="51" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C51" s="217">
+      <c r="C51" s="218">
         <v>42986</v>
       </c>
       <c r="D51" s="149" t="s">
@@ -4032,20 +4032,20 @@
       <c r="G51" s="27">
         <v>29.95</v>
       </c>
-      <c r="H51" s="218">
+      <c r="H51" s="217">
         <f>G51+G52+G53+2.13</f>
         <v>34.380000000000003</v>
       </c>
-      <c r="I51" s="218">
+      <c r="I51" s="217">
         <v>3.03</v>
       </c>
-      <c r="J51" s="218">
+      <c r="J51" s="217">
         <f>H51+I51</f>
         <v>37.410000000000004</v>
       </c>
     </row>
     <row r="52" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C52" s="217"/>
+      <c r="C52" s="218"/>
       <c r="D52" s="149" t="s">
         <v>222</v>
       </c>
@@ -4058,12 +4058,12 @@
       <c r="G52" s="27">
         <v>0.77</v>
       </c>
-      <c r="H52" s="218"/>
-      <c r="I52" s="218"/>
-      <c r="J52" s="218"/>
+      <c r="H52" s="217"/>
+      <c r="I52" s="217"/>
+      <c r="J52" s="217"/>
     </row>
     <row r="53" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C53" s="217"/>
+      <c r="C53" s="218"/>
       <c r="D53" s="149" t="s">
         <v>223</v>
       </c>
@@ -4076,9 +4076,9 @@
       <c r="G53" s="27">
         <v>1.53</v>
       </c>
-      <c r="H53" s="218"/>
-      <c r="I53" s="218"/>
-      <c r="J53" s="218"/>
+      <c r="H53" s="217"/>
+      <c r="I53" s="217"/>
+      <c r="J53" s="217"/>
     </row>
     <row r="54" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="51"/>
@@ -4241,7 +4241,7 @@
       <c r="L62" s="57"/>
     </row>
     <row r="63" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C63" s="217">
+      <c r="C63" s="218">
         <v>43027</v>
       </c>
       <c r="D63" s="149" t="s">
@@ -4256,20 +4256,20 @@
       <c r="G63" s="27">
         <v>2.66</v>
       </c>
-      <c r="H63" s="218">
+      <c r="H63" s="217">
         <f>SUM(G63:G66)</f>
         <v>10.18</v>
       </c>
-      <c r="I63" s="218">
+      <c r="I63" s="217">
         <v>3.75</v>
       </c>
-      <c r="J63" s="218">
+      <c r="J63" s="217">
         <f>H63+I63</f>
         <v>13.93</v>
       </c>
     </row>
     <row r="64" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C64" s="217"/>
+      <c r="C64" s="218"/>
       <c r="D64" s="149" t="s">
         <v>234</v>
       </c>
@@ -4282,12 +4282,12 @@
       <c r="G64" s="27">
         <v>1.53</v>
       </c>
-      <c r="H64" s="218"/>
-      <c r="I64" s="218"/>
-      <c r="J64" s="218"/>
+      <c r="H64" s="217"/>
+      <c r="I64" s="217"/>
+      <c r="J64" s="217"/>
     </row>
     <row r="65" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C65" s="217"/>
+      <c r="C65" s="218"/>
       <c r="D65" s="149" t="s">
         <v>222</v>
       </c>
@@ -4300,12 +4300,12 @@
       <c r="G65" s="27">
         <v>0.77</v>
       </c>
-      <c r="H65" s="218"/>
-      <c r="I65" s="218"/>
-      <c r="J65" s="218"/>
+      <c r="H65" s="217"/>
+      <c r="I65" s="217"/>
+      <c r="J65" s="217"/>
     </row>
     <row r="66" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C66" s="217"/>
+      <c r="C66" s="218"/>
       <c r="D66" s="149" t="s">
         <v>235</v>
       </c>
@@ -4318,9 +4318,9 @@
       <c r="G66" s="27">
         <v>5.22</v>
       </c>
-      <c r="H66" s="218"/>
-      <c r="I66" s="218"/>
-      <c r="J66" s="218"/>
+      <c r="H66" s="217"/>
+      <c r="I66" s="217"/>
+      <c r="J66" s="217"/>
     </row>
     <row r="67" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C67" s="51"/>
@@ -4372,7 +4372,7 @@
       <c r="L69" s="57"/>
     </row>
     <row r="70" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C70" s="217">
+      <c r="C70" s="218">
         <v>43040</v>
       </c>
       <c r="D70" s="149" t="s">
@@ -4387,14 +4387,14 @@
       <c r="G70" s="27">
         <v>0.4</v>
       </c>
-      <c r="H70" s="218">
+      <c r="H70" s="217">
         <f>SUM(G70:G76)</f>
         <v>3.5799999999999996</v>
       </c>
-      <c r="I70" s="218">
+      <c r="I70" s="217">
         <v>3.39</v>
       </c>
-      <c r="J70" s="219">
+      <c r="J70" s="222">
         <f>H70+I70+K71</f>
         <v>7.2206000000000001</v>
       </c>
@@ -4403,7 +4403,7 @@
       </c>
     </row>
     <row r="71" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C71" s="217"/>
+      <c r="C71" s="218"/>
       <c r="D71" s="149" t="s">
         <v>237</v>
       </c>
@@ -4416,9 +4416,9 @@
       <c r="G71" s="27">
         <v>0.9</v>
       </c>
-      <c r="H71" s="218"/>
-      <c r="I71" s="218"/>
-      <c r="J71" s="219"/>
+      <c r="H71" s="217"/>
+      <c r="I71" s="217"/>
+      <c r="J71" s="222"/>
       <c r="K71" s="214">
         <f>SUM(G70:G76)*0.07</f>
         <v>0.25059999999999999</v>
@@ -4426,7 +4426,7 @@
       <c r="L71" s="215"/>
     </row>
     <row r="72" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C72" s="217"/>
+      <c r="C72" s="218"/>
       <c r="D72" s="149" t="s">
         <v>238</v>
       </c>
@@ -4439,12 +4439,12 @@
       <c r="G72" s="27">
         <v>0.64</v>
       </c>
-      <c r="H72" s="218"/>
-      <c r="I72" s="218"/>
-      <c r="J72" s="219"/>
+      <c r="H72" s="217"/>
+      <c r="I72" s="217"/>
+      <c r="J72" s="222"/>
     </row>
     <row r="73" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C73" s="217"/>
+      <c r="C73" s="218"/>
       <c r="D73" s="149" t="s">
         <v>239</v>
       </c>
@@ -4457,12 +4457,12 @@
       <c r="G73" s="27">
         <v>0.4</v>
       </c>
-      <c r="H73" s="218"/>
-      <c r="I73" s="218"/>
-      <c r="J73" s="219"/>
+      <c r="H73" s="217"/>
+      <c r="I73" s="217"/>
+      <c r="J73" s="222"/>
     </row>
     <row r="74" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C74" s="217"/>
+      <c r="C74" s="218"/>
       <c r="D74" s="149" t="s">
         <v>240</v>
       </c>
@@ -4475,12 +4475,12 @@
       <c r="G74" s="27">
         <v>0.32</v>
       </c>
-      <c r="H74" s="218"/>
-      <c r="I74" s="218"/>
-      <c r="J74" s="219"/>
+      <c r="H74" s="217"/>
+      <c r="I74" s="217"/>
+      <c r="J74" s="222"/>
     </row>
     <row r="75" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C75" s="217"/>
+      <c r="C75" s="218"/>
       <c r="D75" s="149" t="s">
         <v>241</v>
       </c>
@@ -4493,12 +4493,12 @@
       <c r="G75" s="27">
         <v>0.46</v>
       </c>
-      <c r="H75" s="218"/>
-      <c r="I75" s="218"/>
-      <c r="J75" s="219"/>
+      <c r="H75" s="217"/>
+      <c r="I75" s="217"/>
+      <c r="J75" s="222"/>
     </row>
     <row r="76" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C76" s="217"/>
+      <c r="C76" s="218"/>
       <c r="D76" s="149" t="s">
         <v>242</v>
       </c>
@@ -4511,9 +4511,9 @@
       <c r="G76" s="27">
         <v>0.46</v>
       </c>
-      <c r="H76" s="218"/>
-      <c r="I76" s="218"/>
-      <c r="J76" s="219"/>
+      <c r="H76" s="217"/>
+      <c r="I76" s="217"/>
+      <c r="J76" s="222"/>
     </row>
     <row r="77" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C77" s="51"/>
@@ -4527,7 +4527,7 @@
       <c r="L77" s="57"/>
     </row>
     <row r="78" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C78" s="217">
+      <c r="C78" s="218">
         <v>43045</v>
       </c>
       <c r="D78" s="202" t="s">
@@ -4542,14 +4542,14 @@
       <c r="G78" s="27">
         <v>0.1</v>
       </c>
-      <c r="H78" s="218">
+      <c r="H78" s="217">
         <f>SUM(G78:G86)</f>
         <v>4.1500000000000004</v>
       </c>
-      <c r="I78" s="218">
+      <c r="I78" s="217">
         <v>3.93</v>
       </c>
-      <c r="J78" s="219">
+      <c r="J78" s="222">
         <f>H78+I78+K79</f>
         <v>8.3497500000000002</v>
       </c>
@@ -4558,7 +4558,7 @@
       </c>
     </row>
     <row r="79" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C79" s="217"/>
+      <c r="C79" s="218"/>
       <c r="D79" s="202" t="s">
         <v>246</v>
       </c>
@@ -4571,16 +4571,16 @@
       <c r="G79" s="27">
         <v>0.4</v>
       </c>
-      <c r="H79" s="218"/>
-      <c r="I79" s="218"/>
-      <c r="J79" s="219"/>
+      <c r="H79" s="217"/>
+      <c r="I79" s="217"/>
+      <c r="J79" s="222"/>
       <c r="K79" s="214">
         <f>SUM(G78:G86)*0.065</f>
         <v>0.26975000000000005</v>
       </c>
     </row>
     <row r="80" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C80" s="217"/>
+      <c r="C80" s="218"/>
       <c r="D80" s="202" t="s">
         <v>247</v>
       </c>
@@ -4593,12 +4593,12 @@
       <c r="G80" s="27">
         <v>0.4</v>
       </c>
-      <c r="H80" s="218"/>
-      <c r="I80" s="218"/>
-      <c r="J80" s="219"/>
+      <c r="H80" s="217"/>
+      <c r="I80" s="217"/>
+      <c r="J80" s="222"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C81" s="217"/>
+      <c r="C81" s="218"/>
       <c r="D81" s="202" t="s">
         <v>248</v>
       </c>
@@ -4611,12 +4611,12 @@
       <c r="G81" s="27">
         <v>0.4</v>
       </c>
-      <c r="H81" s="218"/>
-      <c r="I81" s="218"/>
-      <c r="J81" s="219"/>
+      <c r="H81" s="217"/>
+      <c r="I81" s="217"/>
+      <c r="J81" s="222"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C82" s="217"/>
+      <c r="C82" s="218"/>
       <c r="D82" s="202" t="s">
         <v>249</v>
       </c>
@@ -4629,12 +4629,12 @@
       <c r="G82" s="27">
         <v>0.63</v>
       </c>
-      <c r="H82" s="218"/>
-      <c r="I82" s="218"/>
-      <c r="J82" s="219"/>
+      <c r="H82" s="217"/>
+      <c r="I82" s="217"/>
+      <c r="J82" s="222"/>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C83" s="217"/>
+      <c r="C83" s="218"/>
       <c r="D83" s="202" t="s">
         <v>250</v>
       </c>
@@ -4647,12 +4647,12 @@
       <c r="G83" s="27">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H83" s="218"/>
-      <c r="I83" s="218"/>
-      <c r="J83" s="219"/>
+      <c r="H83" s="217"/>
+      <c r="I83" s="217"/>
+      <c r="J83" s="222"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C84" s="217"/>
+      <c r="C84" s="218"/>
       <c r="D84" s="202" t="s">
         <v>251</v>
       </c>
@@ -4665,12 +4665,12 @@
       <c r="G84" s="27">
         <v>0.86</v>
       </c>
-      <c r="H84" s="218"/>
-      <c r="I84" s="218"/>
-      <c r="J84" s="219"/>
+      <c r="H84" s="217"/>
+      <c r="I84" s="217"/>
+      <c r="J84" s="222"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C85" s="217"/>
+      <c r="C85" s="218"/>
       <c r="D85" s="202" t="s">
         <v>252</v>
       </c>
@@ -4683,12 +4683,12 @@
       <c r="G85" s="27">
         <v>0.61</v>
       </c>
-      <c r="H85" s="218"/>
-      <c r="I85" s="218"/>
-      <c r="J85" s="219"/>
+      <c r="H85" s="217"/>
+      <c r="I85" s="217"/>
+      <c r="J85" s="222"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C86" s="217"/>
+      <c r="C86" s="218"/>
       <c r="D86" s="202" t="s">
         <v>253</v>
       </c>
@@ -4701,9 +4701,9 @@
       <c r="G86" s="27">
         <v>0.2</v>
       </c>
-      <c r="H86" s="218"/>
-      <c r="I86" s="218"/>
-      <c r="J86" s="219"/>
+      <c r="H86" s="217"/>
+      <c r="I86" s="217"/>
+      <c r="J86" s="222"/>
     </row>
     <row r="87" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C87" s="7"/>
@@ -4722,7 +4722,7 @@
       </c>
       <c r="C88" s="41">
         <f ca="1">TODAY()</f>
-        <v>43045</v>
+        <v>43050</v>
       </c>
       <c r="E88" s="29"/>
       <c r="F88" s="29"/>
@@ -4740,7 +4740,7 @@
       </c>
       <c r="L88" s="39">
         <f ca="1">(C88-C4)*0.0328767</f>
-        <v>5.3589020999999999</v>
+        <v>5.5232856000000004</v>
       </c>
       <c r="M88" s="24" t="s">
         <v>25</v>
@@ -4758,7 +4758,7 @@
       </c>
       <c r="J89" s="22">
         <f ca="1">J88/L88</f>
-        <v>57.601416155745781</v>
+        <v>55.887088293967629</v>
       </c>
       <c r="K89" s="32" t="s">
         <v>27</v>
@@ -6191,19 +6191,27 @@
     <sortCondition ref="C4:C19"/>
   </sortState>
   <mergeCells count="50">
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="C4:C10"/>
-    <mergeCell ref="J4:J10"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="H4:H10"/>
-    <mergeCell ref="I4:I10"/>
-    <mergeCell ref="J21:J25"/>
-    <mergeCell ref="H21:H25"/>
-    <mergeCell ref="H27:H29"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="I21:I25"/>
-    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="C78:C86"/>
+    <mergeCell ref="H78:H86"/>
+    <mergeCell ref="I78:I86"/>
+    <mergeCell ref="J78:J86"/>
+    <mergeCell ref="C70:C76"/>
+    <mergeCell ref="H70:H76"/>
+    <mergeCell ref="I70:I76"/>
+    <mergeCell ref="J70:J76"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="H63:H66"/>
+    <mergeCell ref="I63:I66"/>
+    <mergeCell ref="J63:J66"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="H51:H53"/>
+    <mergeCell ref="I51:I53"/>
+    <mergeCell ref="J51:J53"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
     <mergeCell ref="C41:C45"/>
     <mergeCell ref="H41:H45"/>
     <mergeCell ref="I41:I45"/>
@@ -6220,27 +6228,19 @@
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="H38:H39"/>
     <mergeCell ref="I38:I39"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="H63:H66"/>
-    <mergeCell ref="I63:I66"/>
-    <mergeCell ref="J63:J66"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="H51:H53"/>
-    <mergeCell ref="I51:I53"/>
-    <mergeCell ref="J51:J53"/>
-    <mergeCell ref="C78:C86"/>
-    <mergeCell ref="H78:H86"/>
-    <mergeCell ref="I78:I86"/>
-    <mergeCell ref="J78:J86"/>
-    <mergeCell ref="C70:C76"/>
-    <mergeCell ref="H70:H76"/>
-    <mergeCell ref="I70:I76"/>
-    <mergeCell ref="J70:J76"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="C4:C10"/>
+    <mergeCell ref="J4:J10"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="H4:H10"/>
+    <mergeCell ref="I4:I10"/>
+    <mergeCell ref="J21:J25"/>
+    <mergeCell ref="H21:H25"/>
+    <mergeCell ref="H27:H29"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="I21:I25"/>
+    <mergeCell ref="H16:H17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6257,7 +6257,7 @@
   </sheetPr>
   <dimension ref="B3:BG20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -7154,15 +7154,15 @@
       <c r="AO16" s="223"/>
       <c r="AP16" s="223"/>
       <c r="AQ16" s="223"/>
-      <c r="AT16" s="222" t="s">
+      <c r="AT16" s="220" t="s">
         <v>119</v>
       </c>
-      <c r="AU16" s="222"/>
-      <c r="AV16" s="222"/>
-      <c r="AW16" s="222"/>
-      <c r="AX16" s="222"/>
-      <c r="AY16" s="222"/>
-      <c r="AZ16" s="222"/>
+      <c r="AU16" s="220"/>
+      <c r="AV16" s="220"/>
+      <c r="AW16" s="220"/>
+      <c r="AX16" s="220"/>
+      <c r="AY16" s="220"/>
+      <c r="AZ16" s="220"/>
     </row>
     <row r="17" spans="25:59" x14ac:dyDescent="0.25">
       <c r="Y17" s="108" t="s">
@@ -7177,11 +7177,11 @@
       <c r="AB17" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="AJ17" s="222" t="s">
+      <c r="AJ17" s="220" t="s">
         <v>117</v>
       </c>
-      <c r="AK17" s="222"/>
-      <c r="AL17" s="222"/>
+      <c r="AK17" s="220"/>
+      <c r="AL17" s="220"/>
       <c r="AN17" s="223"/>
       <c r="AO17" s="223"/>
       <c r="AP17" s="223"/>

</xml_diff>

<commit_message>
AN ENTIRELY NEW CONCEPT... EPAPER
</commit_message>
<xml_diff>
--- a/BillOfMaterials/INVENTORY.xlsx
+++ b/BillOfMaterials/INVENTORY.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="INVENTORY" sheetId="1" r:id="rId1"/>
@@ -2446,22 +2446,22 @@
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2999,9 +2999,9 @@
   </sheetPr>
   <dimension ref="A1:AB209"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O78" sqref="O78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3088,7 +3088,7 @@
       <c r="L3" s="35"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C4" s="218">
+      <c r="C4" s="217">
         <v>42882</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -3103,26 +3103,26 @@
       <c r="G4" s="27">
         <v>6.99</v>
       </c>
-      <c r="H4" s="219">
+      <c r="H4" s="221">
         <f>SUM(G4:G10)</f>
         <v>48.1</v>
       </c>
-      <c r="I4" s="217">
+      <c r="I4" s="218">
         <v>0</v>
       </c>
-      <c r="J4" s="219">
+      <c r="J4" s="221">
         <f>H4+I4</f>
         <v>48.1</v>
       </c>
-      <c r="K4" s="221">
+      <c r="K4" s="220">
         <f>G4/E4</f>
         <v>6.99</v>
       </c>
-      <c r="L4" s="221"/>
-      <c r="M4" s="221"/>
+      <c r="L4" s="220"/>
+      <c r="M4" s="220"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C5" s="218"/>
+      <c r="C5" s="217"/>
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
@@ -3135,18 +3135,18 @@
       <c r="G5" s="27">
         <v>6.99</v>
       </c>
-      <c r="H5" s="220"/>
-      <c r="I5" s="217"/>
-      <c r="J5" s="220"/>
-      <c r="K5" s="221">
+      <c r="H5" s="222"/>
+      <c r="I5" s="218"/>
+      <c r="J5" s="222"/>
+      <c r="K5" s="220">
         <f t="shared" ref="K5:K10" si="0">G5/E5</f>
         <v>6.99</v>
       </c>
-      <c r="L5" s="221"/>
-      <c r="M5" s="221"/>
+      <c r="L5" s="220"/>
+      <c r="M5" s="220"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C6" s="218"/>
+      <c r="C6" s="217"/>
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
@@ -3159,18 +3159,18 @@
       <c r="G6" s="27">
         <v>4.97</v>
       </c>
-      <c r="H6" s="220"/>
-      <c r="I6" s="217"/>
-      <c r="J6" s="220"/>
-      <c r="K6" s="221">
+      <c r="H6" s="222"/>
+      <c r="I6" s="218"/>
+      <c r="J6" s="222"/>
+      <c r="K6" s="220">
         <f t="shared" si="0"/>
         <v>0.2485</v>
       </c>
-      <c r="L6" s="221"/>
-      <c r="M6" s="221"/>
+      <c r="L6" s="220"/>
+      <c r="M6" s="220"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C7" s="218"/>
+      <c r="C7" s="217"/>
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
@@ -3183,18 +3183,18 @@
       <c r="G7" s="27">
         <v>5.99</v>
       </c>
-      <c r="H7" s="220"/>
-      <c r="I7" s="217"/>
-      <c r="J7" s="220"/>
-      <c r="K7" s="221">
+      <c r="H7" s="222"/>
+      <c r="I7" s="218"/>
+      <c r="J7" s="222"/>
+      <c r="K7" s="220">
         <f t="shared" si="0"/>
         <v>0.29949999999999999</v>
       </c>
-      <c r="L7" s="221"/>
-      <c r="M7" s="221"/>
+      <c r="L7" s="220"/>
+      <c r="M7" s="220"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C8" s="218"/>
+      <c r="C8" s="217"/>
       <c r="D8" s="1" t="s">
         <v>155</v>
       </c>
@@ -3207,18 +3207,18 @@
       <c r="G8" s="27">
         <v>6.25</v>
       </c>
-      <c r="H8" s="220"/>
-      <c r="I8" s="217"/>
-      <c r="J8" s="220"/>
-      <c r="K8" s="221">
+      <c r="H8" s="222"/>
+      <c r="I8" s="218"/>
+      <c r="J8" s="222"/>
+      <c r="K8" s="220">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
-      <c r="L8" s="221"/>
-      <c r="M8" s="221"/>
+      <c r="L8" s="220"/>
+      <c r="M8" s="220"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C9" s="218"/>
+      <c r="C9" s="217"/>
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3231,18 +3231,18 @@
       <c r="G9" s="27">
         <v>11.59</v>
       </c>
-      <c r="H9" s="220"/>
-      <c r="I9" s="217"/>
-      <c r="J9" s="220"/>
-      <c r="K9" s="221">
+      <c r="H9" s="222"/>
+      <c r="I9" s="218"/>
+      <c r="J9" s="222"/>
+      <c r="K9" s="220">
         <f t="shared" si="0"/>
         <v>0.57950000000000002</v>
       </c>
-      <c r="L9" s="221"/>
-      <c r="M9" s="221"/>
+      <c r="L9" s="220"/>
+      <c r="M9" s="220"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C10" s="218"/>
+      <c r="C10" s="217"/>
       <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
@@ -3255,15 +3255,15 @@
       <c r="G10" s="27">
         <v>5.32</v>
       </c>
-      <c r="H10" s="220"/>
-      <c r="I10" s="217"/>
-      <c r="J10" s="220"/>
-      <c r="K10" s="221">
+      <c r="H10" s="222"/>
+      <c r="I10" s="218"/>
+      <c r="J10" s="222"/>
+      <c r="K10" s="220">
         <f t="shared" si="0"/>
         <v>1.0640000000000001</v>
       </c>
-      <c r="L10" s="221"/>
-      <c r="M10" s="221"/>
+      <c r="L10" s="220"/>
+      <c r="M10" s="220"/>
     </row>
     <row r="11" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C11" s="7"/>
@@ -3370,14 +3370,14 @@
       <c r="G16" s="27">
         <v>6.56</v>
       </c>
-      <c r="H16" s="219">
+      <c r="H16" s="221">
         <f>SUM(G16:G17)</f>
         <v>7.55</v>
       </c>
-      <c r="I16" s="217">
+      <c r="I16" s="218">
         <v>0</v>
       </c>
-      <c r="J16" s="219">
+      <c r="J16" s="221">
         <f>H16+I16</f>
         <v>7.55</v>
       </c>
@@ -3398,9 +3398,9 @@
       <c r="G17" s="27">
         <v>0.99</v>
       </c>
-      <c r="H17" s="219"/>
-      <c r="I17" s="217"/>
-      <c r="J17" s="219"/>
+      <c r="H17" s="221"/>
+      <c r="I17" s="218"/>
+      <c r="J17" s="221"/>
     </row>
     <row r="18" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
@@ -3452,7 +3452,7 @@
       <c r="L20" s="35"/>
     </row>
     <row r="21" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C21" s="218">
+      <c r="C21" s="217">
         <v>42925</v>
       </c>
       <c r="D21" s="149" t="s">
@@ -3467,20 +3467,20 @@
       <c r="G21" s="27">
         <v>2.56</v>
       </c>
-      <c r="H21" s="219">
+      <c r="H21" s="221">
         <f>SUM(G21:G25)</f>
         <v>17.230000000000004</v>
       </c>
-      <c r="I21" s="217">
+      <c r="I21" s="218">
         <v>5.65</v>
       </c>
-      <c r="J21" s="219">
+      <c r="J21" s="221">
         <f>H21+I21</f>
         <v>22.880000000000003</v>
       </c>
     </row>
     <row r="22" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C22" s="218"/>
+      <c r="C22" s="217"/>
       <c r="D22" s="149" t="s">
         <v>21</v>
       </c>
@@ -3493,12 +3493,12 @@
       <c r="G22" s="27">
         <v>1.8</v>
       </c>
-      <c r="H22" s="220"/>
-      <c r="I22" s="217"/>
-      <c r="J22" s="220"/>
+      <c r="H22" s="222"/>
+      <c r="I22" s="218"/>
+      <c r="J22" s="222"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C23" s="218"/>
+      <c r="C23" s="217"/>
       <c r="D23" s="1" t="s">
         <v>20</v>
       </c>
@@ -3511,12 +3511,12 @@
       <c r="G23" s="27">
         <v>3.99</v>
       </c>
-      <c r="H23" s="220"/>
-      <c r="I23" s="217"/>
-      <c r="J23" s="220"/>
+      <c r="H23" s="222"/>
+      <c r="I23" s="218"/>
+      <c r="J23" s="222"/>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C24" s="218"/>
+      <c r="C24" s="217"/>
       <c r="D24" s="149" t="s">
         <v>13</v>
       </c>
@@ -3529,12 +3529,12 @@
       <c r="G24" s="27">
         <v>1.97</v>
       </c>
-      <c r="H24" s="220"/>
-      <c r="I24" s="217"/>
-      <c r="J24" s="220"/>
+      <c r="H24" s="222"/>
+      <c r="I24" s="218"/>
+      <c r="J24" s="222"/>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C25" s="218"/>
+      <c r="C25" s="217"/>
       <c r="D25" s="1" t="s">
         <v>2</v>
       </c>
@@ -3547,9 +3547,9 @@
       <c r="G25" s="27">
         <v>6.91</v>
       </c>
-      <c r="H25" s="220"/>
-      <c r="I25" s="217"/>
-      <c r="J25" s="220"/>
+      <c r="H25" s="222"/>
+      <c r="I25" s="218"/>
+      <c r="J25" s="222"/>
     </row>
     <row r="26" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
@@ -3563,7 +3563,7 @@
       <c r="L26" s="35"/>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C27" s="218">
+      <c r="C27" s="217">
         <v>42927</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -3578,20 +3578,20 @@
       <c r="G27" s="27">
         <v>0.75</v>
       </c>
-      <c r="H27" s="219">
+      <c r="H27" s="221">
         <f>SUM(G27:G29)</f>
         <v>3.44</v>
       </c>
-      <c r="I27" s="217">
+      <c r="I27" s="218">
         <v>4.99</v>
       </c>
-      <c r="J27" s="219">
+      <c r="J27" s="221">
         <f>H27+I27</f>
         <v>8.43</v>
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C28" s="218"/>
+      <c r="C28" s="217"/>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
@@ -3604,12 +3604,12 @@
       <c r="G28" s="27">
         <v>0.75</v>
       </c>
-      <c r="H28" s="220"/>
-      <c r="I28" s="217"/>
-      <c r="J28" s="220"/>
+      <c r="H28" s="222"/>
+      <c r="I28" s="218"/>
+      <c r="J28" s="222"/>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C29" s="218"/>
+      <c r="C29" s="217"/>
       <c r="D29" s="1" t="s">
         <v>154</v>
       </c>
@@ -3622,9 +3622,9 @@
       <c r="G29" s="27">
         <v>1.94</v>
       </c>
-      <c r="H29" s="220"/>
-      <c r="I29" s="217"/>
-      <c r="J29" s="220"/>
+      <c r="H29" s="222"/>
+      <c r="I29" s="218"/>
+      <c r="J29" s="222"/>
     </row>
     <row r="30" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="7"/>
@@ -3676,7 +3676,7 @@
       <c r="L32" s="35"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C33" s="218">
+      <c r="C33" s="217">
         <v>42929</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -3691,20 +3691,20 @@
       <c r="G33" s="27">
         <v>0.77</v>
       </c>
-      <c r="H33" s="219">
+      <c r="H33" s="221">
         <f>SUM(G33:G34)</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="I33" s="217">
+      <c r="I33" s="218">
         <v>3.39</v>
       </c>
-      <c r="J33" s="217">
+      <c r="J33" s="218">
         <f>SUM(H33:I34)</f>
         <v>5.6899999999999995</v>
       </c>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C34" s="218"/>
+      <c r="C34" s="217"/>
       <c r="D34" s="1" t="s">
         <v>76</v>
       </c>
@@ -3717,9 +3717,9 @@
       <c r="G34" s="27">
         <v>1.53</v>
       </c>
-      <c r="H34" s="220"/>
-      <c r="I34" s="217"/>
-      <c r="J34" s="217"/>
+      <c r="H34" s="222"/>
+      <c r="I34" s="218"/>
+      <c r="J34" s="218"/>
     </row>
     <row r="35" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="7"/>
@@ -3771,7 +3771,7 @@
       <c r="L37" s="35"/>
     </row>
     <row r="38" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C38" s="218">
+      <c r="C38" s="217">
         <v>42931</v>
       </c>
       <c r="D38" s="149" t="s">
@@ -3786,20 +3786,20 @@
       <c r="G38" s="27">
         <v>5.72</v>
       </c>
-      <c r="H38" s="217">
+      <c r="H38" s="218">
         <f>SUM(G38:G39)</f>
         <v>8.5500000000000007</v>
       </c>
-      <c r="I38" s="217">
+      <c r="I38" s="218">
         <v>4.99</v>
       </c>
-      <c r="J38" s="217">
+      <c r="J38" s="218">
         <f>SUM(H38:I39)</f>
         <v>13.540000000000001</v>
       </c>
     </row>
     <row r="39" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C39" s="218"/>
+      <c r="C39" s="217"/>
       <c r="D39" s="149" t="s">
         <v>122</v>
       </c>
@@ -3812,9 +3812,9 @@
       <c r="G39" s="27">
         <v>2.83</v>
       </c>
-      <c r="H39" s="217"/>
-      <c r="I39" s="217"/>
-      <c r="J39" s="217"/>
+      <c r="H39" s="218"/>
+      <c r="I39" s="218"/>
+      <c r="J39" s="218"/>
     </row>
     <row r="40" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="7"/>
@@ -3828,7 +3828,7 @@
       <c r="L40" s="35"/>
     </row>
     <row r="41" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C41" s="218">
+      <c r="C41" s="217">
         <v>42936</v>
       </c>
       <c r="D41" s="149" t="s">
@@ -3843,20 +3843,20 @@
       <c r="G41" s="27">
         <v>10.58</v>
       </c>
-      <c r="H41" s="217">
+      <c r="H41" s="218">
         <f>SUM(G41:G45)</f>
         <v>18.649999999999999</v>
       </c>
-      <c r="I41" s="217">
+      <c r="I41" s="218">
         <v>0.25</v>
       </c>
-      <c r="J41" s="217">
+      <c r="J41" s="218">
         <f>H41+I41</f>
         <v>18.899999999999999</v>
       </c>
     </row>
     <row r="42" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C42" s="218"/>
+      <c r="C42" s="217"/>
       <c r="D42" s="149" t="s">
         <v>150</v>
       </c>
@@ -3869,12 +3869,12 @@
       <c r="G42" s="27">
         <v>3.86</v>
       </c>
-      <c r="H42" s="217"/>
-      <c r="I42" s="217"/>
-      <c r="J42" s="217"/>
+      <c r="H42" s="218"/>
+      <c r="I42" s="218"/>
+      <c r="J42" s="218"/>
     </row>
     <row r="43" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C43" s="218"/>
+      <c r="C43" s="217"/>
       <c r="D43" s="149" t="s">
         <v>151</v>
       </c>
@@ -3888,12 +3888,12 @@
         <f>1.99-0.1</f>
         <v>1.89</v>
       </c>
-      <c r="H43" s="217"/>
-      <c r="I43" s="217"/>
-      <c r="J43" s="217"/>
+      <c r="H43" s="218"/>
+      <c r="I43" s="218"/>
+      <c r="J43" s="218"/>
     </row>
     <row r="44" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C44" s="218"/>
+      <c r="C44" s="217"/>
       <c r="D44" s="149" t="s">
         <v>152</v>
       </c>
@@ -3907,12 +3907,12 @@
         <f>0.99-0.05</f>
         <v>0.94</v>
       </c>
-      <c r="H44" s="217"/>
-      <c r="I44" s="217"/>
-      <c r="J44" s="217"/>
+      <c r="H44" s="218"/>
+      <c r="I44" s="218"/>
+      <c r="J44" s="218"/>
     </row>
     <row r="45" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C45" s="218"/>
+      <c r="C45" s="217"/>
       <c r="D45" s="149" t="s">
         <v>153</v>
       </c>
@@ -3926,9 +3926,9 @@
         <f>1.45-0.07</f>
         <v>1.38</v>
       </c>
-      <c r="H45" s="217"/>
-      <c r="I45" s="217"/>
-      <c r="J45" s="217"/>
+      <c r="H45" s="218"/>
+      <c r="I45" s="218"/>
+      <c r="J45" s="218"/>
     </row>
     <row r="46" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="51"/>
@@ -4017,7 +4017,7 @@
       <c r="L50" s="57"/>
     </row>
     <row r="51" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C51" s="218">
+      <c r="C51" s="217">
         <v>42986</v>
       </c>
       <c r="D51" s="149" t="s">
@@ -4032,20 +4032,20 @@
       <c r="G51" s="27">
         <v>29.95</v>
       </c>
-      <c r="H51" s="217">
+      <c r="H51" s="218">
         <f>G51+G52+G53+2.13</f>
         <v>34.380000000000003</v>
       </c>
-      <c r="I51" s="217">
+      <c r="I51" s="218">
         <v>3.03</v>
       </c>
-      <c r="J51" s="217">
+      <c r="J51" s="218">
         <f>H51+I51</f>
         <v>37.410000000000004</v>
       </c>
     </row>
     <row r="52" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C52" s="218"/>
+      <c r="C52" s="217"/>
       <c r="D52" s="149" t="s">
         <v>222</v>
       </c>
@@ -4058,12 +4058,12 @@
       <c r="G52" s="27">
         <v>0.77</v>
       </c>
-      <c r="H52" s="217"/>
-      <c r="I52" s="217"/>
-      <c r="J52" s="217"/>
+      <c r="H52" s="218"/>
+      <c r="I52" s="218"/>
+      <c r="J52" s="218"/>
     </row>
     <row r="53" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C53" s="218"/>
+      <c r="C53" s="217"/>
       <c r="D53" s="149" t="s">
         <v>223</v>
       </c>
@@ -4076,9 +4076,9 @@
       <c r="G53" s="27">
         <v>1.53</v>
       </c>
-      <c r="H53" s="217"/>
-      <c r="I53" s="217"/>
-      <c r="J53" s="217"/>
+      <c r="H53" s="218"/>
+      <c r="I53" s="218"/>
+      <c r="J53" s="218"/>
     </row>
     <row r="54" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="51"/>
@@ -4241,7 +4241,7 @@
       <c r="L62" s="57"/>
     </row>
     <row r="63" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C63" s="218">
+      <c r="C63" s="217">
         <v>43027</v>
       </c>
       <c r="D63" s="149" t="s">
@@ -4256,20 +4256,20 @@
       <c r="G63" s="27">
         <v>2.66</v>
       </c>
-      <c r="H63" s="217">
+      <c r="H63" s="218">
         <f>SUM(G63:G66)</f>
         <v>10.18</v>
       </c>
-      <c r="I63" s="217">
+      <c r="I63" s="218">
         <v>3.75</v>
       </c>
-      <c r="J63" s="217">
+      <c r="J63" s="218">
         <f>H63+I63</f>
         <v>13.93</v>
       </c>
     </row>
     <row r="64" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C64" s="218"/>
+      <c r="C64" s="217"/>
       <c r="D64" s="149" t="s">
         <v>234</v>
       </c>
@@ -4282,12 +4282,12 @@
       <c r="G64" s="27">
         <v>1.53</v>
       </c>
-      <c r="H64" s="217"/>
-      <c r="I64" s="217"/>
-      <c r="J64" s="217"/>
+      <c r="H64" s="218"/>
+      <c r="I64" s="218"/>
+      <c r="J64" s="218"/>
     </row>
     <row r="65" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C65" s="218"/>
+      <c r="C65" s="217"/>
       <c r="D65" s="149" t="s">
         <v>222</v>
       </c>
@@ -4300,12 +4300,12 @@
       <c r="G65" s="27">
         <v>0.77</v>
       </c>
-      <c r="H65" s="217"/>
-      <c r="I65" s="217"/>
-      <c r="J65" s="217"/>
+      <c r="H65" s="218"/>
+      <c r="I65" s="218"/>
+      <c r="J65" s="218"/>
     </row>
     <row r="66" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C66" s="218"/>
+      <c r="C66" s="217"/>
       <c r="D66" s="149" t="s">
         <v>235</v>
       </c>
@@ -4318,9 +4318,9 @@
       <c r="G66" s="27">
         <v>5.22</v>
       </c>
-      <c r="H66" s="217"/>
-      <c r="I66" s="217"/>
-      <c r="J66" s="217"/>
+      <c r="H66" s="218"/>
+      <c r="I66" s="218"/>
+      <c r="J66" s="218"/>
     </row>
     <row r="67" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C67" s="51"/>
@@ -4372,7 +4372,7 @@
       <c r="L69" s="57"/>
     </row>
     <row r="70" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C70" s="218">
+      <c r="C70" s="217">
         <v>43040</v>
       </c>
       <c r="D70" s="149" t="s">
@@ -4387,14 +4387,14 @@
       <c r="G70" s="27">
         <v>0.4</v>
       </c>
-      <c r="H70" s="217">
+      <c r="H70" s="218">
         <f>SUM(G70:G76)</f>
         <v>3.5799999999999996</v>
       </c>
-      <c r="I70" s="217">
+      <c r="I70" s="218">
         <v>3.39</v>
       </c>
-      <c r="J70" s="222">
+      <c r="J70" s="219">
         <f>H70+I70+K71</f>
         <v>7.2206000000000001</v>
       </c>
@@ -4403,7 +4403,7 @@
       </c>
     </row>
     <row r="71" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C71" s="218"/>
+      <c r="C71" s="217"/>
       <c r="D71" s="149" t="s">
         <v>237</v>
       </c>
@@ -4416,9 +4416,9 @@
       <c r="G71" s="27">
         <v>0.9</v>
       </c>
-      <c r="H71" s="217"/>
-      <c r="I71" s="217"/>
-      <c r="J71" s="222"/>
+      <c r="H71" s="218"/>
+      <c r="I71" s="218"/>
+      <c r="J71" s="219"/>
       <c r="K71" s="214">
         <f>SUM(G70:G76)*0.07</f>
         <v>0.25059999999999999</v>
@@ -4426,7 +4426,7 @@
       <c r="L71" s="215"/>
     </row>
     <row r="72" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C72" s="218"/>
+      <c r="C72" s="217"/>
       <c r="D72" s="149" t="s">
         <v>238</v>
       </c>
@@ -4439,12 +4439,12 @@
       <c r="G72" s="27">
         <v>0.64</v>
       </c>
-      <c r="H72" s="217"/>
-      <c r="I72" s="217"/>
-      <c r="J72" s="222"/>
+      <c r="H72" s="218"/>
+      <c r="I72" s="218"/>
+      <c r="J72" s="219"/>
     </row>
     <row r="73" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C73" s="218"/>
+      <c r="C73" s="217"/>
       <c r="D73" s="149" t="s">
         <v>239</v>
       </c>
@@ -4457,12 +4457,12 @@
       <c r="G73" s="27">
         <v>0.4</v>
       </c>
-      <c r="H73" s="217"/>
-      <c r="I73" s="217"/>
-      <c r="J73" s="222"/>
+      <c r="H73" s="218"/>
+      <c r="I73" s="218"/>
+      <c r="J73" s="219"/>
     </row>
     <row r="74" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C74" s="218"/>
+      <c r="C74" s="217"/>
       <c r="D74" s="149" t="s">
         <v>240</v>
       </c>
@@ -4475,12 +4475,12 @@
       <c r="G74" s="27">
         <v>0.32</v>
       </c>
-      <c r="H74" s="217"/>
-      <c r="I74" s="217"/>
-      <c r="J74" s="222"/>
+      <c r="H74" s="218"/>
+      <c r="I74" s="218"/>
+      <c r="J74" s="219"/>
     </row>
     <row r="75" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C75" s="218"/>
+      <c r="C75" s="217"/>
       <c r="D75" s="149" t="s">
         <v>241</v>
       </c>
@@ -4493,12 +4493,12 @@
       <c r="G75" s="27">
         <v>0.46</v>
       </c>
-      <c r="H75" s="217"/>
-      <c r="I75" s="217"/>
-      <c r="J75" s="222"/>
+      <c r="H75" s="218"/>
+      <c r="I75" s="218"/>
+      <c r="J75" s="219"/>
     </row>
     <row r="76" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C76" s="218"/>
+      <c r="C76" s="217"/>
       <c r="D76" s="149" t="s">
         <v>242</v>
       </c>
@@ -4511,9 +4511,9 @@
       <c r="G76" s="27">
         <v>0.46</v>
       </c>
-      <c r="H76" s="217"/>
-      <c r="I76" s="217"/>
-      <c r="J76" s="222"/>
+      <c r="H76" s="218"/>
+      <c r="I76" s="218"/>
+      <c r="J76" s="219"/>
     </row>
     <row r="77" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C77" s="51"/>
@@ -4527,10 +4527,10 @@
       <c r="L77" s="57"/>
     </row>
     <row r="78" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C78" s="218">
+      <c r="C78" s="217">
         <v>43045</v>
       </c>
-      <c r="D78" s="202" t="s">
+      <c r="D78" s="149" t="s">
         <v>245</v>
       </c>
       <c r="E78" s="26">
@@ -4542,14 +4542,14 @@
       <c r="G78" s="27">
         <v>0.1</v>
       </c>
-      <c r="H78" s="217">
+      <c r="H78" s="218">
         <f>SUM(G78:G86)</f>
         <v>4.1500000000000004</v>
       </c>
-      <c r="I78" s="217">
+      <c r="I78" s="218">
         <v>3.93</v>
       </c>
-      <c r="J78" s="222">
+      <c r="J78" s="219">
         <f>H78+I78+K79</f>
         <v>8.3497500000000002</v>
       </c>
@@ -4558,8 +4558,8 @@
       </c>
     </row>
     <row r="79" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C79" s="218"/>
-      <c r="D79" s="202" t="s">
+      <c r="C79" s="217"/>
+      <c r="D79" s="149" t="s">
         <v>246</v>
       </c>
       <c r="E79" s="26">
@@ -4571,17 +4571,17 @@
       <c r="G79" s="27">
         <v>0.4</v>
       </c>
-      <c r="H79" s="217"/>
-      <c r="I79" s="217"/>
-      <c r="J79" s="222"/>
+      <c r="H79" s="218"/>
+      <c r="I79" s="218"/>
+      <c r="J79" s="219"/>
       <c r="K79" s="214">
         <f>SUM(G78:G86)*0.065</f>
         <v>0.26975000000000005</v>
       </c>
     </row>
     <row r="80" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C80" s="218"/>
-      <c r="D80" s="202" t="s">
+      <c r="C80" s="217"/>
+      <c r="D80" s="149" t="s">
         <v>247</v>
       </c>
       <c r="E80" s="26">
@@ -4593,13 +4593,13 @@
       <c r="G80" s="27">
         <v>0.4</v>
       </c>
-      <c r="H80" s="217"/>
-      <c r="I80" s="217"/>
-      <c r="J80" s="222"/>
+      <c r="H80" s="218"/>
+      <c r="I80" s="218"/>
+      <c r="J80" s="219"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C81" s="218"/>
-      <c r="D81" s="202" t="s">
+      <c r="C81" s="217"/>
+      <c r="D81" s="149" t="s">
         <v>248</v>
       </c>
       <c r="E81" s="26">
@@ -4611,13 +4611,13 @@
       <c r="G81" s="27">
         <v>0.4</v>
       </c>
-      <c r="H81" s="217"/>
-      <c r="I81" s="217"/>
-      <c r="J81" s="222"/>
+      <c r="H81" s="218"/>
+      <c r="I81" s="218"/>
+      <c r="J81" s="219"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C82" s="218"/>
-      <c r="D82" s="202" t="s">
+      <c r="C82" s="217"/>
+      <c r="D82" s="149" t="s">
         <v>249</v>
       </c>
       <c r="E82" s="26">
@@ -4629,13 +4629,13 @@
       <c r="G82" s="27">
         <v>0.63</v>
       </c>
-      <c r="H82" s="217"/>
-      <c r="I82" s="217"/>
-      <c r="J82" s="222"/>
+      <c r="H82" s="218"/>
+      <c r="I82" s="218"/>
+      <c r="J82" s="219"/>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C83" s="218"/>
-      <c r="D83" s="202" t="s">
+      <c r="C83" s="217"/>
+      <c r="D83" s="149" t="s">
         <v>250</v>
       </c>
       <c r="E83" s="26">
@@ -4647,13 +4647,13 @@
       <c r="G83" s="27">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H83" s="217"/>
-      <c r="I83" s="217"/>
-      <c r="J83" s="222"/>
+      <c r="H83" s="218"/>
+      <c r="I83" s="218"/>
+      <c r="J83" s="219"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C84" s="218"/>
-      <c r="D84" s="202" t="s">
+      <c r="C84" s="217"/>
+      <c r="D84" s="149" t="s">
         <v>251</v>
       </c>
       <c r="E84" s="26">
@@ -4665,13 +4665,13 @@
       <c r="G84" s="27">
         <v>0.86</v>
       </c>
-      <c r="H84" s="217"/>
-      <c r="I84" s="217"/>
-      <c r="J84" s="222"/>
+      <c r="H84" s="218"/>
+      <c r="I84" s="218"/>
+      <c r="J84" s="219"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C85" s="218"/>
-      <c r="D85" s="202" t="s">
+      <c r="C85" s="217"/>
+      <c r="D85" s="149" t="s">
         <v>252</v>
       </c>
       <c r="E85" s="26">
@@ -4683,13 +4683,13 @@
       <c r="G85" s="27">
         <v>0.61</v>
       </c>
-      <c r="H85" s="217"/>
-      <c r="I85" s="217"/>
-      <c r="J85" s="222"/>
+      <c r="H85" s="218"/>
+      <c r="I85" s="218"/>
+      <c r="J85" s="219"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C86" s="218"/>
-      <c r="D86" s="202" t="s">
+      <c r="C86" s="217"/>
+      <c r="D86" s="149" t="s">
         <v>253</v>
       </c>
       <c r="E86" s="26">
@@ -4701,9 +4701,9 @@
       <c r="G86" s="27">
         <v>0.2</v>
       </c>
-      <c r="H86" s="217"/>
-      <c r="I86" s="217"/>
-      <c r="J86" s="222"/>
+      <c r="H86" s="218"/>
+      <c r="I86" s="218"/>
+      <c r="J86" s="219"/>
     </row>
     <row r="87" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C87" s="7"/>
@@ -4722,7 +4722,7 @@
       </c>
       <c r="C88" s="41">
         <f ca="1">TODAY()</f>
-        <v>43050</v>
+        <v>43057</v>
       </c>
       <c r="E88" s="29"/>
       <c r="F88" s="29"/>
@@ -4740,7 +4740,7 @@
       </c>
       <c r="L88" s="39">
         <f ca="1">(C88-C4)*0.0328767</f>
-        <v>5.5232856000000004</v>
+        <v>5.7534225000000001</v>
       </c>
       <c r="M88" s="24" t="s">
         <v>25</v>
@@ -4758,7 +4758,7 @@
       </c>
       <c r="J89" s="22">
         <f ca="1">J88/L88</f>
-        <v>55.887088293967629</v>
+        <v>53.651604762208926</v>
       </c>
       <c r="K89" s="32" t="s">
         <v>27</v>
@@ -6191,27 +6191,19 @@
     <sortCondition ref="C4:C19"/>
   </sortState>
   <mergeCells count="50">
-    <mergeCell ref="C78:C86"/>
-    <mergeCell ref="H78:H86"/>
-    <mergeCell ref="I78:I86"/>
-    <mergeCell ref="J78:J86"/>
-    <mergeCell ref="C70:C76"/>
-    <mergeCell ref="H70:H76"/>
-    <mergeCell ref="I70:I76"/>
-    <mergeCell ref="J70:J76"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="H63:H66"/>
-    <mergeCell ref="I63:I66"/>
-    <mergeCell ref="J63:J66"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="H51:H53"/>
-    <mergeCell ref="I51:I53"/>
-    <mergeCell ref="J51:J53"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="C4:C10"/>
+    <mergeCell ref="J4:J10"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="H4:H10"/>
+    <mergeCell ref="I4:I10"/>
+    <mergeCell ref="J21:J25"/>
+    <mergeCell ref="H21:H25"/>
+    <mergeCell ref="H27:H29"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="I21:I25"/>
+    <mergeCell ref="H16:H17"/>
     <mergeCell ref="C41:C45"/>
     <mergeCell ref="H41:H45"/>
     <mergeCell ref="I41:I45"/>
@@ -6228,19 +6220,27 @@
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="H38:H39"/>
     <mergeCell ref="I38:I39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="C4:C10"/>
-    <mergeCell ref="J4:J10"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="H4:H10"/>
-    <mergeCell ref="I4:I10"/>
-    <mergeCell ref="J21:J25"/>
-    <mergeCell ref="H21:H25"/>
-    <mergeCell ref="H27:H29"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="I21:I25"/>
-    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="H63:H66"/>
+    <mergeCell ref="I63:I66"/>
+    <mergeCell ref="J63:J66"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="H51:H53"/>
+    <mergeCell ref="I51:I53"/>
+    <mergeCell ref="J51:J53"/>
+    <mergeCell ref="C78:C86"/>
+    <mergeCell ref="H78:H86"/>
+    <mergeCell ref="I78:I86"/>
+    <mergeCell ref="J78:J86"/>
+    <mergeCell ref="C70:C76"/>
+    <mergeCell ref="H70:H76"/>
+    <mergeCell ref="I70:I76"/>
+    <mergeCell ref="J70:J76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6257,7 +6257,7 @@
   </sheetPr>
   <dimension ref="B3:BG20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -7154,15 +7154,15 @@
       <c r="AO16" s="223"/>
       <c r="AP16" s="223"/>
       <c r="AQ16" s="223"/>
-      <c r="AT16" s="220" t="s">
+      <c r="AT16" s="222" t="s">
         <v>119</v>
       </c>
-      <c r="AU16" s="220"/>
-      <c r="AV16" s="220"/>
-      <c r="AW16" s="220"/>
-      <c r="AX16" s="220"/>
-      <c r="AY16" s="220"/>
-      <c r="AZ16" s="220"/>
+      <c r="AU16" s="222"/>
+      <c r="AV16" s="222"/>
+      <c r="AW16" s="222"/>
+      <c r="AX16" s="222"/>
+      <c r="AY16" s="222"/>
+      <c r="AZ16" s="222"/>
     </row>
     <row r="17" spans="25:59" x14ac:dyDescent="0.25">
       <c r="Y17" s="108" t="s">
@@ -7177,11 +7177,11 @@
       <c r="AB17" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="AJ17" s="220" t="s">
+      <c r="AJ17" s="222" t="s">
         <v>117</v>
       </c>
-      <c r="AK17" s="220"/>
-      <c r="AL17" s="220"/>
+      <c r="AK17" s="222"/>
+      <c r="AL17" s="222"/>
       <c r="AN17" s="223"/>
       <c r="AO17" s="223"/>
       <c r="AP17" s="223"/>

</xml_diff>

<commit_message>
CONCEPT FOR RISER MOUNTING
</commit_message>
<xml_diff>
--- a/BillOfMaterials/INVENTORY.xlsx
+++ b/BillOfMaterials/INVENTORY.xlsx
@@ -1954,7 +1954,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="228">
+  <cellXfs count="229">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2446,24 +2446,24 @@
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2479,6 +2479,7 @@
     <xf numFmtId="44" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -3001,7 +3002,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O78" sqref="O78"/>
+      <selection pane="bottomLeft" activeCell="N79" sqref="N79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3088,7 +3089,7 @@
       <c r="L3" s="35"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C4" s="217">
+      <c r="C4" s="218">
         <v>42882</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -3103,26 +3104,26 @@
       <c r="G4" s="27">
         <v>6.99</v>
       </c>
-      <c r="H4" s="221">
+      <c r="H4" s="219">
         <f>SUM(G4:G10)</f>
         <v>48.1</v>
       </c>
-      <c r="I4" s="218">
+      <c r="I4" s="217">
         <v>0</v>
       </c>
-      <c r="J4" s="221">
+      <c r="J4" s="219">
         <f>H4+I4</f>
         <v>48.1</v>
       </c>
-      <c r="K4" s="220">
+      <c r="K4" s="221">
         <f>G4/E4</f>
         <v>6.99</v>
       </c>
-      <c r="L4" s="220"/>
-      <c r="M4" s="220"/>
+      <c r="L4" s="221"/>
+      <c r="M4" s="221"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C5" s="217"/>
+      <c r="C5" s="218"/>
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
@@ -3135,18 +3136,18 @@
       <c r="G5" s="27">
         <v>6.99</v>
       </c>
-      <c r="H5" s="222"/>
-      <c r="I5" s="218"/>
-      <c r="J5" s="222"/>
-      <c r="K5" s="220">
+      <c r="H5" s="220"/>
+      <c r="I5" s="217"/>
+      <c r="J5" s="220"/>
+      <c r="K5" s="221">
         <f t="shared" ref="K5:K10" si="0">G5/E5</f>
         <v>6.99</v>
       </c>
-      <c r="L5" s="220"/>
-      <c r="M5" s="220"/>
+      <c r="L5" s="221"/>
+      <c r="M5" s="221"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C6" s="217"/>
+      <c r="C6" s="218"/>
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
@@ -3159,18 +3160,18 @@
       <c r="G6" s="27">
         <v>4.97</v>
       </c>
-      <c r="H6" s="222"/>
-      <c r="I6" s="218"/>
-      <c r="J6" s="222"/>
-      <c r="K6" s="220">
+      <c r="H6" s="220"/>
+      <c r="I6" s="217"/>
+      <c r="J6" s="220"/>
+      <c r="K6" s="221">
         <f t="shared" si="0"/>
         <v>0.2485</v>
       </c>
-      <c r="L6" s="220"/>
-      <c r="M6" s="220"/>
+      <c r="L6" s="221"/>
+      <c r="M6" s="221"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C7" s="217"/>
+      <c r="C7" s="218"/>
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
@@ -3183,18 +3184,18 @@
       <c r="G7" s="27">
         <v>5.99</v>
       </c>
-      <c r="H7" s="222"/>
-      <c r="I7" s="218"/>
-      <c r="J7" s="222"/>
-      <c r="K7" s="220">
+      <c r="H7" s="220"/>
+      <c r="I7" s="217"/>
+      <c r="J7" s="220"/>
+      <c r="K7" s="221">
         <f t="shared" si="0"/>
         <v>0.29949999999999999</v>
       </c>
-      <c r="L7" s="220"/>
-      <c r="M7" s="220"/>
+      <c r="L7" s="221"/>
+      <c r="M7" s="221"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C8" s="217"/>
+      <c r="C8" s="218"/>
       <c r="D8" s="1" t="s">
         <v>155</v>
       </c>
@@ -3207,18 +3208,18 @@
       <c r="G8" s="27">
         <v>6.25</v>
       </c>
-      <c r="H8" s="222"/>
-      <c r="I8" s="218"/>
-      <c r="J8" s="222"/>
-      <c r="K8" s="220">
+      <c r="H8" s="220"/>
+      <c r="I8" s="217"/>
+      <c r="J8" s="220"/>
+      <c r="K8" s="221">
         <f t="shared" si="0"/>
         <v>6.25</v>
       </c>
-      <c r="L8" s="220"/>
-      <c r="M8" s="220"/>
+      <c r="L8" s="221"/>
+      <c r="M8" s="221"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C9" s="217"/>
+      <c r="C9" s="218"/>
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3231,18 +3232,18 @@
       <c r="G9" s="27">
         <v>11.59</v>
       </c>
-      <c r="H9" s="222"/>
-      <c r="I9" s="218"/>
-      <c r="J9" s="222"/>
-      <c r="K9" s="220">
+      <c r="H9" s="220"/>
+      <c r="I9" s="217"/>
+      <c r="J9" s="220"/>
+      <c r="K9" s="221">
         <f t="shared" si="0"/>
         <v>0.57950000000000002</v>
       </c>
-      <c r="L9" s="220"/>
-      <c r="M9" s="220"/>
+      <c r="L9" s="221"/>
+      <c r="M9" s="221"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C10" s="217"/>
+      <c r="C10" s="218"/>
       <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
@@ -3255,15 +3256,15 @@
       <c r="G10" s="27">
         <v>5.32</v>
       </c>
-      <c r="H10" s="222"/>
-      <c r="I10" s="218"/>
-      <c r="J10" s="222"/>
-      <c r="K10" s="220">
+      <c r="H10" s="220"/>
+      <c r="I10" s="217"/>
+      <c r="J10" s="220"/>
+      <c r="K10" s="221">
         <f t="shared" si="0"/>
         <v>1.0640000000000001</v>
       </c>
-      <c r="L10" s="220"/>
-      <c r="M10" s="220"/>
+      <c r="L10" s="221"/>
+      <c r="M10" s="221"/>
     </row>
     <row r="11" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C11" s="7"/>
@@ -3370,14 +3371,14 @@
       <c r="G16" s="27">
         <v>6.56</v>
       </c>
-      <c r="H16" s="221">
+      <c r="H16" s="219">
         <f>SUM(G16:G17)</f>
         <v>7.55</v>
       </c>
-      <c r="I16" s="218">
+      <c r="I16" s="217">
         <v>0</v>
       </c>
-      <c r="J16" s="221">
+      <c r="J16" s="219">
         <f>H16+I16</f>
         <v>7.55</v>
       </c>
@@ -3398,9 +3399,9 @@
       <c r="G17" s="27">
         <v>0.99</v>
       </c>
-      <c r="H17" s="221"/>
-      <c r="I17" s="218"/>
-      <c r="J17" s="221"/>
+      <c r="H17" s="219"/>
+      <c r="I17" s="217"/>
+      <c r="J17" s="219"/>
     </row>
     <row r="18" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
@@ -3452,7 +3453,7 @@
       <c r="L20" s="35"/>
     </row>
     <row r="21" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C21" s="217">
+      <c r="C21" s="218">
         <v>42925</v>
       </c>
       <c r="D21" s="149" t="s">
@@ -3467,20 +3468,20 @@
       <c r="G21" s="27">
         <v>2.56</v>
       </c>
-      <c r="H21" s="221">
+      <c r="H21" s="219">
         <f>SUM(G21:G25)</f>
         <v>17.230000000000004</v>
       </c>
-      <c r="I21" s="218">
+      <c r="I21" s="217">
         <v>5.65</v>
       </c>
-      <c r="J21" s="221">
+      <c r="J21" s="219">
         <f>H21+I21</f>
         <v>22.880000000000003</v>
       </c>
     </row>
     <row r="22" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C22" s="217"/>
+      <c r="C22" s="218"/>
       <c r="D22" s="149" t="s">
         <v>21</v>
       </c>
@@ -3493,12 +3494,12 @@
       <c r="G22" s="27">
         <v>1.8</v>
       </c>
-      <c r="H22" s="222"/>
-      <c r="I22" s="218"/>
-      <c r="J22" s="222"/>
+      <c r="H22" s="220"/>
+      <c r="I22" s="217"/>
+      <c r="J22" s="220"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C23" s="217"/>
+      <c r="C23" s="218"/>
       <c r="D23" s="1" t="s">
         <v>20</v>
       </c>
@@ -3511,12 +3512,12 @@
       <c r="G23" s="27">
         <v>3.99</v>
       </c>
-      <c r="H23" s="222"/>
-      <c r="I23" s="218"/>
-      <c r="J23" s="222"/>
+      <c r="H23" s="220"/>
+      <c r="I23" s="217"/>
+      <c r="J23" s="220"/>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C24" s="217"/>
+      <c r="C24" s="218"/>
       <c r="D24" s="149" t="s">
         <v>13</v>
       </c>
@@ -3529,12 +3530,12 @@
       <c r="G24" s="27">
         <v>1.97</v>
       </c>
-      <c r="H24" s="222"/>
-      <c r="I24" s="218"/>
-      <c r="J24" s="222"/>
+      <c r="H24" s="220"/>
+      <c r="I24" s="217"/>
+      <c r="J24" s="220"/>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C25" s="217"/>
+      <c r="C25" s="218"/>
       <c r="D25" s="1" t="s">
         <v>2</v>
       </c>
@@ -3547,9 +3548,9 @@
       <c r="G25" s="27">
         <v>6.91</v>
       </c>
-      <c r="H25" s="222"/>
-      <c r="I25" s="218"/>
-      <c r="J25" s="222"/>
+      <c r="H25" s="220"/>
+      <c r="I25" s="217"/>
+      <c r="J25" s="220"/>
     </row>
     <row r="26" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
@@ -3563,7 +3564,7 @@
       <c r="L26" s="35"/>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C27" s="217">
+      <c r="C27" s="218">
         <v>42927</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -3578,20 +3579,20 @@
       <c r="G27" s="27">
         <v>0.75</v>
       </c>
-      <c r="H27" s="221">
+      <c r="H27" s="219">
         <f>SUM(G27:G29)</f>
         <v>3.44</v>
       </c>
-      <c r="I27" s="218">
+      <c r="I27" s="217">
         <v>4.99</v>
       </c>
-      <c r="J27" s="221">
+      <c r="J27" s="219">
         <f>H27+I27</f>
         <v>8.43</v>
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C28" s="217"/>
+      <c r="C28" s="218"/>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
@@ -3604,12 +3605,12 @@
       <c r="G28" s="27">
         <v>0.75</v>
       </c>
-      <c r="H28" s="222"/>
-      <c r="I28" s="218"/>
-      <c r="J28" s="222"/>
+      <c r="H28" s="220"/>
+      <c r="I28" s="217"/>
+      <c r="J28" s="220"/>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C29" s="217"/>
+      <c r="C29" s="218"/>
       <c r="D29" s="1" t="s">
         <v>154</v>
       </c>
@@ -3622,9 +3623,9 @@
       <c r="G29" s="27">
         <v>1.94</v>
       </c>
-      <c r="H29" s="222"/>
-      <c r="I29" s="218"/>
-      <c r="J29" s="222"/>
+      <c r="H29" s="220"/>
+      <c r="I29" s="217"/>
+      <c r="J29" s="220"/>
     </row>
     <row r="30" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="7"/>
@@ -3676,7 +3677,7 @@
       <c r="L32" s="35"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C33" s="217">
+      <c r="C33" s="218">
         <v>42929</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -3691,20 +3692,20 @@
       <c r="G33" s="27">
         <v>0.77</v>
       </c>
-      <c r="H33" s="221">
+      <c r="H33" s="219">
         <f>SUM(G33:G34)</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="I33" s="218">
+      <c r="I33" s="217">
         <v>3.39</v>
       </c>
-      <c r="J33" s="218">
+      <c r="J33" s="217">
         <f>SUM(H33:I34)</f>
         <v>5.6899999999999995</v>
       </c>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C34" s="217"/>
+      <c r="C34" s="218"/>
       <c r="D34" s="1" t="s">
         <v>76</v>
       </c>
@@ -3717,9 +3718,9 @@
       <c r="G34" s="27">
         <v>1.53</v>
       </c>
-      <c r="H34" s="222"/>
-      <c r="I34" s="218"/>
-      <c r="J34" s="218"/>
+      <c r="H34" s="220"/>
+      <c r="I34" s="217"/>
+      <c r="J34" s="217"/>
     </row>
     <row r="35" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="7"/>
@@ -3771,7 +3772,7 @@
       <c r="L37" s="35"/>
     </row>
     <row r="38" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C38" s="217">
+      <c r="C38" s="218">
         <v>42931</v>
       </c>
       <c r="D38" s="149" t="s">
@@ -3786,20 +3787,20 @@
       <c r="G38" s="27">
         <v>5.72</v>
       </c>
-      <c r="H38" s="218">
+      <c r="H38" s="217">
         <f>SUM(G38:G39)</f>
         <v>8.5500000000000007</v>
       </c>
-      <c r="I38" s="218">
+      <c r="I38" s="217">
         <v>4.99</v>
       </c>
-      <c r="J38" s="218">
+      <c r="J38" s="217">
         <f>SUM(H38:I39)</f>
         <v>13.540000000000001</v>
       </c>
     </row>
     <row r="39" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C39" s="217"/>
+      <c r="C39" s="218"/>
       <c r="D39" s="149" t="s">
         <v>122</v>
       </c>
@@ -3812,9 +3813,9 @@
       <c r="G39" s="27">
         <v>2.83</v>
       </c>
-      <c r="H39" s="218"/>
-      <c r="I39" s="218"/>
-      <c r="J39" s="218"/>
+      <c r="H39" s="217"/>
+      <c r="I39" s="217"/>
+      <c r="J39" s="217"/>
     </row>
     <row r="40" spans="3:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="7"/>
@@ -3828,7 +3829,7 @@
       <c r="L40" s="35"/>
     </row>
     <row r="41" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C41" s="217">
+      <c r="C41" s="218">
         <v>42936</v>
       </c>
       <c r="D41" s="149" t="s">
@@ -3843,20 +3844,20 @@
       <c r="G41" s="27">
         <v>10.58</v>
       </c>
-      <c r="H41" s="218">
+      <c r="H41" s="217">
         <f>SUM(G41:G45)</f>
         <v>18.649999999999999</v>
       </c>
-      <c r="I41" s="218">
+      <c r="I41" s="217">
         <v>0.25</v>
       </c>
-      <c r="J41" s="218">
+      <c r="J41" s="217">
         <f>H41+I41</f>
         <v>18.899999999999999</v>
       </c>
     </row>
     <row r="42" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C42" s="217"/>
+      <c r="C42" s="218"/>
       <c r="D42" s="149" t="s">
         <v>150</v>
       </c>
@@ -3869,12 +3870,12 @@
       <c r="G42" s="27">
         <v>3.86</v>
       </c>
-      <c r="H42" s="218"/>
-      <c r="I42" s="218"/>
-      <c r="J42" s="218"/>
+      <c r="H42" s="217"/>
+      <c r="I42" s="217"/>
+      <c r="J42" s="217"/>
     </row>
     <row r="43" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C43" s="217"/>
+      <c r="C43" s="218"/>
       <c r="D43" s="149" t="s">
         <v>151</v>
       </c>
@@ -3888,12 +3889,12 @@
         <f>1.99-0.1</f>
         <v>1.89</v>
       </c>
-      <c r="H43" s="218"/>
-      <c r="I43" s="218"/>
-      <c r="J43" s="218"/>
+      <c r="H43" s="217"/>
+      <c r="I43" s="217"/>
+      <c r="J43" s="217"/>
     </row>
     <row r="44" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C44" s="217"/>
+      <c r="C44" s="218"/>
       <c r="D44" s="149" t="s">
         <v>152</v>
       </c>
@@ -3907,12 +3908,12 @@
         <f>0.99-0.05</f>
         <v>0.94</v>
       </c>
-      <c r="H44" s="218"/>
-      <c r="I44" s="218"/>
-      <c r="J44" s="218"/>
+      <c r="H44" s="217"/>
+      <c r="I44" s="217"/>
+      <c r="J44" s="217"/>
     </row>
     <row r="45" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C45" s="217"/>
+      <c r="C45" s="218"/>
       <c r="D45" s="149" t="s">
         <v>153</v>
       </c>
@@ -3926,9 +3927,9 @@
         <f>1.45-0.07</f>
         <v>1.38</v>
       </c>
-      <c r="H45" s="218"/>
-      <c r="I45" s="218"/>
-      <c r="J45" s="218"/>
+      <c r="H45" s="217"/>
+      <c r="I45" s="217"/>
+      <c r="J45" s="217"/>
     </row>
     <row r="46" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="51"/>
@@ -4017,7 +4018,7 @@
       <c r="L50" s="57"/>
     </row>
     <row r="51" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C51" s="217">
+      <c r="C51" s="218">
         <v>42986</v>
       </c>
       <c r="D51" s="149" t="s">
@@ -4032,20 +4033,20 @@
       <c r="G51" s="27">
         <v>29.95</v>
       </c>
-      <c r="H51" s="218">
+      <c r="H51" s="217">
         <f>G51+G52+G53+2.13</f>
         <v>34.380000000000003</v>
       </c>
-      <c r="I51" s="218">
+      <c r="I51" s="217">
         <v>3.03</v>
       </c>
-      <c r="J51" s="218">
+      <c r="J51" s="217">
         <f>H51+I51</f>
         <v>37.410000000000004</v>
       </c>
     </row>
     <row r="52" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C52" s="217"/>
+      <c r="C52" s="218"/>
       <c r="D52" s="149" t="s">
         <v>222</v>
       </c>
@@ -4058,12 +4059,12 @@
       <c r="G52" s="27">
         <v>0.77</v>
       </c>
-      <c r="H52" s="218"/>
-      <c r="I52" s="218"/>
-      <c r="J52" s="218"/>
+      <c r="H52" s="217"/>
+      <c r="I52" s="217"/>
+      <c r="J52" s="217"/>
     </row>
     <row r="53" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C53" s="217"/>
+      <c r="C53" s="218"/>
       <c r="D53" s="149" t="s">
         <v>223</v>
       </c>
@@ -4076,9 +4077,9 @@
       <c r="G53" s="27">
         <v>1.53</v>
       </c>
-      <c r="H53" s="218"/>
-      <c r="I53" s="218"/>
-      <c r="J53" s="218"/>
+      <c r="H53" s="217"/>
+      <c r="I53" s="217"/>
+      <c r="J53" s="217"/>
     </row>
     <row r="54" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="51"/>
@@ -4241,7 +4242,7 @@
       <c r="L62" s="57"/>
     </row>
     <row r="63" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C63" s="217">
+      <c r="C63" s="218">
         <v>43027</v>
       </c>
       <c r="D63" s="149" t="s">
@@ -4256,20 +4257,20 @@
       <c r="G63" s="27">
         <v>2.66</v>
       </c>
-      <c r="H63" s="218">
+      <c r="H63" s="217">
         <f>SUM(G63:G66)</f>
         <v>10.18</v>
       </c>
-      <c r="I63" s="218">
+      <c r="I63" s="217">
         <v>3.75</v>
       </c>
-      <c r="J63" s="218">
+      <c r="J63" s="217">
         <f>H63+I63</f>
         <v>13.93</v>
       </c>
     </row>
     <row r="64" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C64" s="217"/>
+      <c r="C64" s="218"/>
       <c r="D64" s="149" t="s">
         <v>234</v>
       </c>
@@ -4282,12 +4283,12 @@
       <c r="G64" s="27">
         <v>1.53</v>
       </c>
-      <c r="H64" s="218"/>
-      <c r="I64" s="218"/>
-      <c r="J64" s="218"/>
-    </row>
-    <row r="65" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C65" s="217"/>
+      <c r="H64" s="217"/>
+      <c r="I64" s="217"/>
+      <c r="J64" s="217"/>
+    </row>
+    <row r="65" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C65" s="218"/>
       <c r="D65" s="149" t="s">
         <v>222</v>
       </c>
@@ -4300,12 +4301,12 @@
       <c r="G65" s="27">
         <v>0.77</v>
       </c>
-      <c r="H65" s="218"/>
-      <c r="I65" s="218"/>
-      <c r="J65" s="218"/>
-    </row>
-    <row r="66" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C66" s="217"/>
+      <c r="H65" s="217"/>
+      <c r="I65" s="217"/>
+      <c r="J65" s="217"/>
+    </row>
+    <row r="66" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C66" s="218"/>
       <c r="D66" s="149" t="s">
         <v>235</v>
       </c>
@@ -4318,11 +4319,11 @@
       <c r="G66" s="27">
         <v>5.22</v>
       </c>
-      <c r="H66" s="218"/>
-      <c r="I66" s="218"/>
-      <c r="J66" s="218"/>
-    </row>
-    <row r="67" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H66" s="217"/>
+      <c r="I66" s="217"/>
+      <c r="J66" s="217"/>
+    </row>
+    <row r="67" spans="3:14" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C67" s="51"/>
       <c r="D67" s="52"/>
       <c r="E67" s="53"/>
@@ -4333,7 +4334,7 @@
       <c r="J67" s="158"/>
       <c r="L67" s="57"/>
     </row>
-    <row r="68" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C68" s="213">
         <v>43036</v>
       </c>
@@ -4360,7 +4361,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="69" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:14" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C69" s="51"/>
       <c r="D69" s="52"/>
       <c r="E69" s="53"/>
@@ -4371,8 +4372,8 @@
       <c r="J69" s="158"/>
       <c r="L69" s="57"/>
     </row>
-    <row r="70" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C70" s="217">
+    <row r="70" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C70" s="218">
         <v>43040</v>
       </c>
       <c r="D70" s="149" t="s">
@@ -4387,14 +4388,14 @@
       <c r="G70" s="27">
         <v>0.4</v>
       </c>
-      <c r="H70" s="218">
+      <c r="H70" s="217">
         <f>SUM(G70:G76)</f>
         <v>3.5799999999999996</v>
       </c>
-      <c r="I70" s="218">
+      <c r="I70" s="217">
         <v>3.39</v>
       </c>
-      <c r="J70" s="219">
+      <c r="J70" s="222">
         <f>H70+I70+K71</f>
         <v>7.2206000000000001</v>
       </c>
@@ -4402,8 +4403,8 @@
         <v>244</v>
       </c>
     </row>
-    <row r="71" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C71" s="217"/>
+    <row r="71" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C71" s="218"/>
       <c r="D71" s="149" t="s">
         <v>237</v>
       </c>
@@ -4416,17 +4417,17 @@
       <c r="G71" s="27">
         <v>0.9</v>
       </c>
-      <c r="H71" s="218"/>
-      <c r="I71" s="218"/>
-      <c r="J71" s="219"/>
+      <c r="H71" s="217"/>
+      <c r="I71" s="217"/>
+      <c r="J71" s="222"/>
       <c r="K71" s="214">
         <f>SUM(G70:G76)*0.07</f>
         <v>0.25059999999999999</v>
       </c>
       <c r="L71" s="215"/>
     </row>
-    <row r="72" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C72" s="217"/>
+    <row r="72" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C72" s="218"/>
       <c r="D72" s="149" t="s">
         <v>238</v>
       </c>
@@ -4439,12 +4440,12 @@
       <c r="G72" s="27">
         <v>0.64</v>
       </c>
-      <c r="H72" s="218"/>
-      <c r="I72" s="218"/>
-      <c r="J72" s="219"/>
-    </row>
-    <row r="73" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C73" s="217"/>
+      <c r="H72" s="217"/>
+      <c r="I72" s="217"/>
+      <c r="J72" s="222"/>
+    </row>
+    <row r="73" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C73" s="218"/>
       <c r="D73" s="149" t="s">
         <v>239</v>
       </c>
@@ -4457,12 +4458,12 @@
       <c r="G73" s="27">
         <v>0.4</v>
       </c>
-      <c r="H73" s="218"/>
-      <c r="I73" s="218"/>
-      <c r="J73" s="219"/>
-    </row>
-    <row r="74" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C74" s="217"/>
+      <c r="H73" s="217"/>
+      <c r="I73" s="217"/>
+      <c r="J73" s="222"/>
+    </row>
+    <row r="74" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C74" s="218"/>
       <c r="D74" s="149" t="s">
         <v>240</v>
       </c>
@@ -4475,12 +4476,12 @@
       <c r="G74" s="27">
         <v>0.32</v>
       </c>
-      <c r="H74" s="218"/>
-      <c r="I74" s="218"/>
-      <c r="J74" s="219"/>
-    </row>
-    <row r="75" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C75" s="217"/>
+      <c r="H74" s="217"/>
+      <c r="I74" s="217"/>
+      <c r="J74" s="222"/>
+    </row>
+    <row r="75" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C75" s="218"/>
       <c r="D75" s="149" t="s">
         <v>241</v>
       </c>
@@ -4493,12 +4494,13 @@
       <c r="G75" s="27">
         <v>0.46</v>
       </c>
-      <c r="H75" s="218"/>
-      <c r="I75" s="218"/>
-      <c r="J75" s="219"/>
-    </row>
-    <row r="76" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C76" s="217"/>
+      <c r="H75" s="217"/>
+      <c r="I75" s="217"/>
+      <c r="J75" s="222"/>
+      <c r="N75" s="228"/>
+    </row>
+    <row r="76" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C76" s="218"/>
       <c r="D76" s="149" t="s">
         <v>242</v>
       </c>
@@ -4511,11 +4513,11 @@
       <c r="G76" s="27">
         <v>0.46</v>
       </c>
-      <c r="H76" s="218"/>
-      <c r="I76" s="218"/>
-      <c r="J76" s="219"/>
-    </row>
-    <row r="77" spans="3:12" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H76" s="217"/>
+      <c r="I76" s="217"/>
+      <c r="J76" s="222"/>
+    </row>
+    <row r="77" spans="3:14" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C77" s="51"/>
       <c r="D77" s="52"/>
       <c r="E77" s="53"/>
@@ -4526,8 +4528,8 @@
       <c r="J77" s="216"/>
       <c r="L77" s="57"/>
     </row>
-    <row r="78" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C78" s="217">
+    <row r="78" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C78" s="218">
         <v>43045</v>
       </c>
       <c r="D78" s="149" t="s">
@@ -4542,14 +4544,14 @@
       <c r="G78" s="27">
         <v>0.1</v>
       </c>
-      <c r="H78" s="218">
+      <c r="H78" s="217">
         <f>SUM(G78:G86)</f>
         <v>4.1500000000000004</v>
       </c>
-      <c r="I78" s="218">
+      <c r="I78" s="217">
         <v>3.93</v>
       </c>
-      <c r="J78" s="219">
+      <c r="J78" s="222">
         <f>H78+I78+K79</f>
         <v>8.3497500000000002</v>
       </c>
@@ -4557,8 +4559,8 @@
         <v>244</v>
       </c>
     </row>
-    <row r="79" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C79" s="217"/>
+    <row r="79" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C79" s="218"/>
       <c r="D79" s="149" t="s">
         <v>246</v>
       </c>
@@ -4571,16 +4573,16 @@
       <c r="G79" s="27">
         <v>0.4</v>
       </c>
-      <c r="H79" s="218"/>
-      <c r="I79" s="218"/>
-      <c r="J79" s="219"/>
+      <c r="H79" s="217"/>
+      <c r="I79" s="217"/>
+      <c r="J79" s="222"/>
       <c r="K79" s="214">
         <f>SUM(G78:G86)*0.065</f>
         <v>0.26975000000000005</v>
       </c>
     </row>
-    <row r="80" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C80" s="217"/>
+    <row r="80" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C80" s="218"/>
       <c r="D80" s="149" t="s">
         <v>247</v>
       </c>
@@ -4593,12 +4595,12 @@
       <c r="G80" s="27">
         <v>0.4</v>
       </c>
-      <c r="H80" s="218"/>
-      <c r="I80" s="218"/>
-      <c r="J80" s="219"/>
+      <c r="H80" s="217"/>
+      <c r="I80" s="217"/>
+      <c r="J80" s="222"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C81" s="217"/>
+      <c r="C81" s="218"/>
       <c r="D81" s="149" t="s">
         <v>248</v>
       </c>
@@ -4611,12 +4613,12 @@
       <c r="G81" s="27">
         <v>0.4</v>
       </c>
-      <c r="H81" s="218"/>
-      <c r="I81" s="218"/>
-      <c r="J81" s="219"/>
+      <c r="H81" s="217"/>
+      <c r="I81" s="217"/>
+      <c r="J81" s="222"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C82" s="217"/>
+      <c r="C82" s="218"/>
       <c r="D82" s="149" t="s">
         <v>249</v>
       </c>
@@ -4629,12 +4631,12 @@
       <c r="G82" s="27">
         <v>0.63</v>
       </c>
-      <c r="H82" s="218"/>
-      <c r="I82" s="218"/>
-      <c r="J82" s="219"/>
+      <c r="H82" s="217"/>
+      <c r="I82" s="217"/>
+      <c r="J82" s="222"/>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C83" s="217"/>
+      <c r="C83" s="218"/>
       <c r="D83" s="149" t="s">
         <v>250</v>
       </c>
@@ -4647,12 +4649,12 @@
       <c r="G83" s="27">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H83" s="218"/>
-      <c r="I83" s="218"/>
-      <c r="J83" s="219"/>
+      <c r="H83" s="217"/>
+      <c r="I83" s="217"/>
+      <c r="J83" s="222"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C84" s="217"/>
+      <c r="C84" s="218"/>
       <c r="D84" s="149" t="s">
         <v>251</v>
       </c>
@@ -4665,12 +4667,12 @@
       <c r="G84" s="27">
         <v>0.86</v>
       </c>
-      <c r="H84" s="218"/>
-      <c r="I84" s="218"/>
-      <c r="J84" s="219"/>
+      <c r="H84" s="217"/>
+      <c r="I84" s="217"/>
+      <c r="J84" s="222"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C85" s="217"/>
+      <c r="C85" s="218"/>
       <c r="D85" s="149" t="s">
         <v>252</v>
       </c>
@@ -4683,12 +4685,12 @@
       <c r="G85" s="27">
         <v>0.61</v>
       </c>
-      <c r="H85" s="218"/>
-      <c r="I85" s="218"/>
-      <c r="J85" s="219"/>
+      <c r="H85" s="217"/>
+      <c r="I85" s="217"/>
+      <c r="J85" s="222"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C86" s="217"/>
+      <c r="C86" s="218"/>
       <c r="D86" s="149" t="s">
         <v>253</v>
       </c>
@@ -4701,9 +4703,9 @@
       <c r="G86" s="27">
         <v>0.2</v>
       </c>
-      <c r="H86" s="218"/>
-      <c r="I86" s="218"/>
-      <c r="J86" s="219"/>
+      <c r="H86" s="217"/>
+      <c r="I86" s="217"/>
+      <c r="J86" s="222"/>
     </row>
     <row r="87" spans="1:15" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C87" s="7"/>
@@ -4722,7 +4724,7 @@
       </c>
       <c r="C88" s="41">
         <f ca="1">TODAY()</f>
-        <v>43057</v>
+        <v>43062</v>
       </c>
       <c r="E88" s="29"/>
       <c r="F88" s="29"/>
@@ -4740,7 +4742,7 @@
       </c>
       <c r="L88" s="39">
         <f ca="1">(C88-C4)*0.0328767</f>
-        <v>5.7534225000000001</v>
+        <v>5.9178060000000006</v>
       </c>
       <c r="M88" s="24" t="s">
         <v>25</v>
@@ -4758,7 +4760,7 @@
       </c>
       <c r="J89" s="22">
         <f ca="1">J88/L88</f>
-        <v>53.651604762208926</v>
+        <v>52.161282407703119</v>
       </c>
       <c r="K89" s="32" t="s">
         <v>27</v>
@@ -6191,19 +6193,27 @@
     <sortCondition ref="C4:C19"/>
   </sortState>
   <mergeCells count="50">
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="C4:C10"/>
-    <mergeCell ref="J4:J10"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="H4:H10"/>
-    <mergeCell ref="I4:I10"/>
-    <mergeCell ref="J21:J25"/>
-    <mergeCell ref="H21:H25"/>
-    <mergeCell ref="H27:H29"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="I21:I25"/>
-    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="C78:C86"/>
+    <mergeCell ref="H78:H86"/>
+    <mergeCell ref="I78:I86"/>
+    <mergeCell ref="J78:J86"/>
+    <mergeCell ref="C70:C76"/>
+    <mergeCell ref="H70:H76"/>
+    <mergeCell ref="I70:I76"/>
+    <mergeCell ref="J70:J76"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="H63:H66"/>
+    <mergeCell ref="I63:I66"/>
+    <mergeCell ref="J63:J66"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="H51:H53"/>
+    <mergeCell ref="I51:I53"/>
+    <mergeCell ref="J51:J53"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
     <mergeCell ref="C41:C45"/>
     <mergeCell ref="H41:H45"/>
     <mergeCell ref="I41:I45"/>
@@ -6220,27 +6230,19 @@
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="H38:H39"/>
     <mergeCell ref="I38:I39"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="H63:H66"/>
-    <mergeCell ref="I63:I66"/>
-    <mergeCell ref="J63:J66"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="H51:H53"/>
-    <mergeCell ref="I51:I53"/>
-    <mergeCell ref="J51:J53"/>
-    <mergeCell ref="C78:C86"/>
-    <mergeCell ref="H78:H86"/>
-    <mergeCell ref="I78:I86"/>
-    <mergeCell ref="J78:J86"/>
-    <mergeCell ref="C70:C76"/>
-    <mergeCell ref="H70:H76"/>
-    <mergeCell ref="I70:I76"/>
-    <mergeCell ref="J70:J76"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="C4:C10"/>
+    <mergeCell ref="J4:J10"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="H4:H10"/>
+    <mergeCell ref="I4:I10"/>
+    <mergeCell ref="J21:J25"/>
+    <mergeCell ref="H21:H25"/>
+    <mergeCell ref="H27:H29"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="I21:I25"/>
+    <mergeCell ref="H16:H17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7154,15 +7156,15 @@
       <c r="AO16" s="223"/>
       <c r="AP16" s="223"/>
       <c r="AQ16" s="223"/>
-      <c r="AT16" s="222" t="s">
+      <c r="AT16" s="220" t="s">
         <v>119</v>
       </c>
-      <c r="AU16" s="222"/>
-      <c r="AV16" s="222"/>
-      <c r="AW16" s="222"/>
-      <c r="AX16" s="222"/>
-      <c r="AY16" s="222"/>
-      <c r="AZ16" s="222"/>
+      <c r="AU16" s="220"/>
+      <c r="AV16" s="220"/>
+      <c r="AW16" s="220"/>
+      <c r="AX16" s="220"/>
+      <c r="AY16" s="220"/>
+      <c r="AZ16" s="220"/>
     </row>
     <row r="17" spans="25:59" x14ac:dyDescent="0.25">
       <c r="Y17" s="108" t="s">
@@ -7177,11 +7179,11 @@
       <c r="AB17" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="AJ17" s="222" t="s">
+      <c r="AJ17" s="220" t="s">
         <v>117</v>
       </c>
-      <c r="AK17" s="222"/>
-      <c r="AL17" s="222"/>
+      <c r="AK17" s="220"/>
+      <c r="AL17" s="220"/>
       <c r="AN17" s="223"/>
       <c r="AO17" s="223"/>
       <c r="AP17" s="223"/>

</xml_diff>